<commit_message>
get schedule structure fixed w/o css
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -47,16 +47,27 @@
     <t>Finals Week</t>
   </si>
   <si>
-    <t>Topics</t>
-  </si>
-  <si>
     <t>Thanksgiving Break</t>
   </si>
   <si>
-    <t>Preparation</t>
+    <t>HW * Exam</t>
   </si>
   <si>
-    <t>Evaluation</t>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>prep</t>
+  </si>
+  <si>
+    <t>eval</t>
+  </si>
+  <si>
+    <t>This is a test 
+* This is just a test</t>
+  </si>
+  <si>
+    <t>Do this * 
+and this</t>
   </si>
 </sst>
 </file>
@@ -876,7 +887,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -904,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H1" s="40" t="s">
         <v>5</v>
@@ -923,7 +934,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -934,7 +945,16 @@
         <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E2" s="31"/>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="H2" s="31"/>
       <c r="I2" s="5"/>
     </row>
@@ -1389,7 +1409,7 @@
         <v>Tue</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="57"/>
       <c r="F28" s="58"/>

</xml_diff>

<commit_message>
minor mod to schedule template
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="7240" yWindow="240" windowWidth="18360" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -73,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -283,7 +278,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -460,24 +455,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -884,27 +861,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2"/>
-    <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" style="5" customWidth="1"/>
     <col min="5" max="5" width="26" style="24" customWidth="1"/>
     <col min="6" max="6" width="35.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" style="10" customWidth="1"/>
     <col min="8" max="8" width="39.5" style="24" customWidth="1"/>
-    <col min="9" max="9" width="31.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.875" style="2"/>
+    <col min="9" max="9" width="31.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1">
       <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
@@ -934,7 +911,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="31.5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -958,7 +935,7 @@
       <c r="H2" s="31"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="6"/>
       <c r="B3" s="7">
         <f>B2+2</f>
@@ -970,13 +947,13 @@
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="32"/>
-      <c r="F3" s="66"/>
+      <c r="F3" s="60"/>
       <c r="G3" s="14"/>
       <c r="H3" s="32"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
         <f>A2+1</f>
         <v>2</v>
@@ -993,7 +970,7 @@
       <c r="H4" s="31"/>
       <c r="I4" s="29"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="6"/>
       <c r="B5" s="7">
         <f>B4+2</f>
@@ -1005,12 +982,12 @@
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="32"/>
-      <c r="F5" s="66"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="14"/>
       <c r="H5" s="35"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2">
         <f>A4+1</f>
         <v>3</v>
@@ -1027,7 +1004,7 @@
       <c r="H6" s="31"/>
       <c r="I6" s="28"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="6"/>
       <c r="B7" s="7">
         <f>B6+2</f>
@@ -1044,7 +1021,7 @@
       <c r="H7" s="37"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A26" si="1">A6+1</f>
         <v>4</v>
@@ -1063,7 +1040,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="16.5" thickBot="1">
       <c r="A9" s="16"/>
       <c r="B9" s="17">
         <f>B8+2</f>
@@ -1081,7 +1058,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="29"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="11">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1096,12 +1073,12 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="41"/>
-      <c r="F10" s="67"/>
+      <c r="F10" s="61"/>
       <c r="G10" s="15"/>
       <c r="H10" s="45"/>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="6"/>
       <c r="B11" s="7">
         <f>B10+2</f>
@@ -1118,7 +1095,7 @@
       <c r="H11" s="35"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1135,7 +1112,7 @@
       <c r="E12" s="34"/>
       <c r="H12" s="31"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="6"/>
       <c r="B13" s="7">
         <f>B12+2</f>
@@ -1152,7 +1129,7 @@
       <c r="H13" s="32"/>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1167,10 +1144,10 @@
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="34"/>
-      <c r="F14" s="67"/>
+      <c r="F14" s="61"/>
       <c r="H14" s="31"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="6"/>
       <c r="B15" s="7">
         <f>B14+2</f>
@@ -1187,7 +1164,7 @@
       <c r="H15" s="32"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="2">
         <v>8</v>
       </c>
@@ -1201,10 +1178,10 @@
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="34"/>
-      <c r="F16" s="67"/>
+      <c r="F16" s="61"/>
       <c r="H16" s="31"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="6"/>
       <c r="B17" s="7">
         <f>B16+2</f>
@@ -1221,7 +1198,7 @@
       <c r="H17" s="32"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1237,7 +1214,7 @@
       <c r="E18" s="31"/>
       <c r="H18" s="31"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="6"/>
       <c r="B19" s="7">
         <f>B18+2</f>
@@ -1255,7 +1232,7 @@
       <c r="I19" s="42"/>
       <c r="J19" s="29"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="46">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1275,7 +1252,7 @@
       <c r="H20" s="50"/>
       <c r="I20" s="51"/>
     </row>
-    <row r="21" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="16.5" thickBot="1">
       <c r="A21" s="16"/>
       <c r="B21" s="17">
         <f>B20+2</f>
@@ -1292,7 +1269,7 @@
       <c r="H21" s="33"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1307,10 +1284,10 @@
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="34"/>
-      <c r="F22" s="68"/>
+      <c r="F22" s="62"/>
       <c r="H22" s="31"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="6"/>
       <c r="B23" s="7">
         <f>B22+2</f>
@@ -1327,7 +1304,7 @@
       <c r="H23" s="32"/>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="11">
         <f>A22+1</f>
         <v>12</v>
@@ -1346,7 +1323,7 @@
       <c r="H24" s="41"/>
       <c r="I24" s="15"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="6"/>
       <c r="B25" s="7">
         <f>B24+2</f>
@@ -1363,7 +1340,7 @@
       <c r="H25" s="32"/>
       <c r="I25" s="14"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1381,14 +1358,14 @@
       <c r="F26" s="15"/>
       <c r="H26" s="31"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="6"/>
       <c r="B27" s="7">
         <f>B26+2</f>
         <v>41593</v>
       </c>
       <c r="C27" s="8" t="str">
-        <f t="shared" ref="C27:C34" si="3">TEXT(WEEKDAY(B27,1)+1, "ddd")</f>
+        <f t="shared" ref="C27:C33" si="3">TEXT(WEEKDAY(B27,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
       <c r="D27" s="21"/>
@@ -1398,7 +1375,7 @@
       <c r="H27" s="35"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="54"/>
       <c r="B28" s="55">
         <f>B26+7</f>
@@ -1418,109 +1395,91 @@
       <c r="I28" s="58"/>
       <c r="J28" s="53"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="60"/>
-      <c r="B29" s="61">
-        <f>B28+2</f>
-        <v>41600</v>
-      </c>
-      <c r="C29" s="62" t="str">
+    <row r="29" spans="1:10">
+      <c r="A29" s="2">
+        <v>14</v>
+      </c>
+      <c r="B29" s="3">
+        <f>B28+7</f>
+        <v>41605</v>
+      </c>
+      <c r="C29" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Tue</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="38"/>
+      <c r="H29" s="41"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7">
+        <f>B29+2</f>
+        <v>41607</v>
+      </c>
+      <c r="C30" s="8" t="str">
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="53"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>14</v>
-      </c>
-      <c r="B30" s="3">
-        <f>B28+7</f>
-        <v>41605</v>
-      </c>
-      <c r="C30" s="4" t="str">
+      <c r="D30" s="21"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="53"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="11">
+        <f>A29+1</f>
+        <v>15</v>
+      </c>
+      <c r="B31" s="3">
+        <f>B29+7</f>
+        <v>41612</v>
+      </c>
+      <c r="C31" s="12" t="str">
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="38"/>
-      <c r="H30" s="41"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7">
-        <f>B30+2</f>
-        <v>41607</v>
-      </c>
-      <c r="C31" s="8" t="str">
+      <c r="E31" s="31"/>
+      <c r="F31" s="15"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="53"/>
+    </row>
+    <row r="32" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A32" s="16"/>
+      <c r="B32" s="17">
+        <f>B31+2</f>
+        <v>41614</v>
+      </c>
+      <c r="C32" s="18" t="str">
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="53"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
-        <f>A30+1</f>
-        <v>15</v>
-      </c>
-      <c r="B32" s="3">
-        <f>B30+7</f>
-        <v>41612</v>
-      </c>
-      <c r="C32" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>Tue</v>
-      </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="15"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="15"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="53"/>
     </row>
-    <row r="33" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="17">
-        <f>B32+2</f>
-        <v>41614</v>
-      </c>
-      <c r="C33" s="18" t="str">
-        <f t="shared" si="3"/>
-        <v>Thu</v>
-      </c>
-      <c r="D33" s="43"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="53"/>
-    </row>
-    <row r="34" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="33" spans="1:8" ht="31.5">
+      <c r="A33" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B33" s="3">
         <v>41625</v>
       </c>
-      <c r="C34" s="4" t="str">
+      <c r="C33" s="4" t="str">
         <f t="shared" si="3"/>
         <v>Mon</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="15"/>
-      <c r="H34" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="15"/>
+      <c r="H33" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
change schedule to use gsub
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="240" windowWidth="18360" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Day</t>
-  </si>
-  <si>
-    <t>Wk</t>
   </si>
   <si>
     <t>Subject</t>
@@ -63,6 +60,12 @@
   <si>
     <t>Do this * 
 and this</t>
+  </si>
+  <si>
+    <t>A*B*C*D</t>
+  </si>
+  <si>
+    <t>Week</t>
   </si>
 </sst>
 </file>
@@ -863,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -881,9 +884,9 @@
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1">
+    <row r="1" spans="1:10" ht="19" thickBot="1">
       <c r="A1" s="25" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>0</v>
@@ -892,26 +895,26 @@
         <v>2</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="40" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>5</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="31.5">
+    <row r="2" spans="1:10" ht="30">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -923,14 +926,14 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="31"/>
       <c r="I2" s="5"/>
@@ -1040,7 +1043,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="45"/>
     </row>
-    <row r="9" spans="1:10" ht="16.5" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="16"/>
       <c r="B9" s="17">
         <f>B8+2</f>
@@ -1252,7 +1255,7 @@
       <c r="H20" s="50"/>
       <c r="I20" s="51"/>
     </row>
-    <row r="21" spans="1:10" ht="16.5" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="16"/>
       <c r="B21" s="17">
         <f>B20+2</f>
@@ -1386,7 +1389,7 @@
         <v>Tue</v>
       </c>
       <c r="D28" s="57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" s="57"/>
       <c r="F28" s="58"/>
@@ -1448,7 +1451,7 @@
       <c r="I31" s="15"/>
       <c r="J31" s="53"/>
     </row>
-    <row r="32" spans="1:10" ht="16.5" thickBot="1">
+    <row r="32" spans="1:10" ht="16" thickBot="1">
       <c r="A32" s="16"/>
       <c r="B32" s="17">
         <f>B31+2</f>
@@ -1466,9 +1469,9 @@
       <c r="I32" s="20"/>
       <c r="J32" s="53"/>
     </row>
-    <row r="33" spans="1:8" ht="31.5">
+    <row r="33" spans="1:8" ht="30">
       <c r="A33" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="3">
         <v>41625</v>
@@ -1476,6 +1479,9 @@
       <c r="C33" s="4" t="str">
         <f t="shared" si="3"/>
         <v>Mon</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="15"/>

</xml_diff>

<commit_message>
add week 1 and 2
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -47,27 +44,74 @@
     <t>Thanksgiving Break</t>
   </si>
   <si>
-    <t>HW * Exam</t>
-  </si>
-  <si>
     <t>topic</t>
   </si>
   <si>
     <t>eval</t>
   </si>
   <si>
-    <t>This is a test 
-* This is just a test</t>
-  </si>
-  <si>
-    <t>Do this * 
-and this</t>
-  </si>
-  <si>
     <t>A*B*C*D</t>
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t>Overview of the class
+* Software programs
+* Reproducibility</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 1 overview](wk01.html) 
+* [Lec01: Intro to the class](docs/lec01_intro_class.html)
+* [PMA5 Ch 2 &amp; 3](docs/PMA5 Ch 2 and 3.pdf) </t>
+  </si>
+  <si>
+    <t>[Week 2 overview](wk02.html)
+* [Lec02: Data Prep](docs/lec02_data_prep.html)</t>
+  </si>
+  <si>
+    <t>* Create a BBL Blog - Intro/Bio, RR plan (Due 8/28)
+* PMA5 2.2, 2.7 (Due 8/24)
+* Setup laptop for analysis (Due 8/24)</t>
+  </si>
+  <si>
+    <t>Codebooks
+* Data Types
+* Importing Data
+* Choosing research area</t>
+  </si>
+  <si>
+    <t>Read PMA5 CH 3
+* Pick AddHlth sections. Blog your choices.  (Due 8/28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Cleaning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 3 overview](wk03.html)
+* [Lec03: Data Screening](docs/lec03_data_screen.html)
+* [PMA6 Data Viz ch DRAFT](docs/pma6_ch4_draft.pdf)
+* [R Data Viz overview](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
+</t>
+  </si>
+  <si>
+    <t>* Graph 5 vars from Add Health. Blog about it. (Due 9/11)</t>
+  </si>
+  <si>
+    <t>Explore Add Health variables. Blog about choices and potential problems.  (Due 9/4)
+* Start your own Add Health codebook
+* Start your own Add Health data management file</t>
+  </si>
+  <si>
+    <t>* Turn in codebook and DM file (Due 9/4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Screening
+* Univariate Data Visualizations
+</t>
   </si>
 </sst>
 </file>
@@ -159,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +222,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -223,6 +279,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -283,7 +361,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -324,12 +402,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -342,9 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -362,9 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -429,9 +495,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -450,20 +513,74 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -862,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -871,144 +988,168 @@
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" style="2"/>
     <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" style="5" customWidth="1"/>
-    <col min="5" max="5" width="26" style="24" customWidth="1"/>
-    <col min="6" max="6" width="35.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="39.5" style="24" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="21" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="61.125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="27.125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="39.5" style="21" customWidth="1"/>
     <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="58">
         <v>41507</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C2" s="59" t="str">
         <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="30"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E2" s="61"/>
+      <c r="F2" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="7">
+      <c r="B3" s="54">
         <f>B2+2</f>
         <v>41509</v>
       </c>
-      <c r="C3" s="8" t="str">
+      <c r="C3" s="55" t="str">
         <f>TEXT(WEEKDAY(B3,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="31"/>
+      <c r="D3" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="57"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="57"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="64">
         <f>B2+7</f>
         <v>41514</v>
       </c>
-      <c r="C4" s="4" t="str">
+      <c r="C4" s="65" t="str">
         <f>TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="67"/>
+    </row>
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="7">
+      <c r="B5" s="69">
         <f>B4+2</f>
         <v>41516</v>
       </c>
-      <c r="C5" s="8" t="str">
+      <c r="C5" s="70" t="str">
         <f>TEXT(WEEKDAY(B5,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="73"/>
+    </row>
+    <row r="6" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>A4+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="64">
         <f>B4+7</f>
         <v>41521</v>
       </c>
-      <c r="C6" s="4" t="str">
+      <c r="C6" s="65" t="str">
         <f t="shared" ref="C6:C24" si="0">TEXT(WEEKDAY(B6,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="D6" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="67"/>
+      <c r="F6" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="7">
+      <c r="B7" s="69">
         <f>B6+2</f>
         <v>41523</v>
       </c>
-      <c r="C7" s="8" t="str">
+      <c r="C7" s="70" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="36"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1024,34 +1165,34 @@
         <v>Tue</v>
       </c>
       <c r="D8" s="13"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="43"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="39"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15">
         <f>B8+2</f>
         <v>41530</v>
       </c>
-      <c r="C9" s="18" t="str">
+      <c r="C9" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="28"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="38">
         <f>B8+7</f>
         <v>41535</v>
       </c>
@@ -1060,10 +1201,10 @@
         <v>Tue</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="43"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
@@ -1076,10 +1217,10 @@
         <v>Thu</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="34"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1094,9 +1235,9 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="33"/>
-      <c r="H12" s="30"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="29"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -1108,11 +1249,11 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="31"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1127,10 +1268,10 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="59"/>
-      <c r="H14" s="30"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="20"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -1142,11 +1283,11 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="31"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1160,10 +1301,10 @@
         <f t="shared" ref="C16:C17" si="2">TEXT(WEEKDAY(B16,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="59"/>
-      <c r="H16" s="30"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="20"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
@@ -1175,11 +1316,11 @@
         <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="31"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -1194,8 +1335,8 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="H18" s="30"/>
+      <c r="E18" s="26"/>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -1208,46 +1349,46 @@
         <v>Thu</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="28"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="44">
+      <c r="A20" s="40">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B20" s="45">
+      <c r="B20" s="41">
         <f>B18+7</f>
         <v>41570</v>
       </c>
-      <c r="C20" s="46" t="str">
+      <c r="C20" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="48"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="44"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15">
         <f>B20+2</f>
         <v>41572</v>
       </c>
-      <c r="C21" s="18" t="str">
+      <c r="C21" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="32"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
@@ -1262,10 +1403,10 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="60"/>
-      <c r="H22" s="30"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="52"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
@@ -1277,18 +1418,18 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="31"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="27"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <f>A22+1</f>
         <v>12</v>
       </c>
-      <c r="B24" s="42">
+      <c r="B24" s="38">
         <f>B22+7</f>
         <v>41584</v>
       </c>
@@ -1296,10 +1437,10 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="35"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="40"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="31"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="36"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
@@ -1311,11 +1452,11 @@
         <f>TEXT(WEEKDAY(B25,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="31"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -1330,10 +1471,10 @@
         <f>TEXT(WEEKDAY(B26,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="15"/>
-      <c r="H26" s="30"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="13"/>
+      <c r="H26" s="26"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
@@ -1345,30 +1486,30 @@
         <f t="shared" ref="C27:C33" si="3">TEXT(WEEKDAY(B27,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="34"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="53">
+      <c r="A28" s="47"/>
+      <c r="B28" s="48">
         <f>B26+7</f>
         <v>41598</v>
       </c>
-      <c r="C28" s="54" t="str">
+      <c r="C28" s="49" t="str">
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="D28" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="55"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="51"/>
+      <c r="D28" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="50"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="46"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -1382,9 +1523,9 @@
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="37"/>
-      <c r="H29" s="40"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="33"/>
+      <c r="H29" s="36"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
@@ -1396,12 +1537,12 @@
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="51"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
@@ -1416,31 +1557,31 @@
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="15"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="51"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="13"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="46"/>
     </row>
     <row r="32" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15">
         <f>B31+2</f>
         <v>41614</v>
       </c>
-      <c r="C32" s="18" t="str">
+      <c r="C32" s="16" t="str">
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="51"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="46"/>
     </row>
     <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="3">
         <v>41625</v>
@@ -1450,11 +1591,11 @@
         <v>Mon</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="15"/>
-      <c r="H33" s="30"/>
+        <v>8</v>
+      </c>
+      <c r="E33" s="26"/>
+      <c r="F33" s="13"/>
+      <c r="H33" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
reoconfig week 02 and 03
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -35,9 +35,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Corresponding Assignments</t>
-  </si>
-  <si>
     <t>Finals Week</t>
   </si>
   <si>
@@ -71,21 +68,12 @@
   <si>
     <t>[Week 2 overview](wk02.html)
 * [Lec02: Data Prep](docs/lec02_data_prep.html)</t>
-  </si>
-  <si>
-    <t>* Create a BBL Blog - Intro/Bio, RR plan (Due 8/28)
-* PMA5 2.2, 2.7 (Due 8/24)
-* Setup laptop for analysis (Due 8/24)</t>
   </si>
   <si>
     <t>Codebooks
 * Data Types
 * Importing Data
 * Choosing research area</t>
-  </si>
-  <si>
-    <t>Read PMA5 CH 3
-* Pick AddHlth sections. Blog your choices.  (Due 8/28)</t>
   </si>
   <si>
     <t xml:space="preserve">Data Cleaning </t>
@@ -98,20 +86,31 @@
 </t>
   </si>
   <si>
-    <t>* Graph 5 vars from Add Health. Blog about it. (Due 9/11)</t>
-  </si>
-  <si>
-    <t>Explore Add Health variables. Blog about choices and potential problems.  (Due 9/4)
-* Start your own Add Health codebook
-* Start your own Add Health data management file</t>
-  </si>
-  <si>
-    <t>* Turn in codebook and DM file (Due 9/4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data Screening
 * Univariate Data Visualizations
 </t>
+  </si>
+  <si>
+    <t>graded</t>
+  </si>
+  <si>
+    <t>Pick AddHlth sections. Blog your choices.  (Due 8/28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explore Add Health variables. Blog about your choices and potential problems.  (Due 9/4)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a BBL Blog (Due 8/28) 
+* Post Intro/Bio
+* Post RR plan
+</t>
+  </si>
+  <si>
+    <t>Turn in copies of your codebook and DM file (Due 9/4)</t>
+  </si>
+  <si>
+    <t>Blog post describing 5 vars from Add Health.  (Due 9/11)</t>
   </si>
 </sst>
 </file>
@@ -203,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,12 +224,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,7 +354,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -549,38 +542,59 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -979,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -990,15 +1004,15 @@
     <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="21" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="61.125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27.125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="47.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="27.125" style="69" customWidth="1"/>
     <col min="8" max="8" width="39.5" style="21" customWidth="1"/>
     <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>0</v>
@@ -1007,23 +1021,23 @@
         <v>1</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="G1" s="63" t="s">
+        <v>6</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1035,14 +1049,14 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="61"/>
       <c r="F2" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>20</v>
       </c>
       <c r="H2" s="61"/>
     </row>
@@ -1057,98 +1071,98 @@
         <v>Thu</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="57"/>
       <c r="F3" s="62"/>
-      <c r="G3" s="63" t="s">
-        <v>16</v>
+      <c r="G3" s="65" t="s">
+        <v>18</v>
       </c>
       <c r="H3" s="57"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="64">
+      <c r="B4" s="72">
         <f>B2+7</f>
         <v>41514</v>
       </c>
-      <c r="C4" s="65" t="str">
+      <c r="C4" s="73" t="str">
         <f>TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D4" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="67"/>
+      <c r="D4" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="75"/>
+      <c r="F4" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="69">
+      <c r="B5" s="54">
         <f>B4+2</f>
         <v>41516</v>
       </c>
-      <c r="C5" s="70" t="str">
+      <c r="C5" s="55" t="str">
         <f>TEXT(WEEKDAY(B5,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71" t="s">
+      <c r="D5" s="56"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="73"/>
-    </row>
-    <row r="6" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="H5" s="79"/>
+    </row>
+    <row r="6" spans="1:9" ht="126" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>A4+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="64">
+      <c r="B6" s="72">
         <f>B4+7</f>
         <v>41521</v>
       </c>
-      <c r="C6" s="65" t="str">
+      <c r="C6" s="73" t="str">
         <f t="shared" ref="C6:C24" si="0">TEXT(WEEKDAY(B6,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D6" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="66" t="s">
-        <v>19</v>
-      </c>
+      <c r="D6" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="75"/>
+      <c r="F6" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="80"/>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="69">
+      <c r="B7" s="54">
         <f>B6+2</f>
         <v>41523</v>
       </c>
-      <c r="C7" s="70" t="str">
+      <c r="C7" s="55" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="78" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1167,7 +1181,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="36"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="66"/>
       <c r="H8" s="39"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1183,7 +1197,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="28"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="45"/>
       <c r="I9" s="24"/>
     </row>
@@ -1203,7 +1217,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="36"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="66"/>
       <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1219,7 +1233,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="27"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="68"/>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1252,7 +1266,7 @@
       <c r="D13" s="18"/>
       <c r="E13" s="30"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="G13" s="68"/>
       <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1286,7 +1300,7 @@
       <c r="D15" s="18"/>
       <c r="E15" s="30"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="68"/>
       <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1319,7 +1333,7 @@
       <c r="D17" s="18"/>
       <c r="E17" s="30"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="G17" s="68"/>
       <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1351,7 +1365,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="27"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="68"/>
       <c r="H19" s="27"/>
       <c r="I19" s="24"/>
     </row>
@@ -1371,7 +1385,7 @@
       <c r="D20" s="43"/>
       <c r="E20" s="44"/>
       <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="44"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1387,7 +1401,7 @@
       <c r="D21" s="17"/>
       <c r="E21" s="28"/>
       <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1421,7 +1435,7 @@
       <c r="D23" s="18"/>
       <c r="E23" s="30"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="68"/>
       <c r="H23" s="27"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1439,7 +1453,7 @@
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="31"/>
-      <c r="G24" s="13"/>
+      <c r="G24" s="66"/>
       <c r="H24" s="36"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1455,7 +1469,7 @@
       <c r="D25" s="18"/>
       <c r="E25" s="30"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="G25" s="68"/>
       <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1489,7 +1503,7 @@
       <c r="D27" s="18"/>
       <c r="E27" s="30"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="G27" s="68"/>
       <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1503,11 +1517,11 @@
         <v>Tue</v>
       </c>
       <c r="D28" s="50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="50"/>
       <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
+      <c r="G28" s="71"/>
       <c r="H28" s="51"/>
       <c r="I28" s="46"/>
     </row>
@@ -1540,7 +1554,7 @@
       <c r="D30" s="18"/>
       <c r="E30" s="34"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="G30" s="68"/>
       <c r="H30" s="27"/>
       <c r="I30" s="46"/>
     </row>
@@ -1575,13 +1589,13 @@
       <c r="D32" s="37"/>
       <c r="E32" s="28"/>
       <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
+      <c r="G32" s="67"/>
       <c r="H32" s="28"/>
       <c r="I32" s="46"/>
     </row>
     <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" s="3">
         <v>41625</v>
@@ -1591,7 +1605,7 @@
         <v>Mon</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33" s="13"/>

</xml_diff>

<commit_message>
tweak first 3 weeks. finalize schedule
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
   <si>
     <t>date</t>
   </si>
@@ -97,12 +92,6 @@
 * Add Health</t>
   </si>
   <si>
-    <t>Choose area of interest  (Due 8/28)</t>
-  </si>
-  <si>
-    <t>Conducting a lit review, citation fomats</t>
-  </si>
-  <si>
     <t>Personal Codebook/ Research Question Assignment  (Due 8/31)
 * Data management assignment (Due 9/4)</t>
   </si>
@@ -136,9 +125,6 @@
 Rest of class on graphing assignment</t>
   </si>
   <si>
-    <t>Univariate graphing assignment (Due 9/11)</t>
-  </si>
-  <si>
     <t>Writing about empirical research</t>
   </si>
   <si>
@@ -157,12 +143,6 @@
     <t>Bivariate graphing assignment (Due 9/25)</t>
   </si>
   <si>
-    <t>open analysis time</t>
-  </si>
-  <si>
-    <t>Exam 1</t>
-  </si>
-  <si>
     <t>Choosing appropriate analyses</t>
   </si>
   <si>
@@ -181,27 +161,12 @@
     <t>Chi-square</t>
   </si>
   <si>
-    <t>Correlation</t>
-  </si>
-  <si>
-    <t>Linear Regression</t>
-  </si>
-  <si>
-    <t>Moderation</t>
-  </si>
-  <si>
     <t>Multiple Regression</t>
   </si>
   <si>
-    <t>Confounding</t>
-  </si>
-  <si>
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Final Exam</t>
-  </si>
-  <si>
     <t>Presentations</t>
   </si>
   <si>
@@ -214,21 +179,6 @@
     <t>Analysis work time</t>
   </si>
   <si>
-    <t>ANOVA Assignment (Due 10/23)</t>
-  </si>
-  <si>
-    <t>Chi-Square Assignment (Due 10/23)</t>
-  </si>
-  <si>
-    <t>Correlation Assignment (Due 10/30)</t>
-  </si>
-  <si>
-    <t>Moderation Assignment (Due 11/6)</t>
-  </si>
-  <si>
-    <t>Regression Assignment (Due 11/30)</t>
-  </si>
-  <si>
     <t>[Week 11 overview](wk11.html)</t>
   </si>
   <si>
@@ -265,19 +215,70 @@
     <t>[Week 15 overview](wk15.html)</t>
   </si>
   <si>
-    <t>Posters due 12/6</t>
-  </si>
-  <si>
     <t>Foundations assignment (Due 10/9)</t>
   </si>
   <si>
     <t>Inference Assignment (Due 10/11)</t>
+  </si>
+  <si>
+    <t>Univariate graphing assignment (Due 9/14)</t>
+  </si>
+  <si>
+    <t>Moderating and Confounding</t>
+  </si>
+  <si>
+    <t>Midterm</t>
+  </si>
+  <si>
+    <t>Flex time</t>
+  </si>
+  <si>
+    <t>Correlation and Regression</t>
+  </si>
+  <si>
+    <t>Bivariate Inference (Due 10/30)</t>
+  </si>
+  <si>
+    <t>Multiple Regression Assignment (Due 11/13)</t>
+  </si>
+  <si>
+    <t>Logistic Regression Assignment (Due 11/27)</t>
+  </si>
+  <si>
+    <t>Progress check in blog post (Due 10/23)</t>
+  </si>
+  <si>
+    <t>Progress check in blog post (Due 10/2)</t>
+  </si>
+  <si>
+    <t>Progress check in blog post (Due 10/30)</t>
+  </si>
+  <si>
+    <t>Progress check in blog post (Due 11/13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progress check in blog post (Due Thursday 11/30) </t>
+  </si>
+  <si>
+    <t>Special Regression Topics</t>
+  </si>
+  <si>
+    <t>Posters due day before final exam time</t>
+  </si>
+  <si>
+    <t>Impacts of sampling design</t>
+  </si>
+  <si>
+    <t>Lit review  * citation fomats</t>
+  </si>
+  <si>
+    <t>Choose area of interest (Due 8/28) * Personal Codebook/ Research Question Assignment  (Due 9/4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -363,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,13 +385,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +471,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -522,8 +529,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -633,9 +672,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -657,9 +693,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -681,18 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -708,80 +729,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -809,6 +857,22 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -836,9 +900,25 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1174,27 +1254,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2"/>
-    <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="21" customWidth="1"/>
-    <col min="6" max="6" width="47.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="63.25" style="61" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="63.1640625" style="55" customWidth="1"/>
     <col min="8" max="8" width="39.5" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
@@ -1213,7 +1293,7 @@
       <c r="F1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="51" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="35" t="s">
@@ -1221,153 +1301,153 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:9" ht="63">
+      <c r="A2" s="75">
         <v>1</v>
       </c>
-      <c r="B2" s="69">
+      <c r="B2" s="76">
         <v>41507</v>
       </c>
-      <c r="C2" s="70" t="str">
+      <c r="C2" s="77" t="str">
         <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="71" t="s">
+      <c r="E2" s="65"/>
+      <c r="F2" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="72"/>
-    </row>
-    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="53">
+      <c r="H2" s="65"/>
+    </row>
+    <row r="3" spans="1:9" ht="75">
+      <c r="A3" s="79"/>
+      <c r="B3" s="80">
         <f>B2+2</f>
         <v>41509</v>
       </c>
-      <c r="C3" s="54" t="str">
+      <c r="C3" s="81" t="str">
         <f>TEXT(WEEKDAY(B3,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="83" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="68" t="s">
+      <c r="E3" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="66" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="56"/>
+      <c r="G3" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="27"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="75">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="74">
+      <c r="B4" s="83">
         <f>B2+7</f>
         <v>41514</v>
       </c>
-      <c r="C4" s="75" t="str">
+      <c r="C4" s="84" t="str">
         <f>TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="78" t="s">
+      <c r="E4" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="77"/>
-    </row>
-    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="53">
+      <c r="G4" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="66"/>
+    </row>
+    <row r="5" spans="1:9" ht="45">
+      <c r="A5" s="79"/>
+      <c r="B5" s="80">
         <f>B4+2</f>
         <v>41516</v>
       </c>
-      <c r="C5" s="54" t="str">
+      <c r="C5" s="81" t="str">
         <f>TEXT(WEEKDAY(B5,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="59"/>
+      <c r="G5" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="83" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="67"/>
-    </row>
-    <row r="6" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="H5" s="30"/>
+    </row>
+    <row r="6" spans="1:9" ht="90">
+      <c r="A6" s="75">
         <f>A4+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="64">
+      <c r="B6" s="86">
         <f>B4+7</f>
         <v>41521</v>
       </c>
-      <c r="C6" s="65" t="str">
+      <c r="C6" s="87" t="str">
         <f t="shared" ref="C6:C24" si="0">TEXT(WEEKDAY(B6,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D6" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="80" t="s">
+      <c r="D6" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="81" t="s">
-        <v>30</v>
+      <c r="G6" s="73" t="s">
+        <v>60</v>
       </c>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="53">
+    <row r="7" spans="1:9" ht="45">
+      <c r="A7" s="79"/>
+      <c r="B7" s="80">
         <f>B6+2</f>
         <v>41523</v>
       </c>
-      <c r="C7" s="54" t="str">
+      <c r="C7" s="81" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D7" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="55" t="s">
+      <c r="D7" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="66"/>
+      <c r="G7" s="72"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="45">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A26" si="1">A6+1</f>
         <v>4</v>
@@ -1381,44 +1461,44 @@
         <v>Tue</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="39"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15">
+        <v>54</v>
+      </c>
+      <c r="G8" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7">
         <f>B8+2</f>
         <v>41530</v>
       </c>
-      <c r="C9" s="16" t="str">
+      <c r="C9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="45"/>
+      <c r="D9" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30">
       <c r="A10" s="11">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="37">
         <f>B8+7</f>
         <v>41535</v>
       </c>
@@ -1427,20 +1507,20 @@
         <v>Tue</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="39"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="6"/>
       <c r="B11" s="7">
         <f>B10+2</f>
@@ -1450,13 +1530,15 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="68" t="s">
+        <v>45</v>
+      </c>
       <c r="E11" s="27"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="60"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1470,17 +1552,20 @@
         <v>Tue</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>67</v>
+        <v>52</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>69</v>
       </c>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="6"/>
       <c r="B13" s="7">
         <f>B12+2</f>
@@ -1490,15 +1575,15 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>38</v>
+      <c r="D13" s="69" t="s">
+        <v>62</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="60"/>
+      <c r="G13" s="54"/>
       <c r="H13" s="27"/>
     </row>
-    <row r="14" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="78.75">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1512,18 +1597,18 @@
         <v>Tue</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="61" t="s">
-        <v>74</v>
+        <v>51</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>58</v>
       </c>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="47.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7">
         <f>B14+2</f>
@@ -1534,16 +1619,16 @@
         <v>Thu</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="60" t="s">
-        <v>75</v>
+      <c r="G15" s="54" t="s">
+        <v>59</v>
       </c>
       <c r="H15" s="27"/>
     </row>
-    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30">
       <c r="A16" s="2">
         <v>8</v>
       </c>
@@ -1556,15 +1641,18 @@
         <v>Tue</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="55" t="s">
         <v>65</v>
       </c>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="6"/>
       <c r="B17" s="7">
         <f>B16+2</f>
@@ -1575,16 +1663,14 @@
         <v>Thu</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="60" t="s">
-        <v>56</v>
-      </c>
+      <c r="G17" s="54"/>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1598,18 +1684,18 @@
         <v>Tue</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="61" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="G18" s="55" t="s">
+        <v>68</v>
       </c>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" s="6"/>
       <c r="B19" s="7">
         <f>B18+2</f>
@@ -1619,59 +1705,59 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>55</v>
+      <c r="D19" s="60" t="s">
+        <v>64</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="60"/>
+      <c r="G19" s="54"/>
       <c r="H19" s="27"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="40">
+    <row r="20" spans="1:9">
+      <c r="A20" s="39">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="40">
         <f>B18+7</f>
         <v>41570</v>
       </c>
-      <c r="C20" s="42" t="str">
+      <c r="C20" s="41" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D20" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="44"/>
+      <c r="D20" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="43"/>
       <c r="F20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="62" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="44"/>
-    </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15">
+        <v>47</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" s="43"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7">
         <f>B20+2</f>
         <v>41572</v>
       </c>
-      <c r="C21" s="16" t="str">
+      <c r="C21" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="28"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="27"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1684,19 +1770,19 @@
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>47</v>
+      <c r="D22" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="61" t="s">
-        <v>59</v>
+        <v>46</v>
+      </c>
+      <c r="G22" s="55" t="s">
+        <v>66</v>
       </c>
       <c r="H22" s="26"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="6"/>
       <c r="B23" s="7">
         <f>B22+2</f>
@@ -1707,19 +1793,19 @@
         <v>Thu</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E23" s="30"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="60"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="30">
       <c r="A24" s="11">
         <f>A22+1</f>
         <v>12</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B24" s="37">
         <f>B22+7</f>
         <v>41584</v>
       </c>
@@ -1728,18 +1814,18 @@
         <v>Tue</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="G24" s="55" t="s">
+        <v>71</v>
       </c>
       <c r="H24" s="36"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="6"/>
       <c r="B25" s="7">
         <f>B24+2</f>
@@ -1750,14 +1836,14 @@
         <v>Thu</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="60"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1771,15 +1857,18 @@
         <v>Tue</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E26" s="31"/>
       <c r="F26" s="5" t="s">
-        <v>63</v>
+        <v>48</v>
+      </c>
+      <c r="G26" s="55" t="s">
+        <v>67</v>
       </c>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="6"/>
       <c r="B27" s="7">
         <f>B26+2</f>
@@ -1789,34 +1878,34 @@
         <f t="shared" ref="C27:C33" si="3">TEXT(WEEKDAY(B27,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>55</v>
+      <c r="D27" s="68" t="s">
+        <v>45</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="60"/>
+      <c r="G27" s="54"/>
       <c r="H27" s="30"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="48">
+    <row r="28" spans="1:9">
+      <c r="A28" s="45"/>
+      <c r="B28" s="46">
         <f>B26+7</f>
         <v>41598</v>
       </c>
-      <c r="C28" s="49" t="str">
+      <c r="C28" s="47" t="str">
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="46"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E28" s="48"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="44"/>
+    </row>
+    <row r="29" spans="1:9" ht="30">
       <c r="A29" s="2">
         <v>14</v>
       </c>
@@ -1828,16 +1917,19 @@
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>50</v>
+      <c r="D29" s="70" t="s">
+        <v>73</v>
       </c>
       <c r="E29" s="33"/>
       <c r="F29" s="5" t="s">
-        <v>71</v>
+        <v>56</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>72</v>
       </c>
       <c r="H29" s="36"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="6"/>
       <c r="B30" s="7">
         <f>B29+2</f>
@@ -1847,16 +1939,16 @@
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>55</v>
+      <c r="D30" s="68" t="s">
+        <v>45</v>
       </c>
       <c r="E30" s="34"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="60"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="27"/>
-      <c r="I30" s="46"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="44"/>
+    </row>
+    <row r="31" spans="1:9" ht="30">
       <c r="A31" s="11">
         <f>A29+1</f>
         <v>15</v>
@@ -1869,20 +1961,20 @@
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>55</v>
+      <c r="D31" s="70" t="s">
+        <v>75</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" s="61" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>74</v>
       </c>
       <c r="H31" s="36"/>
-      <c r="I31" s="46"/>
-    </row>
-    <row r="32" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I31" s="44"/>
+    </row>
+    <row r="32" spans="1:9" ht="16" thickBot="1">
       <c r="A32" s="14"/>
       <c r="B32" s="15">
         <f>B31+2</f>
@@ -1892,16 +1984,16 @@
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D32" s="37" t="s">
-        <v>52</v>
+      <c r="D32" s="71" t="s">
+        <v>45</v>
       </c>
       <c r="E32" s="28"/>
       <c r="F32" s="17"/>
-      <c r="G32" s="59"/>
+      <c r="G32" s="53"/>
       <c r="H32" s="28"/>
-      <c r="I32" s="46"/>
-    </row>
-    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="I32" s="44"/>
+    </row>
+    <row r="33" spans="1:8" ht="30">
       <c r="A33" s="10" t="s">
         <v>3</v>
       </c>
@@ -1913,7 +2005,7 @@
         <v>Mon</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33" s="13"/>
@@ -1921,7 +2013,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add conference time to schedule
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>date</t>
   </si>
@@ -274,11 +279,14 @@
   <si>
     <t>Choose area of interest (Due 8/28) * Personal Codebook/ Research Question Assignment  (Due 9/4)</t>
   </si>
+  <si>
+    <t>I won't be here - Edward Cover</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -364,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +406,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,7 +576,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -826,6 +840,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -917,8 +946,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1254,27 +1283,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="21" customWidth="1"/>
-    <col min="6" max="6" width="47.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="63.1640625" style="55" customWidth="1"/>
+    <col min="6" max="6" width="47.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="63.125" style="55" customWidth="1"/>
     <col min="8" max="8" width="39.5" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" thickBot="1">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
@@ -1301,7 +1330,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="63">
+    <row r="2" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="75">
         <v>1</v>
       </c>
@@ -1324,7 +1353,7 @@
       </c>
       <c r="H2" s="65"/>
     </row>
-    <row r="3" spans="1:9" ht="75">
+    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
       <c r="B3" s="80">
         <f>B2+2</f>
@@ -1349,7 +1378,7 @@
       <c r="H3" s="27"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="30">
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="75">
         <f>A2+1</f>
         <v>2</v>
@@ -1376,7 +1405,7 @@
       </c>
       <c r="H4" s="66"/>
     </row>
-    <row r="5" spans="1:9" ht="45">
+    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="79"/>
       <c r="B5" s="80">
         <f>B4+2</f>
@@ -1398,7 +1427,7 @@
       </c>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="1:9" ht="90">
+    <row r="6" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
         <f>A4+1</f>
         <v>3</v>
@@ -1425,7 +1454,7 @@
       </c>
       <c r="H6" s="26"/>
     </row>
-    <row r="7" spans="1:9" ht="45">
+    <row r="7" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="79"/>
       <c r="B7" s="80">
         <f>B6+2</f>
@@ -1447,7 +1476,7 @@
       <c r="G7" s="72"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:9" ht="45">
+    <row r="8" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A26" si="1">A6+1</f>
         <v>4</v>
@@ -1474,7 +1503,7 @@
       </c>
       <c r="H8" s="38"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7">
         <f>B8+2</f>
@@ -1493,7 +1522,7 @@
       <c r="H9" s="30"/>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:9" ht="30">
+    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1520,7 +1549,7 @@
       </c>
       <c r="H10" s="38"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7">
         <f>B10+2</f>
@@ -1530,15 +1559,17 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:9" ht="30">
+      <c r="E11" s="90" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="91"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="93"/>
+    </row>
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1565,7 +1596,7 @@
       </c>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7">
         <f>B12+2</f>
@@ -1583,7 +1614,7 @@
       <c r="G13" s="54"/>
       <c r="H13" s="27"/>
     </row>
-    <row r="14" spans="1:9" ht="78.75">
+    <row r="14" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1608,7 +1639,7 @@
       </c>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:9" ht="47.25">
+    <row r="15" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7">
         <f>B14+2</f>
@@ -1628,7 +1659,7 @@
       </c>
       <c r="H15" s="27"/>
     </row>
-    <row r="16" spans="1:9" ht="30">
+    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>8</v>
       </c>
@@ -1652,7 +1683,7 @@
       </c>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7">
         <f>B16+2</f>
@@ -1670,7 +1701,7 @@
       <c r="G17" s="54"/>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1695,7 +1726,7 @@
       </c>
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="1:9" ht="30">
+    <row r="19" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7">
         <f>B18+2</f>
@@ -1714,7 +1745,7 @@
       <c r="H19" s="27"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1739,7 +1770,7 @@
       </c>
       <c r="H20" s="43"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7">
         <f>B20+2</f>
@@ -1757,7 +1788,7 @@
       <c r="G21" s="54"/>
       <c r="H21" s="27"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1782,7 +1813,7 @@
       </c>
       <c r="H22" s="26"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7">
         <f>B22+2</f>
@@ -1800,7 +1831,7 @@
       <c r="G23" s="54"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:9" ht="30">
+    <row r="24" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <f>A22+1</f>
         <v>12</v>
@@ -1825,7 +1856,7 @@
       </c>
       <c r="H24" s="36"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7">
         <f>B24+2</f>
@@ -1843,7 +1874,7 @@
       <c r="G25" s="54"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1868,7 +1899,7 @@
       </c>
       <c r="H26" s="26"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="7">
         <f>B26+2</f>
@@ -1886,7 +1917,7 @@
       <c r="G27" s="54"/>
       <c r="H27" s="30"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="B28" s="46">
         <f>B26+7</f>
@@ -1905,7 +1936,7 @@
       <c r="H28" s="49"/>
       <c r="I28" s="44"/>
     </row>
-    <row r="29" spans="1:9" ht="30">
+    <row r="29" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>14</v>
       </c>
@@ -1929,7 +1960,7 @@
       </c>
       <c r="H29" s="36"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="7">
         <f>B29+2</f>
@@ -1948,7 +1979,7 @@
       <c r="H30" s="27"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:9" ht="30">
+    <row r="31" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <f>A29+1</f>
         <v>15</v>
@@ -1974,7 +2005,7 @@
       <c r="H31" s="36"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:9" ht="16" thickBot="1">
+    <row r="32" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="15">
         <f>B31+2</f>
@@ -1993,7 +2024,7 @@
       <c r="H32" s="28"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:8" ht="30">
+    <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
add medical records instructions
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -277,16 +277,17 @@
     <t>Lit review  * citation fomats</t>
   </si>
   <si>
-    <t>Choose area of interest (Due 8/28) * Personal Codebook/ Research Question Assignment  (Due 9/4)</t>
-  </si>
-  <si>
     <t>I won't be here - Edward Cover</t>
+  </si>
+  <si>
+    <t>Choose area of interest (Due 8/28) 
+* Personal Codebook/ Research Question Assignment  (Due 9/4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -946,8 +947,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1283,11 +1284,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1374,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="61" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" s="27"/>
       <c r="I3" s="10"/>
@@ -1563,7 +1564,7 @@
         <v>45</v>
       </c>
       <c r="E11" s="90" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="91"/>
       <c r="G11" s="92"/>

</xml_diff>

<commit_message>
update some hw and schedule
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -162,9 +162,6 @@
     <t>Inference Assignment (Due 10/11)</t>
   </si>
   <si>
-    <t>Univariate graphing assignment (Due 9/14)</t>
-  </si>
-  <si>
     <t>Moderating and Confounding</t>
   </si>
   <si>
@@ -211,13 +208,6 @@
   </si>
   <si>
     <t>I won't be here - Edward Cover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
-* Blog RR plan  (Due 8/28)
-* Choose area of Add Health interest (Due 8/28) 
-* Personal Codebook/ Research Question Assignment  (Due 9/4)
-</t>
   </si>
   <si>
     <t>Introduction to the class
@@ -234,11 +224,6 @@
     <t>T: Import data, start data prep
 R: 20 min lecture on lit review/citation assignment
 finish data prep</t>
-  </si>
-  <si>
-    <t>Personal Codebook/ Research Question Assignment  (Due 8/31)
-* Data management assignment (Due 9/4)
-* Citation Assignment (Due 9/7)</t>
   </si>
   <si>
     <t xml:space="preserve">Univariate Data Visualizations
@@ -255,6 +240,21 @@
 * [R Data Viz overview](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
 * [Lec03: Data Screening](docs/lec03_data_screen.html)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
+* Blog RR plan  (Due 8/28)
+* Blog area of Add Health research interest (Due 8/28) 
+* Personal Codebook/ Research Question Assignment  (Due 8/28)
+</t>
+  </si>
+  <si>
+    <t>Blog about potential necessary recoding  (Due Thu: 8/31) 
+* Data management assignment (Due 9/4)
+* Citation Assignment (Due 9/7)</t>
+  </si>
+  <si>
+    <t>Univariate graphing assignment (Due 9/18)</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1" s="50" t="s">
         <v>6</v>
@@ -1284,7 +1284,7 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" s="62" t="s">
         <v>11</v>
@@ -1293,7 +1293,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H2" s="62"/>
     </row>
@@ -1311,16 +1311,16 @@
         <v>Tue</v>
       </c>
       <c r="D3" s="77" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="60" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H3" s="63"/>
     </row>
@@ -1338,16 +1338,16 @@
         <v>Tue</v>
       </c>
       <c r="D4" s="80" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F4" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="69" t="s">
         <v>69</v>
-      </c>
-      <c r="G4" s="69" t="s">
-        <v>44</v>
       </c>
       <c r="H4" s="26"/>
     </row>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
-        <f t="shared" ref="A7:A23" si="1">A5+1</f>
+        <f>A5+1</f>
         <v>5</v>
       </c>
       <c r="B7" s="36">
@@ -1438,7 +1438,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="82" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="83"/>
       <c r="G8" s="84"/>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A9:A23" si="1">A7+1</f>
         <v>6</v>
       </c>
       <c r="B9" s="3">
@@ -1467,7 +1467,7 @@
         <v>36</v>
       </c>
       <c r="G9" s="54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H9" s="26"/>
     </row>
@@ -1482,7 +1482,7 @@
         <v>Thu</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="9"/>
@@ -1554,7 +1554,7 @@
         <v>34</v>
       </c>
       <c r="G13" s="54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="26"/>
     </row>
@@ -1597,7 +1597,7 @@
         <v>33</v>
       </c>
       <c r="G15" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="26"/>
     </row>
@@ -1612,7 +1612,7 @@
         <v>Thu</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="9"/>
@@ -1634,14 +1634,14 @@
         <v>Tue</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H17" s="42"/>
     </row>
@@ -1684,7 +1684,7 @@
         <v>30</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H19" s="26"/>
     </row>
@@ -1720,14 +1720,14 @@
         <v>Tue</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="31"/>
       <c r="F21" s="5" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H21" s="35"/>
     </row>
@@ -1770,7 +1770,7 @@
         <v>32</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="26"/>
     </row>
@@ -1824,14 +1824,14 @@
         <v>Tue</v>
       </c>
       <c r="D26" s="67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G26" s="54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="35"/>
     </row>
@@ -1868,14 +1868,14 @@
         <v>Tue</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" s="35"/>
       <c r="I28" s="43"/>

</xml_diff>

<commit_message>
clarify PC/RQ assignment for week 1.
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -236,13 +231,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
-* Blog RR plan  (Due 8/28)
-* Blog area of Add Health research interest (Due 8/28) 
-* Personal Codebook/ Research Question Assignment  (Due 8/28)
-</t>
-  </si>
-  <si>
     <t>Blog about potential necessary recoding  (Due Thu: 8/31) 
 * Data management assignment (Due 9/4)
 * Citation Assignment (Due 9/7)</t>
@@ -261,12 +249,19 @@
   </si>
   <si>
     <t xml:space="preserve">Split class in half. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
+* Blog RR plan  (Due 8/28)
+* Blog area of Add Health research interest (Due 8/25) 
+* Personal Codebook/ Research Question Assignment  (Due 8/28)
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1237,24 +1232,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2"/>
-    <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="21" customWidth="1"/>
-    <col min="6" max="6" width="47.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="63.125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="63.1640625" style="54" customWidth="1"/>
     <col min="8" max="8" width="39.5" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1276,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="75">
       <c r="A2" s="70">
         <v>1</v>
       </c>
@@ -1302,11 +1297,11 @@
         <v>8</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H2" s="62"/>
     </row>
-    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="78.75">
       <c r="A3" s="70">
         <f>A2+1</f>
         <v>2</v>
@@ -1329,11 +1324,11 @@
         <v>9</v>
       </c>
       <c r="G3" s="60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="63"/>
     </row>
-    <row r="4" spans="1:9" ht="126" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="126">
       <c r="A4" s="70">
         <f>A3+1</f>
         <v>3</v>
@@ -1356,11 +1351,11 @@
         <v>64</v>
       </c>
       <c r="G4" s="68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H4" s="26"/>
     </row>
-    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="47.25">
       <c r="A5" s="2">
         <f>A4+1</f>
         <v>4</v>
@@ -1387,7 +1382,7 @@
       </c>
       <c r="H5" s="37"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="6"/>
       <c r="B6" s="7">
         <f>B5+2</f>
@@ -1406,7 +1401,7 @@
       <c r="H6" s="30"/>
       <c r="I6" s="24"/>
     </row>
-    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="31.5">
       <c r="A7" s="11">
         <f>A5+1</f>
         <v>5</v>
@@ -1433,7 +1428,7 @@
       </c>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="31.5">
       <c r="A8" s="6"/>
       <c r="B8" s="7">
         <f>B7+2</f>
@@ -1453,7 +1448,7 @@
       <c r="G8" s="83"/>
       <c r="H8" s="84"/>
     </row>
-    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="31.5">
       <c r="A9" s="2">
         <f t="shared" ref="A9:A23" si="1">A7+1</f>
         <v>6</v>
@@ -1480,7 +1475,7 @@
       </c>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="6"/>
       <c r="B10" s="7">
         <f>B9+2</f>
@@ -1498,7 +1493,7 @@
       <c r="G10" s="53"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="78.75">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1523,7 +1518,7 @@
       </c>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="47.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7">
         <f>B11+2</f>
@@ -1543,7 +1538,7 @@
       </c>
       <c r="H12" s="27"/>
     </row>
-    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="31.5">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -1567,7 +1562,7 @@
       </c>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="6"/>
       <c r="B14" s="7">
         <f>B13+2</f>
@@ -1585,7 +1580,7 @@
       <c r="G14" s="53"/>
       <c r="H14" s="27"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1610,7 +1605,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="31.5">
       <c r="A16" s="6"/>
       <c r="B16" s="7">
         <f>B15+2</f>
@@ -1629,7 +1624,7 @@
       <c r="H16" s="27"/>
       <c r="I16" s="24"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="38">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1654,7 +1649,7 @@
       </c>
       <c r="H17" s="42"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="6"/>
       <c r="B18" s="7">
         <f>B17+2</f>
@@ -1672,7 +1667,7 @@
       <c r="G18" s="53"/>
       <c r="H18" s="27"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1697,7 +1692,7 @@
       </c>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="6"/>
       <c r="B20" s="7">
         <f>B19+2</f>
@@ -1715,7 +1710,7 @@
       <c r="G20" s="53"/>
       <c r="H20" s="27"/>
     </row>
-    <row r="21" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="31.5">
       <c r="A21" s="11">
         <f>A19+1</f>
         <v>12</v>
@@ -1740,7 +1735,7 @@
       </c>
       <c r="H21" s="35"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="6"/>
       <c r="B22" s="7">
         <f>B21+2</f>
@@ -1758,7 +1753,7 @@
       <c r="G22" s="53"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1783,7 +1778,7 @@
       </c>
       <c r="H23" s="26"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="6"/>
       <c r="B24" s="7">
         <f>B23+2</f>
@@ -1801,7 +1796,7 @@
       <c r="G24" s="53"/>
       <c r="H24" s="30"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="44"/>
       <c r="B25" s="45">
         <f>B23+7</f>
@@ -1820,7 +1815,7 @@
       <c r="H25" s="48"/>
       <c r="I25" s="43"/>
     </row>
-    <row r="26" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="31.5">
       <c r="A26" s="2">
         <v>14</v>
       </c>
@@ -1844,7 +1839,7 @@
       </c>
       <c r="H26" s="35"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="6"/>
       <c r="B27" s="7">
         <f>B26+2</f>
@@ -1863,7 +1858,7 @@
       <c r="H27" s="27"/>
       <c r="I27" s="43"/>
     </row>
-    <row r="28" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="31.5">
       <c r="A28" s="11">
         <f>A26+1</f>
         <v>15</v>
@@ -1884,12 +1879,12 @@
         <v>40</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H28" s="35"/>
       <c r="I28" s="43"/>
     </row>
-    <row r="29" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="16.5" thickBot="1">
       <c r="A29" s="14"/>
       <c r="B29" s="15">
         <f>B28+2</f>
@@ -1900,17 +1895,17 @@
         <v>Thu</v>
       </c>
       <c r="D29" s="85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="52"/>
       <c r="H29" s="28"/>
       <c r="I29" s="43"/>
     </row>
-    <row r="30" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="31.5">
       <c r="A30" s="10" t="s">
         <v>3</v>
       </c>
@@ -1922,7 +1917,7 @@
         <v>Mon</v>
       </c>
       <c r="D30" s="86" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="13"/>

</xml_diff>

<commit_message>
reformat schedule, add dm assignment preparation
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>date</t>
   </si>
@@ -43,15 +48,6 @@
   </si>
   <si>
     <t>Week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 1 overview](wk01.html) 
-* [Lec01: Intro to the class](docs/lec01_intro_class.html)
-* [PMA5 Ch 2 &amp; 3](docs/PMA5 Ch 2 and 3.pdf) </t>
-  </si>
-  <si>
-    <t>[Week 2 overview](wk02.html)
-* [Lec02: Data Prep](docs/lec02_data_prep.html)</t>
   </si>
   <si>
     <t>graded</t>
@@ -224,44 +220,63 @@
 R: transformations (10-15 min). Rest of class on graphing assignment</t>
   </si>
   <si>
+    <t>Univariate graphing assignment (Due 9/18)</t>
+  </si>
+  <si>
+    <t>Posters Due 12/6</t>
+  </si>
+  <si>
+    <t>Poster Presentations</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split class in half. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 1 overview](wk01.html) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 2 overview](wk02.html)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">[Week 3 overview](wk03.html)
-* [PMA6 Data Viz ch DRAFT](docs/pma6_ch4_draft.pdf)
-* [R Data Viz overview](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
-* [Lec03: Data Screening](docs/lec03_data_screen.html)
 </t>
   </si>
   <si>
-    <t>Blog about potential necessary recoding  (Due Thu: 8/31) 
-* Data management assignment (Due 9/4)
-* Citation Assignment (Due 9/7)</t>
-  </si>
-  <si>
-    <t>Univariate graphing assignment (Due 9/18)</t>
-  </si>
-  <si>
-    <t>Posters Due 12/6</t>
-  </si>
-  <si>
-    <t>Poster Presentations</t>
-  </si>
-  <si>
-    <t>Final Exam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Split class in half. </t>
+    <t>[Syllabus](docs/syllabus_615_f17_html)
+* [PMA5 Ch 2 &amp; 3](docs/PMA5 Ch 2 and 3.pdf) 
+* [Reproducibility slides](http://benmarwick.github.io/UW-eScience-reproducibility-social-sciences/#/)
+* [Passion Driven Statistics](docs/PDS_Intro_Stat.pdf)
+* [Introduction to the class](docs/lec01_intro_class.html)</t>
+  </si>
+  <si>
+    <t>[Notes on Data Preparation](docs/lec02_data_prep.html)
+* [How to read a Journal Article](docs/How to Read a Journal Article.pdf)
+* [Literature Review notes](docs/lec_lit_review.html)</t>
   </si>
   <si>
     <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
 * Blog RR plan  (Due 8/28)
 * Blog area of Add Health research interest (Due 8/25) 
-* Personal Codebook/ Research Question Assignment  (Due 8/28)
+* Personal Codebook/ Research Question [Assignment](hw/RQ_personal_codebook_assignment.html)   (Due 8/28)
 </t>
+  </si>
+  <si>
+    <t>wknum</t>
+  </si>
+  <si>
+    <t>Blog about data cleaning preparation (Due Thu: 8/31) 
+* Data management code file (Due 9/4)
+* Citation [Assignment](hw/Citation_Assignment.html) (Due 9/7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -892,8 +907,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1229,29 +1244,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="21" customWidth="1"/>
-    <col min="6" max="6" width="47.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="63.1640625" style="54" customWidth="1"/>
-    <col min="8" max="8" width="39.5" style="21" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="27.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.125" style="54" customWidth="1"/>
+    <col min="9" max="9" width="39.5" style="21" customWidth="1"/>
+    <col min="10" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" thickBot="1">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>0</v>
@@ -1266,17 +1282,20 @@
         <v>2</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="75">
+      <c r="I1" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="70">
         <v>1</v>
       </c>
@@ -1288,20 +1307,23 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="73" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="62"/>
-    </row>
-    <row r="3" spans="1:9" ht="78.75">
+        <v>67</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="62"/>
+    </row>
+    <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <f>A2+1</f>
         <v>2</v>
@@ -1315,20 +1337,23 @@
         <v>Tue</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="63"/>
-    </row>
-    <row r="4" spans="1:9" ht="126">
+        <v>68</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
         <f>A3+1</f>
         <v>3</v>
@@ -1342,20 +1367,21 @@
         <v>Tue</v>
       </c>
       <c r="D4" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="61"/>
+      <c r="H4" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="26"/>
-    </row>
-    <row r="5" spans="1:9" ht="47.25">
+      <c r="I4" s="26"/>
+    </row>
+    <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>A4+1</f>
         <v>4</v>
@@ -1369,20 +1395,20 @@
         <v>Tue</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="37"/>
-    </row>
-    <row r="6" spans="1:9">
+        <v>35</v>
+      </c>
+      <c r="H5" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="37"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7">
         <f>B5+2</f>
@@ -1393,15 +1419,16 @@
         <v>Thu</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="24"/>
-    </row>
-    <row r="7" spans="1:9" ht="31.5">
+      <c r="G6" s="9"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <f>A5+1</f>
         <v>5</v>
@@ -1415,20 +1442,20 @@
         <v>Tue</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="37"/>
-    </row>
-    <row r="8" spans="1:9" ht="31.5">
+      <c r="I7" s="37"/>
+    </row>
+    <row r="8" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7">
         <f>B7+2</f>
@@ -1439,16 +1466,17 @@
         <v>Thu</v>
       </c>
       <c r="D8" s="80" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="82"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="84"/>
-    </row>
-    <row r="9" spans="1:9" ht="31.5">
+      <c r="G8" s="82"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="84"/>
+    </row>
+    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" ref="A9:A23" si="1">A7+1</f>
         <v>6</v>
@@ -1462,20 +1490,20 @@
         <v>Tue</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:9">
+        <v>33</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="7">
         <f>B9+2</f>
@@ -1486,14 +1514,15 @@
         <v>Thu</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" spans="1:9" ht="78.75">
+      <c r="G10" s="9"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1507,18 +1536,18 @@
         <v>Tue</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" s="29"/>
       <c r="F11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" ht="47.25">
+        <v>32</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="26"/>
+    </row>
+    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7">
         <f>B11+2</f>
@@ -1529,16 +1558,17 @@
         <v>Thu</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="27"/>
-    </row>
-    <row r="13" spans="1:9" ht="31.5">
+      <c r="G12" s="9"/>
+      <c r="H12" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>8</v>
       </c>
@@ -1551,18 +1581,18 @@
         <v>Tue</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="26"/>
-    </row>
-    <row r="14" spans="1:9">
+        <v>31</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7">
         <f>B13+2</f>
@@ -1573,14 +1603,15 @@
         <v>Thu</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="G14" s="9"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1594,18 +1625,18 @@
         <v>Tue</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="1:9" ht="31.5">
+        <v>30</v>
+      </c>
+      <c r="H15" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7">
         <f>B15+2</f>
@@ -1616,15 +1647,16 @@
         <v>Thu</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="G16" s="9"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1638,18 +1670,18 @@
         <v>Tue</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="42"/>
-    </row>
-    <row r="18" spans="1:9">
+        <v>28</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="42"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7">
         <f>B17+2</f>
@@ -1660,14 +1692,15 @@
         <v>Thu</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="27"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="G18" s="9"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1681,18 +1714,18 @@
         <v>Tue</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="26"/>
-    </row>
-    <row r="20" spans="1:9">
+        <v>27</v>
+      </c>
+      <c r="H19" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="7">
         <f>B19+2</f>
@@ -1703,14 +1736,15 @@
         <v>Thu</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E20" s="30"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="27"/>
-    </row>
-    <row r="21" spans="1:9" ht="31.5">
+      <c r="G20" s="9"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <f>A19+1</f>
         <v>12</v>
@@ -1724,18 +1758,18 @@
         <v>Tue</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21" s="31"/>
       <c r="F21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="H21" s="35"/>
-    </row>
-    <row r="22" spans="1:9">
+        <v>36</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="35"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7">
         <f>B21+2</f>
@@ -1746,14 +1780,15 @@
         <v>Thu</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E22" s="30"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="27"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="G22" s="9"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1767,18 +1802,18 @@
         <v>Tue</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23" s="31"/>
       <c r="F23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="26"/>
-    </row>
-    <row r="24" spans="1:9">
+        <v>29</v>
+      </c>
+      <c r="H23" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7">
         <f>B23+2</f>
@@ -1789,14 +1824,15 @@
         <v>Thu</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="30"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="G24" s="9"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="30"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="45">
         <f>B23+7</f>
@@ -1811,11 +1847,12 @@
       </c>
       <c r="E25" s="47"/>
       <c r="F25" s="49"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="43"/>
-    </row>
-    <row r="26" spans="1:9" ht="31.5">
+      <c r="G25" s="49"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="43"/>
+    </row>
+    <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>14</v>
       </c>
@@ -1828,18 +1865,18 @@
         <v>Tue</v>
       </c>
       <c r="D26" s="67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" s="35"/>
-    </row>
-    <row r="27" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="7">
         <f>B26+2</f>
@@ -1850,15 +1887,16 @@
         <v>Thu</v>
       </c>
       <c r="D27" s="65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E27" s="33"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="43"/>
-    </row>
-    <row r="28" spans="1:9" ht="31.5">
+      <c r="G27" s="9"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="43"/>
+    </row>
+    <row r="28" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <f>A26+1</f>
         <v>15</v>
@@ -1872,19 +1910,19 @@
         <v>Tue</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="35"/>
-      <c r="I28" s="43"/>
-    </row>
-    <row r="29" spans="1:9" ht="16.5" thickBot="1">
+        <v>38</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="35"/>
+      <c r="J28" s="43"/>
+    </row>
+    <row r="29" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="15">
         <f>B28+2</f>
@@ -1895,17 +1933,18 @@
         <v>Thu</v>
       </c>
       <c r="D29" s="85" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F29" s="17"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="43"/>
-    </row>
-    <row r="30" spans="1:9" ht="31.5">
+      <c r="G29" s="17"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="43"/>
+    </row>
+    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>3</v>
       </c>
@@ -1917,11 +1956,12 @@
         <v>Mon</v>
       </c>
       <c r="D30" s="86" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="13"/>
-      <c r="H30" s="26"/>
+      <c r="G30" s="13"/>
+      <c r="I30" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update syllabus, wk02 and 03
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
   <si>
     <t>date</t>
   </si>
@@ -258,19 +258,26 @@
 * [Literature Review notes](docs/lec_lit_review.html)</t>
   </si>
   <si>
+    <t>wknum</t>
+  </si>
+  <si>
+    <t>Blog about data cleaning preparation (Due Thu: 8/31) 
+* Data management code file (Due 9/4)
+* Citation [Assignment](hw/Citation_Assignment.html) (Due 9/7)</t>
+  </si>
+  <si>
+    <t>[PMA6 Data Viz ch DRAFT](docs/pma6_ch4_draft.pdf)
+* [Data Viz tutorial](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
+*[dsmall data](https://norcalbiostat.netlify.com/data/cleaned_data/)
+* [Data Screening](docs/lec03_data_screen.html) notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
 * Blog RR plan  (Due 8/28)
 * Blog area of Add Health research interest (Due 8/25) 
 * Personal Codebook/ Research Question [Assignment](hw/RQ_personal_codebook_assignment.html)   (Due 8/28)
+* [Peer Review](project.html) of RQ post (New: Due 9/4)
 </t>
-  </si>
-  <si>
-    <t>wknum</t>
-  </si>
-  <si>
-    <t>Blog about data cleaning preparation (Due Thu: 8/31) 
-* Data management code file (Due 9/4)
-* Citation [Assignment](hw/Citation_Assignment.html) (Due 9/7)</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1255,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1274,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>0</v>
@@ -1319,7 +1326,7 @@
         <v>70</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I2" s="62"/>
     </row>
@@ -1349,11 +1356,11 @@
         <v>71</v>
       </c>
       <c r="H3" s="60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3" s="63"/>
     </row>
-    <row r="4" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
         <f>A3+1</f>
         <v>3</v>
@@ -1375,7 +1382,9 @@
       <c r="F4" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="61"/>
+      <c r="G4" s="61" t="s">
+        <v>74</v>
+      </c>
       <c r="H4" s="68" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
add PR to schedule
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -60,9 +60,6 @@
     <t>Writing about empirical research</t>
   </si>
   <si>
-    <t>Research plan outline (Due 9/18)</t>
-  </si>
-  <si>
     <t>20 min lecture, start assignment (20 min),  rest open analysis time</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
   </si>
   <si>
     <t>Demonstrate how to do,then go do it</t>
-  </si>
-  <si>
-    <t>Bivariate graphing assignment (Due 9/25)</t>
   </si>
   <si>
     <t>Choosing appropriate analyses</t>
@@ -218,9 +212,6 @@
   <si>
     <t>T: univariate graphics (45 min on graph types). rest of class on creating them in SPC
 R: transformations (10-15 min). Rest of class on graphing assignment</t>
-  </si>
-  <si>
-    <t>Univariate graphing assignment (Due 9/18)</t>
   </si>
   <si>
     <t>Posters Due 12/6</t>
@@ -259,11 +250,6 @@
   </si>
   <si>
     <t>wknum</t>
-  </si>
-  <si>
-    <t>Blog about data cleaning preparation (Due Thu: 8/31) 
-* Data management code file (Due 9/4)
-* Citation [Assignment](hw/Citation_Assignment.html) (Due 9/7)</t>
   </si>
   <si>
     <t>[PMA6 Data Viz ch DRAFT](docs/pma6_ch4_draft.pdf)
@@ -278,6 +264,25 @@
 * Personal Codebook/ Research Question [Assignment](hw/RQ_personal_codebook_assignment.html)   (Due 8/28)
 * [Peer Review](project.html) of RQ post (New: Due 9/4)
 </t>
+  </si>
+  <si>
+    <t>Blog about data management preparation (Due Thu: 8/31) 
+* Peer Review of DM blog post (Due 9/4)
+* Data management code file (Due 9/4)
+* Citation [Assignment](hw/Citation_Assignment.html) (Due 9/7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univariate graphing assignment (Due 9/13)
+* Peer Revew (Due 9/18)
+</t>
+  </si>
+  <si>
+    <t>Research plan outline (Due 9/18)
+* Peer Review (Due 9/20)</t>
+  </si>
+  <si>
+    <t>Bivariate graphing assignment (Due 9/25)
+* Peer Review (Due 10/2)</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1274,7 +1279,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>0</v>
@@ -1292,7 +1297,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>6</v>
@@ -1314,19 +1319,19 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="73" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" s="62" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="56" t="s">
-        <v>70</v>
-      </c>
       <c r="H2" s="57" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I2" s="62"/>
     </row>
@@ -1344,19 +1349,19 @@
         <v>Tue</v>
       </c>
       <c r="D3" s="76" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="59" t="s">
-        <v>71</v>
-      </c>
       <c r="H3" s="60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I3" s="63"/>
     </row>
@@ -1374,19 +1379,19 @@
         <v>Tue</v>
       </c>
       <c r="D4" s="79" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="61" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H4" s="68" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="I4" s="26"/>
     </row>
@@ -1407,13 +1412,13 @@
         <v>10</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" s="69" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="I5" s="37"/>
     </row>
@@ -1428,7 +1433,7 @@
         <v>Thu</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="9"/>
@@ -1451,16 +1456,16 @@
         <v>Tue</v>
       </c>
       <c r="D7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="I7" s="37"/>
     </row>
@@ -1475,10 +1480,10 @@
         <v>Thu</v>
       </c>
       <c r="D8" s="80" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="82"/>
       <c r="G8" s="82"/>
@@ -1499,16 +1504,16 @@
         <v>Tue</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H9" s="54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I9" s="26"/>
     </row>
@@ -1523,7 +1528,7 @@
         <v>Thu</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="9"/>
@@ -1545,14 +1550,14 @@
         <v>Tue</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="29"/>
       <c r="F11" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H11" s="54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I11" s="26"/>
     </row>
@@ -1567,13 +1572,13 @@
         <v>Thu</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="53" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I12" s="27"/>
     </row>
@@ -1590,14 +1595,14 @@
         <v>Tue</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H13" s="54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I13" s="26"/>
     </row>
@@ -1612,7 +1617,7 @@
         <v>Thu</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="9"/>
@@ -1634,14 +1639,14 @@
         <v>Tue</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H15" s="54" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I15" s="26"/>
     </row>
@@ -1656,7 +1661,7 @@
         <v>Thu</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" s="9"/>
@@ -1679,14 +1684,14 @@
         <v>Tue</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" s="42"/>
       <c r="F17" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H17" s="54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I17" s="42"/>
     </row>
@@ -1701,7 +1706,7 @@
         <v>Thu</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18" s="27"/>
       <c r="F18" s="9"/>
@@ -1723,14 +1728,14 @@
         <v>Tue</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H19" s="54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I19" s="26"/>
     </row>
@@ -1745,7 +1750,7 @@
         <v>Thu</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" s="30"/>
       <c r="F20" s="9"/>
@@ -1767,14 +1772,14 @@
         <v>Tue</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" s="31"/>
       <c r="F21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H21" s="54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I21" s="35"/>
     </row>
@@ -1789,7 +1794,7 @@
         <v>Thu</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E22" s="30"/>
       <c r="F22" s="9"/>
@@ -1811,14 +1816,14 @@
         <v>Tue</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E23" s="31"/>
       <c r="F23" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H23" s="54" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I23" s="26"/>
     </row>
@@ -1833,7 +1838,7 @@
         <v>Thu</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="9"/>
@@ -1874,14 +1879,14 @@
         <v>Tue</v>
       </c>
       <c r="D26" s="67" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H26" s="54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I26" s="35"/>
     </row>
@@ -1896,7 +1901,7 @@
         <v>Thu</v>
       </c>
       <c r="D27" s="65" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E27" s="33"/>
       <c r="F27" s="9"/>
@@ -1919,14 +1924,14 @@
         <v>Tue</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H28" s="54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I28" s="35"/>
       <c r="J28" s="43"/>
@@ -1942,10 +1947,10 @@
         <v>Thu</v>
       </c>
       <c r="D29" s="85" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
@@ -1965,7 +1970,7 @@
         <v>Mon</v>
       </c>
       <c r="D30" s="86" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="13"/>

</xml_diff>

<commit_message>
clean up dm file names
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -244,11 +244,6 @@
 * [Introduction to the class](docs/lec01_intro_class.html)</t>
   </si>
   <si>
-    <t>[Notes on Data Preparation](docs/lec02_data_prep.html)
-* [How to read a Journal Article](docs/How to Read a Journal Article.pdf)
-* [Literature Review notes](docs/lec_lit_review.html)</t>
-  </si>
-  <si>
     <t>wknum</t>
   </si>
   <si>
@@ -258,31 +253,37 @@
 * [Data Screening](docs/lec03_data_screen.html) notes</t>
   </si>
   <si>
+    <t xml:space="preserve">Univariate graphing assignment (Due 9/13)
+* Peer Revew (Due 9/18)
+</t>
+  </si>
+  <si>
+    <t>Research plan outline (Due 9/18)
+* Peer Review (Due 9/20)</t>
+  </si>
+  <si>
+    <t>Bivariate graphing assignment (Due 9/25)
+* Peer Review (Due 10/2)</t>
+  </si>
+  <si>
+    <t>[Data Management preparation questions](docs/dm_prep_qs.html)
+* [Doing Data Management](docs/lec02_doing_dm.html)
+* [How to read a Journal Article](docs/How to Read a Journal Article.pdf)
+* [Literature Review notes](docs/lec_lit_review.html)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
 * Blog RR plan  (Due 8/28)
 * Blog area of Add Health research interest (Due 8/25) 
 * Personal Codebook/ Research Question [Assignment](hw/RQ_personal_codebook_assignment.html)   (Due 8/28)
-* [Peer Review](project.html) of RQ post (New: Due 9/4)
 </t>
   </si>
   <si>
-    <t>Blog about data management preparation (Due Thu: 8/31) 
+    <t>[Peer Review](project.html) of RQ post (Due 9/4)
+* Blog about data management preparation (Due Thu: 8/31) 
 * Peer Review of DM blog post (Due 9/4)
 * Data management code file (Due 9/4)
 * Citation [Assignment](hw/Citation_Assignment.html) (Due 9/7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Univariate graphing assignment (Due 9/13)
-* Peer Revew (Due 9/18)
-</t>
-  </si>
-  <si>
-    <t>Research plan outline (Due 9/18)
-* Peer Review (Due 9/20)</t>
-  </si>
-  <si>
-    <t>Bivariate graphing assignment (Due 9/25)
-* Peer Review (Due 10/2)</t>
   </si>
 </sst>
 </file>
@@ -1259,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1280,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>0</v>
@@ -1331,11 +1332,11 @@
         <v>67</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I2" s="62"/>
     </row>
-    <row r="3" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="126" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <f>A2+1</f>
         <v>2</v>
@@ -1358,10 +1359,10 @@
         <v>65</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H3" s="60" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I3" s="63"/>
     </row>
@@ -1388,10 +1389,10 @@
         <v>66</v>
       </c>
       <c r="G4" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="68" t="s">
         <v>70</v>
-      </c>
-      <c r="H4" s="68" t="s">
-        <v>73</v>
       </c>
       <c r="I4" s="26"/>
     </row>
@@ -1418,7 +1419,7 @@
         <v>33</v>
       </c>
       <c r="H5" s="69" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I5" s="37"/>
     </row>
@@ -1465,7 +1466,7 @@
         <v>32</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I7" s="37"/>
     </row>

</xml_diff>

<commit_message>
add wk4, adj wk3
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>date</t>
   </si>
@@ -247,12 +247,6 @@
     <t>wknum</t>
   </si>
   <si>
-    <t>[PMA6 Data Viz ch DRAFT](docs/pma6_ch4_draft.pdf)
-* [Data Viz tutorial](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
-*[dsmall data](https://norcalbiostat.netlify.com/data/cleaned_data/)
-* [Data Screening](docs/lec03_data_screen.html) notes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Univariate graphing assignment (Due 9/13)
 * Peer Revew (Due 9/18)
 </t>
@@ -264,12 +258,6 @@
   <si>
     <t>Bivariate graphing assignment (Due 9/25)
 * Peer Review (Due 10/2)</t>
-  </si>
-  <si>
-    <t>[Data Management preparation questions](docs/dm_prep_qs.html)
-* [Doing Data Management](docs/lec02_doing_dm.html)
-* [How to read a Journal Article](docs/How to Read a Journal Article.pdf)
-* [Literature Review notes](docs/lec_lit_review.html)</t>
   </si>
   <si>
     <t xml:space="preserve">Blog Intro/Bio (Due 8/28)
@@ -284,6 +272,21 @@
 * Peer Review of DM blog post (Due 9/4)
 * Data management code file (Due 9/4)
 * Citation [Assignment](hw/Citation_Assignment.html) (Due 9/7)</t>
+  </si>
+  <si>
+    <t>[PMA6 Data Viz ch DRAFT](docs/pma6_ch4_draft.pdf)
+* [Data Viz tutorial](https://norcalbiostat.github.io/MATH130/materials/day56-data-viz.html)
+* [dsmall data](https://norcalbiostat.netlify.com/data/cleaned_data/)
+* [Data Screening](docs/lec03_data_screen.html) notes</t>
+  </si>
+  <si>
+    <t>[Data Management preparation questions](docs/dm_prep_qs.html)
+* [Doing Data Management](http://www.norcalbiostat.com/lec/lec_doing_dm.html)
+* [How to read a Journal Article](docs/How to Read a Journal Article.pdf)
+* [Literature Review notes](http://www.norcalbiostat.com/lec/lec_lit_review.html)</t>
+  </si>
+  <si>
+    <t>[Writing about empirical research](http://www.norcalbiostat.com/lec/lec_writing_em.html)</t>
   </si>
 </sst>
 </file>
@@ -367,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +410,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,7 +580,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -829,6 +838,30 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1261,7 +1294,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1332,11 +1365,11 @@
         <v>67</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I2" s="62"/>
     </row>
-    <row r="3" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <f>A2+1</f>
         <v>2</v>
@@ -1359,10 +1392,10 @@
         <v>65</v>
       </c>
       <c r="G3" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="60" t="s">
         <v>73</v>
-      </c>
-      <c r="H3" s="60" t="s">
-        <v>75</v>
       </c>
       <c r="I3" s="63"/>
     </row>
@@ -1389,27 +1422,27 @@
         <v>66</v>
       </c>
       <c r="G4" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="68" t="s">
-        <v>70</v>
-      </c>
       <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="87">
         <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="88">
         <f>B4+7</f>
         <v>41528</v>
       </c>
-      <c r="C5" s="4" t="str">
+      <c r="C5" s="89" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="90" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="35" t="s">
@@ -1418,22 +1451,25 @@
       <c r="F5" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="G5" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="H5" s="69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I5" s="37"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7">
+      <c r="A6" s="91"/>
+      <c r="B6" s="92">
         <f>B5+2</f>
         <v>41530</v>
       </c>
-      <c r="C6" s="8" t="str">
+      <c r="C6" s="93" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="94" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="27"/>
@@ -1466,7 +1502,7 @@
         <v>32</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I7" s="37"/>
     </row>

</xml_diff>

<commit_message>
adjust research plan outline submission instructions. fix links
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -247,11 +247,6 @@
     <t>wknum</t>
   </si>
   <si>
-    <t xml:space="preserve">Univariate graphing assignment (Due 9/13)
-* Peer Revew (Due 9/18)
-</t>
-  </si>
-  <si>
     <t>Research plan outline (Due 9/18)
 * Peer Review (Due 9/20)</t>
   </si>
@@ -287,6 +282,11 @@
 * [Doing Data Management](http://www.norcalbiostat.com/lec/doing-dm)
 * [How to read a Journal Article](docs/How to Read a Journal Article.pdf)
 * [Literature Review notes](http://www.norcalbiostat.com/lec/lec_lit_review.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univariate graphing [Assignment](hw/Univ_Graphing.html) (Due 9/13)
+* Peer Revew (Due 9/18)
+</t>
   </si>
 </sst>
 </file>
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1365,7 @@
         <v>67</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I2" s="62"/>
     </row>
@@ -1392,10 +1392,10 @@
         <v>65</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3" s="60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I3" s="63"/>
     </row>
@@ -1422,10 +1422,10 @@
         <v>66</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H4" s="68" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I4" s="26"/>
     </row>
@@ -1452,10 +1452,10 @@
         <v>33</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" s="37"/>
     </row>
@@ -1502,7 +1502,7 @@
         <v>32</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="37"/>
     </row>

</xml_diff>

<commit_message>
add bivariate graphing assignment. not linked yet.
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -415,7 +415,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -953,8 +953,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1290,11 +1290,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add wk5, update research plan  outline
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -370,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,12 +398,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +574,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -789,79 +783,70 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -953,8 +938,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1290,11 +1275,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1342,17 +1327,17 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="70">
+      <c r="A2" s="77">
         <v>1</v>
       </c>
-      <c r="B2" s="71">
+      <c r="B2" s="85">
         <v>41507</v>
       </c>
-      <c r="C2" s="72" t="str">
+      <c r="C2" s="86" t="str">
         <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="87" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="62" t="s">
@@ -1370,19 +1355,19 @@
       <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="70">
+      <c r="A3" s="77">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="74">
+      <c r="B3" s="88">
         <f>B2+7</f>
         <v>41514</v>
       </c>
-      <c r="C3" s="75" t="str">
+      <c r="C3" s="89" t="str">
         <f>TEXT(WEEKDAY(B3,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="90" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="63" t="s">
@@ -1400,19 +1385,19 @@
       <c r="I3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="70">
+      <c r="A4" s="77">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="77">
+      <c r="B4" s="78">
         <f>B3+7</f>
         <v>41521</v>
       </c>
-      <c r="C4" s="78" t="str">
+      <c r="C4" s="79" t="str">
         <f t="shared" ref="C4:C21" si="0">TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="91" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="64" t="s">
@@ -1430,19 +1415,19 @@
       <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="87">
+      <c r="A5" s="77">
         <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="88">
+      <c r="B5" s="78">
         <f>B4+7</f>
         <v>41528</v>
       </c>
-      <c r="C5" s="89" t="str">
+      <c r="C5" s="79" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D5" s="90" t="s">
+      <c r="D5" s="80" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="35" t="s">
@@ -1460,16 +1445,16 @@
       <c r="I5" s="37"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92">
+      <c r="A6" s="81"/>
+      <c r="B6" s="82">
         <f>B5+2</f>
         <v>41530</v>
       </c>
-      <c r="C6" s="93" t="str">
+      <c r="C6" s="83" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D6" s="94" t="s">
+      <c r="D6" s="84" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="27"/>
@@ -1516,16 +1501,16 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="84"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="74"/>
     </row>
     <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1983,7 +1968,7 @@
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D29" s="85" t="s">
+      <c r="D29" s="75" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="28" t="s">
@@ -2006,7 +1991,7 @@
         <f t="shared" si="3"/>
         <v>Mon</v>
       </c>
-      <c r="D30" s="86" t="s">
+      <c r="D30" s="76" t="s">
         <v>62</v>
       </c>
       <c r="E30" s="26"/>

</xml_diff>

<commit_message>
update project page and add poster prep page
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>date</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Exploring bivariate relationships</t>
   </si>
   <si>
-    <t>Demonstrate how to do,then go do it</t>
-  </si>
-  <si>
-    <t>Choosing appropriate analyses</t>
-  </si>
-  <si>
     <t>Afifi chapter 5</t>
   </si>
   <si>
@@ -147,46 +141,22 @@
     <t>Moderating and Confounding</t>
   </si>
   <si>
-    <t>Midterm</t>
-  </si>
-  <si>
     <t>Flex time</t>
   </si>
   <si>
     <t>Correlation and Regression</t>
   </si>
   <si>
-    <t>Bivariate Inference (Due 10/30)</t>
-  </si>
-  <si>
     <t>Multiple Regression Assignment (Due 11/13)</t>
   </si>
   <si>
     <t>Logistic Regression Assignment (Due 11/27)</t>
   </si>
   <si>
-    <t>Progress check in blog post (Due 10/23)</t>
-  </si>
-  <si>
-    <t>Progress check in blog post (Due 10/2)</t>
-  </si>
-  <si>
-    <t>Progress check in blog post (Due 10/30)</t>
-  </si>
-  <si>
-    <t>Progress check in blog post (Due 11/13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progress check in blog post (Due Thursday 11/30) </t>
-  </si>
-  <si>
     <t>Special Regression Topics</t>
   </si>
   <si>
     <t>Impacts of sampling design</t>
-  </si>
-  <si>
-    <t>I won't be here - Edward Cover</t>
   </si>
   <si>
     <t>Introduction to the class
@@ -287,6 +257,30 @@
     <t xml:space="preserve">Univariate graphing [Assignment](hw/Univ_Graphing.html) (Due 9/13)
 * Peer Revew (Due 9/18)
 </t>
+  </si>
+  <si>
+    <t>Poster draft due (12/1)
+* PR poster draft (12/4)</t>
+  </si>
+  <si>
+    <t>Poster prep I (Due 10/6)
+* Peer Review (Due 10/11)</t>
+  </si>
+  <si>
+    <t>Bivariate Inference Assignment (Due 10/25)
+* Poster Prep: Stage II (Due 10/30)
+* Peer Review: Stage II (Due 11/1)</t>
+  </si>
+  <si>
+    <t>Poster Prep: Stage III (Due 11/15)
+* Peer Review: Stage III (Due 11/17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demonstrate how to do,then go do it. Analysis work time on Thursday. Edward Cover. </t>
+  </si>
+  <si>
+    <t>Choosing appropriate analyses
+* Midterm Thu</t>
   </si>
 </sst>
 </file>
@@ -370,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,12 +392,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,7 +562,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -771,9 +759,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -783,70 +768,43 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1276,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1256,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>0</v>
@@ -1316,7 +1274,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>6</v>
@@ -1327,677 +1285,611 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="77">
+      <c r="A2" s="71">
         <v>1</v>
       </c>
-      <c r="B2" s="85">
+      <c r="B2" s="75">
         <v>41507</v>
       </c>
-      <c r="C2" s="86" t="str">
+      <c r="C2" s="76" t="str">
         <f>TEXT(WEEKDAY(B2,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D2" s="87" t="s">
-        <v>54</v>
+      <c r="D2" s="77" t="s">
+        <v>44</v>
       </c>
       <c r="E2" s="62" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="56" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G2" s="56" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="77">
+      <c r="A3" s="71">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="88">
+      <c r="B3" s="78">
         <f>B2+7</f>
         <v>41514</v>
       </c>
-      <c r="C3" s="89" t="str">
+      <c r="C3" s="79" t="str">
         <f>TEXT(WEEKDAY(B3,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D3" s="90" t="s">
-        <v>56</v>
+      <c r="D3" s="80" t="s">
+        <v>46</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F3" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="59" t="s">
-        <v>75</v>
-      </c>
       <c r="H3" s="60" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="I3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="77">
+      <c r="A4" s="71">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="72">
         <f>B3+7</f>
         <v>41521</v>
       </c>
-      <c r="C4" s="79" t="str">
-        <f t="shared" ref="C4:C21" si="0">TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
+      <c r="C4" s="73" t="str">
+        <f t="shared" ref="C4:C18" si="0">TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D4" s="91" t="s">
-        <v>58</v>
+      <c r="D4" s="81" t="s">
+        <v>48</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F4" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="68" t="s">
-        <v>76</v>
-      </c>
       <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="77">
+      <c r="A5" s="71">
         <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="72">
         <f>B4+7</f>
         <v>41528</v>
       </c>
-      <c r="C5" s="79" t="str">
+      <c r="C5" s="73" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="74" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="69" t="s">
-        <v>69</v>
+        <v>64</v>
+      </c>
+      <c r="H5" s="68" t="s">
+        <v>59</v>
       </c>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="81"/>
-      <c r="B6" s="82">
-        <f>B5+2</f>
-        <v>41530</v>
-      </c>
-      <c r="C6" s="83" t="str">
+    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="36">
+        <f>B5+7</f>
+        <v>41535</v>
+      </c>
+      <c r="C6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Tue</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="37"/>
+    </row>
+    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f>A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <f>B6+7</f>
+        <v>41542</v>
+      </c>
+      <c r="C7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Tue</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f>A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <f>B7+7</f>
+        <v>41549</v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Tue</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="26"/>
+    </row>
+    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7">
+        <f>B8+2</f>
+        <v>41551</v>
+      </c>
+      <c r="C9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D6" s="84" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="24"/>
-    </row>
-    <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <f>A5+1</f>
-        <v>5</v>
-      </c>
-      <c r="B7" s="36">
-        <f>B5+7</f>
-        <v>41535</v>
-      </c>
-      <c r="C7" s="12" t="str">
+      <c r="D9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B8+7</f>
+        <v>41556</v>
+      </c>
+      <c r="C10" s="4" t="str">
+        <f t="shared" ref="C10:C11" si="1">TEXT(WEEKDAY(B10,1)+1, "ddd")</f>
+        <v>Tue</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7">
+        <f>B10+2</f>
+        <v>41558</v>
+      </c>
+      <c r="C11" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Thu</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" ref="A12:A20" si="2">A10+1</f>
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <f>B10+7</f>
+        <v>41563</v>
+      </c>
+      <c r="C12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="37"/>
-    </row>
-    <row r="8" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7">
-        <f>B7+2</f>
-        <v>41537</v>
-      </c>
-      <c r="C8" s="8" t="str">
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7">
+        <f>B12+2</f>
+        <v>41565</v>
+      </c>
+      <c r="C13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D8" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="74"/>
-    </row>
-    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <f t="shared" ref="A9:A23" si="1">A7+1</f>
-        <v>6</v>
-      </c>
-      <c r="B9" s="3">
-        <f>B7+7</f>
-        <v>41542</v>
-      </c>
-      <c r="C9" s="4" t="str">
+      <c r="D13" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="24"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="39">
+        <f>B12+7</f>
+        <v>41570</v>
+      </c>
+      <c r="C14" s="40" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="26"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7">
-        <f>B9+2</f>
-        <v>41544</v>
-      </c>
-      <c r="C10" s="8" t="str">
+      <c r="D14" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="42"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7">
+        <f>B14+2</f>
+        <v>41572</v>
+      </c>
+      <c r="C15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D10" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B11" s="3">
-        <f>B9+7</f>
-        <v>41549</v>
-      </c>
-      <c r="C11" s="4" t="str">
+      <c r="D15" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B16" s="3">
+        <f>B14+7</f>
+        <v>41577</v>
+      </c>
+      <c r="C16" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7">
-        <f>B11+2</f>
-        <v>41551</v>
-      </c>
-      <c r="C12" s="8" t="str">
+      <c r="D16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7">
+        <f>B16+2</f>
+        <v>41579</v>
+      </c>
+      <c r="C17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="27"/>
-    </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3">
-        <f>B11+7</f>
-        <v>41556</v>
-      </c>
-      <c r="C13" s="4" t="str">
-        <f t="shared" ref="C13:C14" si="2">TEXT(WEEKDAY(B13,1)+1, "ddd")</f>
-        <v>Tue</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7">
-        <f>B13+2</f>
-        <v>41558</v>
-      </c>
-      <c r="C14" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>Thu</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="27"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B15" s="3">
-        <f>B13+7</f>
-        <v>41563</v>
-      </c>
-      <c r="C15" s="4" t="str">
+      <c r="D17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <f>A16+1</f>
+        <v>12</v>
+      </c>
+      <c r="B18" s="36">
+        <f>B16+7</f>
+        <v>41584</v>
+      </c>
+      <c r="C18" s="12" t="str">
         <f t="shared" si="0"/>
         <v>Tue</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D18" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7">
+        <f>B18+2</f>
+        <v>41586</v>
+      </c>
+      <c r="C19" s="8" t="str">
+        <f>TEXT(WEEKDAY(B19,1)+1, "ddd")</f>
+        <v>Thu</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="30"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B20" s="3">
+        <f>B18+7</f>
+        <v>41591</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f>TEXT(WEEKDAY(B20,1)+1, "ddd")</f>
+        <v>Tue</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="26"/>
-    </row>
-    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7">
-        <f>B15+2</f>
-        <v>41565</v>
-      </c>
-      <c r="C16" s="8" t="str">
-        <f t="shared" si="0"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7">
+        <f>B20+2</f>
+        <v>41593</v>
+      </c>
+      <c r="C21" s="8" t="str">
+        <f t="shared" ref="C21:C27" si="3">TEXT(WEEKDAY(B21,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D21" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="30"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="45">
+        <f>B20+7</f>
+        <v>41598</v>
+      </c>
+      <c r="C22" s="46" t="str">
+        <f t="shared" si="3"/>
+        <v>Tue</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>14</v>
+      </c>
+      <c r="B23" s="3">
+        <f>B22+7</f>
+        <v>41605</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Tue</v>
+      </c>
+      <c r="D23" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="24"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B17" s="39">
-        <f>B15+7</f>
-        <v>41570</v>
-      </c>
-      <c r="C17" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>Tue</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" s="42"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7">
-        <f>B17+2</f>
-        <v>41572</v>
-      </c>
-      <c r="C18" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Thu</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="27"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B19" s="3">
-        <f>B17+7</f>
-        <v>41577</v>
-      </c>
-      <c r="C19" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Tue</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" s="26"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7">
-        <f>B19+2</f>
-        <v>41579</v>
-      </c>
-      <c r="C20" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>Thu</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="27"/>
-    </row>
-    <row r="21" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <f>A19+1</f>
-        <v>12</v>
-      </c>
-      <c r="B21" s="36">
-        <f>B19+7</f>
-        <v>41584</v>
-      </c>
-      <c r="C21" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>Tue</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="35"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7">
-        <f>B21+2</f>
-        <v>41586</v>
-      </c>
-      <c r="C22" s="8" t="str">
-        <f>TEXT(WEEKDAY(B22,1)+1, "ddd")</f>
-        <v>Thu</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="27"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B23" s="3">
-        <f>B21+7</f>
-        <v>41591</v>
-      </c>
-      <c r="C23" s="4" t="str">
-        <f>TEXT(WEEKDAY(B23,1)+1, "ddd")</f>
-        <v>Tue</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="31"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H23" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="I23" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="I23" s="35"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7">
         <f>B23+2</f>
-        <v>41593</v>
+        <v>41607</v>
       </c>
       <c r="C24" s="8" t="str">
-        <f t="shared" ref="C24:C30" si="3">TEXT(WEEKDAY(B24,1)+1, "ddd")</f>
+        <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
       <c r="D24" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="30"/>
+        <v>22</v>
+      </c>
+      <c r="E24" s="33"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="53"/>
-      <c r="I24" s="30"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="45">
+      <c r="I24" s="27"/>
+      <c r="J24" s="43"/>
+    </row>
+    <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <f>A23+1</f>
+        <v>15</v>
+      </c>
+      <c r="B25" s="3">
         <f>B23+7</f>
-        <v>41598</v>
-      </c>
-      <c r="C25" s="46" t="str">
+        <v>41612</v>
+      </c>
+      <c r="C25" s="12" t="str">
         <f t="shared" si="3"/>
         <v>Tue</v>
       </c>
-      <c r="D25" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="48"/>
+      <c r="D25" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="26"/>
+      <c r="F25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="35"/>
       <c r="J25" s="43"/>
     </row>
-    <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>14</v>
-      </c>
-      <c r="B26" s="3">
-        <f>B25+7</f>
-        <v>41605</v>
-      </c>
-      <c r="C26" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>Tue</v>
-      </c>
-      <c r="D26" s="67" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H26" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="35"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7">
-        <f>B26+2</f>
-        <v>41607</v>
-      </c>
-      <c r="C27" s="8" t="str">
+    <row r="26" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15">
+        <f>B25+2</f>
+        <v>41614</v>
+      </c>
+      <c r="C26" s="16" t="str">
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D27" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="43"/>
-    </row>
-    <row r="28" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
-        <f>A26+1</f>
-        <v>15</v>
-      </c>
-      <c r="B28" s="3">
-        <f>B26+7</f>
-        <v>41612</v>
-      </c>
-      <c r="C28" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v>Tue</v>
-      </c>
-      <c r="D28" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="I28" s="35"/>
-      <c r="J28" s="43"/>
-    </row>
-    <row r="29" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15">
-        <f>B28+2</f>
-        <v>41614</v>
-      </c>
-      <c r="C29" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>Thu</v>
-      </c>
-      <c r="D29" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="43"/>
-    </row>
-    <row r="30" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="D26" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="43"/>
+    </row>
+    <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B27" s="3">
         <v>41625</v>
       </c>
-      <c r="C30" s="4" t="str">
+      <c r="C27" s="4" t="str">
         <f t="shared" si="3"/>
         <v>Mon</v>
       </c>
-      <c r="D30" s="76" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="26"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="I30" s="26"/>
+      <c r="D27" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="26"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="I27" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add wk6, merge project pages. add link to schedule.
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>date</t>
   </si>
@@ -282,11 +282,14 @@
     <t>Choosing appropriate analyses
 * Midterm Thu</t>
   </si>
+  <si>
+    <t>[Project page](https://norcalbiostat.github.io/MATH615/project.html)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -896,8 +899,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1233,10 +1236,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1314,11 +1317,11 @@
     </row>
     <row r="3" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A3" s="71">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A8" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="78">
-        <f>B2+7</f>
+        <f t="shared" ref="B3:B8" si="1">B2+7</f>
         <v>41514</v>
       </c>
       <c r="C3" s="79" t="str">
@@ -1344,15 +1347,15 @@
     </row>
     <row r="4" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="72">
-        <f>B3+7</f>
+        <f t="shared" si="1"/>
         <v>41521</v>
       </c>
       <c r="C4" s="73" t="str">
-        <f t="shared" ref="C4:C18" si="0">TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
+        <f t="shared" ref="C4:C18" si="2">TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
       <c r="D4" s="81" t="s">
@@ -1374,15 +1377,15 @@
     </row>
     <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="72">
-        <f>B4+7</f>
+        <f t="shared" si="1"/>
         <v>41528</v>
       </c>
       <c r="C5" s="73" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D5" s="74" t="s">
@@ -1404,15 +1407,15 @@
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="36">
-        <f>B5+7</f>
+        <f t="shared" si="1"/>
         <v>41535</v>
       </c>
       <c r="C6" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -1431,15 +1434,15 @@
     </row>
     <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <f>B6+7</f>
+        <f t="shared" si="1"/>
         <v>41542</v>
       </c>
       <c r="C7" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D7" s="19" t="s">
@@ -1451,6 +1454,9 @@
       <c r="F7" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="G7" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="H7" s="54" t="s">
         <v>68</v>
       </c>
@@ -1458,15 +1464,15 @@
     </row>
     <row r="8" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <f>B7+7</f>
+        <f t="shared" si="1"/>
         <v>41549</v>
       </c>
       <c r="C8" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -1488,7 +1494,7 @@
         <v>41551</v>
       </c>
       <c r="C9" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -1511,7 +1517,7 @@
         <v>41556</v>
       </c>
       <c r="C10" s="4" t="str">
-        <f t="shared" ref="C10:C11" si="1">TEXT(WEEKDAY(B10,1)+1, "ddd")</f>
+        <f t="shared" ref="C10:C11" si="3">TEXT(WEEKDAY(B10,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -1533,7 +1539,7 @@
         <v>41558</v>
       </c>
       <c r="C11" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
       <c r="D11" s="18" t="s">
@@ -1547,7 +1553,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" ref="A12:A20" si="2">A10+1</f>
+        <f t="shared" ref="A12:A20" si="4">A10+1</f>
         <v>9</v>
       </c>
       <c r="B12" s="3">
@@ -1555,7 +1561,7 @@
         <v>41563</v>
       </c>
       <c r="C12" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -1574,7 +1580,7 @@
         <v>41565</v>
       </c>
       <c r="C13" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
       <c r="D13" s="58" t="s">
@@ -1589,7 +1595,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="B14" s="39">
@@ -1597,7 +1603,7 @@
         <v>41570</v>
       </c>
       <c r="C14" s="40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D14" s="41" t="s">
@@ -1616,7 +1622,7 @@
         <v>41572</v>
       </c>
       <c r="C15" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
       <c r="D15" s="65" t="s">
@@ -1630,7 +1636,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="B16" s="3">
@@ -1638,7 +1644,7 @@
         <v>41577</v>
       </c>
       <c r="C16" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D16" s="20" t="s">
@@ -1660,7 +1666,7 @@
         <v>41579</v>
       </c>
       <c r="C17" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -1682,7 +1688,7 @@
         <v>41584</v>
       </c>
       <c r="C18" s="12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D18" s="20" t="s">
@@ -1718,7 +1724,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="B20" s="3">
@@ -1748,7 +1754,7 @@
         <v>41593</v>
       </c>
       <c r="C21" s="8" t="str">
-        <f t="shared" ref="C21:C27" si="3">TEXT(WEEKDAY(B21,1)+1, "ddd")</f>
+        <f t="shared" ref="C21:C27" si="5">TEXT(WEEKDAY(B21,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
       <c r="D21" s="65" t="s">
@@ -1767,7 +1773,7 @@
         <v>41598</v>
       </c>
       <c r="C22" s="46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
       <c r="D22" s="47" t="s">
@@ -1789,7 +1795,7 @@
         <v>41605</v>
       </c>
       <c r="C23" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
       <c r="D23" s="66" t="s">
@@ -1811,7 +1817,7 @@
         <v>41607</v>
       </c>
       <c r="C24" s="8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Thu</v>
       </c>
       <c r="D24" s="65" t="s">
@@ -1834,7 +1840,7 @@
         <v>41612</v>
       </c>
       <c r="C25" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
       <c r="D25" s="66" t="s">
@@ -1857,7 +1863,7 @@
         <v>41614</v>
       </c>
       <c r="C26" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Thu</v>
       </c>
       <c r="D26" s="69" t="s">
@@ -1880,7 +1886,7 @@
         <v>41625</v>
       </c>
       <c r="C27" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
       <c r="D27" s="70" t="s">

</xml_diff>

<commit_message>
update index and schedule
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -263,10 +258,6 @@
 * PR poster draft (12/4)</t>
   </si>
   <si>
-    <t>Poster prep I (Due 10/6)
-* Peer Review (Due 10/11)</t>
-  </si>
-  <si>
     <t>Bivariate Inference Assignment (Due 10/25)
 * Poster Prep: Stage II (Due 10/30)
 * Peer Review: Stage II (Due 11/1)</t>
@@ -284,18 +275,24 @@
   </si>
   <si>
     <t>[Project page](https://norcalbiostat.github.io/MATH615/project.html)</t>
+  </si>
+  <si>
+    <t>Poster prep I (Due 10/6)
+* Peer Review (Due 10/11)
+* Error Assessment (Due 10/6)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1239,25 +1236,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2"/>
-    <col min="3" max="3" width="4.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="21" customWidth="1"/>
-    <col min="6" max="6" width="27.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.1640625" style="54" customWidth="1"/>
     <col min="9" max="9" width="39.5" style="21" customWidth="1"/>
-    <col min="10" max="16384" width="10.875" style="2"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.5" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>58</v>
       </c>
@@ -1287,7 +1284,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="141.75">
       <c r="A2" s="71">
         <v>1</v>
       </c>
@@ -1315,7 +1312,7 @@
       </c>
       <c r="I2" s="62"/>
     </row>
-    <row r="3" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="157.5">
       <c r="A3" s="71">
         <f t="shared" ref="A3:A8" si="0">A2+1</f>
         <v>2</v>
@@ -1345,7 +1342,7 @@
       </c>
       <c r="I3" s="63"/>
     </row>
-    <row r="4" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="173.25">
       <c r="A4" s="71">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1375,7 +1372,7 @@
       </c>
       <c r="I4" s="26"/>
     </row>
-    <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="47.25">
       <c r="A5" s="71">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1405,7 +1402,7 @@
       </c>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="47.25">
       <c r="A6" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1422,7 +1419,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>30</v>
@@ -1432,7 +1429,7 @@
       </c>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1446,7 +1443,7 @@
         <v>Tue</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>13</v>
@@ -1455,14 +1452,14 @@
         <v>29</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="54" t="s">
-        <v>68</v>
-      </c>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="78.75">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1487,7 +1484,7 @@
       </c>
       <c r="I8" s="26"/>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="47.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7">
         <f>B8+2</f>
@@ -1508,7 +1505,7 @@
       </c>
       <c r="I9" s="27"/>
     </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="47.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1528,11 +1525,11 @@
         <v>27</v>
       </c>
       <c r="H10" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="6"/>
       <c r="B11" s="7">
         <f>B10+2</f>
@@ -1551,7 +1548,7 @@
       <c r="H11" s="53"/>
       <c r="I11" s="27"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="2">
         <f t="shared" ref="A12:A20" si="4">A10+1</f>
         <v>9</v>
@@ -1573,7 +1570,7 @@
       </c>
       <c r="I12" s="26"/>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="31.5">
       <c r="A13" s="6"/>
       <c r="B13" s="7">
         <f>B12+2</f>
@@ -1593,7 +1590,7 @@
       <c r="I13" s="27"/>
       <c r="J13" s="24"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="38">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -1615,7 +1612,7 @@
       </c>
       <c r="I14" s="42"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="6"/>
       <c r="B15" s="7">
         <f>B14+2</f>
@@ -1634,7 +1631,7 @@
       <c r="H15" s="53"/>
       <c r="I15" s="27"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="11">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -1659,7 +1656,7 @@
       </c>
       <c r="I16" s="26"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="6"/>
       <c r="B17" s="7">
         <f>B16+2</f>
@@ -1678,7 +1675,7 @@
       <c r="H17" s="53"/>
       <c r="I17" s="27"/>
     </row>
-    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="31.5">
       <c r="A18" s="11">
         <f>A16+1</f>
         <v>12</v>
@@ -1699,11 +1696,11 @@
         <v>32</v>
       </c>
       <c r="H18" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="35"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="6"/>
       <c r="B19" s="7">
         <f>B18+2</f>
@@ -1722,7 +1719,7 @@
       <c r="H19" s="53"/>
       <c r="I19" s="27"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="2">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -1747,7 +1744,7 @@
       </c>
       <c r="I20" s="26"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="6"/>
       <c r="B21" s="7">
         <f>B20+2</f>
@@ -1766,7 +1763,7 @@
       <c r="H21" s="53"/>
       <c r="I21" s="30"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="44"/>
       <c r="B22" s="45">
         <f>B20+7</f>
@@ -1786,7 +1783,7 @@
       <c r="I22" s="48"/>
       <c r="J22" s="43"/>
     </row>
-    <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="31.5">
       <c r="A23" s="2">
         <v>14</v>
       </c>
@@ -1810,7 +1807,7 @@
       </c>
       <c r="I23" s="35"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="6"/>
       <c r="B24" s="7">
         <f>B23+2</f>
@@ -1830,7 +1827,7 @@
       <c r="I24" s="27"/>
       <c r="J24" s="43"/>
     </row>
-    <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="31.5">
       <c r="A25" s="11">
         <f>A23+1</f>
         <v>15</v>
@@ -1856,7 +1853,7 @@
       <c r="I25" s="35"/>
       <c r="J25" s="43"/>
     </row>
-    <row r="26" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="16.5" thickBot="1">
       <c r="A26" s="14"/>
       <c r="B26" s="15">
         <f>B25+2</f>
@@ -1878,7 +1875,7 @@
       <c r="I26" s="28"/>
       <c r="J26" s="43"/>
     </row>
-    <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="31.5">
       <c r="A27" s="10" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
add week 8, bivariate analysis assignment.
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -75,19 +75,10 @@
     <t>Foundations for inference: Probability, Normality, sampling distributions</t>
   </si>
   <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
-    <t>Chi-square</t>
-  </si>
-  <si>
     <t>Multiple Regression</t>
   </si>
   <si>
     <t>Logistic Regression</t>
-  </si>
-  <si>
-    <t>Two sample Inference</t>
   </si>
   <si>
     <t>Indicator variables</t>
@@ -264,23 +255,32 @@
 * Peer Review (Due 10/11)</t>
   </si>
   <si>
-    <t>Bivariate Inference Assignment (Due 10/25)
+    <t>Poster Prep: Stage III (Due 11/15)
+* Peer Review: Stage III (Due 11/17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demonstrate how to do,then go do it. Analysis work time on Thursday. Edward Cover. </t>
+  </si>
+  <si>
+    <t>Choosing appropriate analyses
+* Midterm Thu</t>
+  </si>
+  <si>
+    <t>[Project page](https://norcalbiostat.github.io/MATH615/project.html)</t>
+  </si>
+  <si>
+    <t>[Bivariate Inference Assignment](hw/Bivariate_inference.html) (Due 10/25)
 * Poster Prep: Stage II (Due 10/30)
 * Peer Review: Stage II (Due 11/1)</t>
   </si>
   <si>
-    <t>Poster Prep: Stage III (Due 11/15)
-* Peer Review: Stage III (Due 11/17)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demonstrate how to do,then go do it. Analysis work time on Thursday. Edward Cover. </t>
-  </si>
-  <si>
-    <t>Choosing appropriate analyses
-* Midterm Thu</t>
-  </si>
-  <si>
-    <t>[Project page](https://norcalbiostat.github.io/MATH615/project.html)</t>
+    <t>Chi-squared analysis</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Overview of Bivariate analysis procedures</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -667,26 +667,20 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -694,19 +688,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -721,7 +715,28 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -742,8 +757,14 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -808,19 +829,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1252,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1261,18 +1273,18 @@
     <col min="1" max="1" width="6.5" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" style="7"/>
     <col min="3" max="3" width="4.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" style="80" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="30" customWidth="1"/>
+    <col min="5" max="5" width="26" style="88" customWidth="1"/>
     <col min="6" max="6" width="27.125" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.25" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.125" style="41" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="80" customWidth="1"/>
+    <col min="8" max="8" width="63.125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="39.5" style="88" customWidth="1"/>
     <col min="10" max="16384" width="10.875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1290,7 +1302,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>6</v>
@@ -1312,19 +1324,19 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>56</v>
-      </c>
       <c r="H2" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I2" s="12"/>
     </row>
@@ -1342,19 +1354,19 @@
         <v>Tue</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I3" s="18"/>
     </row>
@@ -1372,19 +1384,19 @@
         <v>Tue</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G4" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="26" t="s">
         <v>62</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>65</v>
       </c>
       <c r="I4" s="27"/>
     </row>
@@ -1408,26 +1420,26 @@
         <v>11</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="81">
+      <c r="A6" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="34">
         <f t="shared" si="1"/>
         <v>41535</v>
       </c>
-      <c r="C6" s="83" t="str">
+      <c r="C6" s="35" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
@@ -1435,13 +1447,13 @@
         <v>12</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="37" t="s">
-        <v>59</v>
+        <v>27</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>56</v>
       </c>
       <c r="I6" s="32"/>
     </row>
@@ -1458,454 +1470,454 @@
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D7" s="84" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="40" t="s">
+      <c r="D7" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="38" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>64</v>
       </c>
       <c r="I7" s="27"/>
     </row>
-    <row r="8" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="21">
         <f t="shared" si="1"/>
         <v>41549</v>
       </c>
-      <c r="C8" s="39" t="str">
+      <c r="C8" s="22" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="41" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>32</v>
       </c>
       <c r="I8" s="27"/>
     </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44">
+    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+      <c r="B9" s="42">
         <f>B8+2</f>
         <v>41551</v>
       </c>
-      <c r="C9" s="45" t="str">
+      <c r="C9" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
-    </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
+    </row>
+    <row r="10" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="49">
         <f>B8+7</f>
         <v>41556</v>
       </c>
-      <c r="C10" s="39" t="str">
+      <c r="C10" s="50" t="str">
         <f t="shared" ref="C10:C11" si="3">TEXT(WEEKDAY(B10,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D10" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="40"/>
+      <c r="D10" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="38"/>
       <c r="F10" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>68</v>
+        <v>24</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>69</v>
       </c>
       <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44">
+      <c r="A11" s="52"/>
+      <c r="B11" s="53">
         <f>B10+2</f>
         <v>41558</v>
       </c>
-      <c r="C11" s="45" t="str">
+      <c r="C11" s="54" t="str">
         <f t="shared" si="3"/>
         <v>Thu</v>
       </c>
-      <c r="D11" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="50"/>
+      <c r="D11" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="48"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <f t="shared" ref="A12:A20" si="4">A10+1</f>
         <v>9</v>
       </c>
-      <c r="B12" s="38">
+      <c r="B12" s="49">
         <f>B10+7</f>
         <v>41563</v>
       </c>
-      <c r="C12" s="39" t="str">
+      <c r="C12" s="50" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="44">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="53">
         <f>B12+2</f>
         <v>41565</v>
       </c>
-      <c r="C13" s="45" t="str">
+      <c r="C13" s="54" t="str">
         <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
-      <c r="D13" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="50"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="52"/>
+      <c r="D13" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="53">
+      <c r="A14" s="58">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="B14" s="54">
+      <c r="B14" s="59">
         <f>B12+7</f>
         <v>41570</v>
       </c>
-      <c r="C14" s="55" t="str">
+      <c r="C14" s="60" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D14" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="57"/>
+      <c r="D14" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="62"/>
       <c r="F14" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="57"/>
+        <v>21</v>
+      </c>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44">
+      <c r="A15" s="52"/>
+      <c r="B15" s="53">
         <f>B14+2</f>
         <v>41572</v>
       </c>
-      <c r="C15" s="45" t="str">
+      <c r="C15" s="54" t="str">
         <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
-      <c r="D15" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="50"/>
+      <c r="D15" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="48"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="33">
+      <c r="A16" s="63">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="49">
         <f>B14+7</f>
         <v>41577</v>
       </c>
-      <c r="C16" s="35" t="str">
+      <c r="C16" s="64" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D16" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="40"/>
+      <c r="D16" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="38"/>
       <c r="F16" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>39</v>
+        <v>20</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>36</v>
       </c>
       <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44">
+      <c r="A17" s="52"/>
+      <c r="B17" s="53">
         <f>B16+2</f>
         <v>41579</v>
       </c>
-      <c r="C17" s="45" t="str">
+      <c r="C17" s="54" t="str">
         <f t="shared" si="2"/>
         <v>Thu</v>
       </c>
-      <c r="D17" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
+      <c r="D17" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
+      <c r="A18" s="63">
         <f>A16+1</f>
         <v>12</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="65">
         <f>B16+7</f>
         <v>41584</v>
       </c>
-      <c r="C18" s="35" t="str">
+      <c r="C18" s="64" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D18" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="59"/>
+      <c r="D18" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="66"/>
       <c r="F18" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>69</v>
+        <v>29</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>65</v>
       </c>
       <c r="I18" s="29"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="44">
+      <c r="A19" s="52"/>
+      <c r="B19" s="53">
         <f>B18+2</f>
         <v>41586</v>
       </c>
-      <c r="C19" s="45" t="str">
+      <c r="C19" s="54" t="str">
         <f>TEXT(WEEKDAY(B19,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D19" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
+      <c r="D19" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="45"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="B20" s="38">
+      <c r="B20" s="49">
         <f>B18+7</f>
         <v>41591</v>
       </c>
-      <c r="C20" s="39" t="str">
+      <c r="C20" s="50" t="str">
         <f>TEXT(WEEKDAY(B20,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D20" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="59"/>
+      <c r="D20" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="66"/>
       <c r="F20" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="H20" s="39" t="s">
+        <v>37</v>
       </c>
       <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="44">
+      <c r="A21" s="52"/>
+      <c r="B21" s="53">
         <f>B20+2</f>
         <v>41593</v>
       </c>
-      <c r="C21" s="45" t="str">
+      <c r="C21" s="54" t="str">
         <f t="shared" ref="C21:C27" si="5">TEXT(WEEKDAY(B21,1)+1, "ddd")</f>
         <v>Thu</v>
       </c>
-      <c r="D21" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="47"/>
+      <c r="D21" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="45"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="60"/>
-      <c r="B22" s="61">
+      <c r="A22" s="67"/>
+      <c r="B22" s="68">
         <f>B20+7</f>
         <v>41598</v>
       </c>
-      <c r="C22" s="62" t="str">
+      <c r="C22" s="69" t="str">
         <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D22" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="67"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="74"/>
     </row>
     <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>14</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="49">
         <f>B22+7</f>
         <v>41605</v>
       </c>
-      <c r="C23" s="39" t="str">
+      <c r="C23" s="50" t="str">
         <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
-      <c r="D23" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="69"/>
+      <c r="D23" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="76"/>
       <c r="F23" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>66</v>
+        <v>30</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>63</v>
       </c>
       <c r="I23" s="29"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="44">
+      <c r="A24" s="52"/>
+      <c r="B24" s="53">
         <f>B23+2</f>
         <v>41607</v>
       </c>
-      <c r="C24" s="45" t="str">
+      <c r="C24" s="54" t="str">
         <f t="shared" si="5"/>
         <v>Thu</v>
       </c>
-      <c r="D24" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="70"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="67"/>
-    </row>
-    <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="33">
+      <c r="D24" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="77"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="74"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="63">
         <f>A23+1</f>
         <v>15</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="49">
         <f>B23+7</f>
         <v>41612</v>
       </c>
-      <c r="C25" s="35" t="str">
+      <c r="C25" s="64" t="str">
         <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
-      <c r="D25" s="68" t="s">
-        <v>42</v>
+      <c r="D25" s="75" t="s">
+        <v>39</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>49</v>
+        <v>31</v>
+      </c>
+      <c r="H25" s="39" t="s">
+        <v>46</v>
       </c>
       <c r="I25" s="29"/>
-      <c r="J25" s="67"/>
+      <c r="J25" s="74"/>
     </row>
     <row r="26" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72">
+      <c r="A26" s="78"/>
+      <c r="B26" s="79">
         <f>B25+2</f>
         <v>41614</v>
       </c>
-      <c r="C26" s="73" t="str">
+      <c r="C26" s="80" t="str">
         <f t="shared" si="5"/>
         <v>Thu</v>
       </c>
-      <c r="D26" s="74" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="75" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="76"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="67"/>
+      <c r="D26" s="81" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="82" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="83"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="74"/>
     </row>
     <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B27" s="49">
         <v>41625</v>
       </c>
-      <c r="C27" s="39" t="str">
+      <c r="C27" s="50" t="str">
         <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
-      <c r="D27" s="79" t="s">
-        <v>51</v>
+      <c r="D27" s="86" t="s">
+        <v>48</v>
       </c>
       <c r="E27" s="27"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="27"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add wk9, linreg and cda materials.
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>date</t>
   </si>
@@ -69,60 +69,9 @@
     <t>Afifi chapter 5</t>
   </si>
   <si>
-    <t>Confidence Intervals and Hypothesis Testing</t>
-  </si>
-  <si>
-    <t>Foundations for inference: Probability, Normality, sampling distributions</t>
-  </si>
-  <si>
-    <t>Multiple Regression</t>
-  </si>
-  <si>
     <t>Logistic Regression</t>
   </si>
   <si>
-    <t>Indicator variables</t>
-  </si>
-  <si>
-    <t>Analysis work time</t>
-  </si>
-  <si>
-    <t>[Week 11 overview](wk11.html)</t>
-  </si>
-  <si>
-    <t>[Week 10 overview](wk10.html)</t>
-  </si>
-  <si>
-    <t>[Week 13 overview](wk13.html)</t>
-  </si>
-  <si>
-    <t>[Week 9 overview](wk09.html)</t>
-  </si>
-  <si>
-    <t>[Week 8 overview](wk08.html)</t>
-  </si>
-  <si>
-    <t>[Week 7 overview](wk07.html)</t>
-  </si>
-  <si>
-    <t>[Week 6 overview](wk06.html)</t>
-  </si>
-  <si>
-    <t>[Week 5 overview](wk05.html)</t>
-  </si>
-  <si>
-    <t>[Week 4 overview](wk04.html)</t>
-  </si>
-  <si>
-    <t>[Week 12 overview](wk12.html)</t>
-  </si>
-  <si>
-    <t>[Week 14 overview](wk14.html)</t>
-  </si>
-  <si>
-    <t>[Week 15 overview](wk15.html)</t>
-  </si>
-  <si>
     <t>Foundations assignment (Due 10/9)</t>
   </si>
   <si>
@@ -132,9 +81,6 @@
     <t>Flex time</t>
   </si>
   <si>
-    <t>Correlation and Regression</t>
-  </si>
-  <si>
     <t>Multiple Regression Assignment (Due 11/13)</t>
   </si>
   <si>
@@ -142,9 +88,6 @@
   </si>
   <si>
     <t>Special Regression Topics</t>
-  </si>
-  <si>
-    <t>Impacts of sampling design</t>
   </si>
   <si>
     <t>Introduction to the class
@@ -175,24 +118,7 @@
     <t>Posters Due 12/6</t>
   </si>
   <si>
-    <t>Poster Presentations</t>
-  </si>
-  <si>
     <t>Final Exam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Split class in half. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 1 overview](wk01.html) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 2 overview](wk02.html)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 3 overview](wk03.html)
-</t>
   </si>
   <si>
     <t>[Syllabus](docs/syllabus_615_f17_html)
@@ -274,13 +200,77 @@
 * Peer Review: Stage II (Due 11/1)</t>
   </si>
   <si>
-    <t>Chi-squared analysis</t>
-  </si>
-  <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
-    <t>Overview of Bivariate analysis procedures</t>
+    <t>Overview of Bivariate analysis procedures.
+* Two sample tests
+* ANOVA</t>
+  </si>
+  <si>
+    <t>Foundations for inference: Probability, Normality, sampling distributions, Confidence Intervals, Hypothesis Testing</t>
+  </si>
+  <si>
+    <t>Bivariate Analysis:
+* Chi-squared analysis
+* Correlation and Regression</t>
+  </si>
+  <si>
+    <t>[Categorical Analysis](docs/lec04_cda.html) notes
+* PMA5 Ch 6 (Corr &amp; Reg) 
+* [Regression](docs/lec05_LinReg.html) notes</t>
+  </si>
+  <si>
+    <t>[Week 10: Oct 23](wk10.html)</t>
+  </si>
+  <si>
+    <t>[Week 09: Oct 16](wk09.html)</t>
+  </si>
+  <si>
+    <t>[Week 11: Oct 30](wk11.html)</t>
+  </si>
+  <si>
+    <t>Multiple Regression
+* Indicator Variables</t>
+  </si>
+  <si>
+    <t>[Week 12: Nov 6](wk12.html)</t>
+  </si>
+  <si>
+    <t>[Week 08: Oct 9](wk08.html)</t>
+  </si>
+  <si>
+    <t>[Week 07: Oct 2](wk07.html)</t>
+  </si>
+  <si>
+    <t>[Week 06: Sep 25](wk06.html)</t>
+  </si>
+  <si>
+    <t>[Week 05: Sep 18](wk05.html)</t>
+  </si>
+  <si>
+    <t>[Week 04: Sep 11](wk04.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 03: Sep 4](wk03.html)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 02: Aug 28](wk02.html)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 01: Aug 21](wk01.html) </t>
+  </si>
+  <si>
+    <t>[Week 13: Nov 13](wk13.html)</t>
+  </si>
+  <si>
+    <t>[Week 14: Nov 27](wk14.html)</t>
+  </si>
+  <si>
+    <t>[Week 15: Dec 6](wk15.html)</t>
+  </si>
+  <si>
+    <t>Impacts of sampling design
+* Poster Presentations</t>
   </si>
 </sst>
 </file>
@@ -371,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,12 +377,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,7 +553,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -592,16 +576,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,13 +597,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -631,13 +615,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -652,7 +636,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -667,19 +651,19 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -688,33 +672,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,24 +686,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -799,40 +744,28 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1262,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1274,17 +1207,17 @@
     <col min="2" max="2" width="10.875" style="7"/>
     <col min="3" max="3" width="4.375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="30" customWidth="1"/>
-    <col min="5" max="5" width="26" style="88" customWidth="1"/>
+    <col min="5" max="5" width="26" style="67" customWidth="1"/>
     <col min="6" max="6" width="27.125" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.25" style="30" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="63.125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="88" customWidth="1"/>
+    <col min="9" max="9" width="39.5" style="67" customWidth="1"/>
     <col min="10" max="16384" width="10.875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1302,7 +1235,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>6</v>
@@ -1324,19 +1257,19 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>50</v>
+      <c r="F2" s="71" t="s">
+        <v>62</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="I2" s="12"/>
     </row>
@@ -1354,19 +1287,19 @@
         <v>Tue</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="I3" s="18"/>
     </row>
@@ -1380,23 +1313,23 @@
         <v>41521</v>
       </c>
       <c r="C4" s="22" t="str">
-        <f t="shared" ref="C4:C18" si="2">TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
+        <f t="shared" ref="C4:C13" si="2">TEXT(WEEKDAY(B4,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>52</v>
+        <v>26</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>60</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="I4" s="27"/>
     </row>
@@ -1419,14 +1352,14 @@
       <c r="E5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>28</v>
+      <c r="F5" s="68" t="s">
+        <v>59</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="I5" s="32"/>
     </row>
@@ -1447,13 +1380,13 @@
         <v>12</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>27</v>
+        <v>42</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>58</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="I6" s="32"/>
     </row>
@@ -1471,23 +1404,23 @@
         <v>Tue</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="30" t="s">
-        <v>26</v>
+      <c r="F7" s="68" t="s">
+        <v>57</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="I7" s="27"/>
     </row>
-    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1501,424 +1434,252 @@
         <v>Tue</v>
       </c>
       <c r="D8" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="38"/>
+      <c r="F8" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>32</v>
-      </c>
       <c r="I8" s="27"/>
     </row>
-    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42">
-        <f>B8+2</f>
-        <v>41551</v>
-      </c>
-      <c r="C9" s="43" t="str">
-        <f t="shared" si="2"/>
-        <v>Thu</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="45"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="48"/>
+    <row r="9" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="21">
+        <f>B8+7</f>
+        <v>41556</v>
+      </c>
+      <c r="C9" s="22" t="str">
+        <f t="shared" ref="C9" si="3">TEXT(WEEKDAY(B9,1)+1, "ddd")</f>
+        <v>Tue</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:10" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>8</v>
-      </c>
-      <c r="B10" s="49">
-        <f>B8+7</f>
-        <v>41556</v>
-      </c>
-      <c r="C10" s="50" t="str">
-        <f t="shared" ref="C10:C11" si="3">TEXT(WEEKDAY(B10,1)+1, "ddd")</f>
-        <v>Tue</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="27"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="53">
-        <f>B10+2</f>
-        <v>41558</v>
-      </c>
-      <c r="C11" s="54" t="str">
-        <f t="shared" si="3"/>
-        <v>Thu</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="48"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <f t="shared" ref="A12:A20" si="4">A10+1</f>
+        <f>A9+1</f>
         <v>9</v>
       </c>
-      <c r="B12" s="49">
-        <f>B10+7</f>
+      <c r="B10" s="42">
+        <f>B9+7</f>
         <v>41563</v>
       </c>
-      <c r="C12" s="50" t="str">
+      <c r="C10" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="27"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="53">
-        <f>B12+2</f>
-        <v>41565</v>
-      </c>
-      <c r="C13" s="54" t="str">
-        <f t="shared" si="2"/>
-        <v>Thu</v>
-      </c>
-      <c r="D13" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="48"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="57"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="58">
-        <f t="shared" si="4"/>
+      <c r="D10" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="41"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="45">
+        <f>A10+1</f>
         <v>10</v>
       </c>
-      <c r="B14" s="59">
-        <f>B12+7</f>
+      <c r="B11" s="46">
+        <f>B10+7</f>
         <v>41570</v>
       </c>
-      <c r="C14" s="60" t="str">
+      <c r="C11" s="47" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D14" s="61" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="62"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="53">
-        <f>B14+2</f>
-        <v>41572</v>
-      </c>
-      <c r="C15" s="54" t="str">
-        <f t="shared" si="2"/>
-        <v>Thu</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="48"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="63">
-        <f t="shared" si="4"/>
+      <c r="D11" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="49"/>
+    </row>
+    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="50">
+        <f>A11+1</f>
         <v>11</v>
       </c>
-      <c r="B16" s="49">
-        <f>B14+7</f>
+      <c r="B12" s="42">
+        <f>B11+7</f>
         <v>41577</v>
       </c>
-      <c r="C16" s="64" t="str">
+      <c r="C12" s="51" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D16" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="27"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="53">
-        <f>B16+2</f>
-        <v>41579</v>
-      </c>
-      <c r="C17" s="54" t="str">
-        <f t="shared" si="2"/>
-        <v>Thu</v>
-      </c>
-      <c r="D17" s="55" t="s">
+      <c r="D12" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="48"/>
-    </row>
-    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="63">
-        <f>A16+1</f>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="50">
+        <f>A12+1</f>
         <v>12</v>
       </c>
-      <c r="B18" s="65">
-        <f>B16+7</f>
+      <c r="B13" s="52">
+        <f>B12+7</f>
         <v>41584</v>
       </c>
-      <c r="C18" s="64" t="str">
+      <c r="C13" s="51" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D18" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="39" t="s">
+      <c r="D13" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="53"/>
+      <c r="F13" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <f>A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="42">
+        <f>B13+7</f>
+        <v>41591</v>
+      </c>
+      <c r="C14" s="43" t="str">
+        <f>TEXT(WEEKDAY(B14,1)+1, "ddd")</f>
+        <v>Tue</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="53"/>
+      <c r="F14" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="55">
+        <f>B14+7</f>
+        <v>41598</v>
+      </c>
+      <c r="C15" s="56" t="str">
+        <f t="shared" ref="C15:C18" si="4">TEXT(WEEKDAY(B15,1)+1, "ddd")</f>
+        <v>Tue</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="61"/>
+    </row>
+    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="42">
+        <f>B15+7</f>
+        <v>41605</v>
+      </c>
+      <c r="C16" s="43" t="str">
+        <f t="shared" si="4"/>
+        <v>Tue</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="63"/>
+      <c r="F16" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="50">
+        <f>A16+1</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="42">
+        <f>B16+7</f>
+        <v>41612</v>
+      </c>
+      <c r="C17" s="51" t="str">
+        <f t="shared" si="4"/>
+        <v>Tue</v>
+      </c>
+      <c r="D17" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="29"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="53">
-        <f>B18+2</f>
-        <v>41586</v>
-      </c>
-      <c r="C19" s="54" t="str">
-        <f>TEXT(WEEKDAY(B19,1)+1, "ddd")</f>
-        <v>Thu</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="48"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="H17" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="61"/>
+    </row>
+    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="42">
+        <v>41625</v>
+      </c>
+      <c r="C18" s="43" t="str">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="B20" s="49">
-        <f>B18+7</f>
-        <v>41591</v>
-      </c>
-      <c r="C20" s="50" t="str">
-        <f>TEXT(WEEKDAY(B20,1)+1, "ddd")</f>
-        <v>Tue</v>
-      </c>
-      <c r="D20" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="I20" s="27"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53">
-        <f>B20+2</f>
-        <v>41593</v>
-      </c>
-      <c r="C21" s="54" t="str">
-        <f t="shared" ref="C21:C27" si="5">TEXT(WEEKDAY(B21,1)+1, "ddd")</f>
-        <v>Thu</v>
-      </c>
-      <c r="D21" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="45"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="67"/>
-      <c r="B22" s="68">
-        <f>B20+7</f>
-        <v>41598</v>
-      </c>
-      <c r="C22" s="69" t="str">
-        <f t="shared" si="5"/>
-        <v>Tue</v>
-      </c>
-      <c r="D22" s="70" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="70"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="74"/>
-    </row>
-    <row r="23" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>14</v>
-      </c>
-      <c r="B23" s="49">
-        <f>B22+7</f>
-        <v>41605</v>
-      </c>
-      <c r="C23" s="50" t="str">
-        <f t="shared" si="5"/>
-        <v>Tue</v>
-      </c>
-      <c r="D23" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="76"/>
-      <c r="F23" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="29"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53">
-        <f>B23+2</f>
-        <v>41607</v>
-      </c>
-      <c r="C24" s="54" t="str">
-        <f t="shared" si="5"/>
-        <v>Thu</v>
-      </c>
-      <c r="D24" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="77"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="74"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="63">
-        <f>A23+1</f>
-        <v>15</v>
-      </c>
-      <c r="B25" s="49">
-        <f>B23+7</f>
-        <v>41612</v>
-      </c>
-      <c r="C25" s="64" t="str">
-        <f t="shared" si="5"/>
-        <v>Tue</v>
-      </c>
-      <c r="D25" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="74"/>
-    </row>
-    <row r="26" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="78"/>
-      <c r="B26" s="79">
-        <f>B25+2</f>
-        <v>41614</v>
-      </c>
-      <c r="C26" s="80" t="str">
-        <f t="shared" si="5"/>
-        <v>Thu</v>
-      </c>
-      <c r="D26" s="81" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="82" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="74"/>
-    </row>
-    <row r="27" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="85" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="49">
-        <v>41625</v>
-      </c>
-      <c r="C27" s="50" t="str">
-        <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
-      <c r="D27" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="I27" s="27"/>
+      <c r="D18" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="27"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="I18" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update week 9, rebuild index
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -213,64 +213,65 @@
 * Correlation and Regression</t>
   </si>
   <si>
+    <t>[Week 10: Oct 23](wk10.html)</t>
+  </si>
+  <si>
+    <t>[Week 09: Oct 16](wk09.html)</t>
+  </si>
+  <si>
+    <t>[Week 11: Oct 30](wk11.html)</t>
+  </si>
+  <si>
+    <t>Multiple Regression
+* Indicator Variables</t>
+  </si>
+  <si>
+    <t>[Week 12: Nov 6](wk12.html)</t>
+  </si>
+  <si>
+    <t>[Week 08: Oct 9](wk08.html)</t>
+  </si>
+  <si>
+    <t>[Week 07: Oct 2](wk07.html)</t>
+  </si>
+  <si>
+    <t>[Week 06: Sep 25](wk06.html)</t>
+  </si>
+  <si>
+    <t>[Week 05: Sep 18](wk05.html)</t>
+  </si>
+  <si>
+    <t>[Week 04: Sep 11](wk04.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 03: Sep 4](wk03.html)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 02: Aug 28](wk02.html)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Week 01: Aug 21](wk01.html) </t>
+  </si>
+  <si>
+    <t>[Week 13: Nov 13](wk13.html)</t>
+  </si>
+  <si>
+    <t>[Week 14: Nov 27](wk14.html)</t>
+  </si>
+  <si>
+    <t>[Week 15: Dec 6](wk15.html)</t>
+  </si>
+  <si>
+    <t>Impacts of sampling design
+* Poster Presentations</t>
+  </si>
+  <si>
     <t>[Categorical Analysis](docs/lec04_cda.html) notes
 * PMA5 Ch 6 (Corr &amp; Reg) 
-* [Regression](docs/lec05_LinReg.html) notes</t>
-  </si>
-  <si>
-    <t>[Week 10: Oct 23](wk10.html)</t>
-  </si>
-  <si>
-    <t>[Week 09: Oct 16](wk09.html)</t>
-  </si>
-  <si>
-    <t>[Week 11: Oct 30](wk11.html)</t>
-  </si>
-  <si>
-    <t>Multiple Regression
-* Indicator Variables</t>
-  </si>
-  <si>
-    <t>[Week 12: Nov 6](wk12.html)</t>
-  </si>
-  <si>
-    <t>[Week 08: Oct 9](wk08.html)</t>
-  </si>
-  <si>
-    <t>[Week 07: Oct 2](wk07.html)</t>
-  </si>
-  <si>
-    <t>[Week 06: Sep 25](wk06.html)</t>
-  </si>
-  <si>
-    <t>[Week 05: Sep 18](wk05.html)</t>
-  </si>
-  <si>
-    <t>[Week 04: Sep 11](wk04.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 03: Sep 4](wk03.html)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 02: Aug 28](wk02.html)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Week 01: Aug 21](wk01.html) </t>
-  </si>
-  <si>
-    <t>[Week 13: Nov 13](wk13.html)</t>
-  </si>
-  <si>
-    <t>[Week 14: Nov 27](wk14.html)</t>
-  </si>
-  <si>
-    <t>[Week 15: Dec 6](wk15.html)</t>
-  </si>
-  <si>
-    <t>Impacts of sampling design
-* Poster Presentations</t>
+* [Regression](docs/lec05_LinReg.html) notes
+* PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1199,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1264,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>29</v>
@@ -1293,7 +1294,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>37</v>
@@ -1323,7 +1324,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" s="25" t="s">
         <v>35</v>
@@ -1353,7 +1354,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="30" t="s">
         <v>36</v>
@@ -1383,7 +1384,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="36" t="s">
         <v>32</v>
@@ -1410,7 +1411,7 @@
         <v>13</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>44</v>
@@ -1438,7 +1439,7 @@
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="39" t="s">
         <v>15</v>
@@ -1450,11 +1451,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="21">
-        <f>B8+7</f>
+        <f t="shared" ref="B9:B17" si="3">B8+7</f>
         <v>41556</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f t="shared" ref="C9" si="3">TEXT(WEEKDAY(B9,1)+1, "ddd")</f>
+        <f t="shared" ref="C9" si="4">TEXT(WEEKDAY(B9,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
       <c r="D9" s="40" t="s">
@@ -1462,20 +1463,20 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H9" s="39" t="s">
         <v>45</v>
       </c>
       <c r="I9" s="27"/>
     </row>
-    <row r="10" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>A9+1</f>
         <v>9</v>
       </c>
       <c r="B10" s="42">
-        <f>B9+7</f>
+        <f t="shared" si="3"/>
         <v>41563</v>
       </c>
       <c r="C10" s="43" t="str">
@@ -1487,10 +1488,10 @@
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="69" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="27"/>
@@ -1501,7 +1502,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="46">
-        <f>B10+7</f>
+        <f t="shared" si="3"/>
         <v>41570</v>
       </c>
       <c r="C11" s="47" t="str">
@@ -1513,7 +1514,7 @@
       </c>
       <c r="E11" s="49"/>
       <c r="F11" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I11" s="49"/>
     </row>
@@ -1523,7 +1524,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="42">
-        <f>B11+7</f>
+        <f t="shared" si="3"/>
         <v>41577</v>
       </c>
       <c r="C12" s="51" t="str">
@@ -1531,11 +1532,11 @@
         <v>Tue</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="68" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="39" t="s">
         <v>18</v>
@@ -1548,7 +1549,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="52">
-        <f>B12+7</f>
+        <f t="shared" si="3"/>
         <v>41584</v>
       </c>
       <c r="C13" s="51" t="str">
@@ -1560,7 +1561,7 @@
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="39" t="s">
         <v>41</v>
@@ -1573,7 +1574,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="42">
-        <f>B13+7</f>
+        <f t="shared" si="3"/>
         <v>41591</v>
       </c>
       <c r="C14" s="43" t="str">
@@ -1585,7 +1586,7 @@
       </c>
       <c r="E14" s="53"/>
       <c r="F14" s="68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="39" t="s">
         <v>19</v>
@@ -1595,11 +1596,11 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
       <c r="B15" s="55">
-        <f>B14+7</f>
+        <f t="shared" si="3"/>
         <v>41598</v>
       </c>
       <c r="C15" s="56" t="str">
-        <f t="shared" ref="C15:C18" si="4">TEXT(WEEKDAY(B15,1)+1, "ddd")</f>
+        <f t="shared" ref="C15:C18" si="5">TEXT(WEEKDAY(B15,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
       <c r="D15" s="57" t="s">
@@ -1617,11 +1618,11 @@
         <v>14</v>
       </c>
       <c r="B16" s="42">
-        <f>B15+7</f>
+        <f t="shared" si="3"/>
         <v>41605</v>
       </c>
       <c r="C16" s="43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
       <c r="D16" s="62" t="s">
@@ -1629,32 +1630,32 @@
       </c>
       <c r="E16" s="63"/>
       <c r="F16" s="68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="39" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="50">
         <f>A16+1</f>
         <v>15</v>
       </c>
       <c r="B17" s="42">
-        <f>B16+7</f>
+        <f t="shared" si="3"/>
         <v>41612</v>
       </c>
       <c r="C17" s="51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
       <c r="D17" s="62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="39" t="s">
         <v>27</v>
@@ -1670,7 +1671,7 @@
         <v>41625</v>
       </c>
       <c r="C18" s="43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
       <c r="D18" s="65" t="s">

</xml_diff>

<commit_message>
adj topic outline. add wk10 starter rmd file
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25610" windowHeight="14510" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -78,9 +78,6 @@
     <t>Moderating and Confounding</t>
   </si>
   <si>
-    <t>Flex time</t>
-  </si>
-  <si>
     <t>Multiple Regression Assignment (Due 11/13)</t>
   </si>
   <si>
@@ -181,10 +178,6 @@
 * Peer Review (Due 10/11)</t>
   </si>
   <si>
-    <t>Poster Prep: Stage III (Due 11/15)
-* Peer Review: Stage III (Due 11/17)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Demonstrate how to do,then go do it. Analysis work time on Thursday. Edward Cover. </t>
   </si>
   <si>
@@ -220,10 +213,6 @@
   </si>
   <si>
     <t>[Week 11: Oct 30](wk11.html)</t>
-  </si>
-  <si>
-    <t>Multiple Regression
-* Indicator Variables</t>
   </si>
   <si>
     <t>[Week 12: Nov 6](wk12.html)</t>
@@ -273,11 +262,22 @@
 * [Regression](docs/lec05_LinReg.html) notes
 * PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
   </si>
+  <si>
+    <t>Multiple Regression</t>
+  </si>
+  <si>
+    <t>Indicator Variables</t>
+  </si>
+  <si>
+    <t>Moderation and Confounding Assignment
+* Poster Prep: Stage III (Due 11/15)
+* Peer Review: Stage III (Due 11/17)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -554,7 +554,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,9 +697,6 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -768,6 +765,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="89">
@@ -858,8 +861,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1195,30 +1198,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="7"/>
-    <col min="3" max="3" width="4.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="7"/>
+    <col min="3" max="3" width="4.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="30" customWidth="1"/>
-    <col min="5" max="5" width="26" style="67" customWidth="1"/>
-    <col min="6" max="6" width="27.125" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="66" customWidth="1"/>
+    <col min="6" max="6" width="27.08203125" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.25" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="67" customWidth="1"/>
-    <col min="10" max="16384" width="10.875" style="7"/>
+    <col min="8" max="8" width="63.08203125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="39.5" style="66" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1236,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>6</v>
@@ -1246,7 +1249,7 @@
       </c>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1258,23 +1261,23 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="71" t="s">
-        <v>61</v>
+      <c r="F2" s="70" t="s">
+        <v>58</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="155" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <f t="shared" ref="A3:A8" si="0">A2+1</f>
         <v>2</v>
@@ -1288,23 +1291,23 @@
         <v>Tue</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>24</v>
-      </c>
       <c r="F3" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1318,23 +1321,23 @@
         <v>Tue</v>
       </c>
       <c r="D4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="70" t="s">
-        <v>59</v>
+      <c r="F4" s="69" t="s">
+        <v>56</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="27"/>
     </row>
-    <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1353,18 +1356,18 @@
       <c r="E5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
-        <v>58</v>
+      <c r="F5" s="67" t="s">
+        <v>55</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1381,17 +1384,17 @@
         <v>12</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="68" t="s">
-        <v>57</v>
+        <v>40</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>54</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1405,23 +1408,23 @@
         <v>Tue</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="68" t="s">
-        <v>56</v>
+      <c r="F7" s="67" t="s">
+        <v>53</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="27"/>
     </row>
-    <row r="8" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1435,18 +1438,18 @@
         <v>Tue</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E8" s="38"/>
-      <c r="F8" s="68" t="s">
-        <v>55</v>
+      <c r="F8" s="67" t="s">
+        <v>52</v>
       </c>
       <c r="H8" s="39" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="27"/>
     </row>
-    <row r="9" spans="1:10" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="62" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1459,18 +1462,18 @@
         <v>Tue</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="38"/>
-      <c r="F9" s="68" t="s">
-        <v>54</v>
+      <c r="F9" s="67" t="s">
+        <v>51</v>
       </c>
       <c r="H9" s="39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" s="27"/>
     </row>
-    <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="124" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <f>A9+1</f>
         <v>9</v>
@@ -1483,20 +1486,20 @@
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="69" t="s">
-        <v>66</v>
+      <c r="G10" s="68" t="s">
+        <v>63</v>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="27"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="45">
         <f>A10+1</f>
         <v>10</v>
@@ -1509,17 +1512,20 @@
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="48"/>
+      <c r="F11" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="49"/>
-    </row>
-    <row r="12" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="50">
+      <c r="I11" s="48"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="49">
         <f>A11+1</f>
         <v>11</v>
       </c>
@@ -1527,48 +1533,45 @@
         <f t="shared" si="3"/>
         <v>41577</v>
       </c>
-      <c r="C12" s="51" t="str">
+      <c r="C12" s="50" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E12" s="38"/>
-      <c r="F12" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>18</v>
+      <c r="F12" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="50">
+    <row r="13" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="49">
         <f>A12+1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="51">
         <f t="shared" si="3"/>
         <v>41584</v>
       </c>
-      <c r="C13" s="51" t="str">
+      <c r="C13" s="50" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D13" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>41</v>
+      <c r="E13" s="52"/>
+      <c r="F13" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="72" t="s">
+        <v>66</v>
       </c>
       <c r="I13" s="29"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <f>A13+1</f>
         <v>13</v>
@@ -1584,36 +1587,36 @@
       <c r="D14" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="68" t="s">
-        <v>62</v>
+      <c r="E14" s="52"/>
+      <c r="F14" s="67" t="s">
+        <v>59</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I14" s="27"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="55">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="53"/>
+      <c r="B15" s="54">
         <f t="shared" si="3"/>
         <v>41598</v>
       </c>
-      <c r="C15" s="56" t="str">
+      <c r="C15" s="55" t="str">
         <f t="shared" ref="C15:C18" si="5">TEXT(WEEKDAY(B15,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="61"/>
-    </row>
-    <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="60"/>
+    </row>
+    <row r="16" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>14</v>
       </c>
@@ -1625,20 +1628,20 @@
         <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
-      <c r="D16" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="63"/>
-      <c r="F16" s="68" t="s">
-        <v>63</v>
+      <c r="D16" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="62"/>
+      <c r="F16" s="67" t="s">
+        <v>60</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="50">
+    <row r="17" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+      <c r="A17" s="49">
         <f>A16+1</f>
         <v>15</v>
       </c>
@@ -1646,25 +1649,25 @@
         <f t="shared" si="3"/>
         <v>41612</v>
       </c>
-      <c r="C17" s="51" t="str">
+      <c r="C17" s="50" t="str">
         <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
-      <c r="D17" s="62" t="s">
-        <v>65</v>
+      <c r="D17" s="61" t="s">
+        <v>62</v>
       </c>
       <c r="E17" s="27"/>
-      <c r="F17" s="68" t="s">
-        <v>64</v>
+      <c r="F17" s="67" t="s">
+        <v>61</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" s="29"/>
-      <c r="J17" s="61"/>
-    </row>
-    <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
+      <c r="J17" s="60"/>
+    </row>
+    <row r="18" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+      <c r="A18" s="63" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="42">
@@ -1674,12 +1677,12 @@
         <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
-      <c r="D18" s="65" t="s">
-        <v>28</v>
+      <c r="D18" s="64" t="s">
+        <v>27</v>
       </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
       <c r="I18" s="27"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add wk10 and moderation assignment.
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -241,10 +241,6 @@
 * PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bivariate Inference Assignment](hw/Bivariate_inference.html) (Due 10/25)
-</t>
-  </si>
-  <si>
     <t>Poster Prep: Stage II (Due 10/30)
 * Peer Review: Stage II (Due 11/1)</t>
   </si>
@@ -293,7 +289,11 @@
 * PMA5 Chapter 7, 9.1-9.3, 9.5</t>
   </si>
   <si>
-    <t>Moderation Assignment (Due 11/6)</t>
+    <t xml:space="preserve">[Bivariate Inference Assignment](hw/Bivariate_Inference.html) (Due 10/25)
+</t>
+  </si>
+  <si>
+    <t>[Moderation Assignment](hw/Moderation.html) (Due 11/1)</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1224,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1491,7 +1491,7 @@
         <v>46</v>
       </c>
       <c r="H9" s="71" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="I9" s="27"/>
     </row>
@@ -1509,7 +1509,7 @@
         <v>Tue</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="67" t="s">
@@ -1519,7 +1519,7 @@
         <v>57</v>
       </c>
       <c r="H10" s="72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="27"/>
     </row>
@@ -1537,16 +1537,16 @@
         <v>Tue</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" s="66" t="s">
         <v>42</v>
       </c>
       <c r="G11" s="66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" s="71" t="s">
         <v>73</v>
@@ -1567,17 +1567,17 @@
         <v>Tue</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="66" t="s">
         <v>44</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H12" s="71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12" s="27"/>
     </row>
@@ -1602,7 +1602,7 @@
         <v>45</v>
       </c>
       <c r="G13" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="29"/>
     </row>
@@ -1620,14 +1620,14 @@
         <v>Tue</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="66" t="s">
         <v>54</v>
       </c>
       <c r="G14" s="66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H14" s="39" t="s">
         <v>36</v>
@@ -1667,14 +1667,14 @@
         <v>Tue</v>
       </c>
       <c r="D16" s="60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="61"/>
       <c r="F16" s="66" t="s">
         <v>55</v>
       </c>
       <c r="G16" s="66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="39" t="s">
         <v>34</v>
@@ -1695,7 +1695,7 @@
         <v>Tue</v>
       </c>
       <c r="D17" s="60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="66" t="s">

</xml_diff>

<commit_message>
add mlr, logreg and reg assignments
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -69,9 +69,6 @@
     <t>Afifi chapter 5</t>
   </si>
   <si>
-    <t>Logistic Regression</t>
-  </si>
-  <si>
     <t>Foundations assignment (Due 10/9)</t>
   </si>
   <si>
@@ -166,10 +163,6 @@
 * Peer Review (Due 10/11)</t>
   </si>
   <si>
-    <t>Poster Prep: Stage III (Due 11/15)
-* Peer Review: Stage III (Due 11/17)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Demonstrate how to do,then go do it. Analysis work time on Thursday. Edward Cover. </t>
   </si>
   <si>
@@ -245,15 +238,7 @@
 * Peer Review: Stage II (Due 11/1)</t>
   </si>
   <si>
-    <t>Regression /Confounding Assignment (Due 11/13)</t>
-  </si>
-  <si>
     <t>Special Analysis Topics</t>
-  </si>
-  <si>
-    <t>Multiple Regression
-* Confounding
-* Indicator Variables</t>
   </si>
   <si>
     <t>Poster Presentations</t>
@@ -273,20 +258,10 @@
 * Correlation and Regression (R) </t>
   </si>
   <si>
-    <t>Model building/ fit</t>
-  </si>
-  <si>
     <t>PMA5 Ch 8</t>
   </si>
   <si>
-    <t>PMA5 Ch 12</t>
-  </si>
-  <si>
     <t>Read Intro for:  PMA15 Ch 13, 14,15, 16, 18</t>
-  </si>
-  <si>
-    <t>[PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
-* PMA5 Chapter 7, 9.1-9.3, 9.5</t>
   </si>
   <si>
     <t xml:space="preserve">[Bivariate Inference Assignment](hw/Bivariate_Inference.html) (Due 10/25)
@@ -294,6 +269,36 @@
   </si>
   <si>
     <t>[Moderation Assignment](hw/Moderation.html) (Due 11/1)</t>
+  </si>
+  <si>
+    <t>[PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
+* Study Design Notes [[HTML]](docs/lec06_StudyDesign.html) [[PDF]](docs/lec06_StudyDesign.pdf)
+* PMA5 Chapter 7, 9.1-9.3, 9.5
+* Multiple Regression Notes [[HTML]](docs/lec07_MLR.html) [[PDF]](docs/lec07_MLR.pdf)</t>
+  </si>
+  <si>
+    <t>Log Linear Models
+* Model building/ fit</t>
+  </si>
+  <si>
+    <t>Study Design
+* Multiple Regression</t>
+  </si>
+  <si>
+    <t>Categorical Variables
+* Logistic Regression</t>
+  </si>
+  <si>
+    <t>Multiple Regression Notes [[HTML]](docs/lec07_MLR.html) [[PDF]](docs/lec07_MLR.pdf)
+* PMA5 Ch 12 (Logistic Regression)
+* Logistic Regression Notes [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)</t>
+  </si>
+  <si>
+    <t>Poster Prep: Stage III (Due 11/17)
+* Peer Review: Stage III (Due 11/27)</t>
+  </si>
+  <si>
+    <t>[Regression Assignment](hw/Regression_Assignment.html) (Due 11/17)</t>
   </si>
 </sst>
 </file>
@@ -576,7 +581,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -707,15 +712,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -785,14 +781,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="89">
@@ -1223,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1233,17 +1241,17 @@
     <col min="2" max="2" width="10.875" style="7"/>
     <col min="3" max="3" width="4.375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="30" customWidth="1"/>
-    <col min="5" max="5" width="26" style="65" customWidth="1"/>
+    <col min="5" max="5" width="26" style="62" customWidth="1"/>
     <col min="6" max="6" width="27.125" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.25" style="30" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="63.125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="65" customWidth="1"/>
+    <col min="9" max="9" width="39.5" style="62" customWidth="1"/>
     <col min="10" max="16384" width="10.875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1261,7 +1269,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>6</v>
@@ -1283,19 +1291,19 @@
         <v>Tue</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="69" t="s">
-        <v>53</v>
+      <c r="F2" s="66" t="s">
+        <v>51</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="12"/>
     </row>
@@ -1313,19 +1321,19 @@
         <v>Tue</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>19</v>
-      </c>
       <c r="F3" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="18"/>
     </row>
@@ -1343,19 +1351,19 @@
         <v>Tue</v>
       </c>
       <c r="D4" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="68" t="s">
-        <v>51</v>
+      <c r="F4" s="65" t="s">
+        <v>49</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="27"/>
     </row>
@@ -1378,14 +1386,14 @@
       <c r="E5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="66" t="s">
-        <v>50</v>
+      <c r="F5" s="63" t="s">
+        <v>48</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="32"/>
     </row>
@@ -1406,13 +1414,13 @@
         <v>12</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>49</v>
+        <v>35</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>47</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="32"/>
     </row>
@@ -1430,19 +1438,19 @@
         <v>Tue</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="66" t="s">
-        <v>48</v>
+      <c r="F7" s="63" t="s">
+        <v>46</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="27"/>
     </row>
@@ -1460,14 +1468,14 @@
         <v>Tue</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="38"/>
-      <c r="F8" s="66" t="s">
-        <v>47</v>
+      <c r="F8" s="63" t="s">
+        <v>45</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" s="27"/>
     </row>
@@ -1484,77 +1492,77 @@
         <v>Tue</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" s="38"/>
-      <c r="F9" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="71" t="s">
-        <v>72</v>
+      <c r="F9" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="67" t="s">
+        <v>65</v>
       </c>
       <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="8">
         <f>A9+1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="21">
         <f t="shared" si="3"/>
         <v>41563</v>
       </c>
-      <c r="C10" s="42" t="str">
+      <c r="C10" s="22" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D10" s="66" t="s">
-        <v>66</v>
+      <c r="D10" s="69" t="s">
+        <v>62</v>
       </c>
       <c r="E10" s="27"/>
-      <c r="F10" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="72" t="s">
-        <v>58</v>
+      <c r="F10" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="68" t="s">
+        <v>56</v>
       </c>
       <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="44">
+      <c r="A11" s="70">
         <f>A10+1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="71">
         <f t="shared" si="3"/>
         <v>41570</v>
       </c>
-      <c r="C11" s="46" t="str">
+      <c r="C11" s="72" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D11" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="71" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="47"/>
+      <c r="D11" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="44"/>
     </row>
-    <row r="12" spans="1:10" ht="63" x14ac:dyDescent="0.25">
-      <c r="A12" s="48">
+    <row r="12" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="45">
         <f>A11+1</f>
         <v>11</v>
       </c>
@@ -1562,47 +1570,47 @@
         <f t="shared" si="3"/>
         <v>41577</v>
       </c>
-      <c r="C12" s="49" t="str">
+      <c r="C12" s="46" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E12" s="38"/>
-      <c r="F12" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="71" t="s">
-        <v>59</v>
+      <c r="F12" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>73</v>
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="48">
+    <row r="13" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="45">
         <f>A12+1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="50">
+      <c r="B13" s="47">
         <f t="shared" si="3"/>
         <v>41584</v>
       </c>
-      <c r="C13" s="49" t="str">
+      <c r="C13" s="46" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="51"/>
-      <c r="F13" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="66" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="F13" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>71</v>
       </c>
       <c r="I13" s="29"/>
     </row>
@@ -1620,39 +1628,39 @@
         <v>Tue</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="51"/>
-      <c r="F14" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>36</v>
+      <c r="E14" s="48"/>
+      <c r="F14" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="67" t="s">
+        <v>72</v>
       </c>
       <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="53">
+      <c r="A15" s="49"/>
+      <c r="B15" s="50">
         <f t="shared" si="3"/>
         <v>41598</v>
       </c>
-      <c r="C15" s="54" t="str">
+      <c r="C15" s="51" t="str">
         <f t="shared" ref="C15:C18" si="5">TEXT(WEEKDAY(B15,1)+1, "ddd")</f>
         <v>Tue</v>
       </c>
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="59"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="56"/>
     </row>
     <row r="16" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
@@ -1666,23 +1674,23 @@
         <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
-      <c r="D16" s="60" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="66" t="s">
-        <v>70</v>
+      <c r="D16" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="58"/>
+      <c r="F16" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="63" t="s">
+        <v>64</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="48">
+      <c r="A17" s="45">
         <f>A16+1</f>
         <v>15</v>
       </c>
@@ -1690,25 +1698,25 @@
         <f t="shared" si="3"/>
         <v>41612</v>
       </c>
-      <c r="C17" s="49" t="str">
+      <c r="C17" s="46" t="str">
         <f t="shared" si="5"/>
         <v>Tue</v>
       </c>
-      <c r="D17" s="60" t="s">
-        <v>62</v>
+      <c r="D17" s="57" t="s">
+        <v>58</v>
       </c>
       <c r="E17" s="27"/>
-      <c r="F17" s="66" t="s">
-        <v>56</v>
+      <c r="F17" s="63" t="s">
+        <v>54</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I17" s="29"/>
-      <c r="J17" s="59"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="59" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="41">
@@ -1718,12 +1726,12 @@
         <f t="shared" si="5"/>
         <v>Mon</v>
       </c>
-      <c r="D18" s="63" t="s">
-        <v>23</v>
+      <c r="D18" s="60" t="s">
+        <v>22</v>
       </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
       <c r="I18" s="27"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add wk11 to index page
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -285,10 +285,6 @@
 * Multiple Regression</t>
   </si>
   <si>
-    <t>Categorical Variables
-* Logistic Regression</t>
-  </si>
-  <si>
     <t>Multiple Regression Notes [[HTML]](docs/lec07_MLR.html) [[PDF]](docs/lec07_MLR.pdf)
 * PMA5 Ch 12 (Logistic Regression)
 * Logistic Regression Notes [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)</t>
@@ -299,12 +295,16 @@
   </si>
   <si>
     <t>[Regression Assignment](hw/Regression_Assignment.html) (Due 11/17)</t>
+  </si>
+  <si>
+    <t>Categorical Predictors
+* Logistic Regression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -891,8 +891,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1228,11 +1228,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1585,7 @@
         <v>67</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="27"/>
     </row>
@@ -1603,14 +1603,14 @@
         <v>Tue</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="63" t="s">
         <v>43</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I13" s="29"/>
     </row>
@@ -1638,7 +1638,7 @@
         <v>63</v>
       </c>
       <c r="H14" s="67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" s="27"/>
     </row>

</xml_diff>

<commit_message>
update schedule, fix link in wk11 and work on reg assignment
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -304,7 +304,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -891,8 +891,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51"/>
-    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1228,11 +1228,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1562,19 +1562,19 @@
       <c r="I11" s="44"/>
     </row>
     <row r="12" spans="1:10" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45">
+      <c r="A12" s="33">
         <f>A11+1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="21">
         <f t="shared" si="3"/>
         <v>41577</v>
       </c>
-      <c r="C12" s="46" t="str">
+      <c r="C12" s="35" t="str">
         <f t="shared" si="2"/>
         <v>Tue</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="40" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="38"/>

</xml_diff>

<commit_message>
finalize mlr notes and regression assignment
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>date</t>
   </si>
@@ -95,9 +95,6 @@
   <si>
     <t>T: univariate graphics (45 min on graph types). rest of class on creating them in SPC
 R: transformations (10-15 min). Rest of class on graphing assignment</t>
-  </si>
-  <si>
-    <t>Posters Due 12/6</t>
   </si>
   <si>
     <t>Final Exam</t>
@@ -238,12 +235,6 @@
 * Peer Review: Stage II (Due 11/1)</t>
   </si>
   <si>
-    <t>Special Analysis Topics</t>
-  </si>
-  <si>
-    <t>Poster Presentations</t>
-  </si>
-  <si>
     <t>open work time Tuesday</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t xml:space="preserve">Bivariate Analysis:
 * Chi-squared analysis (T)
 * Correlation and Regression (R) </t>
-  </si>
-  <si>
-    <t>PMA5 Ch 8</t>
   </si>
   <si>
     <t>Read Intro for:  PMA15 Ch 13, 14,15, 16, 18</t>
@@ -277,19 +265,10 @@
 * Multiple Regression Notes [[HTML]](docs/lec07_MLR.html) [[PDF]](docs/lec07_MLR.pdf)</t>
   </si>
   <si>
-    <t>Log Linear Models
-* Model building/ fit</t>
-  </si>
-  <si>
     <t>Study Design
 * Multiple Regression</t>
   </si>
   <si>
-    <t>Multiple Regression Notes [[HTML]](docs/lec07_MLR.html) [[PDF]](docs/lec07_MLR.pdf)
-* PMA5 Ch 12 (Logistic Regression)
-* Logistic Regression Notes [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)</t>
-  </si>
-  <si>
     <t>Poster Prep: Stage III (Due 11/17)
 * Peer Review: Stage III (Due 11/27)</t>
   </si>
@@ -297,8 +276,40 @@
     <t>[Regression Assignment](hw/Regression_Assignment.html) (Due 11/17)</t>
   </si>
   <si>
+    <t>Thursday, 10-12noon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In class presentations on R 12/7. </t>
+  </si>
+  <si>
+    <t>Special Analysis Topics
+* Poster design</t>
+  </si>
+  <si>
+    <t>Poster Revisions
+* Poster Presentations</t>
+  </si>
+  <si>
+    <t>Final Posters (as printed)  Due 12/7 EOD</t>
+  </si>
+  <si>
+    <t>Logistic Regression
+* Model building/ fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple Regression Notes [[HTML]](docs/lec07_MLR.html) [[PDF]](docs/lec07_MLR.pdf)
+* PMA5 9.3 
+* PMA5 Ch 6
+</t>
+  </si>
+  <si>
+    <t>PMA5 Ch 8
+* Logistic Regression Notes [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)
+* PMA5  Ch 12 (Logistic Regression)</t>
+  </si>
+  <si>
     <t>Categorical Predictors
-* Logistic Regression</t>
+* Log transformed outcome</t>
   </si>
 </sst>
 </file>
@@ -581,7 +592,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -800,6 +811,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1232,7 +1246,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1265,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1297,13 +1311,13 @@
         <v>9</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="12"/>
     </row>
@@ -1327,13 +1341,13 @@
         <v>18</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="18"/>
     </row>
@@ -1357,13 +1371,13 @@
         <v>20</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="27"/>
     </row>
@@ -1387,13 +1401,13 @@
         <v>11</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="32"/>
     </row>
@@ -1414,13 +1428,13 @@
         <v>12</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" s="32"/>
     </row>
@@ -1438,19 +1452,19 @@
         <v>Tue</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="27"/>
     </row>
@@ -1468,11 +1482,11 @@
         <v>Tue</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" s="39" t="s">
         <v>14</v>
@@ -1492,14 +1506,14 @@
         <v>Tue</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="63" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H9" s="67" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I9" s="27"/>
     </row>
@@ -1517,17 +1531,17 @@
         <v>Tue</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="68" t="s">
         <v>55</v>
-      </c>
-      <c r="H10" s="68" t="s">
-        <v>56</v>
       </c>
       <c r="I10" s="27"/>
     </row>
@@ -1545,19 +1559,19 @@
         <v>Tue</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F11" s="63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="63" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I11" s="44"/>
     </row>
@@ -1575,21 +1589,21 @@
         <v>Tue</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="63" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="45">
         <f>A12+1</f>
         <v>12</v>
@@ -1603,18 +1617,18 @@
         <v>Tue</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I13" s="29"/>
     </row>
-    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <f>A13+1</f>
         <v>13</v>
@@ -1628,17 +1642,17 @@
         <v>Tue</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="63" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="H14" s="67" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I14" s="27"/>
     </row>
@@ -1675,21 +1689,21 @@
         <v>Tue</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E16" s="58"/>
       <c r="F16" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="63" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="45">
         <f>A16+1</f>
         <v>15</v>
@@ -1703,14 +1717,17 @@
         <v>Tue</v>
       </c>
       <c r="D17" s="57" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="39" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="G17" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="67" t="s">
+        <v>71</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="56"/>
@@ -1720,17 +1737,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="41">
-        <v>41625</v>
+        <v>41621</v>
       </c>
       <c r="C18" s="42" t="str">
         <f t="shared" si="5"/>
-        <v>Mon</v>
+        <v>Thu</v>
       </c>
       <c r="D18" s="60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="61"/>
+      <c r="F18" s="74" t="s">
+        <v>67</v>
+      </c>
       <c r="G18" s="61"/>
       <c r="I18" s="27"/>
     </row>

</xml_diff>

<commit_message>
add week 13 14, logreg
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -279,9 +279,6 @@
     <t>Thursday, 10-12noon</t>
   </si>
   <si>
-    <t xml:space="preserve">In class presentations on R 12/7. </t>
-  </si>
-  <si>
     <t>Special Analysis Topics
 * Poster design</t>
   </si>
@@ -293,29 +290,31 @@
     <t>Final Posters (as printed)  Due 12/7 EOD</t>
   </si>
   <si>
-    <t>Logistic Regression
-* Model building/ fit</t>
+    <t xml:space="preserve">In class presentations on 12/7. </t>
   </si>
   <si>
     <t xml:space="preserve">Multiple Regression Notes [[HTML]](docs/lec07_MLR.html) [[PDF]](docs/lec07_MLR.pdf)
-* PMA5 9.3 
-* PMA5 Ch 6
+* Logistic Regression Notes [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)
+* PMA5 9.3 (dummy variables)
+* PMA5 Ch 6.9 (transformations)
+* PMA5 Ch 12 (Logistic Regression)
 </t>
   </si>
   <si>
-    <t>PMA5 Ch 8
-* Logistic Regression Notes [[HTML]](docs/lec08_LogReg.html) [[PDF]](docs/lec08_LogReg.pdf)
-* PMA5  Ch 12 (Logistic Regression)</t>
-  </si>
-  <si>
-    <t>Categorical Predictors
-* Log transformed outcome</t>
+    <t xml:space="preserve">Categorical Predictors
+* Log and logit transformations </t>
+  </si>
+  <si>
+    <t>Model building/ fit</t>
+  </si>
+  <si>
+    <t>PMA5 Ch 8 (Variable Selection)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -905,8 +904,8 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Percent 2" xfId="52"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1242,11 +1241,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1602,7 @@
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A13" s="45">
         <f>A12+1</f>
         <v>12</v>
@@ -1617,18 +1616,18 @@
         <v>Tue</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="63" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I13" s="29"/>
     </row>
-    <row r="14" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <f>A13+1</f>
         <v>13</v>
@@ -1642,14 +1641,14 @@
         <v>Tue</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="63" t="s">
         <v>51</v>
       </c>
       <c r="G14" s="63" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H14" s="67" t="s">
         <v>65</v>
@@ -1689,7 +1688,7 @@
         <v>Tue</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" s="58"/>
       <c r="F16" s="63" t="s">
@@ -1717,17 +1716,17 @@
         <v>Tue</v>
       </c>
       <c r="D17" s="57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="63" t="s">
         <v>53</v>
       </c>
       <c r="G17" s="63" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H17" s="67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="56"/>

</xml_diff>

<commit_message>
start to work weekly
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH615/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4B68C695-F904-2A4E-8A1F-75878B280088}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{559657C7-3349-4A45-A662-524A86494C8F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="520" windowWidth="14160" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="122">
   <si>
     <t>Finals Week</t>
   </si>
@@ -241,15 +241,6 @@
   </si>
   <si>
     <t>Thursday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Import and Preparation
-* Literature review </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Univariate Data Visualizations
-* Screening your data for Tranformations
-</t>
   </si>
   <si>
     <t>Writing about empirical research</t>
@@ -298,13 +289,6 @@
   <si>
     <t>Poster Revisions
 * Poster Presentations</t>
-  </si>
-  <si>
-    <t>* [Syllabus](docs/syllabus_615_f18_html)
-* [PMA5 Ch 2 &amp; 3](docs/PMA5 Ch 2 and 3.pdf) 
-* [Reproducibility slides](http://benmarwick.github.io/UW-eScience-reproducibility-social-sciences/#/)
-* [Passion Driven Statistics](docs/PDS_Intro_Stat.pdf)
-* [Introduction to the class](docs/lec01_intro_class.html)</t>
   </si>
   <si>
     <t>* [Data Management preparation questions](docs/dm_prep_qs.html)
@@ -365,22 +349,6 @@
   </si>
   <si>
     <t xml:space="preserve">Literature review, citation assignment. </t>
-  </si>
-  <si>
-    <t>* Make a Slack account and join the math615 workspace. 
-* Post an introduction in the #introductions channel. (Due Sun X/XX)</t>
-  </si>
-  <si>
-    <t>Introduction to the class
-* Choosing a research topic</t>
-  </si>
-  <si>
-    <t>* Introduction to the class requirements and materials
-* Discuss analysis program options</t>
-  </si>
-  <si>
-    <t>* Choose a research topic
-* Decide on a software progam of choice (SPC)</t>
   </si>
   <si>
     <t>* [Peer Review](project.html) of RQ post (Due 9/xx )
@@ -470,6 +438,52 @@
   </si>
   <si>
     <t>wk</t>
+  </si>
+  <si>
+    <t>* Join our Slack team and post an #introduction (Due Sun X/XX)
+* Decide on a software program of choice (SPC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* [Syllabus](docs/syllabus_615_f18_html)
+* [Introduction to the class](docs/lec01_intro_class.html)
+* [PMA5 Ch 2 &amp; 3](docs/PMA5 Ch 2 and 3.pdf) 
+* [Reproducibility slides](http://benmarwick.github.io/UW-eScience-reproducibility-social-sciences/#/)
+* [Passion Driven Statistics](docs/PDS_Intro_Stat.pdf)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Review and discuss available research topics
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Introduction to the class requirements and materials
+* Discuss analysis program options and the need for reproducible materials. </t>
+  </si>
+  <si>
+    <t>Prepare</t>
+  </si>
+  <si>
+    <t>Introduction to the class
+Choosing a research topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Import and Preparation
+Literature review </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univariate Data Visualizations
+Screening your data for Tranformations
+</t>
+  </si>
+  <si>
+    <t>Understand how to be successful in this class
+Learn a new set of collaborative tools
+Understand the importance and need for reproducible research</t>
+  </si>
+  <si>
+    <t>Read over all materials listed
+Buy the textbook
+Familarize yourself with the course website organization</t>
   </si>
 </sst>
 </file>
@@ -752,7 +766,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -880,6 +894,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="92">
@@ -1317,11 +1334,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16"/>
@@ -1329,17 +1346,18 @@
     <col min="1" max="1" width="11.1640625" style="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.1640625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="44" customWidth="1"/>
-    <col min="5" max="5" width="58.5" style="44" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" style="44" customWidth="1"/>
-    <col min="7" max="7" width="32.83203125" style="44" customWidth="1"/>
-    <col min="8" max="8" width="38.1640625" style="44" customWidth="1"/>
-    <col min="9" max="16384" width="14.83203125" style="36"/>
+    <col min="4" max="4" width="18" style="44" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="44" customWidth="1"/>
+    <col min="6" max="6" width="58.5" style="44" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="44" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" style="44" customWidth="1"/>
+    <col min="9" max="9" width="38.1640625" style="44" customWidth="1"/>
+    <col min="10" max="16384" width="14.83203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="25" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>2</v>
@@ -1350,20 +1368,23 @@
       <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="96">
+    <row r="2" spans="1:9" ht="117">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -1371,23 +1392,28 @@
         <v>41878</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>103</v>
+        <v>117</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>113</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="144">
+        <v>115</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="144">
       <c r="A3" s="27">
         <v>2</v>
       </c>
@@ -1395,24 +1421,25 @@
         <f t="shared" ref="B3:B18" si="0">B2+7</f>
         <v>41885</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>71</v>
+      <c r="C3" s="39" t="s">
+        <v>118</v>
       </c>
       <c r="D3" s="29"/>
-      <c r="E3" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>96</v>
+      <c r="E3" s="29"/>
+      <c r="F3" s="38" t="s">
+        <v>84</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="112">
+        <v>93</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="112">
       <c r="A4" s="27">
         <v>3</v>
       </c>
@@ -1420,24 +1447,25 @@
         <f t="shared" si="0"/>
         <v>41892</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>72</v>
+      <c r="C4" s="39" t="s">
+        <v>119</v>
       </c>
       <c r="D4" s="29"/>
-      <c r="E4" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>97</v>
+      <c r="E4" s="29"/>
+      <c r="F4" s="39" t="s">
+        <v>85</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="32">
+        <v>94</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="32">
       <c r="A5" s="27">
         <v>4</v>
       </c>
@@ -1446,21 +1474,22 @@
         <v>41899</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="30"/>
-      <c r="E5" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="40" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="48">
+      <c r="E5" s="30"/>
+      <c r="F5" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="31"/>
+      <c r="I5" s="40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="32">
       <c r="A6" s="27">
         <v>5</v>
       </c>
@@ -1469,17 +1498,18 @@
         <v>41906</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="30"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="24"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="45"/>
       <c r="G6" s="24"/>
-      <c r="H6" s="43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="32">
+      <c r="H6" s="24"/>
+      <c r="I6" s="43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="32">
       <c r="A7" s="27">
         <v>6</v>
       </c>
@@ -1488,17 +1518,18 @@
         <v>41913</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="29"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="24"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="43" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="64">
+      <c r="H7" s="24"/>
+      <c r="I7" s="43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="64">
       <c r="A8" s="27">
         <v>7</v>
       </c>
@@ -1507,17 +1538,18 @@
         <v>41920</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" s="29"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="24"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="24"/>
-      <c r="H8" s="43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="64">
+      <c r="H8" s="24"/>
+      <c r="I8" s="43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="64">
       <c r="A9" s="27">
         <v>8</v>
       </c>
@@ -1526,17 +1558,18 @@
         <v>41927</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="29"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="24"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="24"/>
-      <c r="H9" s="47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="96">
+      <c r="H9" s="24"/>
+      <c r="I9" s="47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="96">
       <c r="A10" s="32">
         <v>9</v>
       </c>
@@ -1545,19 +1578,20 @@
         <v>41934</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="29"/>
-      <c r="E10" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="24"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="43" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="48">
+      <c r="H10" s="24"/>
+      <c r="I10" s="43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="48">
       <c r="A11" s="32">
         <v>10</v>
       </c>
@@ -1566,19 +1600,20 @@
         <v>41941</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D11" s="29"/>
-      <c r="E11" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11" s="24"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="43" t="s">
+        <v>88</v>
+      </c>
       <c r="G11" s="24"/>
-      <c r="H11" s="47" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="144">
+      <c r="H11" s="24"/>
+      <c r="I11" s="47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="144">
       <c r="A12" s="32">
         <v>11</v>
       </c>
@@ -1587,19 +1622,20 @@
         <v>41948</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D12" s="29"/>
-      <c r="E12" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" s="24"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="43" t="s">
+        <v>89</v>
+      </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="47" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="80">
+      <c r="H12" s="24"/>
+      <c r="I12" s="47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="80">
       <c r="A13" s="32">
         <v>12</v>
       </c>
@@ -1608,32 +1644,34 @@
         <v>41955</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" s="29"/>
-      <c r="E13" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="24"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="43" t="s">
+        <v>90</v>
+      </c>
       <c r="G13" s="24"/>
-      <c r="H13" s="45"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13" s="24"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="33"/>
       <c r="B14" s="34">
         <f t="shared" si="0"/>
         <v>41962</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="35"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="46"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="46"/>
-    </row>
-    <row r="15" spans="1:8" ht="32">
+      <c r="H14" s="35"/>
+      <c r="I14" s="46"/>
+    </row>
+    <row r="15" spans="1:9" ht="32">
       <c r="A15" s="32">
         <v>13</v>
       </c>
@@ -1642,19 +1680,20 @@
         <v>41969</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D15" s="29"/>
-      <c r="E15" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="F15" s="24"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="43" t="s">
+        <v>91</v>
+      </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="64">
+      <c r="H15" s="24"/>
+      <c r="I15" s="43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="64">
       <c r="A16" s="32">
         <v>14</v>
       </c>
@@ -1663,19 +1702,20 @@
         <v>41976</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D16" s="29"/>
-      <c r="E16" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="24"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="43" t="s">
+        <v>92</v>
+      </c>
       <c r="G16" s="24"/>
-      <c r="H16" s="43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="32">
+      <c r="H16" s="24"/>
+      <c r="I16" s="43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="32">
       <c r="A17" s="32">
         <v>15</v>
       </c>
@@ -1684,17 +1724,18 @@
         <v>41983</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D17" s="29"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="24"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="43"/>
       <c r="G17" s="24"/>
-      <c r="H17" s="43" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="H17" s="24"/>
+      <c r="I17" s="43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="32" t="s">
         <v>0</v>
       </c>
@@ -1706,10 +1747,11 @@
         <v>0</v>
       </c>
       <c r="D18" s="29"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="43"/>
       <c r="G18" s="29"/>
       <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix assignment links in wks
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D2FA20-DD15-46AD-B85E-54C2331C7957}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCD02D6-EBC8-421B-B9A0-80AA89D03968}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,33 +459,6 @@
 * How to identify categorical vs numerical values in your SPC</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[Syllabus](syllabus_615_f18.html)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Lec 00 - Introduction to the class](lecture/lec00_intro_class.html)
-[Reproducibility slides](http://benmarwick.github.io/UW-eScience-reproducibility-social-sciences/#/)
-[Passion Driven Statistics](reading/PDS_Intro_Stat.pdf)
-[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)
-[Medical Records Data Files](https://norcalbiostat.netlify.com/data/raw_data/)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Familarize yourself with the course website organization
 Buy the textbook (PMA5), read PMA6 draft ch 1-3 (skip 3.4)
 Join Slack workspace: math615.slack.com 
@@ -656,14 +629,48 @@
       <t>Peer Review of RQ assignment (Due Wed 9/19 )</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_615_f18.html)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[Lec 00 - Introduction to the class](lecture/lec00_intro_class.html)
+[Reproducibility slides](http://benmarwick.github.io/UW-eScience-reproducibility-social-sciences/#/)
+[Passion Driven Statistics](reading/PDS_Intro_Stat.pdf)
+[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)
+[Medical Records Data Files](https://norcalbiostat.netlify.com/data/raw_data/)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -886,104 +893,104 @@
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="90" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -997,7 +1004,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="91" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1035,79 +1042,82 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1549,8 +1559,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,19 +1620,19 @@
         <v>102</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="44" t="s">
         <v>109</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>121</v>
       </c>
       <c r="G2" s="25" t="s">
         <v>100</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I2" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -1640,19 +1650,19 @@
         <v>103</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G3" s="44" t="s">
         <v>108</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="255" x14ac:dyDescent="0.25">
@@ -1664,7 +1674,7 @@
         <v>41892</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>104</v>
@@ -1673,16 +1683,16 @@
         <v>107</v>
       </c>
       <c r="F4" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="26" t="s">
         <v>120</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
revise org and add hw
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCD02D6-EBC8-421B-B9A0-80AA89D03968}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6A287-5A26-46B8-B1C5-704FB4286DE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
@@ -32,42 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Robin</author>
-  </authors>
-  <commentList>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{2A116636-9ACC-421C-8181-EA3AC3DCC9AE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Robin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-add interpretations to all graphs in the original document</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="143">
   <si>
     <t>Finals Week</t>
   </si>
@@ -138,66 +104,9 @@
     <t>Exam</t>
   </si>
   <si>
-    <t>Data Camp</t>
-  </si>
-  <si>
-    <t>Multiple Regression</t>
-  </si>
-  <si>
-    <t>Model Building</t>
-  </si>
-  <si>
-    <t>Peer Review Model Building</t>
-  </si>
-  <si>
-    <t>Project Updates</t>
-  </si>
-  <si>
-    <t>Poster Presentations</t>
-  </si>
-  <si>
-    <t>GLM Assignment</t>
-  </si>
-  <si>
-    <t>Peer Review GLM Assignment</t>
-  </si>
-  <si>
-    <t>PCA/FA Assignment</t>
-  </si>
-  <si>
-    <t>Peer Review PCA/FA Assignment</t>
-  </si>
-  <si>
-    <t>Correlated Data</t>
-  </si>
-  <si>
-    <t>Missing Data</t>
-  </si>
-  <si>
-    <t>PR Missing Data</t>
-  </si>
-  <si>
-    <t>QFT Model Building</t>
-  </si>
-  <si>
-    <t>QFT Correlated Data</t>
-  </si>
-  <si>
-    <t>QFT Missing Data</t>
-  </si>
-  <si>
-    <t>QFT Midterm Review</t>
-  </si>
-  <si>
     <t>Midterm</t>
   </si>
   <si>
-    <t>QFT Final Exam</t>
-  </si>
-  <si>
-    <t>PR Correlated Data</t>
-  </si>
-  <si>
     <t>Slack Introductions</t>
   </si>
   <si>
@@ -252,40 +161,16 @@
     <t>Manipulating data:C ase study</t>
   </si>
   <si>
-    <t>PR Spatio-Temporal</t>
-  </si>
-  <si>
-    <t>QFT Spatio-Temporal</t>
-  </si>
-  <si>
-    <t>Spatio-Temporal analysis</t>
-  </si>
-  <si>
     <t>Topic</t>
   </si>
   <si>
-    <t>QFT n&lt;&lt;p</t>
-  </si>
-  <si>
     <t>Research Proposal</t>
   </si>
   <si>
-    <t>Model Writing Practice</t>
-  </si>
-  <si>
-    <t>Classification Practice</t>
-  </si>
-  <si>
     <t>Tuesday</t>
   </si>
   <si>
     <t>Thursday</t>
-  </si>
-  <si>
-    <t>Exploring bivariate relationships</t>
-  </si>
-  <si>
-    <t>Foundations for inference: Probability, Normality, sampling distributions, Confidence Intervals, Hypothesis Testing</t>
   </si>
   <si>
     <t>Overview of Bivariate analysis procedures.
@@ -316,19 +201,6 @@
   </si>
   <si>
     <t>Read Intro for:  PMA15 Ch 13, 14,15, 16, 18</t>
-  </si>
-  <si>
-    <t>Foundations assignment (Due 10/x )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Bivariate Inference Assignment](hw/Bivariate_Inference.html) (Due 10/xx )
-</t>
-  </si>
-  <si>
-    <t>[Moderation Assignment](hw/Moderation_Assignment.html) (Due 11/x )</t>
-  </si>
-  <si>
-    <t>[Regression Assignment](hw/Regression_Assignment.html) (Due 11/xx )</t>
   </si>
   <si>
     <t>wk</t>
@@ -347,54 +219,8 @@
 [PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)</t>
   </si>
   <si>
-    <t xml:space="preserve">[PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
-Study Design Notes [[HTML]](docs/lec06_StudyDesign.html) [[PDF]](docs/lec06_StudyDesign.pdf)
-PMA5 Chapter 7, 9.1-9.3, 9.5
-Multiple Regression Notes (link to 456)
-[Regression Assignment Examples](hw/Regression_Assignment_Examples.html)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMA5 9.3 (dummy variables)
-PMA5 Ch 6.9 (transformations)
-Logistic Regression PMA5 Ch 12, [456 Notebook]()
-</t>
-  </si>
-  <si>
-    <t>Poster Prep: Stage II (Due 10/xx )
-Peer Review: Stage II (Due 11/x )</t>
-  </si>
-  <si>
-    <t>Poster Prep: Stage III (Due 11/xx )
-Peer Review: Stage III (Due 11/xx )</t>
-  </si>
-  <si>
-    <t>Poster draft due (12/x )
-[PR poster draft](https://norcalbiostat.github.io/MATH615/project.html#final_posters) (12/x )</t>
-  </si>
-  <si>
-    <t>Final Posters as printed  (Due 12/x )
-Poster scoring (Due 12/x )</t>
-  </si>
-  <si>
-    <t>Choosing appropriate analyses
-Midterm Thu</t>
-  </si>
-  <si>
-    <t>Research plan outline (Due Mon 9/xx )
-Peer Review (Due Wed 9/xx )
-Poster prep I (Due 10/x )
-Peer Review (Due 10/xx )</t>
-  </si>
-  <si>
     <t>Poster Presentations
 Final Review</t>
-  </si>
-  <si>
-    <t>Poster Design</t>
-  </si>
-  <si>
-    <t>Special Analysis Topics</t>
   </si>
   <si>
     <t xml:space="preserve">* Introduction to the class structure, materials, requirements, expectations and resources. 
@@ -418,13 +244,163 @@
 Create univariate visualizations of data</t>
   </si>
   <si>
-    <t xml:space="preserve">Identify features of data that will need to be changed prior to analysis
-Implement various data prepration tasks in an analysis software program
-Understand and replicate best practices for reading journal articles and citing literature. </t>
-  </si>
-  <si>
     <t>Data Import
 Univariate Data Visualizations</t>
+  </si>
+  <si>
+    <t>* Workflow - Keeping your raw data untouched
+* Using GUI methods to extract code. 
+* Import your raw analysis data set your SPC, keep only variables of interest from your codebook, save an analysis data file to disk
+* How to identify categorical vs numerical values in your SPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Familarize yourself with the course website organization
+Buy the textbook (PMA5), read PMA6 draft ch 1-3 (skip 3.4)
+Join Slack workspace: math615.slack.com 
+Install statistical analysis software before Thursday
+Read through the rest of the posted materials below. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Review basic data structures, types 
+* What's a codebook? Aka a Data Dictionary. Defines each variable definition and the expected values. 
+* Enter [Medical Records](hw/01_DataEntry.html) data and create a codebook.
+* Import your created data set into your software program of choice (SPC) using point and click methods. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Create pretty pictures to win friends and influence people. 
+* Or just to get to know your data. 
+* The text is your reference for what type of graphics are appropriate for each data type. 
+* The important part is to learn how to interpret the graph in plain english - covered in class
+* How to make the graphics in your SPC is done by you outside of class via notes/tutorials. 
+* Analysis code files should be separate. Read in the analysis data set - not the raw data. </t>
+  </si>
+  <si>
+    <t>[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 1.1, 1.3
+[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)</t>
+  </si>
+  <si>
+    <t>Create and interpret appropriate visualizations to examine associations between two variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean up all variables directly related to your research questions
+Read PMA6 DRAFT Ch 4.3, 4.6
+</t>
+  </si>
+  <si>
+    <t>Create a `MATH615`  folder in an easy to find place on your computer. Create the following sub-folders 1) `data`, 2) `code`, 3) `results`
+Download the data set that you are going to be analyzing and save it into your `MATH615\data` folder. 
+Start a code file (`dm.Rmd` or `dm.sps`) and import your chosen analysis data set. Save this code file to your `MATH615\code` folder. 
+Skim AS Notes Chapter 1 notes before Tuesday
+Read PMA6 DRAFT Ch 4.1, 4.2, 4.5 before Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)  </t>
+  </si>
+  <si>
+    <t>Read through the data management prep questions and use your last graphing assignment to start to think about what variables will need to be changed. 
+Read PMA6 DRAFT Chapter 3.4 - Data Recoding
+Read PMA5 Chapter 4 - Transforming your variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploring bivariate relationships
+</t>
+  </si>
+  <si>
+    <t>Poster Prep: Stage II (Due Wed 10/24 )
+Peer Review: Stage II (Due Fri 10/26 )</t>
+  </si>
+  <si>
+    <t>Final Poster</t>
+  </si>
+  <si>
+    <t>PR Poster Draft</t>
+  </si>
+  <si>
+    <t>Poster Draft</t>
+  </si>
+  <si>
+    <t>PR Poster prep III</t>
+  </si>
+  <si>
+    <t>Poster prep III</t>
+  </si>
+  <si>
+    <t>PR Regression</t>
+  </si>
+  <si>
+    <t>PR Moderation</t>
+  </si>
+  <si>
+    <t>PR Poster prep II</t>
+  </si>
+  <si>
+    <t>Poster prep II</t>
+  </si>
+  <si>
+    <t>PR Bivariate Inference</t>
+  </si>
+  <si>
+    <t>Bivariate Inference</t>
+  </si>
+  <si>
+    <t>Foundations Assignment</t>
+  </si>
+  <si>
+    <t>PR Bivariate Graphing</t>
+  </si>
+  <si>
+    <t>Bivariate graphing</t>
+  </si>
+  <si>
+    <t>PR Poster prep I</t>
+  </si>
+  <si>
+    <t>Poster prep I</t>
+  </si>
+  <si>
+    <t>RQ and codebook</t>
+  </si>
+  <si>
+    <t>DM code file</t>
+  </si>
+  <si>
+    <t>PR Univ Graphics</t>
+  </si>
+  <si>
+    <t>Univariate Graphics</t>
+  </si>
+  <si>
+    <t>Data Entry</t>
+  </si>
+  <si>
+    <t>PR Final Poster</t>
+  </si>
+  <si>
+    <t>Slack participation</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Read PMA5 Ch 9.3 (dummy variables)
+Read PMA5 Ch 6.9 (transformations)
+Read PMA5 Ch 12 (Logistic Regression)</t>
+  </si>
+  <si>
+    <t>[AS Notebook]() CH 7</t>
+  </si>
+  <si>
+    <t>[AS Notebook]() CH 8</t>
+  </si>
+  <si>
+    <t>Read PMA5 Chapter 7, 9.1-9.3, 9.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
+Study Design Notes [[HTML]](docs/lec06_StudyDesign.html) [[PDF]](docs/lec06_StudyDesign.pdf)
+AS Notebook [Ch 6]() 
+[Regression Assignment Examples](hw/Regression_Assignment_Examples.html)
+</t>
   </si>
   <si>
     <r>
@@ -435,102 +411,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Bivariate graphing assignment (Due 9/24 )
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Peer Review (Due 9/26 )</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Read through the data management prep questions and use your last graphing assignment to start to think about what variables will need to be changed. </t>
-  </si>
-  <si>
-    <t>* Workflow - Keeping your raw data untouched
-* Using GUI methods to extract code. 
-* Import your raw analysis data set your SPC, keep only variables of interest from your codebook, save an analysis data file to disk
-* How to identify categorical vs numerical values in your SPC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Familarize yourself with the course website organization
-Buy the textbook (PMA5), read PMA6 draft ch 1-3 (skip 3.4)
-Join Slack workspace: math615.slack.com 
-Install statistical analysis software before Thursday
-Read through the rest of the posted materials below. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Review basic data structures, types 
-* What's a codebook? Aka a Data Dictionary. Defines each variable definition and the expected values. 
-* Enter [Medical Records](hw/01_DataEntry.html) data and create a codebook.
-* Import your created data set into your software program of choice (SPC) using point and click methods. </t>
-  </si>
-  <si>
-    <t>Create a `MATH615`  folder in an easy to find place on your computer. Create the following sub-folders 1) `data`, 2) `code`, 3) `results`
-Download the data set that you are going to be analyzing and save it into your `MATH615\data` folder. 
-Start a code file (`dm.Rmd` or `dm.sps`) and import your chosen analysis data set. Save this code file to your `MATH615\code` folder. 
-Skim AS Notes Chapter 1 notes before Tuesday
-Read PMA6 DRAFT Ch 4 before Thursday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Create pretty pictures to win friends and influence people. 
-* Or just to get to know your data. 
-* The text is your reference for what type of graphics are appropriate for each data type. 
-* The important part is to learn how to interpret the graph in plain english - covered in class
-* How to make the graphics in your SPC is done by you outside of class via notes/tutorials. 
-* Analysis code files should be separate. Read in the analysis data set - not the raw data. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* What steps are needed to prepare your data for analysis? 
-* We need to ensure that these steps taken are all recorded in code, such that there are no manual changes conducted. 
-* Often we would like normally distributed data. There are a few ways we can achieve that. We'll cover how to identify non-normally distributed data and what transformations are available. 
-* Work on your `dm` (data management) code file during class. You will turn a copy of this in. Your results must be able to be replicated on my computer. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Univariate graphing Assignment [[HTML]](hw/02_Univariate_Graphing_Assignment.html)[[PDF]](hw/02_Univariate_Graphing_Assignment.pdf) (Due Mon 9/10 )
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Peer Revew (Due Wed 9/12 )</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">* What's the difference between writing about empirical research and other types of writing? 
-* Let's discuss some best practices and tips on how to read journal articles without burning yourself out. 
-* Then you can generate your own research questions based on current literature. </t>
-  </si>
-  <si>
-    <t>Preparing your data for analysis
-Writing about empirical research</t>
-  </si>
-  <si>
-    <t>[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 1.1, 1.3
-[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Decide on a data set to analyze and install your software program of choice (Due Thu 8/30 )
-</t>
+      <t>[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_615_f18.html)</t>
     </r>
     <r>
       <rPr>
@@ -540,105 +421,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Join our [Slack team](http://math615.slack.com) and post an `#introduction` (See instructions in channel) (Due Mon 9/3 )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
-Data entry and Codebook creation [Assignment](hw/01_DataEntry.html) (Due Mon 9/3 )</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[PMA6 DRAFT](reading/PMA6 DRAFT.pdf) Chapter 3.4 - Data Recoding
-**PMA5** Chapter 4 (Transforming your variables) 
-Data Management preparation questions [[HTML]](lecture/lec01_dm_prep_questions.html)[[PDF]](lecture/lec01_dm_prep_questions.pdf)
-[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 1
-How to read a Journal Article[[PDF]](reading/How to Read a Journal Article.pdf)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Writing about empirical research [[HTML]](lecture/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lec02a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_writing_em.html)[[PDF]](lecture/lec02a_writing_em.pdf)
-Literature Review notes [[HTML]](lecture/lec02b_lit_review.html)[[PDF]](lecture/lec02b_lit_review.pdf)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Data management code file (Due Mon 9/17 ) 
-Research Question and Codebook Assignment [[HTML]](hw/03_RQ_codebook_assignment.html)[[PDF]](hw/03_RQ_codebook_assignment.pdf)  (Due Mon 9/17 )
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Peer Review of RQ assignment (Due Wed 9/19 )</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_615_f18.html)
 </t>
     </r>
     <r>
@@ -656,28 +439,226 @@
 [Medical Records Data Files](https://norcalbiostat.netlify.com/data/raw_data/)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Univariate graphing assignment [[HTML]](hw/02_univariate_graphing_assignment.html)[[PDF]](hw/02_univariate_graphing_assignment.pdf) (Due Mon 9/10 )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Peer Revew (Due Wed 9/12 )
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Decide on a data set to analyze and install your software program of choice (Due Thu 8/30 )
+Take [this survey](https://goo.gl/forms/qLBv2jMF6fBv3BTR2) to help me set my OH (Due Thu 8/30 )
+Join our [Slack team](http://math615.slack.com) and post an `#introduction` (See instructions in channel) (Due Mon 9/3 )
+Data entry assignment [[HTML]](hw/01_data_entry.html)[[PDF]](hw/01_data_entry.pdf) (Due Mon 9/3 )</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Bivariate graphing assignment [[HTML]](hw/04_bivariate_graphing_assignment.html)[[PDF]](hw/04_bivariate_graphing_assignment.pdf) (Due Mon 9/24 )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peer Review (Due Wed 9/26 )</t>
+    </r>
+  </si>
+  <si>
+    <t>Final Posters as printed  (Due Mon 12/10 )
+Poster scoring (Due Fri 12/14 )</t>
+  </si>
+  <si>
+    <t>Poster Design
+Special Analysis Topics</t>
+  </si>
+  <si>
+    <t>Model building tactics</t>
+  </si>
+  <si>
+    <t>Open work session</t>
+  </si>
+  <si>
+    <t>Poster Prep: Stage III (Due Fri 11/30 )
+Peer Review: Stage III (Due Sun 12/2 )</t>
+  </si>
+  <si>
+    <t>Poster draft (Due Friday 12/7 )
+[PR poster draft](https://norcalbiostat.github.io/MATH615/project.html#final_posters) (Due Sun 12/9 )</t>
+  </si>
+  <si>
+    <t>Preparing your data for analysis
+Recoding, data editing and transformations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify features of data that will need to be changed prior to analysis
+Implement various data prepration tasks in an analysis software program
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)  
+**PMA5** Chapter 4 
+Data Management preparation questions [[HTML]](lecture/lec01_dm_prep_questions.html)[[PDF]](lecture/lec01_dm_prep_questions.pdf)
+[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What's the difference between writing about empirical research and other types of writing? 
+* Let's discuss some best practices and tips on how to read journal articles without burning yourself out. 
+* Then you can refine your own research questions based on current literature. </t>
+  </si>
+  <si>
+    <t>* Choosing appropriate citations
+* How to prepare to write your research proposal</t>
+  </si>
+  <si>
+    <t>* Appropriate methods to visualize combinations of categorical variables, C~C, C~Q</t>
+  </si>
+  <si>
+    <t>* Appropriate methods to visualize combinations of quantitative variables (Q~Q)
+* Creating Multivariate graphics. 
+* Best practices for informative graphics (no chart junk)</t>
+  </si>
+  <si>
+    <t>* Hypothesis Testing &amp; p-values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What steps are needed to prepare your data for analysis? 
+* We need to ensure that these steps taken are all recorded in code, such that there are no manual changes conducted. 
+* Often we would like normally distributed data. There are a few ways we can achieve that. We'll cover how to identify non-normally distributed data and what transformations are available. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Work on your `dm` (data management) code file during class. You will turn a copy of this in. Your results must be able to be replicated on my computer. </t>
+  </si>
+  <si>
+    <t>Foundations worksheet</t>
+  </si>
+  <si>
+    <t>Research proposal examples [[PDF]](reading/Research Proposal Examples.pdf)</t>
+  </si>
+  <si>
+    <t>* Probability of exploding kittens
+* Sampling Distributions
+* Confidence intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probability &amp; Confidence Intervals
+Foundations for inference
+</t>
+  </si>
+  <si>
+    <t>Midterm
+Normality and Hypothesis Testing</t>
+  </si>
+  <si>
+    <t>Understand and implement best practices for reading journal articles and citing literature. 
+Write a testable hypothesis that is supported by the literature
+Identify areas of new research</t>
+  </si>
+  <si>
+    <t>Writing about empirical research [[HTML]](lecture/lec02a_writing_em.html)[[PDF]](lecture/lec02a_writing_em.pdf)
+Literature Review notes [[HTML]](lecture/lec02b_lit_review.html)[[PDF]](lecture/lec02b_lit_review.pdf)
+How to read a Journal Article[[PDF]](reading/How to Read a Journal Article.pdf)
+Citation Assignment (not assigned)[[PDF]](reading/Citation_Assignment.pdf)
+Citation Assignment Example [[PDF]](reading/Citation Assignment Example.pdf)</t>
+  </si>
+  <si>
+    <t>PR Research Proposal</t>
+  </si>
+  <si>
+    <t>Foundations assignment (Due Fri 10/4 )</t>
+  </si>
+  <si>
+    <t>Research Propsal Prep</t>
+  </si>
+  <si>
+    <t>PR Research proposal prep</t>
+  </si>
+  <si>
+    <t>Writing about empirical research
+Research proposal preparation</t>
+  </si>
+  <si>
+    <t>Research proposal [[HTML]](hw/06_research_proposal.html)[[PDF]](hw/06_research_proposal.pdf) (Due Mon 10/8 )
+PR Research proposal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bivariate inference assignment [[HTML]](hw/07_bivariate_Inference.html)[[PDF]](hw/07_bivariate_Inference.pdf) (Due Mon 10/22 )
+Peer Review (Due Wed 10/24 )
+</t>
+  </si>
+  <si>
+    <t>Moderation assignment [[HTML]](hw/08_moderation.html)[[PDF]](hw/08_moderation.pdf) (Due Mon 10/29 )
+Peer Review (Due Wed 10/31 )</t>
+  </si>
+  <si>
+    <t>Regression assignment [[HTML]](hw/09_regression.html)[[PDF]](hw/09_regression.pdf) (Due Mon 11/12 )
+Peer Review (Due Wed 11/14)</t>
+  </si>
+  <si>
+    <t>Proposal preparation assignment [[HTML]](hw/05_proposal_prep.html)[[PDF]](hw/05_proposal_prep.pdf)(Due Mon 10/1 )
+Peer Review (Due Wed 10/3 )</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data management code file (Due Mon 9/17 ) 
+Research Question and Codebook Assignment [[HTML]](hw/03_research_codebook.html)[[PDF]](hw/03_research_codebook.pdf)  (Due Mon 9/17 )</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Poster Prep: Stage I (Due Wed 9/19 )
+Peer Review: Stage I (Due Fri 9/20 )</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -777,34 +758,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -893,104 +846,104 @@
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="90" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1004,7 +957,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="91" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1042,79 +995,70 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1555,31 +1499,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5" style="24" customWidth="1"/>
     <col min="2" max="2" width="10.125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="26.125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="24" customWidth="1"/>
     <col min="4" max="4" width="27.375" style="32" customWidth="1"/>
     <col min="5" max="5" width="31.875" style="32" customWidth="1"/>
-    <col min="6" max="6" width="54.5" style="32" customWidth="1"/>
+    <col min="6" max="6" width="45.875" style="32" customWidth="1"/>
     <col min="7" max="7" width="30.125" style="32" customWidth="1"/>
     <col min="8" max="8" width="32.875" style="32" customWidth="1"/>
-    <col min="9" max="9" width="39" style="32" customWidth="1"/>
+    <col min="9" max="9" width="54.75" style="32" customWidth="1"/>
     <col min="10" max="16384" width="14.875" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>2</v>
@@ -1591,52 +1535,52 @@
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="F1" s="33" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="I1" s="33" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A2" s="47">
+      <c r="A2" s="44">
         <v>1</v>
       </c>
       <c r="B2" s="36">
         <v>41878</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>121</v>
+        <v>61</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>105</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="48" t="s">
-        <v>118</v>
+        <v>59</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="47">
+      <c r="A3" s="44">
         <v>2</v>
       </c>
       <c r="B3" s="36">
@@ -1644,28 +1588,28 @@
         <v>41885</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>112</v>
+        <v>62</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>67</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="35">
         <v>3</v>
       </c>
@@ -1673,49 +1617,59 @@
         <f t="shared" si="0"/>
         <v>41892</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>119</v>
+      <c r="E4" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>117</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="35">
         <v>4</v>
       </c>
       <c r="B5" s="36">
-        <f t="shared" si="0"/>
+        <f>B4+7</f>
         <v>41899</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C5" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="35">
         <v>5</v>
       </c>
@@ -1723,19 +1677,27 @@
         <f t="shared" si="0"/>
         <v>41906</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="28"/>
+      <c r="C6" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>130</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="F6" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="35">
         <v>6</v>
       </c>
@@ -1743,19 +1705,23 @@
         <f t="shared" si="0"/>
         <v>41913</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="C7" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="35">
         <v>7</v>
       </c>
@@ -1764,15 +1730,21 @@
         <v>41920</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="29" t="s">
-        <v>82</v>
+      <c r="F8" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" s="45" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1783,21 +1755,19 @@
         <f t="shared" si="0"/>
         <v>41927</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>74</v>
+      <c r="C9" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
-      <c r="F9" s="27" t="s">
-        <v>87</v>
-      </c>
+      <c r="F9" s="27"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I9" s="29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="37">
         <v>9</v>
       </c>
@@ -1806,20 +1776,20 @@
         <v>41934</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
-      <c r="F10" s="27" t="s">
-        <v>88</v>
+      <c r="F10" s="45" t="s">
+        <v>56</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
-      <c r="I10" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="I10" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="37">
         <v>10</v>
       </c>
@@ -1827,21 +1797,21 @@
         <f t="shared" si="0"/>
         <v>41941</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>76</v>
+      <c r="C11" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="37">
         <v>11</v>
       </c>
@@ -1849,19 +1819,23 @@
         <f t="shared" si="0"/>
         <v>41948</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>77</v>
+      <c r="C12" s="26" t="s">
+        <v>49</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27" t="s">
-        <v>90</v>
+      <c r="E12" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>104</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="27"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I12" s="45" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="37">
         <v>12</v>
       </c>
@@ -1870,18 +1844,18 @@
         <v>41955</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27" t="s">
-        <v>79</v>
+      <c r="E13" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>102</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
-      <c r="I13" s="27" t="s">
-        <v>92</v>
-      </c>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
@@ -1897,7 +1871,7 @@
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="37">
         <v>13</v>
       </c>
@@ -1905,17 +1879,25 @@
         <f t="shared" si="0"/>
         <v>41969</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>99</v>
+      <c r="C15" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="27"/>
+      <c r="E15" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="37">
@@ -1926,15 +1908,17 @@
         <v>41976</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="E16" s="27" t="s">
+        <v>53</v>
+      </c>
       <c r="F16" s="27"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
-      <c r="I16" s="27" t="s">
-        <v>93</v>
+      <c r="I16" s="45" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1946,15 +1930,15 @@
         <v>41983</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
-      <c r="I17" s="27" t="s">
-        <v>94</v>
+      <c r="I17" s="45" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1976,34 +1960,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFAA633-0D4B-46C7-9CFF-955F6192B7FE}">
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:D12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="6"/>
+    <col min="1" max="1" width="8.875" style="6"/>
     <col min="2" max="2" width="32.125" style="6" customWidth="1"/>
     <col min="3" max="3" width="11.125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="6"/>
+    <col min="4" max="4" width="8.875" style="6"/>
     <col min="5" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="10" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="3"/>
+    <col min="8" max="8" width="8.875" style="3"/>
     <col min="9" max="9" width="4.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -2026,60 +2009,60 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="21">
+        <v>24</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="15">
         <v>5</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="18">
-        <f>SUMIF($C$2:$C$89,F2,$D$2:$D$89)</f>
-        <v>120</v>
+        <f>SUMIF($C$2:$C$91,F2,$D$2:$D$91)</f>
+        <v>80</v>
       </c>
       <c r="H2" s="20">
         <f>G2/$G$6</f>
-        <v>0.25</v>
+        <v>0.24242424242424243</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="21">
-        <v>20</v>
+        <v>96</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="15">
+        <v>10</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="21">
-        <f>SUMIF($C$2:$C$89,F3,$D$2:$D$89)</f>
-        <v>100</v>
+        <f>SUMIF($C$2:$C$91,F3,$D$2:$D$91)</f>
+        <v>50</v>
       </c>
       <c r="H3" s="23">
         <f>G3/$G$6</f>
-        <v>0.20833333333333334</v>
+        <v>0.15151515151515152</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>17</v>
@@ -2091,424 +2074,453 @@
         <v>22</v>
       </c>
       <c r="G4" s="12">
-        <f>SUMIF($C$2:$C$89,F4,$D$2:$D$89)</f>
-        <v>200</v>
+        <f>SUMIF($C$2:$C$91,F4,$D$2:$D$91)</f>
+        <v>100</v>
       </c>
       <c r="H4" s="14">
         <f>G4/$G$6</f>
-        <v>0.41666666666666669</v>
+        <v>0.30303030303030304</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="11">
-        <f>SUMIF($C$2:$C$89,F5,$D$2:$D$89)</f>
-        <v>60</v>
+        <f>SUMIF($C$2:$C$91,F5,$D$2:$D$91)</f>
+        <v>100</v>
       </c>
       <c r="H5" s="17">
         <f>G5/$G$6</f>
-        <v>0.125</v>
+        <v>0.30303030303030304</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>2.2000000000000002</v>
+        <v>3.1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G6" s="8">
         <f>SUM(G2:G5)</f>
-        <v>480</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>2.2999999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="21">
-        <v>5</v>
+        <v>92</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="11">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="11">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="15">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>3.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="21">
-        <v>5</v>
+        <v>134</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="11">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>4</v>
+        <v>5.2</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="21">
-        <v>5</v>
-      </c>
-      <c r="G13"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>4.0999999999999996</v>
+        <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>4.2</v>
+        <v>7.1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="21">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="12">
+        <v>50</v>
       </c>
       <c r="G15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>5</v>
+        <v>7.2</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="21">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="11">
+        <v>20</v>
       </c>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>5.0999999999999996</v>
+        <v>7.3</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="12">
-        <v>100</v>
+        <v>132</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="21">
+        <v>5</v>
       </c>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>6</v>
+        <v>8.1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="11">
-        <v>20</v>
+        <v>86</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="15">
+        <v>10</v>
       </c>
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>7</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="15">
-        <v>20</v>
+        <v>84</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="11">
+        <v>10</v>
       </c>
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>7.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>8</v>
+        <v>10.1</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="21">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="15">
+        <v>10</v>
       </c>
       <c r="G22"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>8.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="15">
-        <v>20</v>
+        <v>82</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="21">
+        <v>4</v>
       </c>
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>8.1999999999999993</v>
+        <v>12.1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="21">
-        <v>5</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="15">
+        <v>10</v>
+      </c>
+      <c r="G24"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>9</v>
+        <v>12.2</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="21">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G25"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>9.1</v>
+        <v>13.1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="15">
-        <v>20</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="11">
+        <v>10</v>
+      </c>
+      <c r="G26"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>9.1999999999999993</v>
+        <v>13.2</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>10</v>
+        <v>14.1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="11">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>11</v>
+        <v>14.2</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D29" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>11.1</v>
+        <v>15.1</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>16</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="D32" s="12">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="3">
+        <v>16</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="21">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
@@ -2551,7 +2563,6 @@
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
@@ -2564,6 +2575,7 @@
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -2594,14 +2606,12 @@
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="9"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="9"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
@@ -2714,9 +2724,6 @@
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="9"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="6"/>
-      <c r="H66" s="6"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -2724,39 +2731,42 @@
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="9"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
-      <c r="E68" s="5"/>
-      <c r="I68" s="6"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
-      <c r="E69" s="5"/>
-      <c r="I69" s="6"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="9"/>
+      <c r="E70" s="5"/>
+      <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="9"/>
+      <c r="E71" s="5"/>
+      <c r="I71" s="6"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -2791,18 +2801,20 @@
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
+      <c r="E76" s="9"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="9"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
@@ -2827,16 +2839,12 @@
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
-      <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
-      <c r="E83" s="7"/>
-      <c r="G83"/>
-      <c r="H83"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
@@ -2850,6 +2858,7 @@
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
+      <c r="E85" s="7"/>
       <c r="G85"/>
       <c r="H85"/>
     </row>
@@ -2858,8 +2867,7 @@
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
-      <c r="G86"/>
-      <c r="H86"/>
+      <c r="E86" s="7"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
@@ -2914,12 +2922,16 @@
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
+      <c r="G93"/>
+      <c r="H93"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
+      <c r="G94"/>
+      <c r="H94"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
@@ -2940,14 +2952,23 @@
       <c r="D97" s="4"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="10"/>
-      <c r="B98" s="10"/>
-      <c r="D98" s="10"/>
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="10"/>
+      <c r="B100" s="10"/>
+      <c r="D100" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D100">
-    <sortCondition ref="A2:A100"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3023,33 +3044,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3057,13 +3078,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3071,7 +3092,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3079,7 +3100,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3087,10 +3108,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3098,7 +3119,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3106,7 +3127,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3114,7 +3135,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3122,7 +3143,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3130,7 +3151,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
render hw and rebuild
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6A287-5A26-46B8-B1C5-704FB4286DE8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5598F9C2-4D0E-42A5-91A6-D0CA5CE30E2C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="assignments" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
@@ -656,9 +656,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -846,104 +853,104 @@
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="90" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -957,7 +964,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="91" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -995,73 +1002,73 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1504,7 +1511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,7 +1728,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="35">
         <v>7</v>
       </c>
@@ -1747,7 +1754,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="35">
         <v>8</v>
       </c>
@@ -1968,7 +1975,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
rebuild up through week 4
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A82BB62-BB93-4B40-82F0-48F258D7D78A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CC2DC4-BBB8-4661-AE02-8D1F41012C1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="150">
   <si>
     <t>Finals Week</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Points</t>
-  </si>
-  <si>
-    <t>Learning</t>
   </si>
   <si>
     <t>Exam</t>
@@ -249,14 +246,6 @@
 * Import your created data set into your software program of choice (SPC) using point and click methods. </t>
   </si>
   <si>
-    <t xml:space="preserve">* Create pretty pictures to win friends and influence people. 
-* Or just to get to know your data. 
-* The text is your reference for what type of graphics are appropriate for each data type. 
-* The important part is to learn how to interpret the graph in plain english - covered in class
-* How to make the graphics in your SPC is done by you outside of class via notes/tutorials. 
-* Analysis code files should be separate. Read in the analysis data set - not the raw data. </t>
-  </si>
-  <si>
     <t>[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 1.1, 1.3
 [PMA6 DRAFT](reading/PMA6 DRAFT.pdf)</t>
   </si>
@@ -442,9 +431,6 @@
 * We need to ensure that these steps taken are all recorded in code, such that there are no manual changes conducted. 
 * Often we would like normally distributed data. There are a few ways we can achieve that. We'll cover how to identify non-normally distributed data and what transformations are available. 
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Work on your `dm` (data management) code file during class. You will turn a copy of this in. Your results must be able to be replicated on my computer. </t>
   </si>
   <si>
     <t>Foundations worksheet</t>
@@ -566,18 +552,36 @@
     <t>BBL Entry</t>
   </si>
   <si>
+    <t>Participation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Create pretty pictures to win friends and influence people. 
+* Or just to get to know your data. 
+* The text is your reference for what type of graphics are appropriate for each data type. 
+* The important part is to learn how to interpret the graph in plain english
+* How to make the graphics in your SPC is done by you outside of class via notes/tutorials. 
+* Analysis code files should be separate. Read in the analysis data set - not the raw data. </t>
+  </si>
+  <si>
     <t>Univariate graphing assignment [[HTML]](hw/02_univariate_graphing_assignment.html)[[PDF]](hw/02_univariate_graphing_assignment.pdf) (Due Mon 9/10 )
-Peer Revew (Due Wed 9/12 )</t>
-  </si>
-  <si>
-    <t>Data management code file (Due Mon 9/17 ) 
-Research Question and Codebook Assignment [[HTML]](hw/03_research_codebook.html)[[PDF]](hw/03_research_codebook.pdf)  (Due Mon 9/17 )
-Poster Prep: Stage I (Due Wed 9/19 )
-Peer Review: Stage I (Due Fri 9/20 )</t>
-  </si>
-  <si>
-    <t>Bivariate graphing assignment [[HTML]](hw/04_bivariate_graphing_assignment.html)[[PDF]](hw/04_bivariate_graphing_assignment.pdf) (Due Mon 9/24 )
+Peer Revew of Univariate Graphs (Due Wed 9/12 )
+Research Question and Codebook Assignment [[HTML]](hw/03_research_codebook.html)[[PDF]](hw/03_research_codebook.pdf)  (Due Wed 9/12 )</t>
+  </si>
+  <si>
+    <t>In use, % based</t>
+  </si>
+  <si>
+    <t>Bivariate graphing assignment [[HTML]](hw/05_bivariate_graphing_assignment.html)[[PDF]](hw/05_bivariate_graphing_assignment.pdf) (Due Mon 9/24 )
 Peer Review (Due Wed 9/26 )</t>
+  </si>
+  <si>
+    <t>Data management code file [[HTML]](hw/04_data_management.html)[[PDF]](hw/04_data_management.pdf) (Due Mon 9/17 ) 
+Poster Prep: Stage I (Due Wed 9/19 ) [Drop a note in BBL when done] 
+Peer Review: Stage I (Due Fri 9/21 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Work on your `dm` (data management) code file during class. You will turn a copy of this in. Your results must be able to be replicated on my computer. 
+* Start to build your analysis story. Descriptive analysis always comes first. Setting the stage. </t>
   </si>
 </sst>
 </file>
@@ -585,11 +589,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -783,104 +794,104 @@
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="90" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -894,7 +905,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="91" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -928,108 +939,113 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="92">
@@ -1469,460 +1485,460 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="24" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="24.625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="32" customWidth="1"/>
-    <col min="5" max="5" width="31.875" style="32" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="32" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="32" customWidth="1"/>
-    <col min="8" max="8" width="32.875" style="32" customWidth="1"/>
-    <col min="9" max="9" width="54.75" style="32" customWidth="1"/>
-    <col min="10" max="16384" width="14.875" style="24"/>
+    <col min="1" max="1" width="4.5" style="23" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="27.375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="31.875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="45.875" style="31" customWidth="1"/>
+    <col min="7" max="7" width="30.125" style="31" customWidth="1"/>
+    <col min="8" max="8" width="32.875" style="31" customWidth="1"/>
+    <col min="9" max="9" width="54.75" style="31" customWidth="1"/>
+    <col min="10" max="16384" width="14.875" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="F1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A2" s="43">
+        <v>1</v>
+      </c>
+      <c r="B2" s="35">
+        <v>41878</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A3" s="43">
         <v>2</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A2" s="44">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36">
-        <v>41878</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="44">
-        <v>2</v>
-      </c>
-      <c r="B3" s="36">
+      <c r="B3" s="35">
         <f t="shared" ref="B3:B18" si="0">B2+7</f>
         <v>41885</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>146</v>
+      <c r="H3" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
+      <c r="A4" s="34">
         <v>3</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="35">
         <f t="shared" si="0"/>
         <v>41892</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>147</v>
+      <c r="C4" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="35">
+      <c r="A5" s="34">
         <v>4</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="35">
         <f>B4+7</f>
         <v>41899</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="28" t="s">
+      <c r="C5" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>148</v>
+      <c r="G5" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" s="35">
+      <c r="A6" s="34">
         <v>5</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="35">
         <f t="shared" si="0"/>
         <v>41906</v>
       </c>
-      <c r="C6" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>131</v>
+      <c r="C6" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
+      <c r="A7" s="34">
         <v>6</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="35">
         <f t="shared" si="0"/>
         <v>41913</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="H7" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>123</v>
+      <c r="C7" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
+      <c r="A8" s="34">
         <v>7</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="35">
         <f t="shared" si="0"/>
         <v>41920</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="G8" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>127</v>
+      <c r="C8" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
+      <c r="A9" s="34">
         <v>8</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="35">
         <f t="shared" si="0"/>
         <v>41927</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="28" t="s">
-        <v>128</v>
+      <c r="C9" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="27" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+      <c r="A10" s="36">
         <v>9</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="35">
         <f t="shared" si="0"/>
         <v>41934</v>
       </c>
-      <c r="C10" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="28" t="s">
-        <v>70</v>
+      <c r="C10" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="27" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="37">
+      <c r="A11" s="36">
         <v>10</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="35">
         <f t="shared" si="0"/>
         <v>41941</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="28" t="s">
-        <v>129</v>
+      <c r="C11" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="27" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A12" s="37">
+      <c r="A12" s="36">
         <v>11</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="35">
         <f t="shared" si="0"/>
         <v>41948</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="28" t="s">
-        <v>130</v>
+      <c r="C12" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="27" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="37">
+      <c r="A13" s="36">
         <v>12</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="35">
         <f t="shared" si="0"/>
         <v>41955</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="45" t="s">
+      <c r="C13" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="29"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="39">
+      <c r="A14" s="37"/>
+      <c r="B14" s="38">
         <f t="shared" si="0"/>
         <v>41962</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="35">
         <f t="shared" si="0"/>
         <v>41969</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="46" t="s">
+      <c r="F15" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="45" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="37">
+      <c r="A16" s="36">
         <v>14</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="35">
         <f t="shared" si="0"/>
         <v>41976</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="45" t="s">
-        <v>106</v>
+      <c r="C16" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="44" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="37">
+      <c r="A17" s="36">
         <v>15</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="35">
         <f t="shared" si="0"/>
         <v>41983</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="45" t="s">
-        <v>101</v>
+      <c r="C17" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="44" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="35">
         <f t="shared" si="0"/>
         <v>41990</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1934,16 +1950,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFAA633-0D4B-46C7-9CFF-955F6192B7FE}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.875" style="6"/>
-    <col min="2" max="3" width="32.125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="32.125" style="52" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="6" customWidth="1"/>
     <col min="6" max="6" width="8.875" style="6"/>
     <col min="7" max="7" width="5.125" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
@@ -1954,16 +1971,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>145</v>
+        <v>137</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -1986,15 +2003,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="52">
+        <v>23</v>
+      </c>
+      <c r="D2" s="51">
         <v>41884</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="15">
+      <c r="E2" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="21">
         <v>5</v>
       </c>
       <c r="H2" s="19" t="s">
@@ -2002,11 +2019,11 @@
       </c>
       <c r="I2" s="18">
         <f>SUMIF($E$2:$E$91,H2,$F$2:$F$91)</f>
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="J2" s="20">
         <f>I2/$I$6</f>
-        <v>0.21052631578947367</v>
+        <v>9.8591549295774641E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2014,30 +2031,30 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="52">
+        <v>89</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="51">
         <v>41884</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="15">
-        <v>10</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="H3" s="56" t="s">
+        <v>143</v>
       </c>
       <c r="I3" s="21">
         <f>SUMIF($E$2:$E$91,H3,$F$2:$F$91)</f>
-        <v>50</v>
-      </c>
-      <c r="J3" s="23">
+        <v>65</v>
+      </c>
+      <c r="J3" s="22">
         <f>I3/$I$6</f>
-        <v>0.13157894736842105</v>
+        <v>0.18309859154929578</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,17 +2062,22 @@
         <v>2.1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="49"/>
+        <v>88</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="51">
+        <v>41891</v>
+      </c>
       <c r="E4" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="12">
         <f>SUMIF($E$2:$E$91,H4,$F$2:$F$91)</f>
@@ -2063,7 +2085,7 @@
       </c>
       <c r="J4" s="14">
         <f>I4/$I$6</f>
-        <v>0.26315789473684209</v>
+        <v>0.28169014084507044</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2071,68 +2093,83 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="D5" s="51">
+        <v>41893</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F5" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="11">
         <f>SUMIF($E$2:$E$91,H5,$F$2:$F$91)</f>
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="J5" s="17">
         <f>I5/$I$6</f>
-        <v>0.39473684210526316</v>
+        <v>0.43661971830985913</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="49"/>
-      <c r="E6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="15">
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="51">
+        <v>41893</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="11">
+        <v>10</v>
       </c>
       <c r="I6" s="8">
         <f>SUM(I2:I5)</f>
-        <v>380</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="51">
+        <v>41898</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="11">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>143</v>
+        <v>84</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="51">
+        <v>41900</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>18</v>
@@ -2143,16 +2180,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="D9" s="51">
+        <v>41902</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F9" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2160,14 +2200,14 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="49"/>
+        <v>82</v>
+      </c>
+      <c r="C10" s="48"/>
       <c r="E10" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2175,13 +2215,13 @@
         <v>4.2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F11" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2189,9 +2229,9 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="49"/>
+        <v>121</v>
+      </c>
+      <c r="C12" s="48"/>
       <c r="E12" s="11" t="s">
         <v>18</v>
       </c>
@@ -2204,13 +2244,13 @@
         <v>5.2</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F13" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2218,13 +2258,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I14"/>
     </row>
@@ -2233,10 +2273,10 @@
         <v>7.1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="12">
         <v>50</v>
@@ -2248,12 +2288,12 @@
         <v>7.2</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>142</v>
-      </c>
-      <c r="D16" s="53"/>
+        <v>42</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="52"/>
       <c r="E16" s="11" t="s">
         <v>18</v>
       </c>
@@ -2267,10 +2307,10 @@
         <v>7.3</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F17" s="21">
         <v>5</v>
@@ -2282,16 +2322,16 @@
         <v>8.1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>144</v>
+        <v>79</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>141</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I18"/>
     </row>
@@ -2300,13 +2340,13 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F19" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I19"/>
     </row>
@@ -2315,10 +2355,10 @@
         <v>9.1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>144</v>
+        <v>77</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>141</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>18</v>
@@ -2333,13 +2373,13 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F21" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I21"/>
     </row>
@@ -2348,16 +2388,16 @@
         <v>10.1</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>144</v>
+        <v>45</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>141</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I22"/>
     </row>
@@ -2366,13 +2406,13 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F23" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I23"/>
     </row>
@@ -2381,16 +2421,16 @@
         <v>12.1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="49" t="s">
-        <v>141</v>
+        <v>31</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>138</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I24"/>
     </row>
@@ -2399,13 +2439,13 @@
         <v>12.2</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F25" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I25"/>
     </row>
@@ -2414,10 +2454,10 @@
         <v>13.1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>144</v>
+        <v>73</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>141</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>18</v>
@@ -2432,13 +2472,13 @@
         <v>13.2</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F27" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2446,7 +2486,7 @@
         <v>14.1</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>18</v>
@@ -2460,13 +2500,13 @@
         <v>14.2</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F29" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2474,7 +2514,7 @@
         <v>15.1</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>18</v>
@@ -2488,10 +2528,10 @@
         <v>15.2</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="F31" s="21">
         <v>5</v>
@@ -2505,7 +2545,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F32" s="12">
         <v>50</v>
@@ -2516,10 +2556,10 @@
         <v>16</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F33" s="21">
         <v>10</v>
@@ -2535,7 +2575,7 @@
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="54"/>
+      <c r="D36" s="53"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
@@ -2543,7 +2583,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="54"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
@@ -2551,7 +2591,7 @@
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="54"/>
+      <c r="D38" s="53"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
@@ -2559,7 +2599,7 @@
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="54"/>
+      <c r="D39" s="53"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
@@ -2567,7 +2607,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="54"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
@@ -2575,7 +2615,7 @@
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="54"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
@@ -2583,7 +2623,7 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="54"/>
+      <c r="D42" s="53"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
@@ -2591,7 +2631,7 @@
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="54"/>
+      <c r="D43" s="53"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
@@ -2599,7 +2639,7 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="54"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="9"/>
@@ -2608,7 +2648,7 @@
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="54"/>
+      <c r="D45" s="53"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
@@ -2616,7 +2656,7 @@
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="54"/>
+      <c r="D46" s="53"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
@@ -2624,7 +2664,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="54"/>
+      <c r="D47" s="53"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
@@ -2632,7 +2672,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="54"/>
+      <c r="D48" s="53"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
@@ -2640,7 +2680,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="54"/>
+      <c r="D49" s="53"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
@@ -2648,7 +2688,7 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="54"/>
+      <c r="D50" s="53"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
@@ -2656,7 +2696,7 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="54"/>
+      <c r="D51" s="53"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="9"/>
@@ -2665,7 +2705,7 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="54"/>
+      <c r="D52" s="53"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="9"/>
@@ -2674,7 +2714,7 @@
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="54"/>
+      <c r="D53" s="53"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="9"/>
@@ -2683,7 +2723,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="54"/>
+      <c r="D54" s="53"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="9"/>
@@ -2692,7 +2732,7 @@
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="54"/>
+      <c r="D55" s="53"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="9"/>
@@ -2701,7 +2741,7 @@
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="54"/>
+      <c r="D56" s="53"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="9"/>
@@ -2710,7 +2750,7 @@
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="54"/>
+      <c r="D57" s="53"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="9"/>
@@ -2719,7 +2759,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="54"/>
+      <c r="D58" s="53"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="9"/>
@@ -2728,7 +2768,7 @@
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="54"/>
+      <c r="D59" s="53"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="9"/>
@@ -2737,7 +2777,7 @@
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="54"/>
+      <c r="D60" s="53"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="9"/>
@@ -2746,7 +2786,7 @@
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="54"/>
+      <c r="D61" s="53"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="9"/>
@@ -2755,7 +2795,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="54"/>
+      <c r="D62" s="53"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="9"/>
@@ -2764,7 +2804,7 @@
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="54"/>
+      <c r="D63" s="53"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="9"/>
@@ -2773,7 +2813,7 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
-      <c r="D64" s="54"/>
+      <c r="D64" s="53"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="9"/>
@@ -2782,7 +2822,7 @@
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
-      <c r="D65" s="54"/>
+      <c r="D65" s="53"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="9"/>
@@ -2791,7 +2831,7 @@
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
-      <c r="D66" s="54"/>
+      <c r="D66" s="53"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="9"/>
@@ -2800,7 +2840,7 @@
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
-      <c r="D67" s="54"/>
+      <c r="D67" s="53"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="9"/>
@@ -2809,7 +2849,7 @@
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
-      <c r="D68" s="54"/>
+      <c r="D68" s="53"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="9"/>
@@ -2821,7 +2861,7 @@
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
-      <c r="D69" s="54"/>
+      <c r="D69" s="53"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="9"/>
@@ -2833,7 +2873,7 @@
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
-      <c r="D70" s="54"/>
+      <c r="D70" s="53"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="5"/>
@@ -2843,7 +2883,7 @@
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-      <c r="D71" s="54"/>
+      <c r="D71" s="53"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="5"/>
@@ -2853,7 +2893,7 @@
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
-      <c r="D72" s="54"/>
+      <c r="D72" s="53"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="9"/>
@@ -2862,7 +2902,7 @@
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="54"/>
+      <c r="D73" s="53"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="9"/>
@@ -2871,7 +2911,7 @@
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="54"/>
+      <c r="D74" s="53"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="9"/>
@@ -2880,7 +2920,7 @@
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="54"/>
+      <c r="D75" s="53"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="9"/>
@@ -2889,7 +2929,7 @@
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="54"/>
+      <c r="D76" s="53"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="9"/>
@@ -2898,7 +2938,7 @@
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="54"/>
+      <c r="D77" s="53"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="9"/>
@@ -2907,7 +2947,7 @@
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="54"/>
+      <c r="D78" s="53"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
@@ -2915,7 +2955,7 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
-      <c r="D79" s="55"/>
+      <c r="D79" s="54"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
     </row>
@@ -2923,7 +2963,7 @@
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
-      <c r="D80" s="55"/>
+      <c r="D80" s="54"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
     </row>
@@ -2931,7 +2971,7 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="55"/>
+      <c r="D81" s="54"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
     </row>
@@ -2939,7 +2979,7 @@
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
-      <c r="D82" s="55"/>
+      <c r="D82" s="54"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
     </row>
@@ -2947,7 +2987,7 @@
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
-      <c r="D83" s="55"/>
+      <c r="D83" s="54"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
     </row>
@@ -2955,7 +2995,7 @@
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
-      <c r="D84" s="55"/>
+      <c r="D84" s="54"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="7"/>
@@ -2964,7 +3004,7 @@
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
-      <c r="D85" s="55"/>
+      <c r="D85" s="54"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="7"/>
@@ -2975,7 +3015,7 @@
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
-      <c r="D86" s="55"/>
+      <c r="D86" s="54"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="7"/>
@@ -2984,7 +3024,7 @@
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="55"/>
+      <c r="D87" s="54"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="I87"/>
@@ -2994,7 +3034,7 @@
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
-      <c r="D88" s="55"/>
+      <c r="D88" s="54"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="I88"/>
@@ -3004,7 +3044,7 @@
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
-      <c r="D89" s="55"/>
+      <c r="D89" s="54"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
       <c r="I89"/>
@@ -3014,7 +3054,7 @@
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
-      <c r="D90" s="55"/>
+      <c r="D90" s="54"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="I90"/>
@@ -3024,7 +3064,7 @@
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
-      <c r="D91" s="55"/>
+      <c r="D91" s="54"/>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="I91"/>
@@ -3034,7 +3074,7 @@
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
-      <c r="D92" s="55"/>
+      <c r="D92" s="54"/>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="I92"/>
@@ -3044,7 +3084,7 @@
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
-      <c r="D93" s="55"/>
+      <c r="D93" s="54"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="I93"/>
@@ -3054,7 +3094,7 @@
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
-      <c r="D94" s="55"/>
+      <c r="D94" s="54"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="I94"/>
@@ -3064,7 +3104,7 @@
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
-      <c r="D95" s="55"/>
+      <c r="D95" s="54"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
     </row>
@@ -3072,7 +3112,7 @@
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
-      <c r="D96" s="55"/>
+      <c r="D96" s="54"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
     </row>
@@ -3080,7 +3120,7 @@
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
-      <c r="D97" s="55"/>
+      <c r="D97" s="54"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
     </row>
@@ -3088,7 +3128,7 @@
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
-      <c r="D98" s="55"/>
+      <c r="D98" s="54"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4"/>
     </row>
@@ -3096,7 +3136,7 @@
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
-      <c r="D99" s="55"/>
+      <c r="D99" s="54"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4"/>
     </row>
@@ -3104,10 +3144,13 @@
       <c r="A100" s="10"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
-      <c r="D100" s="56"/>
+      <c r="D100" s="55"/>
       <c r="F100" s="10"/>
     </row>
   </sheetData>
+  <sortState ref="A2:F100">
+    <sortCondition ref="A2:A100"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3184,33 +3227,33 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>6200</v>
       </c>
       <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
         <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
       </c>
       <c r="G5">
         <v>3950</v>
@@ -3218,13 +3261,13 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>7150</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6">
         <v>5250</v>
@@ -3232,7 +3275,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7">
         <v>3600</v>
@@ -3240,7 +3283,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8">
         <v>6250</v>
@@ -3248,10 +3291,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
       </c>
       <c r="G10">
         <v>4500</v>
@@ -3259,7 +3302,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11">
         <v>4600</v>
@@ -3267,7 +3310,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12">
         <v>3600</v>
@@ -3275,7 +3318,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13">
         <v>4450</v>
@@ -3283,7 +3326,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14">
         <v>3550</v>
@@ -3291,7 +3334,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15">
         <v>4000</v>

</xml_diff>

<commit_message>
swap hw2 and 3
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="147">
   <si>
     <t>Finals Week</t>
   </si>
@@ -219,10 +219,6 @@
 Create univariate visualizations of data</t>
   </si>
   <si>
-    <t>Data Import
-Univariate Data Visualizations</t>
-  </si>
-  <si>
     <t>* Workflow - Keeping your raw data untouched
 * Using GUI methods to extract code. 
 * Import your raw analysis data set your SPC, keep only variables of interest from your codebook, save an analysis data file to disk
@@ -242,10 +238,6 @@
 * Import your created data set into your software program of choice (SPC) using point and click methods. </t>
   </si>
   <si>
-    <t>[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 1.1, 1.3
-[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)</t>
-  </si>
-  <si>
     <t>Create and interpret appropriate visualizations to examine associations between two variables</t>
   </si>
   <si>
@@ -254,13 +246,6 @@
 </t>
   </si>
   <si>
-    <t>Create a `MATH615`  folder in an easy to find place on your computer. Create the following sub-folders 1) `data`, 2) `code`, 3) `results`
-Download the data set that you are going to be analyzing and save it into your `MATH615\data` folder. 
-Start a code file (`dm.Rmd` or `dm.sps`) and import your chosen analysis data set. Save this code file to your `MATH615\code` folder. 
-Skim AS Notes Chapter 1 notes before Tuesday
-Read PMA6 DRAFT Ch 4.1, 4.2, 4.5 before Thursday</t>
-  </si>
-  <si>
     <t xml:space="preserve">[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)  </t>
   </si>
   <si>
@@ -288,31 +273,16 @@
     <t>Poster prep III</t>
   </si>
   <si>
-    <t>PR Regression</t>
-  </si>
-  <si>
-    <t>PR Moderation</t>
-  </si>
-  <si>
     <t>PR Poster prep II</t>
   </si>
   <si>
     <t>Poster prep II</t>
   </si>
   <si>
-    <t>PR Bivariate Inference</t>
-  </si>
-  <si>
-    <t>PR Bivariate Graphing</t>
-  </si>
-  <si>
     <t>PR Poster prep I</t>
   </si>
   <si>
     <t>Poster prep I</t>
-  </si>
-  <si>
-    <t>PR Univ Graphics</t>
   </si>
   <si>
     <t>PR Final Poster</t>
@@ -343,12 +313,6 @@
 AS Notebook [Ch 6]() 
 [Regression Assignment Examples](hw/Regression_Assignment_Examples.html)
 </t>
-  </si>
-  <si>
-    <t>Decide on a data set to analyze and install your software program of choice (Due Thu 8/30 )
-Take [this survey](https://goo.gl/forms/qLBv2jMF6fBv3BTR2) to help me set my OH (Due Thu 8/30 )
-Join our [Slack team](http://math615.slack.com) and post an `#introduction` (See instructions in channel) (Due Mon 9/3 )
-Data entry assignment [[HTML]](hw/01_data_entry.html)[[PDF]](hw/01_data_entry.pdf) (Due Mon 9/3 )</t>
   </si>
   <si>
     <t>Final Posters as printed  (Due Mon 12/10 )
@@ -494,21 +458,11 @@
 * Analysis code files should be separate. Read in the analysis data set - not the raw data. </t>
   </si>
   <si>
-    <t>Univariate graphing assignment [[HTML]](hw/02_univariate_graphing_assignment.html)[[PDF]](hw/02_univariate_graphing_assignment.pdf) (Due Mon 9/10 )
-Peer Revew of Univariate Graphs (Due Wed 9/12 )
-Research Question and Codebook Assignment [[HTML]](hw/03_research_codebook.html)[[PDF]](hw/03_research_codebook.pdf)  (Due Wed 9/12 )</t>
-  </si>
-  <si>
     <t>In use, % based</t>
   </si>
   <si>
     <t>Bivariate graphing assignment [[HTML]](hw/05_bivariate_graphing_assignment.html)[[PDF]](hw/05_bivariate_graphing_assignment.pdf) (Due Mon 9/24 )
 Peer Review (Due Wed 9/26 )</t>
-  </si>
-  <si>
-    <t>Data management code file [[HTML]](hw/04_data_management.html)[[PDF]](hw/04_data_management.pdf) (Due Mon 9/17 ) 
-Poster Prep: Stage I (Due Wed 9/19 ) [Drop a note in BBL when done] 
-Peer Review: Stage I (Due Fri 9/21 )</t>
   </si>
   <si>
     <t xml:space="preserve">* Work on your `dm` (data management) code file during class. You will turn a copy of this in. Your results must be able to be replicated on my computer. 
@@ -558,12 +512,6 @@
     <t>01 Data Entry</t>
   </si>
   <si>
-    <t>02 Univariate Graphics</t>
-  </si>
-  <si>
-    <t>03 RQ and codebook</t>
-  </si>
-  <si>
     <t>04 Data Management</t>
   </si>
   <si>
@@ -583,6 +531,52 @@
   </si>
   <si>
     <t>10 Regression</t>
+  </si>
+  <si>
+    <t>Create a `MATH615`  folder in an easy to find place on your computer. Create the following sub-folders 1) `data`, 2) `code`, 3) `results`
+Download the data set that you are going to be analyzing and save it into your `MATH615\data` folder. 
+Start a code file (`dm_dataset.Rmd` or `dm_data.sps`) and import your chosen analysis data set (replace the word `dataset` with the name (one word) of your research data set. Save this code file to your `MATH615\code` folder. 
+Skim AS Notes Chapter 1 notes before Tuesday
+Read PMA6 DRAFT Ch 4.1, 4.2, 4.5 before Thursday</t>
+  </si>
+  <si>
+    <t>[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 1.1, 1.3
+[PMA6 DRAFT](reading/PMA6 DRAFT.pdf)
+Math 130 week 4 on [data visualization](https://norcalbiostat.github.io/MATH130/)</t>
+  </si>
+  <si>
+    <t>Reproducible Research
+Univariate Data Visualizations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univariate graphing assignment [[HTML]](hw/02_univariate_graphing_assignment.html)[[PDF]](hw/02_univariate_graphing_assignment.pdf) (Due Mon 9/10 )
+</t>
+  </si>
+  <si>
+    <t>Decide on a data set to analyze and install your software program of choice (Due Thu 8/30 )
+Take [this survey](https://goo.gl/forms/qLBv2jMF6fBv3BTR2) to help me set my OH (Due Thu 8/30 )
+Join our [Slack team](http://math615.slack.com) and post an `#introduction` (See instructions in channel) (Due Mon 9/3 )
+Data entry assignment [[HTML]](hw/01_data_entry.html)[[PDF]](hw/01_data_entry.pdf) (Due Mon 9/3 )
+Research Question and Codebook Assignment [[HTML]](hw/02_research_codebook.html)[[PDF]](hw/02_research_codebook.pdf)  (Due Wed 9/5 )
+Peer review of Research Question (Due Fri 9/7 )</t>
+  </si>
+  <si>
+    <t>02 RQ and codebook</t>
+  </si>
+  <si>
+    <t>03 Univariate Graphics</t>
+  </si>
+  <si>
+    <t>PR Research Question</t>
+  </si>
+  <si>
+    <t>PR Data Management</t>
+  </si>
+  <si>
+    <t>Data management [[HTML]](hw/04_data_management.html)[[PDF]](hw/04_data_management.pdf) (Due Mon 9/17 ) 
+Peer Review Data management (Due Wed 9/19 )
+Poster Prep: Stage I (Due Wed 9/19 ) 
+Peer Review: Stage I (Due Fri 9/21 )</t>
   </si>
 </sst>
 </file>
@@ -913,7 +907,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -963,143 +957,146 @@
     <xf numFmtId="14" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="90" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="91" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="92">
@@ -1587,8 +1584,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+    <row r="2" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
       <c r="B2" s="13">
@@ -1600,50 +1597,50 @@
       <c r="D2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>111</v>
+      <c r="E2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>60</v>
+      <c r="H2" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
         <v>2</v>
       </c>
       <c r="B3" s="13">
         <f t="shared" ref="B3:B18" si="0">B2+7</f>
         <v>41885</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>57</v>
+      <c r="C3" s="63" t="s">
+        <v>139</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>126</v>
+      <c r="E3" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -1654,26 +1651,26 @@
         <f t="shared" si="0"/>
         <v>41892</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>118</v>
+      <c r="C4" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>109</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1684,26 +1681,26 @@
         <f>B4+7</f>
         <v>41899</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>112</v>
+      <c r="C5" s="23" t="s">
+        <v>103</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>65</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="270" x14ac:dyDescent="0.25">
@@ -1714,26 +1711,26 @@
         <f t="shared" si="0"/>
         <v>41906</v>
       </c>
-      <c r="C6" s="59" t="s">
-        <v>132</v>
+      <c r="C6" s="58" t="s">
+        <v>121</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F6" s="61" t="s">
-        <v>139</v>
+        <v>122</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>128</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1744,22 +1741,22 @@
         <f t="shared" si="0"/>
         <v>41913</v>
       </c>
-      <c r="C7" s="24" t="s">
-        <v>113</v>
+      <c r="C7" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="22"/>
+        <v>126</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1771,16 +1768,16 @@
         <v>41920</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23" t="s">
+      <c r="F8" s="21"/>
+      <c r="G8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>102</v>
+      <c r="H8" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="I8" s="5"/>
     </row>
@@ -1793,7 +1790,7 @@
         <v>41927</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1801,7 +1798,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1812,18 +1809,18 @@
         <f t="shared" si="0"/>
         <v>41934</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>115</v>
+      <c r="C10" s="23" t="s">
+        <v>106</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="21" t="s">
         <v>50</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1845,7 +1842,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -1857,19 +1854,19 @@
         <v>41948</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>89</v>
+      <c r="E12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1881,14 +1878,14 @@
         <v>41955</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>87</v>
+      <c r="E13" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1923,17 +1920,17 @@
       <c r="E15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="22" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1945,7 +1942,7 @@
         <v>41976</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
@@ -1954,8 +1951,8 @@
       <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="22" t="s">
-        <v>96</v>
+      <c r="I16" s="21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1974,8 +1971,8 @@
       <c r="F17" s="4"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="22" t="s">
-        <v>91</v>
+      <c r="I17" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2002,1196 +1999,1151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="32"/>
-    <col min="2" max="2" width="29.375" style="32" customWidth="1"/>
-    <col min="3" max="3" width="30.125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="32" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="32"/>
-    <col min="7" max="7" width="5.125" style="29" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="29" customWidth="1"/>
-    <col min="9" max="9" width="10" style="31" customWidth="1"/>
-    <col min="10" max="10" width="8.875" style="31"/>
-    <col min="11" max="11" width="4.625" style="31" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="29"/>
+    <col min="1" max="1" width="8.875" style="31"/>
+    <col min="2" max="2" width="29.375" style="31" customWidth="1"/>
+    <col min="3" max="3" width="30.125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="31" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="31"/>
+    <col min="7" max="7" width="5.125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="28" customWidth="1"/>
+    <col min="9" max="9" width="10" style="30" customWidth="1"/>
+    <col min="10" max="10" width="8.875" style="30"/>
+    <col min="11" max="11" width="4.625" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="32">
+        <v>41884</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="33">
+        <v>5</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="35">
+        <f>SUMIF($E$2:$E$86,H2,$F$2:$F$86)</f>
+        <v>35</v>
+      </c>
+      <c r="J2" s="36">
+        <f>I2/$I$6</f>
+        <v>0.109375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>1.2</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="32">
+        <v>41884</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="38">
+        <v>5</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="33">
+        <f>SUMIF($E$2:$E$86,H3,$F$2:$F$86)</f>
+        <v>45</v>
+      </c>
+      <c r="J3" s="40">
+        <f>I3/$I$6</f>
+        <v>0.140625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>1.3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="32">
+        <v>41886</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="45">
+        <v>10</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="42">
+        <f>SUMIF($E$2:$E$86,H4,$F$2:$F$86)</f>
+        <v>100</v>
+      </c>
+      <c r="J4" s="43">
+        <f>I4/$I$6</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
+        <v>1.4</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="32">
+        <v>41888</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="33">
+        <v>5</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="45">
+        <f>SUMIF($E$2:$E$86,H5,$F$2:$F$86)</f>
+        <v>140</v>
+      </c>
+      <c r="J5" s="46">
+        <f>I5/$I$6</f>
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30">
+        <v>2.1</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="32">
+        <v>41891</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="38">
+        <v>5</v>
+      </c>
+      <c r="I6" s="47">
+        <f>SUM(I2:I5)</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>3.1</v>
+      </c>
+      <c r="B7" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="32">
+        <v>41898</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>3.2</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>3.3</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="32">
+        <v>41900</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
+        <v>3.4</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="32">
+        <v>41902</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="32">
+        <v>41905</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="27" t="s">
+      <c r="D12" s="49">
+        <v>41919</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="45">
         <v>20</v>
       </c>
-      <c r="H1" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="30" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
+        <v>5.2</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="32">
+        <v>41923</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="33">
+        <v>5</v>
+      </c>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
+        <v>6</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="32">
+        <v>41916</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="38">
+        <v>5</v>
+      </c>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <v>7.1</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="32">
+        <v>41920</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="42">
+        <v>50</v>
+      </c>
+      <c r="I15" s="28"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="30">
+        <v>8.1</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="38">
+        <v>5</v>
+      </c>
+      <c r="I16" s="28"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="30">
+        <v>9.1</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="45">
         <v>20</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="I17" s="28"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="30">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="33">
+        <v>5</v>
+      </c>
+      <c r="I18" s="28"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="30">
+        <v>10.1</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="38">
+        <v>5</v>
+      </c>
+      <c r="I19" s="28"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="30">
+        <v>12.1</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="38">
+        <v>5</v>
+      </c>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="30">
+        <v>13.1</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="45">
+        <v>20</v>
+      </c>
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="30">
+        <v>13.2</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="33">
+        <v>5</v>
+      </c>
+      <c r="I22" s="28"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="30">
+        <v>14.1</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="45">
+        <v>10</v>
+      </c>
+      <c r="I23" s="28"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="30">
+        <v>14.2</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="33">
+        <v>5</v>
+      </c>
+      <c r="I24" s="28"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="30">
+        <v>15.1</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="45">
+        <v>30</v>
+      </c>
+      <c r="I25" s="28"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="30">
+        <v>15.2</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="30">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="33">
-        <v>41884</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="34">
-        <v>5</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="36">
-        <f>SUMIF($E$2:$E$89,H2,$F$2:$F$89)</f>
-        <v>35</v>
-      </c>
-      <c r="J2" s="37">
-        <f>I2/$I$6</f>
-        <v>0.1044776119402985</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
-        <v>1.2</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="33">
-        <v>41884</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="39">
-        <v>5</v>
-      </c>
-      <c r="H3" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="I3" s="34">
-        <f>SUMIF($E$2:$E$89,H3,$F$2:$F$89)</f>
-        <v>60</v>
-      </c>
-      <c r="J3" s="41">
-        <f>I3/$I$6</f>
-        <v>0.17910447761194029</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
-        <v>2.1</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="33">
-        <v>41891</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="39">
-        <v>5</v>
-      </c>
-      <c r="H4" s="42" t="s">
+      <c r="B27" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="43">
-        <f>SUMIF($E$2:$E$89,H4,$F$2:$F$89)</f>
-        <v>100</v>
-      </c>
-      <c r="J4" s="44">
-        <f>I4/$I$6</f>
-        <v>0.29850746268656714</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="33">
-        <v>41893</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F5" s="34">
-        <v>5</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="46">
-        <f>SUMIF($E$2:$E$89,H5,$F$2:$F$89)</f>
-        <v>140</v>
-      </c>
-      <c r="J5" s="47">
-        <f>I5/$I$6</f>
-        <v>0.41791044776119401</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="33">
-        <v>41893</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="46">
+      <c r="F27" s="42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="30">
+        <v>16</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="33">
         <v>10</v>
       </c>
-      <c r="I6" s="48">
-        <f>SUM(I2:I5)</f>
-        <v>335</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>3.1</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="33">
-        <v>41898</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="46">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
-        <v>3.2</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="33">
-        <v>41900</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="46">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>3.3</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="33">
-        <v>41902</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="33">
-        <v>41905</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
-        <v>4.2</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="33">
-        <v>41907</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="50">
-        <v>41919</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="46">
-        <v>20</v>
-      </c>
-      <c r="I12" s="29"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
-        <v>5.2</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="33">
-        <v>41923</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="34">
-        <v>5</v>
-      </c>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="31">
-        <v>6</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="33">
-        <v>41916</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="39">
-        <v>5</v>
-      </c>
-      <c r="I14" s="29"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="31">
-        <v>7.1</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="33">
-        <v>41920</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="43">
-        <v>50</v>
-      </c>
-      <c r="I15" s="29"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="31">
-        <v>8.1</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="39">
-        <v>5</v>
-      </c>
-      <c r="I16" s="29"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="31">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F17" s="34">
-        <v>5</v>
-      </c>
-      <c r="I17" s="29"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="31">
-        <v>9.1</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="46">
-        <v>20</v>
-      </c>
-      <c r="I18" s="29"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="31">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" s="34">
-        <v>5</v>
-      </c>
-      <c r="I19" s="29"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="31">
-        <v>10.1</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="39">
-        <v>5</v>
-      </c>
-      <c r="I20" s="29"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="31">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="34">
-        <v>5</v>
-      </c>
-      <c r="I21" s="29"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="31">
-        <v>12.1</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="39">
-        <v>5</v>
-      </c>
-      <c r="I22" s="29"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="31">
-        <v>12.2</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" s="34">
-        <v>5</v>
-      </c>
-      <c r="I23" s="29"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="31">
-        <v>13.1</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="E24" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="46">
-        <v>20</v>
-      </c>
-      <c r="I24" s="29"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="31">
-        <v>13.2</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="31">
-        <v>14.1</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="46">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="31">
-        <v>14.2</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="31">
-        <v>15.1</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="46">
-        <v>30</v>
-      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="31">
-        <v>15.2</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F29" s="34">
-        <v>5</v>
-      </c>
+      <c r="A29" s="30"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="31">
-        <v>16</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="43">
-        <v>50</v>
-      </c>
+      <c r="A30" s="30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="31">
-        <v>16</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="34">
-        <v>10</v>
-      </c>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="51"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="52"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="51"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="51"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="52"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="52"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="52"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="52"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="52"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="52"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="31"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="51"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="52"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="31"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="52"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="31"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="51"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="52"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="51"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="52"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="52"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="31"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="52"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="31"/>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="51"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="52"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="52"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="51"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="52"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="51"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="52"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="51"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="51"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="51"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="51"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="51"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="51"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="51"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="51"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="51"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="51"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="51"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="51"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="51"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="30"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="51"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="30"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="51"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="30"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="31"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="30"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="31"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="52"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="53"/>
+      <c r="K65" s="31"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="31"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="31"/>
-      <c r="D66" s="51"/>
-      <c r="E66" s="31"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="52"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="32"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="53"/>
+      <c r="K66" s="31"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="31"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="51"/>
-      <c r="E67" s="31"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="52"/>
-      <c r="H67" s="53"/>
-      <c r="I67" s="32"/>
-      <c r="J67" s="32"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="30"/>
+      <c r="G67" s="51"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="51"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="54"/>
-      <c r="K68" s="32"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="51"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="51"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="54"/>
-      <c r="K69" s="32"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="51"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="52"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="51"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="51"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="52"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="51"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
-      <c r="B72" s="31"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="52"/>
+      <c r="A72" s="30"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="51"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="52"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="30"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
-      <c r="B74" s="31"/>
-      <c r="C74" s="31"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="52"/>
+      <c r="A74" s="54"/>
+      <c r="B74" s="54"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="54"/>
+      <c r="F74" s="54"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="31"/>
-      <c r="B75" s="31"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="51"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="52"/>
+      <c r="A75" s="54"/>
+      <c r="B75" s="54"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="55"/>
+      <c r="E75" s="54"/>
+      <c r="F75" s="54"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="31"/>
-      <c r="B76" s="31"/>
-      <c r="C76" s="31"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="31"/>
-      <c r="F76" s="31"/>
+      <c r="A76" s="54"/>
+      <c r="B76" s="54"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="55"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="54"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="55"/>
-      <c r="B77" s="55"/>
-      <c r="C77" s="55"/>
-      <c r="D77" s="56"/>
-      <c r="E77" s="55"/>
-      <c r="F77" s="55"/>
+      <c r="A77" s="54"/>
+      <c r="B77" s="54"/>
+      <c r="C77" s="54"/>
+      <c r="D77" s="55"/>
+      <c r="E77" s="54"/>
+      <c r="F77" s="54"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="55"/>
-      <c r="B78" s="55"/>
-      <c r="C78" s="55"/>
-      <c r="D78" s="56"/>
-      <c r="E78" s="55"/>
-      <c r="F78" s="55"/>
+      <c r="A78" s="54"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="54"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="54"/>
+      <c r="F78" s="54"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="55"/>
-      <c r="B79" s="55"/>
-      <c r="C79" s="55"/>
-      <c r="D79" s="56"/>
-      <c r="E79" s="55"/>
-      <c r="F79" s="55"/>
+      <c r="A79" s="54"/>
+      <c r="B79" s="54"/>
+      <c r="C79" s="54"/>
+      <c r="D79" s="55"/>
+      <c r="E79" s="54"/>
+      <c r="F79" s="54"/>
+      <c r="G79" s="52"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="55"/>
-      <c r="B80" s="55"/>
-      <c r="C80" s="55"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="55"/>
-      <c r="F80" s="55"/>
+      <c r="A80" s="54"/>
+      <c r="B80" s="54"/>
+      <c r="C80" s="54"/>
+      <c r="D80" s="55"/>
+      <c r="E80" s="54"/>
+      <c r="F80" s="54"/>
+      <c r="G80" s="52"/>
+      <c r="I80" s="28"/>
+      <c r="J80" s="28"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="55"/>
-      <c r="B81" s="55"/>
-      <c r="C81" s="55"/>
-      <c r="D81" s="56"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55"/>
+      <c r="A81" s="54"/>
+      <c r="B81" s="54"/>
+      <c r="C81" s="54"/>
+      <c r="D81" s="55"/>
+      <c r="E81" s="54"/>
+      <c r="F81" s="54"/>
+      <c r="G81" s="52"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="55"/>
-      <c r="B82" s="55"/>
-      <c r="C82" s="55"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="55"/>
-      <c r="F82" s="55"/>
-      <c r="G82" s="53"/>
+      <c r="A82" s="54"/>
+      <c r="B82" s="54"/>
+      <c r="C82" s="54"/>
+      <c r="D82" s="55"/>
+      <c r="E82" s="54"/>
+      <c r="F82" s="54"/>
+      <c r="I82" s="28"/>
+      <c r="J82" s="28"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="55"/>
-      <c r="B83" s="55"/>
-      <c r="C83" s="55"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="55"/>
-      <c r="F83" s="55"/>
-      <c r="G83" s="53"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="29"/>
+      <c r="A83" s="54"/>
+      <c r="B83" s="54"/>
+      <c r="C83" s="54"/>
+      <c r="D83" s="55"/>
+      <c r="E83" s="54"/>
+      <c r="F83" s="54"/>
+      <c r="I83" s="28"/>
+      <c r="J83" s="28"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="55"/>
-      <c r="B84" s="55"/>
-      <c r="C84" s="55"/>
-      <c r="D84" s="56"/>
-      <c r="E84" s="55"/>
-      <c r="F84" s="55"/>
-      <c r="G84" s="53"/>
+      <c r="A84" s="54"/>
+      <c r="B84" s="54"/>
+      <c r="C84" s="54"/>
+      <c r="D84" s="55"/>
+      <c r="E84" s="54"/>
+      <c r="F84" s="54"/>
+      <c r="I84" s="28"/>
+      <c r="J84" s="28"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="55"/>
-      <c r="B85" s="55"/>
-      <c r="C85" s="55"/>
-      <c r="D85" s="56"/>
-      <c r="E85" s="55"/>
-      <c r="F85" s="55"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29"/>
+      <c r="A85" s="54"/>
+      <c r="B85" s="54"/>
+      <c r="C85" s="54"/>
+      <c r="D85" s="55"/>
+      <c r="E85" s="54"/>
+      <c r="F85" s="54"/>
+      <c r="I85" s="28"/>
+      <c r="J85" s="28"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="55"/>
-      <c r="B86" s="55"/>
-      <c r="C86" s="55"/>
-      <c r="D86" s="56"/>
-      <c r="E86" s="55"/>
-      <c r="F86" s="55"/>
-      <c r="I86" s="29"/>
-      <c r="J86" s="29"/>
+      <c r="A86" s="54"/>
+      <c r="B86" s="54"/>
+      <c r="C86" s="54"/>
+      <c r="D86" s="55"/>
+      <c r="E86" s="54"/>
+      <c r="F86" s="54"/>
+      <c r="I86" s="28"/>
+      <c r="J86" s="28"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="55"/>
-      <c r="B87" s="55"/>
-      <c r="C87" s="55"/>
-      <c r="D87" s="56"/>
-      <c r="E87" s="55"/>
-      <c r="F87" s="55"/>
-      <c r="I87" s="29"/>
-      <c r="J87" s="29"/>
+      <c r="A87" s="54"/>
+      <c r="B87" s="54"/>
+      <c r="C87" s="54"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="54"/>
+      <c r="F87" s="54"/>
+      <c r="I87" s="28"/>
+      <c r="J87" s="28"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="55"/>
-      <c r="B88" s="55"/>
-      <c r="C88" s="55"/>
-      <c r="D88" s="56"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="55"/>
-      <c r="I88" s="29"/>
-      <c r="J88" s="29"/>
+      <c r="A88" s="54"/>
+      <c r="B88" s="54"/>
+      <c r="C88" s="54"/>
+      <c r="D88" s="55"/>
+      <c r="E88" s="54"/>
+      <c r="F88" s="54"/>
+      <c r="I88" s="28"/>
+      <c r="J88" s="28"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="55"/>
-      <c r="B89" s="55"/>
-      <c r="C89" s="55"/>
-      <c r="D89" s="56"/>
-      <c r="E89" s="55"/>
-      <c r="F89" s="55"/>
-      <c r="I89" s="29"/>
-      <c r="J89" s="29"/>
+      <c r="A89" s="54"/>
+      <c r="B89" s="54"/>
+      <c r="C89" s="54"/>
+      <c r="D89" s="55"/>
+      <c r="E89" s="54"/>
+      <c r="F89" s="54"/>
+      <c r="I89" s="28"/>
+      <c r="J89" s="28"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="55"/>
-      <c r="B90" s="55"/>
-      <c r="C90" s="55"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="55"/>
-      <c r="F90" s="55"/>
-      <c r="I90" s="29"/>
-      <c r="J90" s="29"/>
+      <c r="A90" s="54"/>
+      <c r="B90" s="54"/>
+      <c r="C90" s="54"/>
+      <c r="D90" s="55"/>
+      <c r="E90" s="54"/>
+      <c r="F90" s="54"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="55"/>
-      <c r="B91" s="55"/>
-      <c r="C91" s="55"/>
-      <c r="D91" s="56"/>
-      <c r="E91" s="55"/>
-      <c r="F91" s="55"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="29"/>
+      <c r="A91" s="54"/>
+      <c r="B91" s="54"/>
+      <c r="C91" s="54"/>
+      <c r="D91" s="55"/>
+      <c r="E91" s="54"/>
+      <c r="F91" s="54"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="55"/>
-      <c r="B92" s="55"/>
-      <c r="C92" s="55"/>
-      <c r="D92" s="56"/>
-      <c r="E92" s="55"/>
-      <c r="F92" s="55"/>
-      <c r="I92" s="29"/>
-      <c r="J92" s="29"/>
+      <c r="A92" s="54"/>
+      <c r="B92" s="54"/>
+      <c r="C92" s="54"/>
+      <c r="D92" s="55"/>
+      <c r="E92" s="54"/>
+      <c r="F92" s="54"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="55"/>
-      <c r="B93" s="55"/>
-      <c r="C93" s="55"/>
-      <c r="D93" s="56"/>
-      <c r="E93" s="55"/>
-      <c r="F93" s="55"/>
+      <c r="A93" s="54"/>
+      <c r="B93" s="54"/>
+      <c r="C93" s="54"/>
+      <c r="D93" s="55"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="54"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="55"/>
-      <c r="B94" s="55"/>
-      <c r="C94" s="55"/>
-      <c r="D94" s="56"/>
-      <c r="E94" s="55"/>
-      <c r="F94" s="55"/>
+      <c r="A94" s="54"/>
+      <c r="B94" s="54"/>
+      <c r="C94" s="54"/>
+      <c r="D94" s="55"/>
+      <c r="E94" s="54"/>
+      <c r="F94" s="54"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="55"/>
-      <c r="B95" s="55"/>
-      <c r="C95" s="55"/>
-      <c r="D95" s="56"/>
-      <c r="E95" s="55"/>
-      <c r="F95" s="55"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="55"/>
-      <c r="B96" s="55"/>
-      <c r="C96" s="55"/>
-      <c r="D96" s="56"/>
-      <c r="E96" s="55"/>
-      <c r="F96" s="55"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="55"/>
-      <c r="B97" s="55"/>
-      <c r="C97" s="55"/>
-      <c r="D97" s="56"/>
-      <c r="E97" s="55"/>
-      <c r="F97" s="55"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="57"/>
-      <c r="B98" s="57"/>
-      <c r="C98" s="57"/>
-      <c r="D98" s="58"/>
-      <c r="F98" s="57"/>
+      <c r="A95" s="56"/>
+      <c r="B95" s="56"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="57"/>
+      <c r="F95" s="56"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F100">
-    <sortCondition ref="A2:A100"/>
+  <sortState ref="A2:F99">
+    <sortCondition ref="A2:A99"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
build to wk 7
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41111B89-1151-4DA1-A657-2E7D07C82751}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B718774C-FD98-49ED-9F1F-86DD0B2711A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="149">
   <si>
     <t>Finals Week</t>
   </si>
@@ -326,9 +326,6 @@
     <t>* Appropriate methods to visualize combinations of quantitative variables (Q~Q)
 * Creating Multivariate graphics. 
 * Best practices for informative graphics (no chart junk)</t>
-  </si>
-  <si>
-    <t>* Hypothesis Testing &amp; p-values</t>
   </si>
   <si>
     <t xml:space="preserve">* What steps are needed to prepare your data for analysis? 
@@ -583,6 +580,11 @@
   <si>
     <t>Poster Prep: Stage II (Due Wed 10/24 ) (PR Friday 10/26 ) (Final Sunday 10/28 )</t>
   </si>
+  <si>
+    <t>Choosing appropriate analyses
+Typical assumptions
+Hypothesis testing  and p-values</t>
+  </si>
 </sst>
 </file>
 
@@ -591,9 +593,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -827,290 +836,293 @@
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="90" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="91" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1553,7 +1565,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,7 +1628,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>53</v>
@@ -1625,7 +1637,7 @@
         <v>58</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="270" x14ac:dyDescent="0.25">
@@ -1637,25 +1649,25 @@
         <v>41885</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G3" s="62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -1670,22 +1682,22 @@
         <v>84</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1697,13 +1709,13 @@
         <v>41899</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>60</v>
@@ -1715,7 +1727,7 @@
         <v>86</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="270" x14ac:dyDescent="0.25">
@@ -1727,25 +1739,25 @@
         <v>41906</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -1757,23 +1769,23 @@
         <v>41913</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -1785,20 +1797,20 @@
         <v>41920</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="64" t="s">
         <v>144</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>145</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="22" t="s">
-        <v>87</v>
+      <c r="H8" s="65" t="s">
+        <v>148</v>
       </c>
       <c r="I8" s="5"/>
     </row>
@@ -1811,7 +1823,7 @@
         <v>41927</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1819,7 +1831,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -1831,7 +1843,7 @@
         <v>41934</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1841,7 +1853,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1863,7 +1875,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -1875,19 +1887,19 @@
         <v>41948</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="21" t="s">
         <v>77</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1899,7 +1911,7 @@
         <v>41955</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="21" t="s">
@@ -2050,10 +2062,10 @@
         <v>17</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>19</v>
@@ -2082,7 +2094,7 @@
         <v>41884</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="33">
         <v>5</v>
@@ -2104,10 +2116,10 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" s="32">
         <v>41884</v>
@@ -2119,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="33">
         <f>SUMIF($E$2:$E$86,H3,$F$2:$F$86)</f>
@@ -2135,10 +2147,10 @@
         <v>1.3</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="32">
         <v>41886</v>
@@ -2166,13 +2178,13 @@
         <v>1.4</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="32">
         <v>41888</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="33">
         <v>5</v>
@@ -2194,10 +2206,10 @@
         <v>2.1</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="32">
         <v>41891</v>
@@ -2218,7 +2230,7 @@
         <v>3.1</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="32">
         <v>41898</v>
@@ -2235,10 +2247,10 @@
         <v>3.2</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="33">
         <v>5</v>
@@ -2252,7 +2264,7 @@
         <v>70</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="32">
         <v>41900</v>
@@ -2275,7 +2287,7 @@
         <v>41902</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" s="33">
         <v>5</v>
@@ -2286,7 +2298,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="32">
@@ -2304,10 +2316,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="49">
         <v>41919</v>
@@ -2324,13 +2336,13 @@
         <v>5.2</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="32">
         <v>41923</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" s="33">
         <v>5</v>
@@ -2342,7 +2354,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D14" s="32">
         <v>41916</v>
@@ -2378,10 +2390,10 @@
         <v>8.1</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>17</v>
@@ -2399,7 +2411,7 @@
         <v>68</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>18</v>
@@ -2417,7 +2429,7 @@
         <v>67</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" s="33">
         <v>5</v>
@@ -2429,10 +2441,10 @@
         <v>10.1</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>17</v>
@@ -2447,10 +2459,10 @@
         <v>12.1</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>17</v>
@@ -2468,7 +2480,7 @@
         <v>66</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>18</v>
@@ -2486,7 +2498,7 @@
         <v>65</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F22" s="33">
         <v>5</v>
@@ -2516,7 +2528,7 @@
         <v>63</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" s="33">
         <v>5</v>
@@ -2546,7 +2558,7 @@
         <v>71</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F26" s="33">
         <v>5</v>

</xml_diff>

<commit_message>
add wk6 and foundations assignmnet
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH615/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B718774C-FD98-49ED-9F1F-86DD0B2711A1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58307BD9-6484-A44F-B6AC-C0D0EC6E5BD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -18,13 +18,8 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
   <si>
     <t>Finals Week</t>
   </si>
@@ -332,14 +327,6 @@
 * We need to ensure that these steps taken are all recorded in code, such that there are no manual changes conducted. 
 * Often we would like normally distributed data. There are a few ways we can achieve that. We'll cover how to identify non-normally distributed data and what transformations are available. 
 </t>
-  </si>
-  <si>
-    <t>Foundations worksheet</t>
-  </si>
-  <si>
-    <t>* Probability of exploding kittens
-* Sampling Distributions
-* Confidence intervals</t>
   </si>
   <si>
     <t>PR Research Proposal</t>
@@ -584,6 +571,20 @@
     <t>Choosing appropriate analyses
 Typical assumptions
 Hypothesis testing  and p-values</t>
+  </si>
+  <si>
+    <t>[Shiny app for statistics education](http://www2.stat.duke.edu/~mc301/shinyed/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Demonstrate probability using exploding kittens
+* What's considered an "unusual" event?
+* How to use the normal distribution to calculate probabilities
+* Explore the behavior of sample means and proportions calculated on many samples (Sampling Distribution, CLT)
+* How to use Confidence intervals to quantify uncertainty about a mean. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* What are the basic steps of a hypothesis test? 
+* In class Foundations worksheet - the only time you'll do a hypothesis test by hand. </t>
   </si>
 </sst>
 </file>
@@ -928,7 +929,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1123,6 +1124,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1563,26 +1567,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="31.875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="30.125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="32.875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="54.625" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="14.875" style="1"/>
+    <col min="2" max="2" width="10.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="54.6640625" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="14.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>48</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1628,7 +1632,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>53</v>
@@ -1637,10 +1641,10 @@
         <v>58</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1649,28 +1653,28 @@
         <v>41885</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F3" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="G3" s="62" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="208" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1682,25 +1686,25 @@
         <v>84</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>61</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>87</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1709,13 +1713,13 @@
         <v>41899</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>60</v>
@@ -1727,10 +1731,10 @@
         <v>86</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="270" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="288" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1739,28 +1743,28 @@
         <v>41906</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="192" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1769,26 +1773,28 @@
         <v>41913</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="21"/>
+        <v>112</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>147</v>
+      </c>
       <c r="G7" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>88</v>
+        <v>148</v>
+      </c>
+      <c r="H7" s="65" t="s">
+        <v>149</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1797,24 +1803,24 @@
         <v>41920</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="65" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>41927</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1831,10 +1837,10 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>41934</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1853,10 +1859,10 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -1875,10 +1881,10 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -1887,22 +1893,22 @@
         <v>41948</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="21" t="s">
         <v>77</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -1911,7 +1917,7 @@
         <v>41955</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="21" t="s">
@@ -1924,7 +1930,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="15"/>
       <c r="B14" s="16">
         <f t="shared" si="0"/>
@@ -1938,7 +1944,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
         <v>13</v>
       </c>
@@ -1966,7 +1972,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
         <v>14</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>15</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>0</v>
       </c>
@@ -2038,23 +2044,23 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="31"/>
-    <col min="2" max="2" width="29.375" style="31" customWidth="1"/>
-    <col min="3" max="3" width="30.125" style="31" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="31" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="31"/>
-    <col min="7" max="7" width="5.125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="31"/>
+    <col min="2" max="2" width="29.33203125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="31"/>
+    <col min="7" max="7" width="5.1640625" style="28" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="28" customWidth="1"/>
     <col min="9" max="9" width="10" style="30" customWidth="1"/>
-    <col min="10" max="10" width="8.875" style="30"/>
-    <col min="11" max="11" width="4.625" style="30" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="28"/>
+    <col min="10" max="10" width="8.83203125" style="30"/>
+    <col min="11" max="11" width="4.6640625" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>41</v>
       </c>
@@ -2062,10 +2068,10 @@
         <v>17</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>19</v>
@@ -2083,7 +2089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30">
         <v>1.1000000000000001</v>
       </c>
@@ -2094,7 +2100,7 @@
         <v>41884</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" s="33">
         <v>5</v>
@@ -2111,15 +2117,15 @@
         <v>0.109375</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>1.2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="32">
         <v>41884</v>
@@ -2131,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I3" s="33">
         <f>SUMIF($E$2:$E$86,H3,$F$2:$F$86)</f>
@@ -2142,15 +2148,15 @@
         <v>0.140625</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>1.3</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" s="32">
         <v>41886</v>
@@ -2173,18 +2179,18 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>1.4</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D5" s="32">
         <v>41888</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F5" s="33">
         <v>5</v>
@@ -2201,15 +2207,15 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>2.1</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="32">
         <v>41891</v>
@@ -2225,12 +2231,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
         <v>3.1</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D7" s="32">
         <v>41898</v>
@@ -2242,21 +2248,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="30">
         <v>3.2</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F8" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="30">
         <v>3.3</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>70</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D9" s="32">
         <v>41900</v>
@@ -2276,7 +2282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="30">
         <v>3.4</v>
       </c>
@@ -2287,18 +2293,18 @@
         <v>41902</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
         <v>4.0999999999999996</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="32">
@@ -2311,15 +2317,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
         <v>5.0999999999999996</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D12" s="49">
         <v>41919</v>
@@ -2331,30 +2337,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
         <v>5.2</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D13" s="32">
         <v>41923</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F13" s="33">
         <v>5</v>
       </c>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
         <v>6</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D14" s="32">
         <v>41916</v>
@@ -2367,7 +2373,7 @@
       </c>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="30">
         <v>7.1</v>
       </c>
@@ -2385,15 +2391,15 @@
       </c>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="30">
         <v>8.1</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>17</v>
@@ -2403,7 +2409,7 @@
       </c>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="30">
         <v>9.1</v>
       </c>
@@ -2411,7 +2417,7 @@
         <v>68</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>18</v>
@@ -2421,7 +2427,7 @@
       </c>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="30">
         <v>9.1999999999999993</v>
       </c>
@@ -2429,22 +2435,22 @@
         <v>67</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F18" s="33">
         <v>5</v>
       </c>
       <c r="I18" s="28"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
         <v>10.1</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>17</v>
@@ -2454,15 +2460,15 @@
       </c>
       <c r="I19" s="28"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
         <v>12.1</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>17</v>
@@ -2472,7 +2478,7 @@
       </c>
       <c r="I20" s="28"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="30">
         <v>13.1</v>
       </c>
@@ -2480,7 +2486,7 @@
         <v>66</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>18</v>
@@ -2490,7 +2496,7 @@
       </c>
       <c r="I21" s="28"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
         <v>13.2</v>
       </c>
@@ -2498,14 +2504,14 @@
         <v>65</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F22" s="33">
         <v>5</v>
       </c>
       <c r="I22" s="28"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
         <v>14.1</v>
       </c>
@@ -2520,7 +2526,7 @@
       </c>
       <c r="I23" s="28"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
         <v>14.2</v>
       </c>
@@ -2528,14 +2534,14 @@
         <v>63</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F24" s="33">
         <v>5</v>
       </c>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
         <v>15.1</v>
       </c>
@@ -2550,7 +2556,7 @@
       </c>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
         <v>15.2</v>
       </c>
@@ -2558,13 +2564,13 @@
         <v>71</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F26" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
         <v>16</v>
       </c>
@@ -2578,7 +2584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
         <v>16</v>
       </c>
@@ -2592,13 +2598,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="30"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="30"/>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
@@ -2606,7 +2612,7 @@
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="30"/>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
@@ -2614,7 +2620,7 @@
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -2622,7 +2628,7 @@
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
@@ -2630,7 +2636,7 @@
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -2638,7 +2644,7 @@
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="30"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
@@ -2646,7 +2652,7 @@
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="30"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -2654,7 +2660,7 @@
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -2662,7 +2668,7 @@
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -2671,7 +2677,7 @@
       <c r="F39" s="30"/>
       <c r="G39" s="51"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -2679,7 +2685,7 @@
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -2687,7 +2693,7 @@
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -2695,7 +2701,7 @@
       <c r="E42" s="30"/>
       <c r="F42" s="30"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
@@ -2703,7 +2709,7 @@
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
@@ -2711,7 +2717,7 @@
       <c r="E44" s="30"/>
       <c r="F44" s="30"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
@@ -2719,7 +2725,7 @@
       <c r="E45" s="30"/>
       <c r="F45" s="30"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="30"/>
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
@@ -2728,7 +2734,7 @@
       <c r="F46" s="30"/>
       <c r="G46" s="51"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -2737,7 +2743,7 @@
       <c r="F47" s="30"/>
       <c r="G47" s="51"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
@@ -2746,7 +2752,7 @@
       <c r="F48" s="30"/>
       <c r="G48" s="51"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
@@ -2755,7 +2761,7 @@
       <c r="F49" s="30"/>
       <c r="G49" s="51"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
@@ -2764,7 +2770,7 @@
       <c r="F50" s="30"/>
       <c r="G50" s="51"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="30"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
@@ -2773,7 +2779,7 @@
       <c r="F51" s="30"/>
       <c r="G51" s="51"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
@@ -2782,7 +2788,7 @@
       <c r="F52" s="30"/>
       <c r="G52" s="51"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="30"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -2791,7 +2797,7 @@
       <c r="F53" s="30"/>
       <c r="G53" s="51"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
@@ -2800,7 +2806,7 @@
       <c r="F54" s="30"/>
       <c r="G54" s="51"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="30"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
@@ -2809,7 +2815,7 @@
       <c r="F55" s="30"/>
       <c r="G55" s="51"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
@@ -2818,7 +2824,7 @@
       <c r="F56" s="30"/>
       <c r="G56" s="51"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="30"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
@@ -2827,7 +2833,7 @@
       <c r="F57" s="30"/>
       <c r="G57" s="51"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="30"/>
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
@@ -2836,7 +2842,7 @@
       <c r="F58" s="30"/>
       <c r="G58" s="51"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
@@ -2845,7 +2851,7 @@
       <c r="F59" s="30"/>
       <c r="G59" s="51"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
       <c r="B60" s="30"/>
       <c r="C60" s="30"/>
@@ -2854,7 +2860,7 @@
       <c r="F60" s="30"/>
       <c r="G60" s="51"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
@@ -2863,7 +2869,7 @@
       <c r="F61" s="30"/>
       <c r="G61" s="51"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
@@ -2872,7 +2878,7 @@
       <c r="F62" s="30"/>
       <c r="G62" s="51"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="30"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
@@ -2884,7 +2890,7 @@
       <c r="I63" s="31"/>
       <c r="J63" s="31"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="30"/>
       <c r="B64" s="30"/>
       <c r="C64" s="30"/>
@@ -2896,7 +2902,7 @@
       <c r="I64" s="31"/>
       <c r="J64" s="31"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
@@ -2906,7 +2912,7 @@
       <c r="G65" s="53"/>
       <c r="K65" s="31"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="30"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
@@ -2916,7 +2922,7 @@
       <c r="G66" s="53"/>
       <c r="K66" s="31"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
@@ -2925,7 +2931,7 @@
       <c r="F67" s="30"/>
       <c r="G67" s="51"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="30"/>
       <c r="B68" s="30"/>
       <c r="C68" s="30"/>
@@ -2934,7 +2940,7 @@
       <c r="F68" s="30"/>
       <c r="G68" s="51"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="30"/>
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
@@ -2943,7 +2949,7 @@
       <c r="F69" s="30"/>
       <c r="G69" s="51"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="30"/>
       <c r="B70" s="30"/>
       <c r="C70" s="30"/>
@@ -2952,7 +2958,7 @@
       <c r="F70" s="30"/>
       <c r="G70" s="51"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="30"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30"/>
@@ -2961,7 +2967,7 @@
       <c r="F71" s="30"/>
       <c r="G71" s="51"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="30"/>
       <c r="B72" s="30"/>
       <c r="C72" s="30"/>
@@ -2970,7 +2976,7 @@
       <c r="F72" s="30"/>
       <c r="G72" s="51"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="30"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
@@ -2978,7 +2984,7 @@
       <c r="E73" s="30"/>
       <c r="F73" s="30"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="54"/>
       <c r="B74" s="54"/>
       <c r="C74" s="54"/>
@@ -2986,7 +2992,7 @@
       <c r="E74" s="54"/>
       <c r="F74" s="54"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="54"/>
       <c r="B75" s="54"/>
       <c r="C75" s="54"/>
@@ -2994,7 +3000,7 @@
       <c r="E75" s="54"/>
       <c r="F75" s="54"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="54"/>
       <c r="B76" s="54"/>
       <c r="C76" s="54"/>
@@ -3002,7 +3008,7 @@
       <c r="E76" s="54"/>
       <c r="F76" s="54"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="54"/>
       <c r="B77" s="54"/>
       <c r="C77" s="54"/>
@@ -3010,7 +3016,7 @@
       <c r="E77" s="54"/>
       <c r="F77" s="54"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="54"/>
       <c r="B78" s="54"/>
       <c r="C78" s="54"/>
@@ -3018,7 +3024,7 @@
       <c r="E78" s="54"/>
       <c r="F78" s="54"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="54"/>
       <c r="B79" s="54"/>
       <c r="C79" s="54"/>
@@ -3027,7 +3033,7 @@
       <c r="F79" s="54"/>
       <c r="G79" s="52"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="54"/>
       <c r="B80" s="54"/>
       <c r="C80" s="54"/>
@@ -3038,7 +3044,7 @@
       <c r="I80" s="28"/>
       <c r="J80" s="28"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="54"/>
       <c r="B81" s="54"/>
       <c r="C81" s="54"/>
@@ -3047,7 +3053,7 @@
       <c r="F81" s="54"/>
       <c r="G81" s="52"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="54"/>
       <c r="B82" s="54"/>
       <c r="C82" s="54"/>
@@ -3057,7 +3063,7 @@
       <c r="I82" s="28"/>
       <c r="J82" s="28"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="54"/>
       <c r="B83" s="54"/>
       <c r="C83" s="54"/>
@@ -3067,7 +3073,7 @@
       <c r="I83" s="28"/>
       <c r="J83" s="28"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="54"/>
       <c r="B84" s="54"/>
       <c r="C84" s="54"/>
@@ -3077,7 +3083,7 @@
       <c r="I84" s="28"/>
       <c r="J84" s="28"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="54"/>
       <c r="B85" s="54"/>
       <c r="C85" s="54"/>
@@ -3087,7 +3093,7 @@
       <c r="I85" s="28"/>
       <c r="J85" s="28"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="54"/>
       <c r="B86" s="54"/>
       <c r="C86" s="54"/>
@@ -3097,7 +3103,7 @@
       <c r="I86" s="28"/>
       <c r="J86" s="28"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="54"/>
       <c r="B87" s="54"/>
       <c r="C87" s="54"/>
@@ -3107,7 +3113,7 @@
       <c r="I87" s="28"/>
       <c r="J87" s="28"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="54"/>
       <c r="B88" s="54"/>
       <c r="C88" s="54"/>
@@ -3117,7 +3123,7 @@
       <c r="I88" s="28"/>
       <c r="J88" s="28"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="54"/>
       <c r="B89" s="54"/>
       <c r="C89" s="54"/>
@@ -3127,7 +3133,7 @@
       <c r="I89" s="28"/>
       <c r="J89" s="28"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="54"/>
       <c r="B90" s="54"/>
       <c r="C90" s="54"/>
@@ -3135,7 +3141,7 @@
       <c r="E90" s="54"/>
       <c r="F90" s="54"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="54"/>
       <c r="B91" s="54"/>
       <c r="C91" s="54"/>
@@ -3143,7 +3149,7 @@
       <c r="E91" s="54"/>
       <c r="F91" s="54"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="54"/>
       <c r="B92" s="54"/>
       <c r="C92" s="54"/>
@@ -3151,7 +3157,7 @@
       <c r="E92" s="54"/>
       <c r="F92" s="54"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="54"/>
       <c r="B93" s="54"/>
       <c r="C93" s="54"/>
@@ -3159,7 +3165,7 @@
       <c r="E93" s="54"/>
       <c r="F93" s="54"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="54"/>
       <c r="B94" s="54"/>
       <c r="C94" s="54"/>
@@ -3167,7 +3173,7 @@
       <c r="E94" s="54"/>
       <c r="F94" s="54"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="56"/>
       <c r="B95" s="56"/>
       <c r="C95" s="56"/>
@@ -3191,13 +3197,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3208,7 +3214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3216,7 +3222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3224,7 +3230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3245,14 +3251,14 @@
       <selection activeCell="G5" sqref="G5:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -3269,7 +3275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -3286,7 +3292,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -3300,7 +3306,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
         <v>32</v>
       </c>
@@ -3308,7 +3314,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
         <v>33</v>
       </c>
@@ -3316,7 +3322,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>34</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
         <v>36</v>
       </c>
@@ -3335,7 +3341,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
         <v>37</v>
       </c>
@@ -3343,7 +3349,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>38</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>4450</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>39</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>3550</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F15" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
update due dates add biv assignment
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH615/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58307BD9-6484-A44F-B6AC-C0D0EC6E5BD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E061355C-399B-4346-897A-AEDC85FDF733}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,13 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="151">
   <si>
     <t>Finals Week</t>
   </si>
@@ -178,12 +183,6 @@
   </si>
   <si>
     <t>Prepare</t>
-  </si>
-  <si>
-    <t>[Categorical Data Analysis Notes](notes/lec04_cda.html)
-PMA5 Ch 6 (Corr &amp; Reg) 
-[Regression](docs/lec05_LinReg.html) notes
-PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
   </si>
   <si>
     <t>[Moderation Notes](notes/Moderation.html)
@@ -303,14 +302,6 @@
     <t>Open work session</t>
   </si>
   <si>
-    <t>Poster Prep: Stage III (Due Fri 11/30 )
-Peer Review: Stage III (Due Sun 12/2 )</t>
-  </si>
-  <si>
-    <t>Poster draft (Due Friday 12/7 )
-[PR poster draft](https://norcalbiostat.github.io/MATH615/project.html#final_posters) (Due Sun 12/9 )</t>
-  </si>
-  <si>
     <t>Preparing your data for analysis
 Recoding, data editing and transformations</t>
   </si>
@@ -330,14 +321,6 @@
   </si>
   <si>
     <t>PR Research Proposal</t>
-  </si>
-  <si>
-    <t>Moderation assignment [[HTML]](hw/08_moderation.html)[[PDF]](hw/08_moderation.pdf) (Due Mon 10/29 )
-Peer Review (Due Wed 10/31 )</t>
-  </si>
-  <si>
-    <t>Regression assignment [[HTML]](hw/09_regression.html)[[PDF]](hw/09_regression.pdf) (Due Mon 11/12 )
-Peer Review (Due Wed 11/14)</t>
   </si>
   <si>
     <t>[Syllabus](https://norcalbiostat.github.io/MATH615/syllabus_615_f18.html)
@@ -419,9 +402,6 @@
   </si>
   <si>
     <t>Created, % based - needs descriptions.</t>
-  </si>
-  <si>
-    <t>Foundations assignment [[PDF]](hw/07_foundations_for_inference.pdf) (Due Fri 10/5 )</t>
   </si>
   <si>
     <t>Identify one binary and one continuous variable in your data set of interest. 
@@ -559,15 +539,6 @@
 </t>
   </si>
   <si>
-    <t>(Optional) Error Assessment [PDF](https://norcalbiostat.github.io/MATH315/notes.html)</t>
-  </si>
-  <si>
-    <t>Bivariate inference assignment [[HTML]](hw/07_bivariate_Inference.html)[[PDF]](hw/07_bivariate_Inference.pdf) (Due Mon 10/22 )</t>
-  </si>
-  <si>
-    <t>Poster Prep: Stage II (Due Wed 10/24 ) (PR Friday 10/26 ) (Final Sunday 10/28 )</t>
-  </si>
-  <si>
     <t>Choosing appropriate analyses
 Typical assumptions
 Hypothesis testing  and p-values</t>
@@ -585,6 +556,46 @@
   <si>
     <t xml:space="preserve">* What are the basic steps of a hypothesis test? 
 * In class Foundations worksheet - the only time you'll do a hypothesis test by hand. </t>
+  </si>
+  <si>
+    <t>Foundations assignment [[PDF]](hw/07_foundations_for_inference.pdf) (Due Tue 10/9 )</t>
+  </si>
+  <si>
+    <t>Dowload and take the non-coding part of the sample exam. 
+Review my comments on your prior homeworks. 
+Bring any questions to one of the extra OH (Sunday 5pm over Zoom, Monday 9am) sessions
+For Thursday: Read PMA5 Chapter 5</t>
+  </si>
+  <si>
+    <t>PMA5 Ch 6 (Corr &amp; Reg) 
+[Lectures notes on Categorical Data Analysis](notes/lec04_cda.html)
+[Lecture notes on Regression](docs/lec05_LinReg.html) notes
+[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 5
+PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
+  </si>
+  <si>
+    <t>Poster draft (Due Thursday 12/6 )
+[PR poster draft](https://norcalbiostat.github.io/MATH615/project.html#final_posters) (Due Sat 12/8 )</t>
+  </si>
+  <si>
+    <t>Moderation assignment [[HTML]](hw/09_moderation.html)[[PDF]](hw/09_moderation.pdf) (Due Mon 11/5 )</t>
+  </si>
+  <si>
+    <t>Poster Prep: Stage III (Draft Thu 11/29 ) (PR Due Sat 12/1 ) (Final Due Mon 12/3)</t>
+  </si>
+  <si>
+    <t>Regression assignment [[HTML]](hw/10_regression.html)[[PDF]](hw/10_regression.pdf) (Due Mon 11/19 )</t>
+  </si>
+  <si>
+    <t>Bivariate inference assignment [[HTML]](hw/08_bivariate_inference.html)[[PDF]](hw/08_bivariate_inference.pdf) (Due Mon 10/29 )
+Poster Prep: Stage II (Due Wed 10/31 ) (PR Friday 11/2 ) (Final Monday 11/5 )</t>
+  </si>
+  <si>
+    <t>(Optional) Analyzing Exam Errors [PDF](https://norcalbiostat.github.io/MATH615/notes.html) (Due Fri 10/26 )</t>
+  </si>
+  <si>
+    <t>Analyzing Exam Errors [PDF](https://norcalbiostat.github.io/MATH615/notes.html)
+**PMA5** Chapter 5</t>
   </si>
 </sst>
 </file>
@@ -594,9 +605,23 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -837,293 +862,299 @@
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="90" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="91" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1567,26 +1598,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="45.83203125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="30.1640625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="32.83203125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="54.6640625" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="14.83203125" style="1"/>
+    <col min="1" max="1" width="5.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="31.875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="45.875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="30.125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="32.875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="54.625" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="14.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>48</v>
       </c>
@@ -1615,7 +1646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="208" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1623,28 +1654,28 @@
         <v>41878</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="E2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="I2" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1653,28 +1684,28 @@
         <v>41885</v>
       </c>
       <c r="C3" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="61" t="s">
+      <c r="G3" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="62" t="s">
-        <v>128</v>
-      </c>
       <c r="H3" s="24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="208" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1683,28 +1714,28 @@
         <v>41892</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1713,28 +1744,28 @@
         <v>41899</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>60</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="288" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1743,28 +1774,28 @@
         <v>41906</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="192" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1773,28 +1804,28 @@
         <v>41913</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" s="66" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H7" s="65" t="s">
-        <v>149</v>
-      </c>
       <c r="I7" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1803,24 +1834,28 @@
         <v>41920</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D8" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="21" t="s">
-        <v>143</v>
+      <c r="F8" s="68" t="s">
+        <v>150</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1829,7 +1864,7 @@
         <v>41927</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1837,10 +1872,10 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -1849,20 +1884,18 @@
         <v>41934</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="21" t="s">
-        <v>50</v>
+      <c r="F10" s="67" t="s">
+        <v>143</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -1876,15 +1909,15 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="144" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -1893,22 +1926,22 @@
         <v>41948</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" s="64" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -1917,20 +1950,20 @@
         <v>41955</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="16">
         <f t="shared" si="0"/>
@@ -1944,7 +1977,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>13</v>
       </c>
@@ -1960,19 +1993,19 @@
         <v>46</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="I15" s="67" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>14</v>
       </c>
@@ -1981,7 +2014,7 @@
         <v>41976</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
@@ -1990,11 +2023,11 @@
       <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="I16" s="67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>15</v>
       </c>
@@ -2003,7 +2036,7 @@
         <v>41983</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2011,10 +2044,10 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>0</v>
       </c>
@@ -2041,26 +2074,26 @@
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="31"/>
-    <col min="2" max="2" width="29.33203125" style="31" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" style="31" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="31" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="31"/>
-    <col min="7" max="7" width="5.1640625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="31"/>
+    <col min="2" max="2" width="29.375" style="31" customWidth="1"/>
+    <col min="3" max="3" width="30.125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="31" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="31"/>
+    <col min="7" max="7" width="5.125" style="28" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="28" customWidth="1"/>
     <col min="9" max="9" width="10" style="30" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="30"/>
-    <col min="11" max="11" width="4.6640625" style="30" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="28"/>
+    <col min="10" max="10" width="8.875" style="30"/>
+    <col min="11" max="11" width="4.625" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>41</v>
       </c>
@@ -2068,10 +2101,10 @@
         <v>17</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>19</v>
@@ -2089,7 +2122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>1.1000000000000001</v>
       </c>
@@ -2100,7 +2133,7 @@
         <v>41884</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F2" s="33">
         <v>5</v>
@@ -2117,15 +2150,15 @@
         <v>0.109375</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>1.2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D3" s="32">
         <v>41884</v>
@@ -2137,7 +2170,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I3" s="33">
         <f>SUMIF($E$2:$E$86,H3,$F$2:$F$86)</f>
@@ -2148,15 +2181,15 @@
         <v>0.140625</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>1.3</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D4" s="32">
         <v>41886</v>
@@ -2179,18 +2212,18 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>1.4</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D5" s="32">
         <v>41888</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F5" s="33">
         <v>5</v>
@@ -2207,15 +2240,15 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30">
         <v>2.1</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D6" s="32">
         <v>41891</v>
@@ -2231,12 +2264,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>3.1</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D7" s="32">
         <v>41898</v>
@@ -2248,29 +2281,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>3.2</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F8" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>3.3</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D9" s="32">
         <v>41900</v>
@@ -2282,29 +2315,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>3.4</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="32">
         <v>41902</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F10" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>4.0999999999999996</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="32">
@@ -2317,15 +2350,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>5.0999999999999996</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D12" s="49">
         <v>41919</v>
@@ -2337,30 +2370,30 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
         <v>5.2</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D13" s="32">
         <v>41923</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F13" s="33">
         <v>5</v>
       </c>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>6</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D14" s="32">
         <v>41916</v>
@@ -2373,7 +2406,7 @@
       </c>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
         <v>7.1</v>
       </c>
@@ -2391,15 +2424,15 @@
       </c>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
         <v>8.1</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>17</v>
@@ -2409,15 +2442,15 @@
       </c>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="30">
         <v>9.1</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>18</v>
@@ -2427,30 +2460,30 @@
       </c>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="30">
         <v>9.1999999999999993</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F18" s="33">
         <v>5</v>
       </c>
       <c r="I18" s="28"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
         <v>10.1</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>17</v>
@@ -2460,15 +2493,15 @@
       </c>
       <c r="I19" s="28"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>12.1</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>17</v>
@@ -2478,15 +2511,15 @@
       </c>
       <c r="I20" s="28"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>13.1</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>18</v>
@@ -2496,27 +2529,27 @@
       </c>
       <c r="I21" s="28"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="30">
         <v>13.2</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F22" s="33">
         <v>5</v>
       </c>
       <c r="I22" s="28"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="30">
         <v>14.1</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="45" t="s">
         <v>18</v>
@@ -2526,27 +2559,27 @@
       </c>
       <c r="I23" s="28"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="30">
         <v>14.2</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F24" s="33">
         <v>5</v>
       </c>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="30">
         <v>15.1</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" s="45" t="s">
         <v>18</v>
@@ -2556,21 +2589,21 @@
       </c>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="30">
         <v>15.2</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F26" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="30">
         <v>16</v>
       </c>
@@ -2584,27 +2617,27 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="30">
         <v>16</v>
       </c>
       <c r="B28" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="F28" s="33">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="30"/>
       <c r="C31" s="30"/>
@@ -2612,7 +2645,7 @@
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
@@ -2620,7 +2653,7 @@
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -2628,7 +2661,7 @@
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
@@ -2636,7 +2669,7 @@
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -2644,7 +2677,7 @@
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
@@ -2652,7 +2685,7 @@
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -2660,7 +2693,7 @@
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -2668,7 +2701,7 @@
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -2677,7 +2710,7 @@
       <c r="F39" s="30"/>
       <c r="G39" s="51"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -2685,7 +2718,7 @@
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -2693,7 +2726,7 @@
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -2701,7 +2734,7 @@
       <c r="E42" s="30"/>
       <c r="F42" s="30"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
@@ -2709,7 +2742,7 @@
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
@@ -2717,7 +2750,7 @@
       <c r="E44" s="30"/>
       <c r="F44" s="30"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
@@ -2725,7 +2758,7 @@
       <c r="E45" s="30"/>
       <c r="F45" s="30"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
@@ -2734,7 +2767,7 @@
       <c r="F46" s="30"/>
       <c r="G46" s="51"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -2743,7 +2776,7 @@
       <c r="F47" s="30"/>
       <c r="G47" s="51"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
@@ -2752,7 +2785,7 @@
       <c r="F48" s="30"/>
       <c r="G48" s="51"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="30"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
@@ -2761,7 +2794,7 @@
       <c r="F49" s="30"/>
       <c r="G49" s="51"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
@@ -2770,7 +2803,7 @@
       <c r="F50" s="30"/>
       <c r="G50" s="51"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="30"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
@@ -2779,7 +2812,7 @@
       <c r="F51" s="30"/>
       <c r="G51" s="51"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="30"/>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
@@ -2788,7 +2821,7 @@
       <c r="F52" s="30"/>
       <c r="G52" s="51"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="30"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -2797,7 +2830,7 @@
       <c r="F53" s="30"/>
       <c r="G53" s="51"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="30"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
@@ -2806,7 +2839,7 @@
       <c r="F54" s="30"/>
       <c r="G54" s="51"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="30"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
@@ -2815,7 +2848,7 @@
       <c r="F55" s="30"/>
       <c r="G55" s="51"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
@@ -2824,7 +2857,7 @@
       <c r="F56" s="30"/>
       <c r="G56" s="51"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
@@ -2833,7 +2866,7 @@
       <c r="F57" s="30"/>
       <c r="G57" s="51"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="30"/>
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
@@ -2842,7 +2875,7 @@
       <c r="F58" s="30"/>
       <c r="G58" s="51"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
@@ -2851,7 +2884,7 @@
       <c r="F59" s="30"/>
       <c r="G59" s="51"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="30"/>
       <c r="B60" s="30"/>
       <c r="C60" s="30"/>
@@ -2860,7 +2893,7 @@
       <c r="F60" s="30"/>
       <c r="G60" s="51"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="30"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
@@ -2869,7 +2902,7 @@
       <c r="F61" s="30"/>
       <c r="G61" s="51"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="30"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
@@ -2878,7 +2911,7 @@
       <c r="F62" s="30"/>
       <c r="G62" s="51"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="30"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
@@ -2890,7 +2923,7 @@
       <c r="I63" s="31"/>
       <c r="J63" s="31"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="30"/>
       <c r="B64" s="30"/>
       <c r="C64" s="30"/>
@@ -2902,7 +2935,7 @@
       <c r="I64" s="31"/>
       <c r="J64" s="31"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="30"/>
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
@@ -2912,7 +2945,7 @@
       <c r="G65" s="53"/>
       <c r="K65" s="31"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="30"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
@@ -2922,7 +2955,7 @@
       <c r="G66" s="53"/>
       <c r="K66" s="31"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="30"/>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
@@ -2931,7 +2964,7 @@
       <c r="F67" s="30"/>
       <c r="G67" s="51"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="30"/>
       <c r="B68" s="30"/>
       <c r="C68" s="30"/>
@@ -2940,7 +2973,7 @@
       <c r="F68" s="30"/>
       <c r="G68" s="51"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="30"/>
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
@@ -2949,7 +2982,7 @@
       <c r="F69" s="30"/>
       <c r="G69" s="51"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="30"/>
       <c r="B70" s="30"/>
       <c r="C70" s="30"/>
@@ -2958,7 +2991,7 @@
       <c r="F70" s="30"/>
       <c r="G70" s="51"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="30"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30"/>
@@ -2967,7 +3000,7 @@
       <c r="F71" s="30"/>
       <c r="G71" s="51"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="30"/>
       <c r="B72" s="30"/>
       <c r="C72" s="30"/>
@@ -2976,7 +3009,7 @@
       <c r="F72" s="30"/>
       <c r="G72" s="51"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="30"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
@@ -2984,7 +3017,7 @@
       <c r="E73" s="30"/>
       <c r="F73" s="30"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="54"/>
       <c r="B74" s="54"/>
       <c r="C74" s="54"/>
@@ -2992,7 +3025,7 @@
       <c r="E74" s="54"/>
       <c r="F74" s="54"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="54"/>
       <c r="B75" s="54"/>
       <c r="C75" s="54"/>
@@ -3000,7 +3033,7 @@
       <c r="E75" s="54"/>
       <c r="F75" s="54"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="54"/>
       <c r="B76" s="54"/>
       <c r="C76" s="54"/>
@@ -3008,7 +3041,7 @@
       <c r="E76" s="54"/>
       <c r="F76" s="54"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="54"/>
       <c r="B77" s="54"/>
       <c r="C77" s="54"/>
@@ -3016,7 +3049,7 @@
       <c r="E77" s="54"/>
       <c r="F77" s="54"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="54"/>
       <c r="B78" s="54"/>
       <c r="C78" s="54"/>
@@ -3024,7 +3057,7 @@
       <c r="E78" s="54"/>
       <c r="F78" s="54"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="54"/>
       <c r="B79" s="54"/>
       <c r="C79" s="54"/>
@@ -3033,7 +3066,7 @@
       <c r="F79" s="54"/>
       <c r="G79" s="52"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="54"/>
       <c r="B80" s="54"/>
       <c r="C80" s="54"/>
@@ -3044,7 +3077,7 @@
       <c r="I80" s="28"/>
       <c r="J80" s="28"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="54"/>
       <c r="B81" s="54"/>
       <c r="C81" s="54"/>
@@ -3053,7 +3086,7 @@
       <c r="F81" s="54"/>
       <c r="G81" s="52"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="54"/>
       <c r="B82" s="54"/>
       <c r="C82" s="54"/>
@@ -3063,7 +3096,7 @@
       <c r="I82" s="28"/>
       <c r="J82" s="28"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="54"/>
       <c r="B83" s="54"/>
       <c r="C83" s="54"/>
@@ -3073,7 +3106,7 @@
       <c r="I83" s="28"/>
       <c r="J83" s="28"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="54"/>
       <c r="B84" s="54"/>
       <c r="C84" s="54"/>
@@ -3083,7 +3116,7 @@
       <c r="I84" s="28"/>
       <c r="J84" s="28"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="54"/>
       <c r="B85" s="54"/>
       <c r="C85" s="54"/>
@@ -3093,7 +3126,7 @@
       <c r="I85" s="28"/>
       <c r="J85" s="28"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="54"/>
       <c r="B86" s="54"/>
       <c r="C86" s="54"/>
@@ -3103,7 +3136,7 @@
       <c r="I86" s="28"/>
       <c r="J86" s="28"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="54"/>
       <c r="B87" s="54"/>
       <c r="C87" s="54"/>
@@ -3113,7 +3146,7 @@
       <c r="I87" s="28"/>
       <c r="J87" s="28"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="54"/>
       <c r="B88" s="54"/>
       <c r="C88" s="54"/>
@@ -3123,7 +3156,7 @@
       <c r="I88" s="28"/>
       <c r="J88" s="28"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="54"/>
       <c r="B89" s="54"/>
       <c r="C89" s="54"/>
@@ -3133,7 +3166,7 @@
       <c r="I89" s="28"/>
       <c r="J89" s="28"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="54"/>
       <c r="B90" s="54"/>
       <c r="C90" s="54"/>
@@ -3141,7 +3174,7 @@
       <c r="E90" s="54"/>
       <c r="F90" s="54"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="54"/>
       <c r="B91" s="54"/>
       <c r="C91" s="54"/>
@@ -3149,7 +3182,7 @@
       <c r="E91" s="54"/>
       <c r="F91" s="54"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="54"/>
       <c r="B92" s="54"/>
       <c r="C92" s="54"/>
@@ -3157,7 +3190,7 @@
       <c r="E92" s="54"/>
       <c r="F92" s="54"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="54"/>
       <c r="B93" s="54"/>
       <c r="C93" s="54"/>
@@ -3165,7 +3198,7 @@
       <c r="E93" s="54"/>
       <c r="F93" s="54"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="54"/>
       <c r="B94" s="54"/>
       <c r="C94" s="54"/>
@@ -3173,7 +3206,7 @@
       <c r="E94" s="54"/>
       <c r="F94" s="54"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="56"/>
       <c r="B95" s="56"/>
       <c r="C95" s="56"/>
@@ -3197,13 +3230,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3214,7 +3247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3222,7 +3255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3230,7 +3263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3251,14 +3284,14 @@
       <selection activeCell="G5" sqref="G5:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -3275,7 +3308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -3292,7 +3325,7 @@
         <v>3950</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -3306,7 +3339,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>32</v>
       </c>
@@ -3314,7 +3347,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>33</v>
       </c>
@@ -3322,7 +3355,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>34</v>
       </c>
@@ -3333,7 +3366,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>36</v>
       </c>
@@ -3341,7 +3374,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>37</v>
       </c>
@@ -3349,7 +3382,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>38</v>
       </c>
@@ -3357,7 +3390,7 @@
         <v>4450</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>39</v>
       </c>
@@ -3365,7 +3398,7 @@
         <v>3550</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
update idx for week 8
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D2590E-2361-4266-96FA-18FFF85710D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="155">
   <si>
     <t>Finals Week</t>
   </si>
@@ -562,13 +561,6 @@
 For Thursday: Read PMA5 Chapter 5</t>
   </si>
   <si>
-    <t>PMA5 Ch 6 (Corr &amp; Reg) 
-[Lectures notes on Categorical Data Analysis](notes/lec04_cda.html)
-[Lecture notes on Regression](docs/lec05_LinReg.html) notes
-[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 5
-PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
-  </si>
-  <si>
     <t>Poster draft (Due Thursday 12/6 )
 [PR poster draft](https://norcalbiostat.github.io/MATH615/project.html#final_posters) (Due Sat 12/8 )</t>
   </si>
@@ -598,17 +590,51 @@
 * Project Updates
 </t>
   </si>
+  <si>
+    <t>Comments on foundations assignment, generalizability and statements about the population
+Testing the difference between two means</t>
+  </si>
+  <si>
+    <t>Type I and II errors
+Multiple Comparisons
+Theoretical framework of ANOVA</t>
+  </si>
+  <si>
+    <t>Statisically test the association between two means
+Give an example of a Type I and II error
+Explain the problem of multiple comparisons
+Explain how we can make a claim about the difference between multiple means by analyzing variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Open Intro Statistics](https://www.openintro.org/stat/textbook.php) Chapter 4 for Inference on a single mean, Chapter 5.5 for ANOVA
+Math 315 Course Packet [ANOVA Chapter 6.4](https://norcalbiostat.github.io/MATH315/reading/RAD_course_notes.pdf)
+P-hacking [XKCD](https://xkcd.com/882/) style
+</t>
+  </si>
+  <si>
+    <t>[Lectures notes on Categorical Data Analysis](notes/lec03_cda.html)
+PMA5 Ch 6 (Corr &amp; Reg) 
+[AS Notebook](https://norcalbiostat.github.io/AppliedStatistics_notes/) Chapter 5
+PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -863,299 +889,305 @@
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="90" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="91" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="90" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="90" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="90" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="8" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="89" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="91" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1254,9 +1286,9 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
     <cellStyle name="Percent" xfId="89" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Percent 2" xfId="52"/>
     <cellStyle name="Total" xfId="91" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1599,12 +1631,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,19 +1879,19 @@
         <v>141</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="69" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1870,16 +1902,24 @@
       <c r="C9" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="70" t="s">
+        <v>152</v>
+      </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="71" t="s">
+        <v>151</v>
+      </c>
       <c r="I9" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -1892,8 +1932,8 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="67" t="s">
-        <v>142</v>
+      <c r="F10" s="70" t="s">
+        <v>154</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1918,7 +1958,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -1942,7 +1982,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2006,7 +2046,7 @@
         <v>80</v>
       </c>
       <c r="I15" s="67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2028,7 +2068,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2074,11 +2114,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2438,6 +2478,9 @@
       <c r="C16" s="37" t="s">
         <v>97</v>
       </c>
+      <c r="D16" s="32">
+        <v>41940</v>
+      </c>
       <c r="E16" s="38" t="s">
         <v>17</v>
       </c>
@@ -2456,6 +2499,9 @@
       <c r="C17" s="37" t="s">
         <v>97</v>
       </c>
+      <c r="D17" s="32">
+        <v>41947</v>
+      </c>
       <c r="E17" s="45" t="s">
         <v>18</v>
       </c>
@@ -2471,6 +2517,9 @@
       <c r="B18" s="31" t="s">
         <v>66</v>
       </c>
+      <c r="D18" s="32">
+        <v>41944</v>
+      </c>
       <c r="E18" s="33" t="s">
         <v>99</v>
       </c>
@@ -2488,6 +2537,9 @@
       </c>
       <c r="C19" s="37" t="s">
         <v>97</v>
+      </c>
+      <c r="D19" s="32">
+        <v>41947</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>17</v>
@@ -3227,7 +3279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3281,7 +3333,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add study design notes
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -166,9 +166,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Moderation</t>
-  </si>
-  <si>
     <t>Model building/ fit</t>
   </si>
   <si>
@@ -339,10 +336,6 @@
   <si>
     <t>Bivariate analysis: Chi-squared
 Bivariate analysis: Correlation and Regression</t>
-  </si>
-  <si>
-    <t>Study Design
-Multiple Regression</t>
   </si>
   <si>
     <t xml:space="preserve">Categorical Predictors
@@ -512,12 +505,6 @@
 Open work period</t>
   </si>
   <si>
-    <t>[PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
-Study Design Notes [[HTML]](docs/lec06_StudyDesign.html) [[PDF]](docs/lec06_StudyDesign.pdf)
-AS Notebook [Ch 6]() 
-[Regression Assignment Examples](hw/Regression_Assignment_Examples.html)</t>
-  </si>
-  <si>
     <t>Explain the basic fundamentals of probability. 
 Calculate marginal and conditional probabilities. 
 Perform the steps and calculations needed to construct a confidence interval and hypothesis test. 
@@ -632,8 +619,21 @@
 PDS [[Correlation]](https://www.youtube.com/watch?v=qBwjKfytls8&amp;list=PLDEF0B9CBD27AD37E&amp;index=60) video (11 min)</t>
   </si>
   <si>
-    <t>[Lecture notes on Moderation](lecture/lec04_moderation.html)
-[PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)</t>
+    <t>Moderation
+Study Design</t>
+  </si>
+  <si>
+    <t>Multiple Regression</t>
+  </si>
+  <si>
+    <t>Lecture notes on Moderation [[HTML]](lecture/lec04_moderation.html) [[PDF]](lecture/lec04_moderation.pdf)
+[PDS video 14](http://passiondrivenstatistics.com/2016/08/20/r-chapter-14/)(21 min)
+Lecture notes on Study Design [[HTML]](lecture/lec05_studydesign.html) [[PDF]](lecture/lec05_studydesign.pdf)</t>
+  </si>
+  <si>
+    <t>[PDS video 17](http://passiondrivenstatistics.com/2016/10/06/r-chapter-17/) (57 min)
+AS Notebook [Ch 6](https://norcalbiostat.github.io/AppliedStatistics_notes/multiple-linear-regression.html) 
+[Regression Assignment Examples](hw/hw09_regression.html)</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1020,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1242,6 +1242,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1686,8 +1689,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1709,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>2</v>
@@ -1718,7 +1721,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>4</v>
@@ -1741,25 +1744,25 @@
         <v>41878</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="I2" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="270" hidden="1" x14ac:dyDescent="0.25">
@@ -1771,25 +1774,25 @@
         <v>41885</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F3" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>122</v>
-      </c>
-      <c r="G3" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="195" hidden="1" x14ac:dyDescent="0.25">
@@ -1801,25 +1804,25 @@
         <v>41892</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
@@ -1831,25 +1834,25 @@
         <v>41899</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>58</v>
-      </c>
       <c r="G5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="I5" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="270" hidden="1" x14ac:dyDescent="0.25">
@@ -1861,25 +1864,25 @@
         <v>41906</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="180" hidden="1" x14ac:dyDescent="0.25">
@@ -1891,25 +1894,25 @@
         <v>41913</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="66" t="s">
+      <c r="G7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H7" s="65" t="s">
-        <v>138</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="135" hidden="1" x14ac:dyDescent="0.25">
@@ -1921,25 +1924,25 @@
         <v>41920</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E8" s="68" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="69" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -1951,25 +1954,25 @@
         <v>41927</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="70" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E9" s="72" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F9" s="70" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G9" s="71" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H9" s="71" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -1981,26 +1984,26 @@
         <v>41934</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F10" s="74" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G10" s="73" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H10" s="73" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -2008,21 +2011,21 @@
         <f t="shared" si="0"/>
         <v>41941</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>44</v>
+      <c r="C11" s="75" t="s">
+        <v>156</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="75" t="s">
-        <v>159</v>
+      <c r="F11" s="76" t="s">
+        <v>158</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -2031,19 +2034,19 @@
         <v>41948</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="64" t="s">
-        <v>132</v>
+        <v>74</v>
+      </c>
+      <c r="F12" s="76" t="s">
+        <v>159</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2055,14 +2058,14 @@
         <v>41955</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2091,23 +2094,23 @@
         <v>41969</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="22" t="s">
-        <v>79</v>
-      </c>
       <c r="I15" s="67" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2119,17 +2122,17 @@
         <v>41976</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2141,7 +2144,7 @@
         <v>41983</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2149,7 +2152,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2206,10 +2209,10 @@
         <v>17</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>19</v>
@@ -2238,7 +2241,7 @@
         <v>41884</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="33">
         <v>5</v>
@@ -2260,10 +2263,10 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D3" s="32">
         <v>41884</v>
@@ -2275,7 +2278,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I3" s="33">
         <f>SUMIF($E$2:$E$86,H3,$F$2:$F$86)</f>
@@ -2291,10 +2294,10 @@
         <v>1.3</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D4" s="32">
         <v>41886</v>
@@ -2322,13 +2325,13 @@
         <v>1.4</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D5" s="32">
         <v>41888</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="33">
         <v>5</v>
@@ -2350,10 +2353,10 @@
         <v>2.1</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D6" s="32">
         <v>41891</v>
@@ -2374,7 +2377,7 @@
         <v>3.1</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="32">
         <v>41898</v>
@@ -2391,10 +2394,10 @@
         <v>3.2</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F8" s="33">
         <v>5</v>
@@ -2405,10 +2408,10 @@
         <v>3.3</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="32">
         <v>41900</v>
@@ -2425,13 +2428,13 @@
         <v>3.4</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="32">
         <v>41902</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F10" s="33">
         <v>5</v>
@@ -2442,7 +2445,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="32">
@@ -2460,10 +2463,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D12" s="49">
         <v>41919</v>
@@ -2480,13 +2483,13 @@
         <v>5.2</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="32">
         <v>41923</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F13" s="33">
         <v>5</v>
@@ -2498,7 +2501,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D14" s="32">
         <v>41916</v>
@@ -2534,10 +2537,10 @@
         <v>8.1</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D16" s="32">
         <v>41940</v>
@@ -2555,10 +2558,10 @@
         <v>9.1</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D17" s="32">
         <v>41947</v>
@@ -2576,13 +2579,13 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="32">
         <v>41944</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F18" s="33">
         <v>5</v>
@@ -2594,10 +2597,10 @@
         <v>10.1</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D19" s="32">
         <v>41947</v>
@@ -2615,10 +2618,10 @@
         <v>12.1</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>17</v>
@@ -2633,10 +2636,10 @@
         <v>13.1</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>18</v>
@@ -2651,10 +2654,10 @@
         <v>13.2</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F22" s="33">
         <v>5</v>
@@ -2666,7 +2669,7 @@
         <v>14.1</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="45" t="s">
         <v>18</v>
@@ -2681,10 +2684,10 @@
         <v>14.2</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F24" s="33">
         <v>5</v>
@@ -2696,7 +2699,7 @@
         <v>15.1</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="45" t="s">
         <v>18</v>
@@ -2711,10 +2714,10 @@
         <v>15.2</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F26" s="33">
         <v>5</v>
@@ -2739,10 +2742,10 @@
         <v>16</v>
       </c>
       <c r="B28" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="33" t="s">
         <v>70</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>71</v>
       </c>
       <c r="F28" s="33">
         <v>10</v>

</xml_diff>

<commit_message>
change link color, update project page
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68CCDB7-811E-4A80-86A6-DEEA0E40267A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E63778-689D-49F5-8F5C-DD1515EC68B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33270" yWindow="720" windowWidth="24000" windowHeight="12915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -366,9 +366,6 @@
 Data entry &amp; Codebook creation</t>
   </si>
   <si>
-    <t>PMA5 Ch 1, 2</t>
-  </si>
-  <si>
     <t>Formulating testable hypothesis
 Preparing data for analysis</t>
   </si>
@@ -438,6 +435,10 @@
   <si>
     <t>Multiple Regression analysis
 Confounding</t>
+  </si>
+  <si>
+    <t>PMA5 Ch 1, 2
+[Lec00](lecture/lec00_intro_class.html)</t>
   </si>
 </sst>
 </file>
@@ -1258,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1308,7 @@
         <v>107</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="F2" s="36" t="s">
         <v>76</v>
@@ -1324,10 +1325,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>77</v>
@@ -1348,7 +1349,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="36" t="s">
         <v>78</v>
@@ -1365,10 +1366,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="36" t="s">
         <v>81</v>
@@ -1415,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="36" t="s">
@@ -1433,7 +1434,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F9" s="36" t="s">
         <v>89</v>
@@ -1463,10 +1464,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>92</v>
@@ -1483,7 +1484,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" s="36" t="s">
         <v>94</v>
@@ -1500,7 +1501,7 @@
         <v>62</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13" s="36" t="s">
         <v>95</v>
@@ -1527,7 +1528,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" s="36" t="s">
         <v>99</v>
@@ -1544,10 +1545,10 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16" s="36" t="s">
         <v>97</v>
@@ -1567,7 +1568,7 @@
         <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F17" s="36" t="s">
         <v>101</v>
@@ -1581,7 +1582,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1606,7 +1607,7 @@
         <v>66</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F20" s="36" t="s">
         <v>102</v>
@@ -1620,7 +1621,7 @@
         <v>106</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,7 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add checklist to lec00
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A05EAE6-63EE-4029-B90C-E2113C3E54CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4DF894-6696-452A-BB2C-CFBEA29EFD12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32460" yWindow="1485" windowWidth="24000" windowHeight="12915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -432,14 +432,15 @@
 Confounding</t>
   </si>
   <si>
-    <t>PMA5 Ch 1, 2
-[Lec00](lecture/lec00_intro_class.html)</t>
-  </si>
-  <si>
     <t>Introduction to the class
 Data types, architecture
 Data entry &amp; Codebook creation
 Choosing project research data</t>
+  </si>
+  <si>
+    <t>PMA5 Ch 1, 2
+[Lec00](lecture/lec00_intro_class.html)
+[Lec01](https://hackmd.io/@norcalbiostat/math615_lec01)</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1262,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1306,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="38" t="s">
         <v>126</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="F2" s="36" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
add lec02 and hw02
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EECAF43-2FC8-4100-B907-1DE9FC2F8D51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8297DF-15BD-4B67-BC89-B22D5FC65A21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30660" yWindow="810" windowWidth="24000" windowHeight="12915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -265,9 +265,6 @@
     <t>03 RR / DM</t>
   </si>
   <si>
-    <t>[hw01_introduction](hw/hw01_introduction.html) (Due 09/01 )</t>
-  </si>
-  <si>
     <t>Quiz 01 (Due 09/02 )</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
   </si>
   <si>
     <t>[hw04_univ_graphing](hw/hw04_univ_graphing.html) (Draft Due 9/20, PR 9/21, Final 9/22 )</t>
-  </si>
-  <si>
-    <t>[hw02_rq_formulation](hw/hw02_rq_formulation.html) (Draft Due 9/6, PR 9/11, Final 9/08 )</t>
   </si>
   <si>
     <t>[Poster prep Stage I](project.html) (Draft Due 9/17, PR 9/19, Final 9/21 )</t>
@@ -363,10 +357,6 @@
   <si>
     <t>Formulating testable hypothesis
 Preparing data for analysis</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 3
-ASCN Ch 1</t>
   </si>
   <si>
     <t>PMA6 Ch 4
@@ -444,6 +434,17 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>[HW01 Data Entry](hw/01_data_entry.html) (Due 09/01 )</t>
+  </si>
+  <si>
+    <t>[HW02 RQ Formulation](hw/02_rq_formulation.html) (Draft Due 9/6, PR 9/11, Final 9/08 )</t>
+  </si>
+  <si>
+    <t>[Lec02](https://hackmd.io/@norcalbiostat/math615_lec02)
+[ASCN Ch 1](https://norcalbiostat.github.io/AppliedStatistics_notes/data-prep.html)
+PMA6 Ch 3</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1267,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1311,16 +1312,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>125</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1331,16 +1332,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>127</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,13 +1356,13 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F4" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="39" t="s">
         <v>78</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1372,16 +1373,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F5" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="39" t="s">
         <v>81</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1394,7 +1395,7 @@
       <c r="E6" s="40"/>
       <c r="F6" s="34"/>
       <c r="G6" s="40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1405,13 +1406,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1422,14 +1423,14 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1440,13 +1441,13 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1459,7 +1460,7 @@
       <c r="E10" s="40"/>
       <c r="F10" s="34"/>
       <c r="G10" s="40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1470,16 +1471,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1490,10 +1491,10 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1507,10 +1508,10 @@
         <v>62</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1523,7 +1524,7 @@
       <c r="E14" s="40"/>
       <c r="F14" s="34"/>
       <c r="G14" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1534,13 +1535,13 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1551,16 +1552,16 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1574,10 +1575,10 @@
         <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1588,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,10 +1614,10 @@
         <v>66</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1624,10 +1625,10 @@
         <v>15.2</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1654,7 +1655,7 @@
         <v>69</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1668,7 +1669,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1679,7 +1680,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1795,10 +1796,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
make hack md required
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8297DF-15BD-4B67-BC89-B22D5FC65A21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357EF986-11DF-48BF-B767-EBABA6495DF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30660" yWindow="810" windowWidth="24000" windowHeight="12915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="1050" windowWidth="24000" windowHeight="12915" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="128">
   <si>
     <t>Assignments</t>
   </si>
@@ -1266,7 +1266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1869,6 +1869,12 @@
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="C5" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="E5" s="18" t="s">
         <v>1</v>
       </c>
@@ -1902,6 +1908,9 @@
       </c>
       <c r="B6" s="12" t="s">
         <v>31</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
clean up reading and fix typo
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357EF986-11DF-48BF-B767-EBABA6495DF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D5C3A1-A7A7-4655-AEF5-56719844ECD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1050" windowWidth="24000" windowHeight="12915" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -439,12 +439,12 @@
     <t>[HW01 Data Entry](hw/01_data_entry.html) (Due 09/01 )</t>
   </si>
   <si>
-    <t>[HW02 RQ Formulation](hw/02_rq_formulation.html) (Draft Due 9/6, PR 9/11, Final 9/08 )</t>
-  </si>
-  <si>
     <t>[Lec02](https://hackmd.io/@norcalbiostat/math615_lec02)
 [ASCN Ch 1](https://norcalbiostat.github.io/AppliedStatistics_notes/data-prep.html)
 PMA6 Ch 3</t>
+  </si>
+  <si>
+    <t>[HW02 RQ Formulation](hw/02_rq_formulation.html) (Draft Due 9/6, PR 9/7, Final 9/8 )</t>
   </si>
 </sst>
 </file>
@@ -1266,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1335,13 +1335,13 @@
         <v>105</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" s="36" t="s">
         <v>76</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix syllabus add quiz01
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D5C3A1-A7A7-4655-AEF5-56719844ECD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F5B5BF-6D05-40BE-8D18-BE0F1000B6C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="1245" windowWidth="21090" windowHeight="13665" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -265,9 +265,6 @@
     <t>03 RR / DM</t>
   </si>
   <si>
-    <t>Quiz 01 (Due 09/02 )</t>
-  </si>
-  <si>
     <t>Quiz 02 (Due 09/09 )</t>
   </si>
   <si>
@@ -445,6 +442,9 @@
   </si>
   <si>
     <t>[HW02 RQ Formulation](hw/02_rq_formulation.html) (Draft Due 9/6, PR 9/7, Final 9/8 )</t>
+  </si>
+  <si>
+    <t>[Quiz 01](https://forms.gle/KaKtWNULi58BX37y5) (Due 09/02 )</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1267,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1312,16 +1312,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="38" t="s">
-        <v>123</v>
-      </c>
       <c r="F2" s="36" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1332,16 +1332,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>126</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,13 +1356,13 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="39" t="s">
         <v>77</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1373,16 +1373,16 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="39" t="s">
         <v>80</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
       <c r="E6" s="40"/>
       <c r="F6" s="34"/>
       <c r="G6" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1406,13 +1406,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F7" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="39" t="s">
         <v>83</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1423,14 +1423,14 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1441,13 +1441,13 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F9" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="39" t="s">
         <v>87</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
       <c r="E10" s="40"/>
       <c r="F10" s="34"/>
       <c r="G10" s="40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1471,16 +1471,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="39" t="s">
         <v>90</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1491,10 +1491,10 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1508,10 +1508,10 @@
         <v>62</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1524,7 +1524,7 @@
       <c r="E14" s="40"/>
       <c r="F14" s="34"/>
       <c r="G14" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1535,13 +1535,13 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1552,16 +1552,16 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F16" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="39" t="s">
         <v>95</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1575,10 +1575,10 @@
         <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1614,10 +1614,10 @@
         <v>66</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1625,10 +1625,10 @@
         <v>15.2</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
         <v>69</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1669,7 +1669,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1796,10 +1796,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>1</v>
@@ -1870,10 +1870,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>1</v>
@@ -1910,7 +1910,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
upd hw03 add quiz3 link
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH615/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB475D7-209A-C746-98A5-DF0C1391D066}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A2D79F-2342-49D3-B8AB-DC761AA0406B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="620" windowWidth="24160" windowHeight="14300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30375" yWindow="450" windowWidth="24165" windowHeight="14295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
     <sheet name="points" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="128">
   <si>
     <t>Assignments</t>
   </si>
@@ -255,9 +263,6 @@
   </si>
   <si>
     <t>03 RR / DM</t>
-  </si>
-  <si>
-    <t>Quiz 03 (Due 09/16 )</t>
   </si>
   <si>
     <t>Describing relationships (Q~C, Q~Q)</t>
@@ -431,13 +436,16 @@
     <t>[[Quiz 01]](https://forms.gle/KaKtWNULi58BX37y5) (Due 09/02 )</t>
   </si>
   <si>
-    <t>[hw03_data_management](hw/03_data_management.html) (Draft Due 9/13, PR 9/14, Final 9/15 )</t>
-  </si>
-  <si>
     <t>[hw04_univ_graphing](hw/04_univ_graphing.html) (Draft Due 9/20, PR 9/21, Final 9/22 )</t>
   </si>
   <si>
     <t>[hw05_biv_graphing](hw/05_biv_graphing.html) (Draft Due 9/27, PR 9/28, Final 9/29 )</t>
+  </si>
+  <si>
+    <t>[[Quiz 03]](https://forms.gle/P7hah7kJJidU3z2TA) (Due 09/16 )</t>
+  </si>
+  <si>
+    <t>[hw03_data_management](hw/03_data_management.html) (Due 9/15 ) PR removed due to illness</t>
   </si>
 </sst>
 </file>
@@ -1263,21 +1271,21 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="2"/>
+    <col min="1" max="2" width="8.875" style="2"/>
     <col min="3" max="3" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="38" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="79.6640625" style="38" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="38"/>
+    <col min="4" max="4" width="31.625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="25.125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="79.625" style="38" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1300,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -1308,19 +1316,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="38" t="s">
-        <v>118</v>
-      </c>
       <c r="F2" s="43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2.1</v>
       </c>
@@ -1328,19 +1336,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="43" t="s">
-        <v>123</v>
-      </c>
       <c r="G3" s="42" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3.1</v>
       </c>
@@ -1352,16 +1360,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>75</v>
+        <v>101</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>126</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -1369,19 +1377,19 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4.3</v>
       </c>
@@ -1391,10 +1399,10 @@
       <c r="E6" s="40"/>
       <c r="F6" s="34"/>
       <c r="G6" s="40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5.0999999999999996</v>
       </c>
@@ -1402,16 +1410,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6.1</v>
       </c>
@@ -1419,17 +1427,17 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7.1</v>
       </c>
@@ -1437,16 +1445,16 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F9" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7.3</v>
       </c>
@@ -1456,10 +1464,10 @@
       <c r="E10" s="40"/>
       <c r="F10" s="34"/>
       <c r="G10" s="40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8.1</v>
       </c>
@@ -1467,19 +1475,19 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="39" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9.1</v>
       </c>
@@ -1487,13 +1495,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10.1</v>
       </c>
@@ -1504,13 +1512,13 @@
         <v>62</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>10.199999999999999</v>
       </c>
@@ -1520,10 +1528,10 @@
       <c r="E14" s="40"/>
       <c r="F14" s="34"/>
       <c r="G14" s="40" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>11.1</v>
       </c>
@@ -1531,16 +1539,16 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>12.1</v>
       </c>
@@ -1548,19 +1556,19 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>13.1</v>
       </c>
@@ -1571,13 +1579,13 @@
         <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>13.2</v>
       </c>
@@ -1585,10 +1593,10 @@
         <v>16</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>14.1</v>
       </c>
@@ -1599,7 +1607,7 @@
       <c r="F19" s="35"/>
       <c r="G19" s="41"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>15.1</v>
       </c>
@@ -1610,24 +1618,24 @@
         <v>66</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>15.2</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>15.3</v>
       </c>
@@ -1640,7 +1648,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>16.100000000000001</v>
       </c>
@@ -1651,10 +1659,10 @@
         <v>69</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>17.100000000000001</v>
       </c>
@@ -1665,10 +1673,10 @@
         <v>15</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>17.2</v>
       </c>
@@ -1676,11 +1684,11 @@
         <v>8</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
     <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1696,23 +1704,23 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="12"/>
-    <col min="2" max="2" width="36.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="12"/>
-    <col min="7" max="7" width="5.1640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="12"/>
+    <col min="2" max="2" width="36.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="12"/>
+    <col min="7" max="7" width="5.125" style="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="11" customWidth="1"/>
     <col min="9" max="9" width="10" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="12"/>
-    <col min="11" max="11" width="4.6640625" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="11"/>
+    <col min="10" max="10" width="8.875" style="12"/>
+    <col min="11" max="11" width="4.625" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -1750,7 +1758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1784,7 +1792,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1.2</v>
       </c>
@@ -1792,10 +1800,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>1</v>
@@ -1824,7 +1832,7 @@
         <v>0.12698412698412698</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1.3</v>
       </c>
@@ -1858,7 +1866,7 @@
         <v>0.31746031746031744</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1866,10 +1874,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>1</v>
@@ -1898,7 +1906,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2.1</v>
       </c>
@@ -1906,7 +1914,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>10</v>
@@ -1930,7 +1938,7 @@
       </c>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -1938,7 +1946,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>11</v>
@@ -1951,7 +1959,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -1959,7 +1967,7 @@
         <v>74</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>1</v>
@@ -1968,7 +1976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>3.1</v>
       </c>
@@ -1982,7 +1990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>3.1</v>
       </c>
@@ -1996,7 +2004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>3.2</v>
       </c>
@@ -2010,7 +2018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>4</v>
       </c>
@@ -2024,7 +2032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>4.2</v>
       </c>
@@ -2038,7 +2046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>4.3</v>
       </c>
@@ -2052,7 +2060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -2066,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>5</v>
       </c>
@@ -2080,7 +2088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>5.0999999999999996</v>
       </c>
@@ -2095,7 +2103,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>5.2</v>
       </c>
@@ -2110,7 +2118,7 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>6</v>
       </c>
@@ -2126,7 +2134,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>6.1</v>
       </c>
@@ -2142,7 +2150,7 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>6.2</v>
       </c>
@@ -2157,7 +2165,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>7</v>
       </c>
@@ -2172,7 +2180,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>7.1</v>
       </c>
@@ -2187,7 +2195,7 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>7.2</v>
       </c>
@@ -2202,7 +2210,7 @@
       </c>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>7.3</v>
       </c>
@@ -2217,7 +2225,7 @@
       </c>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>8</v>
       </c>
@@ -2232,7 +2240,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>8.1</v>
       </c>
@@ -2247,7 +2255,7 @@
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>8.1999999999999993</v>
       </c>
@@ -2262,7 +2270,7 @@
       </c>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>8.3000000000000007</v>
       </c>
@@ -2277,7 +2285,7 @@
       </c>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>8.4</v>
       </c>
@@ -2292,7 +2300,7 @@
       </c>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>8.5</v>
       </c>
@@ -2307,7 +2315,7 @@
       </c>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>8.6</v>
       </c>
@@ -2322,7 +2330,7 @@
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>9</v>
       </c>
@@ -2337,7 +2345,7 @@
       </c>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>9.1</v>
       </c>
@@ -2359,7 +2367,7 @@
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>9.1999999999999993</v>
       </c>
@@ -2381,7 +2389,7 @@
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
     </row>
-    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>10</v>
       </c>
@@ -2403,7 +2411,7 @@
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
     </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>10.1</v>
       </c>
@@ -2425,7 +2433,7 @@
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>10.199999999999999</v>
       </c>
@@ -2439,7 +2447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>10.3</v>
       </c>
@@ -2453,7 +2461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>10.4</v>
       </c>
@@ -2467,7 +2475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>10.5</v>
       </c>
@@ -2481,7 +2489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>10.6</v>
       </c>
@@ -2495,7 +2503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>11</v>
       </c>
@@ -2509,7 +2517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>11.2</v>
       </c>
@@ -2523,7 +2531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>12</v>
       </c>
@@ -2537,7 +2545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>12.1</v>
       </c>
@@ -2551,7 +2559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>13</v>
       </c>
@@ -2565,7 +2573,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" s="13"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
@@ -2575,7 +2583,7 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="13"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -2585,7 +2593,7 @@
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" s="13"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
@@ -2595,7 +2603,7 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="13"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
@@ -2605,7 +2613,7 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" s="13"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -2615,7 +2623,7 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="13"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
@@ -2625,7 +2633,7 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D58" s="13"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
@@ -2635,7 +2643,7 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D59" s="13"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -2645,7 +2653,7 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D60" s="13"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
@@ -2655,7 +2663,7 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D61" s="13"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
@@ -2665,7 +2673,7 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="13"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
@@ -2675,7 +2683,7 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="13"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -2685,7 +2693,7 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="13"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
@@ -2695,7 +2703,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" s="13"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -2705,7 +2713,7 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" s="13"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
@@ -2715,7 +2723,7 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D67" s="13"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
@@ -2725,7 +2733,7 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D84" s="13"/>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
@@ -2737,7 +2745,7 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D85" s="13"/>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -2747,7 +2755,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D86" s="13"/>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
@@ -2759,7 +2767,7 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D87" s="13"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
@@ -2771,7 +2779,7 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D88" s="13"/>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -2783,7 +2791,7 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D89" s="13"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -2795,7 +2803,7 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D90" s="13"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
@@ -2807,7 +2815,7 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D91" s="13"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
@@ -2819,7 +2827,7 @@
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D92" s="13"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -2831,7 +2839,7 @@
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D93" s="13"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
@@ -2843,7 +2851,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D94" s="13"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
@@ -2853,7 +2861,7 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D95" s="13"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -2863,7 +2871,7 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D96" s="13"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
@@ -2873,7 +2881,7 @@
       <c r="O96" s="11"/>
       <c r="P96" s="11"/>
     </row>
-    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D97" s="13"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
@@ -2883,7 +2891,7 @@
       <c r="O97" s="11"/>
       <c r="P97" s="11"/>
     </row>
-    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D98" s="13"/>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
@@ -2894,7 +2902,7 @@
       <c r="P98" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F101">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>

<commit_message>
fix poster prep dates
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FE0A44-D337-48DC-A048-526291481D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8585D976-3905-4978-95E1-FBC800E6B582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -268,12 +268,6 @@
     <t>Describing relationships (Q~C, Q~Q)</t>
   </si>
   <si>
-    <t>Quiz 04 (Due 09/23 )</t>
-  </si>
-  <si>
-    <t>[Poster prep Stage I](project.html) (Draft Due 9/17, PR 9/19, Final 9/21 )</t>
-  </si>
-  <si>
     <t>Quiz 05 (Due 09/30 )</t>
   </si>
   <si>
@@ -446,6 +440,12 @@
   </si>
   <si>
     <t>[HW03 Data Management](hw/03_data_management.html) (Due 9/15 ) PR removed due to illness</t>
+  </si>
+  <si>
+    <t>[Poster prep Stage I](project.html) (Draft Due 9/24, PR 9/26, Final 9/28 )</t>
+  </si>
+  <si>
+    <t>[[Quiz 04]](https://forms.gle/8tLFYadDErC9h7499) (Due 09/23 )</t>
   </si>
 </sst>
 </file>
@@ -1270,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1316,16 +1316,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E2" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>117</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1336,16 +1336,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1360,13 +1360,13 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F4" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="42" t="s">
         <v>125</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1377,46 +1377,46 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>127</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>4.3</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="40" t="s">
-        <v>77</v>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>124</v>
+        <v>5.2</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="40"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="40" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1427,14 +1427,14 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1445,13 +1445,13 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
       <c r="E10" s="40"/>
       <c r="F10" s="34"/>
       <c r="G10" s="40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1475,16 +1475,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1495,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1512,10 +1512,10 @@
         <v>62</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
       <c r="E14" s="40"/>
       <c r="F14" s="34"/>
       <c r="G14" s="40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1539,13 +1539,13 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1556,16 +1556,16 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1579,10 +1579,10 @@
         <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1593,7 +1593,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1618,10 +1618,10 @@
         <v>66</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1629,10 +1629,10 @@
         <v>15.2</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1659,7 +1659,7 @@
         <v>69</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1673,7 +1673,7 @@
         <v>15</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1684,7 +1684,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1800,10 +1800,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>1</v>
@@ -1874,10 +1874,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>1</v>
@@ -1914,7 +1914,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>10</v>
@@ -1946,7 +1946,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>11</v>
@@ -1967,7 +1967,7 @@
         <v>74</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
add link to lec04
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH615/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8538C3CE-30E9-42B3-AF07-32A423CC916B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7F7B7C-3250-4C43-959C-27CB7DA7BD45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
     <sheet name="points" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -38,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="129">
   <si>
     <t>Assignments</t>
   </si>
@@ -446,6 +438,9 @@
   </si>
   <si>
     <t>[HW05 Graphing Relationships](hw/05_bivariate_graphing_assignment.html) (Draft Due 9/27, PR 9/28, Final 9/29 )</t>
+  </si>
+  <si>
+    <t>[Lec04](https://hackmd.io/@norcalbiostat/math615_lec04)</t>
   </si>
 </sst>
 </file>
@@ -1271,21 +1266,21 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.875" style="2"/>
+    <col min="1" max="2" width="8.83203125" style="2"/>
     <col min="3" max="3" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="31.625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="25.125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="79.625" style="38" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="38"/>
+    <col min="4" max="4" width="31.6640625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="79.6640625" style="38" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -1328,7 +1323,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2.1</v>
       </c>
@@ -1338,7 +1333,7 @@
       <c r="D3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="8" t="s">
         <v>118</v>
       </c>
       <c r="F3" s="43" t="s">
@@ -1348,7 +1343,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3.1</v>
       </c>
@@ -1369,7 +1364,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -1389,7 +1384,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5.0999999999999996</v>
       </c>
@@ -1399,6 +1394,9 @@
       <c r="D6" s="38" t="s">
         <v>75</v>
       </c>
+      <c r="E6" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="F6" s="43" t="s">
         <v>126</v>
       </c>
@@ -1406,7 +1404,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5.2</v>
       </c>
@@ -1419,7 +1417,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6.1</v>
       </c>
@@ -1437,7 +1435,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7.1</v>
       </c>
@@ -1454,7 +1452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>7.3</v>
       </c>
@@ -1467,7 +1465,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>8.1</v>
       </c>
@@ -1487,7 +1485,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>9.1</v>
       </c>
@@ -1501,7 +1499,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>10.1</v>
       </c>
@@ -1518,7 +1516,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>10.199999999999999</v>
       </c>
@@ -1531,7 +1529,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>11.1</v>
       </c>
@@ -1548,7 +1546,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>12.1</v>
       </c>
@@ -1568,7 +1566,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>13.1</v>
       </c>
@@ -1585,7 +1583,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>13.2</v>
       </c>
@@ -1596,7 +1594,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>14.1</v>
       </c>
@@ -1607,7 +1605,7 @@
       <c r="F19" s="35"/>
       <c r="G19" s="41"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>15.1</v>
       </c>
@@ -1624,7 +1622,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>15.2</v>
       </c>
@@ -1635,7 +1633,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>15.3</v>
       </c>
@@ -1648,7 +1646,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>16.100000000000001</v>
       </c>
@@ -1662,7 +1660,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>17.100000000000001</v>
       </c>
@@ -1676,7 +1674,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>17.2</v>
       </c>
@@ -1688,7 +1686,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
+  <sortState ref="A2:G25">
     <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1704,23 +1702,23 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="12"/>
-    <col min="2" max="2" width="36.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="12"/>
-    <col min="7" max="7" width="5.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="12"/>
+    <col min="2" max="2" width="36.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="12"/>
+    <col min="7" max="7" width="5.1640625" style="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="11" customWidth="1"/>
     <col min="9" max="9" width="10" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.875" style="12"/>
-    <col min="11" max="11" width="4.625" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="11"/>
+    <col min="10" max="10" width="8.83203125" style="12"/>
+    <col min="11" max="11" width="4.6640625" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -1758,7 +1756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1792,7 +1790,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1.2</v>
       </c>
@@ -1832,7 +1830,7 @@
         <v>0.12698412698412698</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>1.3</v>
       </c>
@@ -1866,7 +1864,7 @@
         <v>0.31746031746031744</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1906,7 +1904,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>2.1</v>
       </c>
@@ -1938,7 +1936,7 @@
       </c>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -1959,7 +1957,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -1976,7 +1974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>3.1</v>
       </c>
@@ -1990,7 +1988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>3.1</v>
       </c>
@@ -2004,7 +2002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>3.2</v>
       </c>
@@ -2018,7 +2016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>4</v>
       </c>
@@ -2032,7 +2030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>4.2</v>
       </c>
@@ -2046,7 +2044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>4.3</v>
       </c>
@@ -2060,7 +2058,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -2074,7 +2072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>5</v>
       </c>
@@ -2088,7 +2086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>5.0999999999999996</v>
       </c>
@@ -2103,7 +2101,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>5.2</v>
       </c>
@@ -2118,7 +2116,7 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>6</v>
       </c>
@@ -2134,7 +2132,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>6.1</v>
       </c>
@@ -2150,7 +2148,7 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>6.2</v>
       </c>
@@ -2165,7 +2163,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>7</v>
       </c>
@@ -2180,7 +2178,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>7.1</v>
       </c>
@@ -2195,7 +2193,7 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>7.2</v>
       </c>
@@ -2210,7 +2208,7 @@
       </c>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <v>7.3</v>
       </c>
@@ -2225,7 +2223,7 @@
       </c>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>8</v>
       </c>
@@ -2240,7 +2238,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>8.1</v>
       </c>
@@ -2255,7 +2253,7 @@
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <v>8.1999999999999993</v>
       </c>
@@ -2270,7 +2268,7 @@
       </c>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>8.3000000000000007</v>
       </c>
@@ -2285,7 +2283,7 @@
       </c>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
         <v>8.4</v>
       </c>
@@ -2300,7 +2298,7 @@
       </c>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>8.5</v>
       </c>
@@ -2315,7 +2313,7 @@
       </c>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
         <v>8.6</v>
       </c>
@@ -2330,7 +2328,7 @@
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>9</v>
       </c>
@@ -2345,7 +2343,7 @@
       </c>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12">
         <v>9.1</v>
       </c>
@@ -2367,7 +2365,7 @@
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12">
         <v>9.1999999999999993</v>
       </c>
@@ -2389,7 +2387,7 @@
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
     </row>
-    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12">
         <v>10</v>
       </c>
@@ -2411,7 +2409,7 @@
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
     </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12">
         <v>10.1</v>
       </c>
@@ -2433,7 +2431,7 @@
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>10.199999999999999</v>
       </c>
@@ -2447,7 +2445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="12">
         <v>10.3</v>
       </c>
@@ -2461,7 +2459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="12">
         <v>10.4</v>
       </c>
@@ -2475,7 +2473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="12">
         <v>10.5</v>
       </c>
@@ -2489,7 +2487,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="12">
         <v>10.6</v>
       </c>
@@ -2503,7 +2501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
         <v>11</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="12">
         <v>11.2</v>
       </c>
@@ -2531,7 +2529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="12">
         <v>12</v>
       </c>
@@ -2545,7 +2543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="12">
         <v>12.1</v>
       </c>
@@ -2559,7 +2557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="12">
         <v>13</v>
       </c>
@@ -2573,7 +2571,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D52" s="13"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
@@ -2583,7 +2581,7 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D53" s="13"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -2593,7 +2591,7 @@
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D54" s="13"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
@@ -2603,7 +2601,7 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D55" s="13"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
@@ -2613,7 +2611,7 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D56" s="13"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -2623,7 +2621,7 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D57" s="13"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
@@ -2633,7 +2631,7 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D58" s="13"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
@@ -2643,7 +2641,7 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D59" s="13"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -2653,7 +2651,7 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D60" s="13"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
@@ -2663,7 +2661,7 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D61" s="13"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
@@ -2673,7 +2671,7 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D62" s="13"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
@@ -2683,7 +2681,7 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D63" s="13"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -2693,7 +2691,7 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D64" s="13"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
@@ -2703,7 +2701,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D65" s="13"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -2713,7 +2711,7 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D66" s="13"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
@@ -2723,7 +2721,7 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D67" s="13"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
@@ -2733,7 +2731,7 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D84" s="13"/>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
@@ -2745,7 +2743,7 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D85" s="13"/>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -2755,7 +2753,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D86" s="13"/>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
@@ -2767,7 +2765,7 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D87" s="13"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
@@ -2779,7 +2777,7 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D88" s="13"/>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -2791,7 +2789,7 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D89" s="13"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -2803,7 +2801,7 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D90" s="13"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
@@ -2815,7 +2813,7 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D91" s="13"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
@@ -2827,7 +2825,7 @@
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D92" s="13"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -2839,7 +2837,7 @@
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D93" s="13"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
@@ -2851,7 +2849,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D94" s="13"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
@@ -2861,7 +2859,7 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D95" s="13"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -2871,7 +2869,7 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D96" s="13"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
@@ -2881,7 +2879,7 @@
       <c r="O96" s="11"/>
       <c r="P96" s="11"/>
     </row>
-    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D97" s="13"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
@@ -2891,7 +2889,7 @@
       <c r="O97" s="11"/>
       <c r="P97" s="11"/>
     </row>
-    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D98" s="13"/>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
@@ -2902,7 +2900,7 @@
       <c r="P98" s="11"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
+  <sortState ref="A2:F101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>

<commit_message>
add wk7 lecture and hw files
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH615/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7F7B7C-3250-4C43-959C-27CB7DA7BD45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057F9DA7-C8CD-4BEA-B1E6-57635564F4B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="435" windowWidth="24765" windowHeight="14595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
     <sheet name="points" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -260,25 +268,13 @@
     <t>Describing relationships (Q~C, Q~Q)</t>
   </si>
   <si>
-    <t>[hw06 research proposal outline](hw/hw06_research_proposal_outline.html)(Draft Due 10/4, PR 10/5, Final 10/6 )</t>
-  </si>
-  <si>
     <t>Quiz 06 (Due 10/07 )</t>
   </si>
   <si>
     <t>Quiz 07 (Due 10/14 )</t>
   </si>
   <si>
-    <t>[hw07_foundations](hw/hw07_foundations.html) (Due 10/13 )</t>
-  </si>
-  <si>
-    <t>Poster prep Stage II* (Draft Due 10/08, PR 10/10, Final 10/12 )</t>
-  </si>
-  <si>
     <t>Quiz 08 (Due 10/21 )</t>
-  </si>
-  <si>
-    <t>[hw08_biv_inference](hw/hw08_biv_inference.html) (Draft Due 11/01, PR 11/02, Final 11/03 )</t>
   </si>
   <si>
     <t>Quiz 09 (Due 10/28 )</t>
@@ -358,24 +354,6 @@
   <si>
     <t>Describing distributions
 Describing relationships (C~C)</t>
-  </si>
-  <si>
-    <t>Writing about empirical research
-Probabilty Distributions
-Sampling distributions</t>
-  </si>
-  <si>
-    <t>Interval estimates
-Foundations for Inference</t>
-  </si>
-  <si>
-    <t>Hypothesis testing
-T-tests
-ANOVA</t>
-  </si>
-  <si>
-    <t>Chi-squared analysis
-Correlation analysis</t>
   </si>
   <si>
     <t>Moderation
@@ -441,6 +419,35 @@
   </si>
   <si>
     <t>[Lec04](https://hackmd.io/@norcalbiostat/math615_lec04)</t>
+  </si>
+  <si>
+    <t>Populations vs Samples
+Probabilty Distributions
+Quantifying Uncertainty</t>
+  </si>
+  <si>
+    <t>Hypothesis testing Foundations
+T-tests</t>
+  </si>
+  <si>
+    <t>ANOVA
+Chi-squared analysis</t>
+  </si>
+  <si>
+    <t>Correlation and Regression</t>
+  </si>
+  <si>
+    <t>[Bivariate Inference](hw/08_biv_inference.html) (Draft Due 10/25, PR 10/26, Final 10/27 )</t>
+  </si>
+  <si>
+    <t>[HW07 Foundations for Inference](hw/07_foundations.html) and  
+[Interval Estimation Activity](hw/activity_interval_estimation) (Due 10/13 )</t>
+  </si>
+  <si>
+    <t>[OpenIntro Statistics textbook Ch5](https://leanpub.com/openintro-statistics) or Dr. D's [Math 315 course notes Ch4](https://norcalbiostat.github.io/MATH315/reading/RAD_course_notes_f19.pdf).</t>
+  </si>
+  <si>
+    <t>[Poster prep Stage II](project.html) (Draft Due 10/08, PR 10/10, Final 10/12 )</t>
   </si>
 </sst>
 </file>
@@ -723,7 +730,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="81" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -841,6 +848,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1265,22 +1275,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="2"/>
+    <col min="1" max="2" width="8.875" style="2"/>
     <col min="3" max="3" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="38" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="79.6640625" style="38" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="38"/>
+    <col min="4" max="4" width="31.625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="25.125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="79.625" style="38" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1303,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -1311,19 +1321,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E2" s="38" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2.1</v>
       </c>
@@ -1331,19 +1341,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3.1</v>
       </c>
@@ -1355,16 +1365,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -1372,19 +1382,19 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5.0999999999999996</v>
       </c>
@@ -1395,16 +1405,16 @@
         <v>75</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5.2</v>
       </c>
@@ -1414,10 +1424,10 @@
       <c r="E7" s="40"/>
       <c r="F7" s="34"/>
       <c r="G7" s="40" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6.1</v>
       </c>
@@ -1425,17 +1435,19 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>121</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>127</v>
+      </c>
       <c r="F8" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="39" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="G8" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7.1</v>
       </c>
@@ -1443,16 +1455,14 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7.3</v>
       </c>
@@ -1462,10 +1472,10 @@
       <c r="E10" s="40"/>
       <c r="F10" s="34"/>
       <c r="G10" s="40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8.1</v>
       </c>
@@ -1473,19 +1483,19 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9.1</v>
       </c>
@@ -1493,13 +1503,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10.1</v>
       </c>
@@ -1510,13 +1520,13 @@
         <v>62</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>10.199999999999999</v>
       </c>
@@ -1526,10 +1536,10 @@
       <c r="E14" s="40"/>
       <c r="F14" s="34"/>
       <c r="G14" s="40" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>11.1</v>
       </c>
@@ -1537,16 +1547,16 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>12.1</v>
       </c>
@@ -1554,19 +1564,19 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>13.1</v>
       </c>
@@ -1577,13 +1587,13 @@
         <v>64</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>13.2</v>
       </c>
@@ -1591,10 +1601,10 @@
         <v>16</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>14.1</v>
       </c>
@@ -1605,7 +1615,7 @@
       <c r="F19" s="35"/>
       <c r="G19" s="41"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>15.1</v>
       </c>
@@ -1616,24 +1626,24 @@
         <v>66</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>15.2</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>15.3</v>
       </c>
@@ -1646,7 +1656,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>16.100000000000001</v>
       </c>
@@ -1657,10 +1667,10 @@
         <v>69</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>17.100000000000001</v>
       </c>
@@ -1671,10 +1681,10 @@
         <v>15</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>17.2</v>
       </c>
@@ -1682,11 +1692,11 @@
         <v>8</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
     <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1702,23 +1712,23 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="12"/>
-    <col min="2" max="2" width="36.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="12"/>
-    <col min="7" max="7" width="5.1640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="12"/>
+    <col min="2" max="2" width="36.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="12"/>
+    <col min="7" max="7" width="5.125" style="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="11" customWidth="1"/>
     <col min="9" max="9" width="10" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="12"/>
-    <col min="11" max="11" width="4.6640625" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="11"/>
+    <col min="10" max="10" width="8.875" style="12"/>
+    <col min="11" max="11" width="4.625" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -1756,7 +1766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1790,7 +1800,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1.2</v>
       </c>
@@ -1798,10 +1808,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>1</v>
@@ -1830,7 +1840,7 @@
         <v>0.12698412698412698</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1.3</v>
       </c>
@@ -1864,7 +1874,7 @@
         <v>0.31746031746031744</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1872,10 +1882,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>1</v>
@@ -1904,7 +1914,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2.1</v>
       </c>
@@ -1912,7 +1922,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>10</v>
@@ -1936,7 +1946,7 @@
       </c>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -1944,7 +1954,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>11</v>
@@ -1957,7 +1967,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -1965,7 +1975,7 @@
         <v>74</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>1</v>
@@ -1974,7 +1984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>3.1</v>
       </c>
@@ -1988,7 +1998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>3.1</v>
       </c>
@@ -2002,7 +2012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>3.2</v>
       </c>
@@ -2016,7 +2026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>4</v>
       </c>
@@ -2030,7 +2040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>4.2</v>
       </c>
@@ -2044,7 +2054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>4.3</v>
       </c>
@@ -2058,7 +2068,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -2072,7 +2082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>5</v>
       </c>
@@ -2086,7 +2096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>5.0999999999999996</v>
       </c>
@@ -2101,7 +2111,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>5.2</v>
       </c>
@@ -2116,7 +2126,7 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>6</v>
       </c>
@@ -2132,7 +2142,7 @@
       </c>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>6.1</v>
       </c>
@@ -2148,7 +2158,7 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>6.2</v>
       </c>
@@ -2163,7 +2173,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>7</v>
       </c>
@@ -2178,7 +2188,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>7.1</v>
       </c>
@@ -2193,7 +2203,7 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>7.2</v>
       </c>
@@ -2208,7 +2218,7 @@
       </c>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>7.3</v>
       </c>
@@ -2223,7 +2233,7 @@
       </c>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>8</v>
       </c>
@@ -2238,7 +2248,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>8.1</v>
       </c>
@@ -2253,7 +2263,7 @@
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>8.1999999999999993</v>
       </c>
@@ -2268,7 +2278,7 @@
       </c>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>8.3000000000000007</v>
       </c>
@@ -2283,7 +2293,7 @@
       </c>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>8.4</v>
       </c>
@@ -2298,7 +2308,7 @@
       </c>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>8.5</v>
       </c>
@@ -2313,7 +2323,7 @@
       </c>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>8.6</v>
       </c>
@@ -2328,7 +2338,7 @@
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>9</v>
       </c>
@@ -2343,7 +2353,7 @@
       </c>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>9.1</v>
       </c>
@@ -2365,7 +2375,7 @@
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>9.1999999999999993</v>
       </c>
@@ -2387,7 +2397,7 @@
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
     </row>
-    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>10</v>
       </c>
@@ -2409,7 +2419,7 @@
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
     </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>10.1</v>
       </c>
@@ -2431,7 +2441,7 @@
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>10.199999999999999</v>
       </c>
@@ -2445,7 +2455,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>10.3</v>
       </c>
@@ -2459,7 +2469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>10.4</v>
       </c>
@@ -2473,7 +2483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>10.5</v>
       </c>
@@ -2487,7 +2497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>10.6</v>
       </c>
@@ -2501,7 +2511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>11</v>
       </c>
@@ -2515,7 +2525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>11.2</v>
       </c>
@@ -2529,7 +2539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>12</v>
       </c>
@@ -2543,7 +2553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>12.1</v>
       </c>
@@ -2557,7 +2567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>13</v>
       </c>
@@ -2571,7 +2581,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" s="13"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
@@ -2581,7 +2591,7 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="13"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -2591,7 +2601,7 @@
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" s="13"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
@@ -2601,7 +2611,7 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="13"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
@@ -2611,7 +2621,7 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" s="13"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -2621,7 +2631,7 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="13"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
@@ -2631,7 +2641,7 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D58" s="13"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
@@ -2641,7 +2651,7 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D59" s="13"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -2651,7 +2661,7 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D60" s="13"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
@@ -2661,7 +2671,7 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D61" s="13"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
@@ -2671,7 +2681,7 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="13"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
@@ -2681,7 +2691,7 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="13"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -2691,7 +2701,7 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="13"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
@@ -2701,7 +2711,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" s="13"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -2711,7 +2721,7 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" s="13"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
@@ -2721,7 +2731,7 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D67" s="13"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
@@ -2731,7 +2741,7 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D84" s="13"/>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
@@ -2743,7 +2753,7 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D85" s="13"/>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -2753,7 +2763,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D86" s="13"/>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
@@ -2765,7 +2775,7 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D87" s="13"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
@@ -2777,7 +2787,7 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D88" s="13"/>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -2789,7 +2799,7 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D89" s="13"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -2801,7 +2811,7 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D90" s="13"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
@@ -2813,7 +2823,7 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D91" s="13"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
@@ -2825,7 +2835,7 @@
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D92" s="13"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -2837,7 +2847,7 @@
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D93" s="13"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
@@ -2849,7 +2859,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D94" s="13"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
@@ -2859,7 +2869,7 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D95" s="13"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -2869,7 +2879,7 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D96" s="13"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
@@ -2879,7 +2889,7 @@
       <c r="O96" s="11"/>
       <c r="P96" s="11"/>
     </row>
-    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D97" s="13"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
@@ -2889,7 +2899,7 @@
       <c r="O97" s="11"/>
       <c r="P97" s="11"/>
     </row>
-    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D98" s="13"/>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
@@ -2900,7 +2910,7 @@
       <c r="P98" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F101">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>

<commit_message>
add hw9 and wk11
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/MATH615/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419A6FDA-E3ED-41EA-A7BA-607C99C3F47B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2728FCD1-7D82-894E-B406-63540BAE8271}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
     <sheet name="points" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -38,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="131">
   <si>
     <t>Assignments</t>
   </si>
@@ -244,9 +236,6 @@
     <t>Poster prep Stage IV* (Draft Due 12/03, PR 12/05, Final 12/07 )</t>
   </si>
   <si>
-    <t>Develop Research Poster</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -275,9 +264,6 @@
   </si>
   <si>
     <t>e-Poster*  (Draft Due 12/13 , PR 12/15, Final 12/19 10am )</t>
-  </si>
-  <si>
-    <t>Thursday 12/19, 10-12 noon.  I'll bring snacks!</t>
   </si>
   <si>
     <t>What to watch out for</t>
@@ -306,11 +292,6 @@
   <si>
     <t>Describing distributions
 Describing relationships (C~C)</t>
-  </si>
-  <si>
-    <t>Moderation
-Study Design
-Causation</t>
   </si>
   <si>
     <t>Multiple Regression analysis
@@ -406,9 +387,6 @@
 PMA5 Ch 5 [Lec08](https://hackmd.io/@norcalbiostat/math615_lec08)</t>
   </si>
   <si>
-    <t>[hw09_moderation](hw/hw09_moderation.html) (Draft Due 11/07, PR 11/09, Final 11/11 )</t>
-  </si>
-  <si>
     <t>[HW08 Bivariate Inference](hw/08_bivariate_inference.html) (Draft Due 10/31, PR 11/02, Final 11/04 )</t>
   </si>
   <si>
@@ -456,6 +434,23 @@
   <si>
     <t>PMA5 Ch 7
 ASCN Ch 9</t>
+  </si>
+  <si>
+    <t>[HW 09 Moderation](hw/09_moderation.html) (Draft Due 11/07, PR 11/09, Final 11/11 )</t>
+  </si>
+  <si>
+    <t>ASCN 9.2, 9.3</t>
+  </si>
+  <si>
+    <t>Develop Research Poster
+Study Design &amp; Causation</t>
+  </si>
+  <si>
+    <t>Thursday 12/19, 10-12 noon. THMA 116  I'll bring snacks!</t>
+  </si>
+  <si>
+    <t>Stratification
+Moderation</t>
   </si>
 </sst>
 </file>
@@ -1284,21 +1279,21 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.875" style="2"/>
+    <col min="1" max="2" width="8.83203125" style="2"/>
     <col min="3" max="3" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="31.625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="25.125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="79.625" style="38" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="38"/>
+    <col min="4" max="4" width="31.6640625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="38" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="79.6640625" style="38" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1312,7 +1307,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="33" t="s">
         <v>11</v>
@@ -1321,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -1329,19 +1324,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2.1</v>
       </c>
@@ -1349,19 +1344,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3.1</v>
       </c>
@@ -1373,16 +1368,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -1390,19 +1385,19 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5.0999999999999996</v>
       </c>
@@ -1410,19 +1405,19 @@
         <v>5</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5.2</v>
       </c>
@@ -1432,10 +1427,10 @@
       <c r="E7" s="40"/>
       <c r="F7" s="34"/>
       <c r="G7" s="40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6.1</v>
       </c>
@@ -1443,19 +1438,19 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>109</v>
-      </c>
       <c r="G8" s="44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7.1</v>
       </c>
@@ -1463,17 +1458,17 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G9" s="42"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>7.3</v>
       </c>
@@ -1483,10 +1478,10 @@
       <c r="E10" s="40"/>
       <c r="F10" s="34"/>
       <c r="G10" s="40" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>8.1</v>
       </c>
@@ -1494,17 +1489,17 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F11" s="43"/>
       <c r="G11" s="38" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>9.1</v>
       </c>
@@ -1512,16 +1507,16 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F12" s="43" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>10.1</v>
       </c>
@@ -1529,16 +1524,16 @@
         <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>10.199999999999999</v>
       </c>
@@ -1548,10 +1543,10 @@
       <c r="E14" s="40"/>
       <c r="F14" s="34"/>
       <c r="G14" s="40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>11.1</v>
       </c>
@@ -1559,16 +1554,19 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>88</v>
+        <v>130</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>127</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>12.1</v>
       </c>
@@ -1576,19 +1574,19 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>13.1</v>
       </c>
@@ -1599,13 +1597,13 @@
         <v>63</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>13.2</v>
       </c>
@@ -1613,10 +1611,10 @@
         <v>16</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>14.1</v>
       </c>
@@ -1627,7 +1625,7 @@
       <c r="F19" s="35"/>
       <c r="G19" s="41"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>15.1</v>
       </c>
@@ -1638,24 +1636,24 @@
         <v>65</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F20" s="36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>15.2</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>15.3</v>
       </c>
@@ -1668,21 +1666,21 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>16.100000000000001</v>
       </c>
       <c r="B23" s="2">
         <v>15</v>
       </c>
-      <c r="D23" s="38" t="s">
-        <v>68</v>
+      <c r="D23" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>17.100000000000001</v>
       </c>
@@ -1693,10 +1691,10 @@
         <v>15</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>17.2</v>
       </c>
@@ -1704,11 +1702,11 @@
         <v>8</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
+  <sortState ref="A2:G25">
     <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1724,23 +1722,23 @@
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="12"/>
-    <col min="2" max="2" width="36.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="12"/>
-    <col min="7" max="7" width="5.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="12"/>
+    <col min="2" max="2" width="36.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="12"/>
+    <col min="7" max="7" width="5.1640625" style="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="11" customWidth="1"/>
     <col min="9" max="9" width="10" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.875" style="12"/>
-    <col min="11" max="11" width="4.625" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="11"/>
+    <col min="10" max="10" width="8.83203125" style="12"/>
+    <col min="11" max="11" width="4.6640625" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1812,7 +1810,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1.2</v>
       </c>
@@ -1820,10 +1818,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>1</v>
@@ -1852,7 +1850,7 @@
         <v>0.12698412698412698</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>1.3</v>
       </c>
@@ -1886,7 +1884,7 @@
         <v>0.31746031746031744</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1894,10 +1892,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>1</v>
@@ -1926,7 +1924,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>2.1</v>
       </c>
@@ -1934,7 +1932,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>10</v>
@@ -1958,7 +1956,7 @@
       </c>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -1966,7 +1964,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>11</v>
@@ -1979,15 +1977,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>3</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>1</v>
@@ -1996,7 +1994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>3.1</v>
       </c>
@@ -2010,7 +2008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>3.1</v>
       </c>
@@ -2024,7 +2022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>3.2</v>
       </c>
@@ -2038,7 +2036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>4</v>
       </c>
@@ -2052,7 +2050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>4.2</v>
       </c>
@@ -2066,7 +2064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>4.3</v>
       </c>
@@ -2080,7 +2078,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -2094,7 +2092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>5</v>
       </c>
@@ -2108,7 +2106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>5.0999999999999996</v>
       </c>
@@ -2123,7 +2121,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>5.2</v>
       </c>
@@ -2138,12 +2136,12 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>6</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="18" t="s">
@@ -2152,7 +2150,7 @@
       <c r="F19" s="18"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>6.1</v>
       </c>
@@ -2168,7 +2166,7 @@
       </c>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>6.2</v>
       </c>
@@ -2183,12 +2181,12 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>7</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>1</v>
@@ -2198,7 +2196,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>7.1</v>
       </c>
@@ -2213,7 +2211,7 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>7.2</v>
       </c>
@@ -2228,7 +2226,7 @@
       </c>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <v>7.3</v>
       </c>
@@ -2243,7 +2241,7 @@
       </c>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>8</v>
       </c>
@@ -2258,7 +2256,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>8.1</v>
       </c>
@@ -2273,7 +2271,7 @@
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <v>8.1999999999999993</v>
       </c>
@@ -2288,7 +2286,7 @@
       </c>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>8.3000000000000007</v>
       </c>
@@ -2303,7 +2301,7 @@
       </c>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
         <v>8.4</v>
       </c>
@@ -2318,7 +2316,7 @@
       </c>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>8.5</v>
       </c>
@@ -2333,7 +2331,7 @@
       </c>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
         <v>8.6</v>
       </c>
@@ -2348,7 +2346,7 @@
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>9</v>
       </c>
@@ -2363,7 +2361,7 @@
       </c>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12">
         <v>9.1</v>
       </c>
@@ -2385,7 +2383,7 @@
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="12">
         <v>9.1999999999999993</v>
       </c>
@@ -2407,7 +2405,7 @@
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
     </row>
-    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="12">
         <v>10</v>
       </c>
@@ -2429,7 +2427,7 @@
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
     </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12">
         <v>10.1</v>
       </c>
@@ -2451,7 +2449,7 @@
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>10.199999999999999</v>
       </c>
@@ -2465,7 +2463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="12">
         <v>10.3</v>
       </c>
@@ -2479,12 +2477,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="12">
         <v>10.4</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E40" s="31" t="s">
         <v>11</v>
@@ -2493,7 +2491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="12">
         <v>10.5</v>
       </c>
@@ -2507,7 +2505,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="12">
         <v>10.6</v>
       </c>
@@ -2521,7 +2519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
         <v>11</v>
       </c>
@@ -2535,7 +2533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="12">
         <v>11.2</v>
       </c>
@@ -2549,7 +2547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="12">
         <v>12</v>
       </c>
@@ -2563,7 +2561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="12">
         <v>12.1</v>
       </c>
@@ -2577,7 +2575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="12">
         <v>13</v>
       </c>
@@ -2591,7 +2589,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D52" s="13"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
@@ -2601,7 +2599,7 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D53" s="13"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -2611,7 +2609,7 @@
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D54" s="13"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
@@ -2621,7 +2619,7 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D55" s="13"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
@@ -2631,7 +2629,7 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D56" s="13"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -2641,7 +2639,7 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D57" s="13"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
@@ -2651,7 +2649,7 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D58" s="13"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
@@ -2661,7 +2659,7 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D59" s="13"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -2671,7 +2669,7 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D60" s="13"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
@@ -2681,7 +2679,7 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D61" s="13"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
@@ -2691,7 +2689,7 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D62" s="13"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
@@ -2701,7 +2699,7 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D63" s="13"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -2711,7 +2709,7 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D64" s="13"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
@@ -2721,7 +2719,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D65" s="13"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -2731,7 +2729,7 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D66" s="13"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
@@ -2741,7 +2739,7 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D67" s="13"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
@@ -2751,7 +2749,7 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D84" s="13"/>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
@@ -2763,7 +2761,7 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D85" s="13"/>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -2773,7 +2771,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D86" s="13"/>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
@@ -2785,7 +2783,7 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D87" s="13"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
@@ -2797,7 +2795,7 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D88" s="13"/>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -2809,7 +2807,7 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D89" s="13"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -2821,7 +2819,7 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D90" s="13"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
@@ -2833,7 +2831,7 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D91" s="13"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
@@ -2845,7 +2843,7 @@
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D92" s="13"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -2857,7 +2855,7 @@
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D93" s="13"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
@@ -2869,7 +2867,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D94" s="13"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
@@ -2879,7 +2877,7 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D95" s="13"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -2889,7 +2887,7 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D96" s="13"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
@@ -2899,7 +2897,7 @@
       <c r="O96" s="11"/>
       <c r="P96" s="11"/>
     </row>
-    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D97" s="13"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
@@ -2909,7 +2907,7 @@
       <c r="O97" s="11"/>
       <c r="P97" s="11"/>
     </row>
-    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D98" s="13"/>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
@@ -2920,7 +2918,7 @@
       <c r="P98" s="11"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
+  <sortState ref="A2:F101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>

</xml_diff>

<commit_message>
change pts for 615
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A419A7D-F94F-4AD8-8D89-16A181A57C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="1005" windowWidth="22590" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
     <sheet name="points" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
@@ -30,9 +27,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -463,7 +457,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
@@ -940,11 +934,11 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 2" xfId="51"/>
+    <cellStyle name="Normal 3" xfId="79"/>
     <cellStyle name="Percent" xfId="82" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Percent 3" xfId="80" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Percent 2" xfId="52"/>
+    <cellStyle name="Percent 3" xfId="80"/>
     <cellStyle name="Total" xfId="78" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1281,25 +1275,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B12" zoomScale="110" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="8.875" style="2"/>
+    <col min="1" max="2" width="8.83203125" style="2"/>
     <col min="3" max="3" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="31.625" style="37" customWidth="1"/>
-    <col min="5" max="5" width="25.125" style="37" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="79.625" style="37" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="37"/>
+    <col min="4" max="4" width="31.6640625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="79.6640625" style="37" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1322,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="63">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -1342,7 +1336,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="173.25">
       <c r="A3" s="6">
         <v>2.1</v>
       </c>
@@ -1362,7 +1356,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="7">
         <v>3.1</v>
       </c>
@@ -1383,7 +1377,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="31.5">
       <c r="A5" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -1403,7 +1397,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="47.25">
       <c r="A6" s="6">
         <v>5.0999999999999996</v>
       </c>
@@ -1423,7 +1417,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="6">
         <v>5.2</v>
       </c>
@@ -1436,7 +1430,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="173.25">
       <c r="A8" s="6">
         <v>6.1</v>
       </c>
@@ -1456,7 +1450,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="47.25">
       <c r="A9" s="6">
         <v>7.1</v>
       </c>
@@ -1474,7 +1468,7 @@
       </c>
       <c r="G9" s="40"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="6">
         <v>7.3</v>
       </c>
@@ -1487,7 +1481,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="126">
       <c r="A11" s="6">
         <v>8.1</v>
       </c>
@@ -1505,7 +1499,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="31.5">
       <c r="A12" s="6">
         <v>9.1</v>
       </c>
@@ -1522,7 +1516,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="31.5">
       <c r="A13" s="6">
         <v>10.1</v>
       </c>
@@ -1539,7 +1533,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="6">
         <v>10.199999999999999</v>
       </c>
@@ -1552,7 +1546,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="31.5">
       <c r="A15" s="6">
         <v>11.1</v>
       </c>
@@ -1572,7 +1566,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="31.5">
       <c r="A16" s="6">
         <v>12.1</v>
       </c>
@@ -1592,7 +1586,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="31.5">
       <c r="A17" s="6">
         <v>13.1</v>
       </c>
@@ -1609,7 +1603,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="31.5">
       <c r="A18" s="6">
         <v>13.2</v>
       </c>
@@ -1620,7 +1614,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="6">
         <v>14.1</v>
       </c>
@@ -1631,7 +1625,7 @@
       <c r="F19" s="35"/>
       <c r="G19" s="39"/>
     </row>
-    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="31.5">
       <c r="A20" s="6">
         <v>15.1</v>
       </c>
@@ -1645,7 +1639,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="6">
         <v>15.2</v>
       </c>
@@ -1656,7 +1650,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="6">
         <v>15.3</v>
       </c>
@@ -1669,7 +1663,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="31.5">
       <c r="A23" s="6">
         <v>16.100000000000001</v>
       </c>
@@ -1683,7 +1677,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="6">
         <v>17.100000000000001</v>
       </c>
@@ -1697,7 +1691,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="6">
         <v>17.2</v>
       </c>
@@ -1709,39 +1703,44 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
+  <sortState ref="A2:G25">
     <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="12"/>
-    <col min="2" max="2" width="36.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="12"/>
-    <col min="7" max="7" width="5.125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="12"/>
+    <col min="2" max="2" width="36.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="12"/>
+    <col min="7" max="7" width="5.1640625" style="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="11" customWidth="1"/>
     <col min="9" max="9" width="10" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.875" style="12"/>
-    <col min="11" max="11" width="4.625" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="11"/>
+    <col min="10" max="10" width="8.83203125" style="12"/>
+    <col min="11" max="11" width="4.6640625" style="12" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="18" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="16.5" thickTop="1">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1801,7 +1800,7 @@
       </c>
       <c r="J2" s="17">
         <f>I2/$I$7</f>
-        <v>0.18367346938775511</v>
+        <v>0.19148936170212766</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>1</v>
@@ -1813,7 +1812,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="12">
         <v>1.2</v>
       </c>
@@ -1837,11 +1836,11 @@
       </c>
       <c r="I3" s="14">
         <f>SUMIF($E$2:$E$89,H3,$F$2:$F$89)</f>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="J3" s="20">
         <f>I3/$I$7</f>
-        <v>0.16326530612244897</v>
+        <v>0.1276595744680851</v>
       </c>
       <c r="N3" s="19" t="s">
         <v>10</v>
@@ -1853,7 +1852,7 @@
         <v>0.12698412698412698</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="12">
         <v>1.3</v>
       </c>
@@ -1875,7 +1874,7 @@
       </c>
       <c r="J4" s="24">
         <f>I4/$I$7</f>
-        <v>0.20408163265306123</v>
+        <v>0.21276595744680851</v>
       </c>
       <c r="N4" s="22" t="s">
         <v>6</v>
@@ -1887,7 +1886,7 @@
         <v>0.31746031746031744</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1915,7 +1914,7 @@
       </c>
       <c r="J5" s="32">
         <f>I5/$I$7</f>
-        <v>0.24489795918367346</v>
+        <v>0.25531914893617019</v>
       </c>
       <c r="N5" s="25" t="s">
         <v>7</v>
@@ -1927,7 +1926,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
       <c r="A6" s="12">
         <v>2.1</v>
       </c>
@@ -1952,14 +1951,14 @@
       </c>
       <c r="J6" s="26">
         <f>I6/$I$7</f>
-        <v>0.20408163265306123</v>
+        <v>0.21276595744680851</v>
       </c>
       <c r="O6" s="27">
         <v>315</v>
       </c>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="17.25" thickTop="1" thickBot="1">
       <c r="A7" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -1977,10 +1976,10 @@
       </c>
       <c r="I7" s="27">
         <f>SUM(I2:I6)</f>
-        <v>490</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16.5" thickTop="1">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="12">
         <v>3.1</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="12">
         <v>3.1</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="12">
         <v>3.2</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="12">
         <v>4</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="12">
         <v>4.2</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="12">
         <v>4.3</v>
       </c>
@@ -2081,7 +2080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="12">
         <v>4.4000000000000004</v>
       </c>
@@ -2092,10 +2091,10 @@
         <v>10</v>
       </c>
       <c r="F15" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="12">
         <v>5</v>
       </c>
@@ -2109,7 +2108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="12">
         <v>5.0999999999999996</v>
       </c>
@@ -2124,7 +2123,7 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="12">
         <v>5.2</v>
       </c>
@@ -2139,7 +2138,7 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="12">
         <v>6</v>
       </c>
@@ -2153,7 +2152,7 @@
       <c r="F19" s="18"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="12">
         <v>6.1</v>
       </c>
@@ -2164,12 +2163,10 @@
       <c r="E20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="14">
-        <v>4</v>
-      </c>
+      <c r="F20" s="14"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="12">
         <v>6.2</v>
       </c>
@@ -2184,7 +2181,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="12">
         <v>7</v>
       </c>
@@ -2199,7 +2196,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="12">
         <v>7.1</v>
       </c>
@@ -2214,7 +2211,7 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="12">
         <v>7.2</v>
       </c>
@@ -2225,11 +2222,11 @@
         <v>10</v>
       </c>
       <c r="F24" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="12">
         <v>7.3</v>
       </c>
@@ -2244,7 +2241,7 @@
       </c>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="12">
         <v>8</v>
       </c>
@@ -2259,7 +2256,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="12">
         <v>8.1</v>
       </c>
@@ -2274,7 +2271,7 @@
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="12">
         <v>8.1999999999999993</v>
       </c>
@@ -2289,7 +2286,7 @@
       </c>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="12">
         <v>8.3000000000000007</v>
       </c>
@@ -2304,7 +2301,7 @@
       </c>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="12">
         <v>8.4</v>
       </c>
@@ -2319,7 +2316,7 @@
       </c>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="12">
         <v>8.5</v>
       </c>
@@ -2334,7 +2331,7 @@
       </c>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="12">
         <v>8.6</v>
       </c>
@@ -2345,11 +2342,11 @@
         <v>10</v>
       </c>
       <c r="F32" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" s="12">
         <v>9</v>
       </c>
@@ -2364,7 +2361,7 @@
       </c>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="12" customFormat="1">
       <c r="A34" s="12">
         <v>9.1</v>
       </c>
@@ -2386,7 +2383,7 @@
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
     </row>
-    <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="12" customFormat="1">
       <c r="A35" s="12">
         <v>9.1999999999999993</v>
       </c>
@@ -2408,7 +2405,7 @@
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
     </row>
-    <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="12" customFormat="1">
       <c r="A36" s="12">
         <v>10</v>
       </c>
@@ -2430,7 +2427,7 @@
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
     </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="12" customFormat="1">
       <c r="A37" s="12">
         <v>10.1</v>
       </c>
@@ -2452,7 +2449,7 @@
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="12">
         <v>10.199999999999999</v>
       </c>
@@ -2466,7 +2463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" s="12">
         <v>10.3</v>
       </c>
@@ -2480,7 +2477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" s="12">
         <v>10.4</v>
       </c>
@@ -2490,7 +2487,7 @@
       <c r="E40" s="31"/>
       <c r="F40" s="31"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" s="12">
         <v>10.5</v>
       </c>
@@ -2504,7 +2501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" s="12">
         <v>10.6</v>
       </c>
@@ -2515,10 +2512,10 @@
         <v>10</v>
       </c>
       <c r="F42" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" s="12">
         <v>11</v>
       </c>
@@ -2532,7 +2529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="A44" s="12">
         <v>11.2</v>
       </c>
@@ -2546,7 +2543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="A45" s="12">
         <v>12</v>
       </c>
@@ -2560,7 +2557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="A46" s="12">
         <v>12.1</v>
       </c>
@@ -2574,7 +2571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="A47" s="12">
         <v>13</v>
       </c>
@@ -2588,7 +2585,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:16" s="12" customFormat="1">
       <c r="D52" s="13"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
@@ -2598,7 +2595,7 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:16" s="12" customFormat="1">
       <c r="D53" s="13"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
@@ -2608,7 +2605,7 @@
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:16" s="12" customFormat="1">
       <c r="D54" s="13"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
@@ -2618,7 +2615,7 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:16" s="12" customFormat="1">
       <c r="D55" s="13"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
@@ -2628,7 +2625,7 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:16" s="12" customFormat="1">
       <c r="D56" s="13"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
@@ -2638,7 +2635,7 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:16" s="12" customFormat="1">
       <c r="D57" s="13"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
@@ -2648,7 +2645,7 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:16" s="12" customFormat="1">
       <c r="D58" s="13"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
@@ -2658,7 +2655,7 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:16" s="12" customFormat="1">
       <c r="D59" s="13"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
@@ -2668,7 +2665,7 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:16" s="12" customFormat="1">
       <c r="D60" s="13"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
@@ -2678,7 +2675,7 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:16" s="12" customFormat="1">
       <c r="D61" s="13"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
@@ -2688,7 +2685,7 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:16" s="12" customFormat="1">
       <c r="D62" s="13"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
@@ -2698,7 +2695,7 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:16" s="12" customFormat="1">
       <c r="D63" s="13"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
@@ -2708,7 +2705,7 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:16" s="12" customFormat="1">
       <c r="D64" s="13"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
@@ -2718,7 +2715,7 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:16" s="12" customFormat="1">
       <c r="D65" s="13"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
@@ -2728,7 +2725,7 @@
       <c r="O65" s="11"/>
       <c r="P65" s="11"/>
     </row>
-    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:16" s="12" customFormat="1">
       <c r="D66" s="13"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
@@ -2738,7 +2735,7 @@
       <c r="O66" s="11"/>
       <c r="P66" s="11"/>
     </row>
-    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:16" s="12" customFormat="1">
       <c r="D67" s="13"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
@@ -2748,7 +2745,7 @@
       <c r="O67" s="11"/>
       <c r="P67" s="11"/>
     </row>
-    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:16" s="12" customFormat="1">
       <c r="D84" s="13"/>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
@@ -2760,7 +2757,7 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:16" s="12" customFormat="1">
       <c r="D85" s="13"/>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
@@ -2770,7 +2767,7 @@
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:16" s="12" customFormat="1">
       <c r="D86" s="13"/>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
@@ -2782,7 +2779,7 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:16" s="12" customFormat="1">
       <c r="D87" s="13"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
@@ -2794,7 +2791,7 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:16" s="12" customFormat="1">
       <c r="D88" s="13"/>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
@@ -2806,7 +2803,7 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:16" s="12" customFormat="1">
       <c r="D89" s="13"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
@@ -2818,7 +2815,7 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:16" s="12" customFormat="1">
       <c r="D90" s="13"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
@@ -2830,7 +2827,7 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:16" s="12" customFormat="1">
       <c r="D91" s="13"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
@@ -2842,7 +2839,7 @@
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:16" s="12" customFormat="1">
       <c r="D92" s="13"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
@@ -2854,7 +2851,7 @@
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:16" s="12" customFormat="1">
       <c r="D93" s="13"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
@@ -2866,7 +2863,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:16" s="12" customFormat="1">
       <c r="D94" s="13"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
@@ -2876,7 +2873,7 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:16" s="12" customFormat="1">
       <c r="D95" s="13"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
@@ -2886,7 +2883,7 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:16" s="12" customFormat="1">
       <c r="D96" s="13"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
@@ -2896,7 +2893,7 @@
       <c r="O96" s="11"/>
       <c r="P96" s="11"/>
     </row>
-    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:16" s="12" customFormat="1">
       <c r="D97" s="13"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
@@ -2906,7 +2903,7 @@
       <c r="O97" s="11"/>
       <c r="P97" s="11"/>
     </row>
-    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:16" s="12" customFormat="1">
       <c r="D98" s="13"/>
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
@@ -2917,11 +2914,16 @@
       <c r="P98" s="11"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
+  <sortState ref="A2:F101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
start refresh for F22
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CE4B76-C117-4E8F-A85D-EAD18C73FD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866A44AD-7150-4D01-A0DF-F1F5D8343D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31215" yWindow="1200" windowWidth="22590" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
   <si>
     <t>Assignments</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>Take home final exam (Due 12/20 )</t>
+  </si>
+  <si>
+    <t>EC</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D12" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -1721,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1804,7 @@
       </c>
       <c r="J2" s="17">
         <f>I2/$I$7</f>
-        <v>0.19148936170212766</v>
+        <v>0.19823788546255505</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>1</v>
@@ -1837,11 +1840,11 @@
       </c>
       <c r="I3" s="14">
         <f>SUMIF($E$2:$E$89,H3,$F$2:$F$89)</f>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="J3" s="20">
         <f>I3/$I$7</f>
-        <v>0.1702127659574468</v>
+        <v>0.14096916299559473</v>
       </c>
       <c r="N3" s="19" t="s">
         <v>10</v>
@@ -1875,7 +1878,7 @@
       </c>
       <c r="J4" s="24">
         <f>I4/$I$7</f>
-        <v>0.21276595744680851</v>
+        <v>0.22026431718061673</v>
       </c>
       <c r="N4" s="22" t="s">
         <v>6</v>
@@ -1915,7 +1918,7 @@
       </c>
       <c r="J5" s="32">
         <f>I5/$I$7</f>
-        <v>0.21276595744680851</v>
+        <v>0.22026431718061673</v>
       </c>
       <c r="N5" s="25" t="s">
         <v>7</v>
@@ -1952,7 +1955,7 @@
       </c>
       <c r="J6" s="26">
         <f>I6/$I$7</f>
-        <v>0.21276595744680851</v>
+        <v>0.22026431718061673</v>
       </c>
       <c r="O6" s="27">
         <v>315</v>
@@ -1977,7 +1980,7 @@
       </c>
       <c r="I7" s="27">
         <f>SUM(I2:I6)</f>
-        <v>470</v>
+        <v>454</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -2092,7 +2095,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2225,7 +2228,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I24" s="11"/>
     </row>
@@ -2345,7 +2348,7 @@
         <v>10</v>
       </c>
       <c r="F32" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I32" s="11"/>
     </row>
@@ -2441,10 +2444,10 @@
       <c r="E37" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="14">
-        <v>4</v>
-      </c>
-      <c r="G37" s="11"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="11" t="s">
+        <v>130</v>
+      </c>
       <c r="H37" s="11"/>
       <c r="L37" s="11"/>
       <c r="M37" s="11"/>
@@ -2497,7 +2500,7 @@
         <v>7</v>
       </c>
       <c r="F41" s="21">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -2511,7 +2514,7 @@
         <v>10</v>
       </c>
       <c r="F42" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -2539,7 +2542,7 @@
         <v>10</v>
       </c>
       <c r="F44" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -2553,7 +2556,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="21">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -2567,7 +2570,7 @@
         <v>10</v>
       </c>
       <c r="F46" s="14">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finalize schedule, move syllabus to help page
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MATH615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866A44AD-7150-4D01-A0DF-F1F5D8343D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041D74CD-FC2F-46CC-BB92-037EF21A126F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="127">
   <si>
     <t>Assignments</t>
   </si>
@@ -55,9 +55,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>Slack Introductions</t>
-  </si>
-  <si>
     <t>Exam</t>
   </si>
   <si>
@@ -103,21 +100,6 @@
     <t>05 Bivariate graphing</t>
   </si>
   <si>
-    <t>08 Bivariate Inference</t>
-  </si>
-  <si>
-    <t>PR Poster prep II</t>
-  </si>
-  <si>
-    <t>09 Moderation</t>
-  </si>
-  <si>
-    <t>10 Regression</t>
-  </si>
-  <si>
-    <t>PR Poster prep III</t>
-  </si>
-  <si>
     <t>Poster Draft</t>
   </si>
   <si>
@@ -133,36 +115,6 @@
     <t>wknum</t>
   </si>
   <si>
-    <t>PR 02</t>
-  </si>
-  <si>
-    <t>PR 03</t>
-  </si>
-  <si>
-    <t>PR 04</t>
-  </si>
-  <si>
-    <t>PR PP1</t>
-  </si>
-  <si>
-    <t>PR 05</t>
-  </si>
-  <si>
-    <t>PR 06</t>
-  </si>
-  <si>
-    <t>PR Poster prep IV</t>
-  </si>
-  <si>
-    <t>PR 09</t>
-  </si>
-  <si>
-    <t>PR 10</t>
-  </si>
-  <si>
-    <t>PR 08</t>
-  </si>
-  <si>
     <t>01 Data Structure and Entry</t>
   </si>
   <si>
@@ -214,9 +166,6 @@
     <t>Quiz 12</t>
   </si>
   <si>
-    <t>Quiz 13</t>
-  </si>
-  <si>
     <t>04 Univariate Graphics</t>
   </si>
   <si>
@@ -238,31 +187,13 @@
     <t>Project Stage IV: Multivariable Analysis &amp; Conclusions</t>
   </si>
   <si>
-    <t>Poster prep Stage IV* (Draft Due 12/03, PR 12/05, Final 12/07 )</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
-    <t>06 Research Proposal Outline</t>
-  </si>
-  <si>
-    <t>07 Foundations for Inference</t>
-  </si>
-  <si>
-    <t>Quiz 14</t>
-  </si>
-  <si>
     <t>03 RR / DM</t>
   </si>
   <si>
     <t>Describing relationships (Q~C, Q~Q)</t>
-  </si>
-  <si>
-    <t>Poster prep Stage III* (Draft Due 11/05, PR 11/07, Final 11/09 )</t>
-  </si>
-  <si>
-    <t>e-Poster*  (Draft Due 12/13 , PR 12/15, Final 12/19 10am )</t>
   </si>
   <si>
     <t>What to watch out for</t>
@@ -298,48 +229,12 @@
 [Lec01](https://hackmd.io/@norcalbiostat/math615_lec01)</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>[HW01 Data Entry](hw/01_data_entry.html) (Due 09/01 )</t>
-  </si>
-  <si>
-    <t>[HW02 RQ Formulation](hw/02_rq_formulation.html) (Draft Due 9/6, PR 9/7, Final 9/8 )</t>
-  </si>
-  <si>
     <t>[Lec02](https://hackmd.io/@norcalbiostat/math615_lec02)
 [ASCN Ch 1](https://norcalbiostat.github.io/AppliedStatistics_notes/data-prep.html)
 PMA6 Ch 3
 [Lec03](https://hackmd.io/@norcalbiostat/math615_lec03)</t>
   </si>
   <si>
-    <t>[[Quiz 02]](https://forms.gle/oowUHf421qFPS7Eu7) (Due 09/09 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 01]](https://forms.gle/KaKtWNULi58BX37y5) (Due 09/02 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 03]](https://forms.gle/P7hah7kJJidU3z2TA) (Due 09/16 )</t>
-  </si>
-  <si>
-    <t>[HW04 Describing Data Univariately](hw/04_univariate_graphing.html) (Draft Due 9/20, PR 9/21, Final 9/22 )</t>
-  </si>
-  <si>
-    <t>[HW03 Data Management](hw/03_data_management.html) (Due 9/15 ) PR removed due to illness</t>
-  </si>
-  <si>
-    <t>[Poster prep Stage I](project.html) (Draft Due 9/24, PR 9/26, Final 9/28 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 04]](https://forms.gle/8tLFYadDErC9h7499) (Due 09/23 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 05]](https://forms.gle/JCiibRkibNnaJgY79) (Due 09/30 )</t>
-  </si>
-  <si>
-    <t>[HW05 Graphing Relationships](hw/05_bivariate_graphing_assignment.html) (Draft Due 9/27, PR 9/28, Final 9/29 )</t>
-  </si>
-  <si>
     <t>[Lec04](https://hackmd.io/@norcalbiostat/math615_lec04)</t>
   </si>
   <si>
@@ -348,23 +243,10 @@
 Quantifying Uncertainty</t>
   </si>
   <si>
-    <t>[Poster prep Stage II](project.html) (Draft Due 10/08, PR 10/10, Final 10/12 )</t>
-  </si>
-  <si>
     <t>[OpenIntro Statistics textbook Ch5](https://leanpub.com/openintro-statistics) or Dr. D's [Math 315 course notes Ch4](https://norcalbiostat.github.io/MATH315/reading/RAD_course_notes_f19.pdf) 
 [Lec05](https://hackmd.io/@norcalbiostat/math615_lec05)</t>
   </si>
   <si>
-    <t>[[Quiz 06]](https://forms.gle/vxFAYZbzsRdGRf487)(Due 10/09 )</t>
-  </si>
-  <si>
-    <t>[HW07 Foundations for Inference](hw/07_foundations.html) and  
-[Interval Estimation Activity](hw/activity_interval_estimation.docx) (Due 10/10 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 07]](https://forms.gle/oQ85KTf6b3rH6C7cA) (Due 10/14 )</t>
-  </si>
-  <si>
     <t>Interval Estimation 
 Hypothesis testing Foundations</t>
   </si>
@@ -374,9 +256,6 @@
   <si>
     <t>PMA5 Ch 4 [Lec07](https://hackmd.io/@norcalbiostat/math615_lec07)
 PMA5 Ch 5 [Lec08](https://hackmd.io/@norcalbiostat/math615_lec08)</t>
-  </si>
-  <si>
-    <t>[HW08 Bivariate Inference](hw/08_bivariate_inference.html) (Draft Due 10/31, PR 11/02, Final 11/04 )</t>
   </si>
   <si>
     <t>ANOVA
@@ -392,15 +271,6 @@
 Regression analysis</t>
   </si>
   <si>
-    <t>Quiz includes T-tests</t>
-  </si>
-  <si>
-    <t>[[Quiz 08]](https://forms.gle/csRZSV4CA2d9BeVU8) (Due 10/28 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 09]](https://forms.gle/1Qx4LKfLDRCu5HwaA) (Due 11/04 )</t>
-  </si>
-  <si>
     <t>PMA5 Ch 6
 ASCN Ch 7</t>
   </si>
@@ -409,9 +279,6 @@
 ASCN Ch 10</t>
   </si>
   <si>
-    <t>[HW 09 Moderation](hw/09_moderation.html) (Draft Due 11/07, PR 11/09, Final 11/11 )</t>
-  </si>
-  <si>
     <t>ASCN 9.2, 9.3</t>
   </si>
   <si>
@@ -419,16 +286,10 @@
 Study Design &amp; Causation</t>
   </si>
   <si>
-    <t>Thursday 12/19, 10-12 noon. THMA 116  I'll bring snacks!</t>
-  </si>
-  <si>
     <t>Stratification
 Moderation</t>
   </si>
   <si>
-    <t>[[Quiz 10]](https://forms.gle/VUjPT5yMzPbexGmd6) (Due 11/11 )</t>
-  </si>
-  <si>
     <t>PMA5 Ch 7
 ASCN Ch 8, 9.5</t>
   </si>
@@ -448,19 +309,145 @@
     <t>PMA6 Ch 10.2, 10.5</t>
   </si>
   <si>
-    <t>[HW10 Regression](hw/10_MLR_confounding.html) (Draft Due 11/22, PR 11/23, Final 11/24 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 11]](https://forms.gle/a6nfb4UGuhworGtU7) (Due 11/20 )</t>
-  </si>
-  <si>
-    <t>[[Quiz 12]](https://forms.gle/AWATge25tb4gPcvW8) (Due 12/04 )</t>
-  </si>
-  <si>
-    <t>Take home final exam (Due 12/20 )</t>
-  </si>
-  <si>
-    <t>EC</t>
+    <t>03 PR</t>
+  </si>
+  <si>
+    <t>04 PR</t>
+  </si>
+  <si>
+    <t>05 PR</t>
+  </si>
+  <si>
+    <t>06 Foundations for Inference</t>
+  </si>
+  <si>
+    <t>07 Bivariate Inference</t>
+  </si>
+  <si>
+    <t>07 PR</t>
+  </si>
+  <si>
+    <t>08 Moderation</t>
+  </si>
+  <si>
+    <t>08 PR</t>
+  </si>
+  <si>
+    <t>09 PR</t>
+  </si>
+  <si>
+    <t>09 Multiple Regression</t>
+  </si>
+  <si>
+    <t>10 GLM and Categorical Predictors</t>
+  </si>
+  <si>
+    <t>10 PR</t>
+  </si>
+  <si>
+    <t>02 PR</t>
+  </si>
+  <si>
+    <t>PP I: PR</t>
+  </si>
+  <si>
+    <t>PP II: PR</t>
+  </si>
+  <si>
+    <t>PP III: PR</t>
+  </si>
+  <si>
+    <t>PP IV: PR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monday 6pm-8pm. I will work to get this changed. </t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>[HW01 Data Entry](hw/01_data_entry.html)</t>
+  </si>
+  <si>
+    <t>[HW02 RQ Formulation](hw/02_rq_formulation.html)</t>
+  </si>
+  <si>
+    <t>[HW03 Data Management](hw/03_data_management.html)</t>
+  </si>
+  <si>
+    <t>[HW04 Describing Data Univariately](hw/04_univariate_graphing.html)</t>
+  </si>
+  <si>
+    <t>[HW05 Graphing Relationships](hw/05_bivariate_graphing_assignment.html)</t>
+  </si>
+  <si>
+    <t>[Poster prep Stage I](project.html)</t>
+  </si>
+  <si>
+    <t>[HW06 Foundations for Inference](hw/06_foundations.html)</t>
+  </si>
+  <si>
+    <t>[Poster prep Stage II](project.html)</t>
+  </si>
+  <si>
+    <t>[HW07 Bivariate Inference](hw/07_bivariate_inference.html)</t>
+  </si>
+  <si>
+    <t>[[Quiz 2]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 1]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 3]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 4]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 5]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 6]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 7]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 8]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 09]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 10]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 11]]()</t>
+  </si>
+  <si>
+    <t>[[Quiz 12]]()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poster prep Stage IV* </t>
+  </si>
+  <si>
+    <t>[HW10 GLM &amp; Categorical](hw/10_GLM_catpreds.html)</t>
+  </si>
+  <si>
+    <t>Take home final exam</t>
+  </si>
+  <si>
+    <t>[HW09 Multiple Regression](hw/09_MLR_confounding.html)</t>
+  </si>
+  <si>
+    <t>[HW 08 Moderation](hw/08_moderation.html)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage III*</t>
+  </si>
+  <si>
+    <t>Poster*</t>
   </si>
 </sst>
 </file>
@@ -615,7 +602,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFE6D6BA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,7 +730,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="81" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,12 +811,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="78" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -861,8 +842,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -952,6 +942,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE6D6BA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1285,47 +1280,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="D12" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.875" style="2"/>
     <col min="3" max="3" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="31.625" style="37" customWidth="1"/>
-    <col min="5" max="5" width="25.125" style="37" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="79.625" style="37" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="37"/>
+    <col min="4" max="4" width="31.625" style="35" customWidth="1"/>
+    <col min="5" max="6" width="25.125" style="35" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="79.625" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="8.875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1.1000000000000001</v>
       </c>
@@ -1333,19 +1331,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2.1</v>
       </c>
@@ -1353,19 +1351,20 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3.1</v>
       </c>
@@ -1373,20 +1372,21 @@
         <v>3</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="37" t="s">
-        <v>13</v>
+      <c r="D4" s="35" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -1394,52 +1394,55 @@
         <v>4</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>72</v>
+      <c r="D6" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5.2</v>
       </c>
-      <c r="D7" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="D7" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6.1</v>
       </c>
@@ -1447,19 +1450,20 @@
         <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7.1</v>
       </c>
@@ -1467,30 +1471,32 @@
         <v>7</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="40"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7.3</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="D10" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8.1</v>
       </c>
@@ -1498,17 +1504,18 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9.1</v>
       </c>
@@ -1516,16 +1523,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10.1</v>
       </c>
@@ -1533,29 +1537,31 @@
         <v>10</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>10.199999999999999</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D14" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>11.1</v>
       </c>
@@ -1563,19 +1569,19 @@
         <v>11</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="40" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>12.1</v>
       </c>
@@ -1583,58 +1589,65 @@
         <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F16" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>13.1</v>
       </c>
       <c r="B17" s="2">
         <v>13</v>
       </c>
-      <c r="D17" s="37" t="s">
-        <v>63</v>
+      <c r="D17" s="35" t="s">
+        <v>46</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>13.2</v>
       </c>
-      <c r="D18" s="37" t="s">
-        <v>16</v>
+      <c r="D18" s="35" t="s">
+        <v>15</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>14.1</v>
       </c>
-      <c r="D19" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="39"/>
-    </row>
-    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D19" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>15.1</v>
       </c>
@@ -1642,37 +1655,40 @@
         <v>14</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>122</v>
+        <v>76</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>15.2</v>
       </c>
-      <c r="D21" s="37" t="s">
-        <v>75</v>
+      <c r="D21" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>15.3</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D22" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>16.100000000000001</v>
       </c>
@@ -1680,39 +1696,39 @@
         <v>15</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" s="37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>17.100000000000001</v>
       </c>
       <c r="B24" s="2">
         <v>16</v>
       </c>
-      <c r="D24" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D24" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>17.2</v>
       </c>
-      <c r="D25" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>129</v>
+      <c r="D25" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H25">
     <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1722,20 +1738,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.875" style="12"/>
-    <col min="2" max="2" width="36.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="12"/>
+    <col min="2" max="2" width="36.875" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="12"/>
+    <col min="5" max="5" width="13.375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.125" style="11" customWidth="1"/>
     <col min="8" max="8" width="13.5" style="11" customWidth="1"/>
     <col min="9" max="9" width="10" style="12" customWidth="1"/>
@@ -1744,24 +1760,24 @@
     <col min="12" max="16384" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>3</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>2</v>
@@ -1772,615 +1788,660 @@
       <c r="J1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="T1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="14">
-        <v>2</v>
+      <c r="B2" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="18">
+        <v>10</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="16">
-        <f>SUMIF($E$2:$E$89,H2,$F$2:$F$89)</f>
-        <v>90</v>
+        <f>SUMIF($C$2:$C$86,H2,$D$2:$D$86)</f>
+        <v>100</v>
       </c>
       <c r="J2" s="17">
         <f>I2/$I$7</f>
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="16">
+        <v>90</v>
+      </c>
+      <c r="R2" s="17">
         <v>0.19823788546255505</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="16">
+      <c r="U2" s="16">
         <v>35</v>
       </c>
-      <c r="P2" s="17">
+      <c r="V2" s="17">
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <v>1.2</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="29">
         <v>10</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" s="14">
-        <f>SUMIF($E$2:$E$89,H3,$F$2:$F$89)</f>
-        <v>64</v>
+        <f>SUMIF($C$2:$C$86,H3,$D$2:$D$86)</f>
+        <v>60</v>
       </c>
       <c r="J3" s="20">
         <f>I3/$I$7</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>64</v>
+      </c>
+      <c r="R3" s="20">
         <v>0.14096916299559473</v>
       </c>
-      <c r="N3" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="14">
+      <c r="T3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="14">
         <v>40</v>
       </c>
-      <c r="P3" s="20">
+      <c r="V3" s="20">
         <v>0.12698412698412698</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <v>1.3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="31">
+        <v>2</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18">
         <v>10</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" s="23">
-        <f>SUMIF($E$2:$E$89,H4,$F$2:$F$89)</f>
-        <v>100</v>
+        <f>SUMIF($C$2:$C$86,H4,$D$2:$D$86)</f>
+        <v>50</v>
       </c>
       <c r="J4" s="24">
         <f>I4/$I$7</f>
+        <v>0.11904761904761904</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>100</v>
+      </c>
+      <c r="R4" s="24">
         <v>0.22026431718061673</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="T4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="23">
+        <v>100</v>
+      </c>
+      <c r="V4" s="24">
+        <v>0.31746031746031744</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="29">
+        <f>SUMIF($C$2:$C$86,H5,$D$2:$D$86)-10</f>
+        <v>110</v>
+      </c>
+      <c r="J5" s="30">
+        <f>I5/$I$7</f>
+        <v>0.26190476190476192</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="29">
+        <v>100</v>
+      </c>
+      <c r="R5" s="30">
+        <v>0.22026431718061673</v>
+      </c>
+      <c r="T5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="23">
-        <v>100</v>
-      </c>
-      <c r="P4" s="24">
-        <v>0.31746031746031744</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>2</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="18">
-        <v>10</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="31">
-        <f>SUMIF($E$2:$E$89,H5,$F$2:$F$89)-2*10</f>
-        <v>100</v>
-      </c>
-      <c r="J5" s="32">
-        <f>I5/$I$7</f>
-        <v>0.22026431718061673</v>
-      </c>
-      <c r="N5" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="21">
+      <c r="U5" s="21">
         <v>140</v>
       </c>
-      <c r="P5" s="26">
+      <c r="V5" s="26">
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2.1</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="14">
-        <v>4</v>
+      <c r="C6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="29">
+        <v>10</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="21">
-        <f>SUMIF($E$2:$E$89,H6,$F$2:$F$89)</f>
+        <f>SUMIF($C$2:$C$86,H6,$D$2:$D$86)</f>
         <v>100</v>
       </c>
       <c r="J6" s="26">
         <f>I6/$I$7</f>
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>100</v>
+      </c>
+      <c r="R6" s="26">
         <v>0.22026431718061673</v>
       </c>
-      <c r="O6" s="27">
+      <c r="U6" s="27">
         <v>315</v>
       </c>
-      <c r="P6" s="12"/>
-    </row>
-    <row r="7" spans="1:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V6" s="12"/>
+    </row>
+    <row r="7" spans="1:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="31">
+        <v>3</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18">
         <v>10</v>
       </c>
       <c r="I7" s="27">
         <f>SUM(I2:I6)</f>
+        <v>420</v>
+      </c>
+      <c r="Q7" s="27">
+        <f>SUM(Q2:Q6)</f>
         <v>454</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="12"/>
+    </row>
+    <row r="8" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
+        <v>3.2</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="14">
         <v>3</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>3.1</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="14">
+      <c r="C9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>3.1</v>
-      </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>3.2</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
-        <v>4</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="18" t="s">
+        <v>4.2</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>4.3</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>5</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>4.2</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="31">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>4.3</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
-        <v>5</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="18">
-        <v>10</v>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="14">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="14">
-        <v>4</v>
+        <v>5.2</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="29">
+        <v>10</v>
       </c>
       <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
-        <v>5.2</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="31">
+        <v>6.1</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="29">
         <v>10</v>
       </c>
       <c r="I18" s="11"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
-        <v>6</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="18" t="s">
+        <v>6.2</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="D19" s="18">
+        <v>10</v>
+      </c>
       <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
-        <v>6.1</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="14">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="21">
+        <v>20</v>
       </c>
       <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
-        <v>6.2</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="31">
-        <v>10</v>
+        <v>7.1</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="44">
+        <v>6</v>
       </c>
       <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
-        <v>7</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="18">
+        <v>7.2</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="29">
         <v>10</v>
       </c>
       <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
-        <v>7.1</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="21">
-        <v>20</v>
+        <v>7.3</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="18">
+        <v>10</v>
       </c>
       <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
-        <v>7.2</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="14">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="14">
+        <v>3</v>
       </c>
       <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
-        <v>7.3</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="31">
+        <v>8.1</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="29">
         <v>10</v>
       </c>
       <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
-        <v>8</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="18">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="29">
         <v>10</v>
       </c>
       <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
-        <v>8.1</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="14">
-        <v>4</v>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="29">
+        <v>10</v>
       </c>
       <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="31">
-        <v>10</v>
+        <v>8.4</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="21">
+        <v>20</v>
       </c>
       <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="31">
-        <v>10</v>
+        <v>8.5</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="44">
+        <v>6</v>
       </c>
       <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
-        <v>8.4</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="31">
+        <v>8.6</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="18">
         <v>10</v>
       </c>
       <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
-        <v>8.5</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="21">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="14">
+        <v>3</v>
       </c>
       <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
-        <v>8.6</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="14">
-        <v>4</v>
+        <v>9.1</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="29">
+        <v>10</v>
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
-        <v>9</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="18" t="s">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F33" s="18">
-        <v>10</v>
-      </c>
-      <c r="I33" s="11"/>
+      <c r="D33" s="18">
+        <v>10</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
     </row>
     <row r="34" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
-        <v>9.1</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="14">
-        <v>4</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="14">
+        <v>3</v>
+      </c>
+      <c r="F34" s="13"/>
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="L34" s="11"/>
@@ -2391,18 +2452,18 @@
     </row>
     <row r="35" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="31">
-        <v>10</v>
-      </c>
+        <v>10.1</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="29">
+        <v>10</v>
+      </c>
+      <c r="F35" s="13"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="L35" s="11"/>
@@ -2413,18 +2474,18 @@
     </row>
     <row r="36" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
-        <v>10</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="18" t="s">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F36" s="18">
-        <v>10</v>
-      </c>
+      <c r="D36" s="18">
+        <v>10</v>
+      </c>
+      <c r="F36" s="13"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="L36" s="11"/>
@@ -2433,162 +2494,154 @@
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
     </row>
-    <row r="37" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
-        <v>10.1</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="21">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="31">
-        <v>10</v>
+        <v>10.5</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="44">
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
-        <v>10.3</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
+        <v>10.6</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="21">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
-        <v>10.4</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
+        <v>11</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
-        <v>10.5</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="21">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="44">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
-        <v>10.6</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="14">
-        <v>4</v>
+        <v>11.2</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="21">
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
-        <v>11</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E43" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="21">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="44">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
-        <v>11.2</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="12">
-        <v>12</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="21" t="s">
+        <v>12.1</v>
+      </c>
+      <c r="B44" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="12">
-        <v>12.1</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="12">
-        <v>13</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D52" s="13"/>
+      <c r="C44" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="42"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+    </row>
+    <row r="50" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="42"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+    </row>
+    <row r="51" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="42"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+    </row>
+    <row r="52" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="42"/>
+      <c r="F52" s="13"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
       <c r="L52" s="11"/>
@@ -2597,8 +2650,9 @@
       <c r="O52" s="11"/>
       <c r="P52" s="11"/>
     </row>
-    <row r="53" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="13"/>
+    <row r="53" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="42"/>
+      <c r="F53" s="13"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
       <c r="L53" s="11"/>
@@ -2607,8 +2661,9 @@
       <c r="O53" s="11"/>
       <c r="P53" s="11"/>
     </row>
-    <row r="54" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D54" s="13"/>
+    <row r="54" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="42"/>
+      <c r="F54" s="13"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
       <c r="L54" s="11"/>
@@ -2617,8 +2672,9 @@
       <c r="O54" s="11"/>
       <c r="P54" s="11"/>
     </row>
-    <row r="55" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D55" s="13"/>
+    <row r="55" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="42"/>
+      <c r="F55" s="13"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="L55" s="11"/>
@@ -2627,8 +2683,9 @@
       <c r="O55" s="11"/>
       <c r="P55" s="11"/>
     </row>
-    <row r="56" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D56" s="13"/>
+    <row r="56" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="42"/>
+      <c r="F56" s="13"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="L56" s="11"/>
@@ -2637,8 +2694,9 @@
       <c r="O56" s="11"/>
       <c r="P56" s="11"/>
     </row>
-    <row r="57" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="13"/>
+    <row r="57" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="42"/>
+      <c r="F57" s="13"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="L57" s="11"/>
@@ -2647,8 +2705,9 @@
       <c r="O57" s="11"/>
       <c r="P57" s="11"/>
     </row>
-    <row r="58" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="13"/>
+    <row r="58" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="42"/>
+      <c r="F58" s="13"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="L58" s="11"/>
@@ -2657,8 +2716,9 @@
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
     </row>
-    <row r="59" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D59" s="13"/>
+    <row r="59" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="42"/>
+      <c r="F59" s="13"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="L59" s="11"/>
@@ -2667,8 +2727,9 @@
       <c r="O59" s="11"/>
       <c r="P59" s="11"/>
     </row>
-    <row r="60" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D60" s="13"/>
+    <row r="60" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="42"/>
+      <c r="F60" s="13"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="L60" s="11"/>
@@ -2677,8 +2738,9 @@
       <c r="O60" s="11"/>
       <c r="P60" s="11"/>
     </row>
-    <row r="61" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D61" s="13"/>
+    <row r="61" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="42"/>
+      <c r="F61" s="13"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
       <c r="L61" s="11"/>
@@ -2687,8 +2749,9 @@
       <c r="O61" s="11"/>
       <c r="P61" s="11"/>
     </row>
-    <row r="62" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D62" s="13"/>
+    <row r="62" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="42"/>
+      <c r="F62" s="13"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
       <c r="L62" s="11"/>
@@ -2697,8 +2760,9 @@
       <c r="O62" s="11"/>
       <c r="P62" s="11"/>
     </row>
-    <row r="63" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D63" s="13"/>
+    <row r="63" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="42"/>
+      <c r="F63" s="13"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
       <c r="L63" s="11"/>
@@ -2707,8 +2771,9 @@
       <c r="O63" s="11"/>
       <c r="P63" s="11"/>
     </row>
-    <row r="64" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D64" s="13"/>
+    <row r="64" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="42"/>
+      <c r="F64" s="13"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
       <c r="L64" s="11"/>
@@ -2717,38 +2782,46 @@
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
     </row>
-    <row r="65" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="13"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="11"/>
-      <c r="N65" s="11"/>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-    </row>
-    <row r="66" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D66" s="13"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="L66" s="11"/>
-      <c r="M66" s="11"/>
-      <c r="N66" s="11"/>
-      <c r="O66" s="11"/>
-      <c r="P66" s="11"/>
-    </row>
-    <row r="67" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D67" s="13"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="11"/>
-      <c r="N67" s="11"/>
-      <c r="O67" s="11"/>
-      <c r="P67" s="11"/>
-    </row>
-    <row r="84" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D84" s="13"/>
+    <row r="81" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="42"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
+      <c r="L81" s="11"/>
+      <c r="M81" s="11"/>
+      <c r="N81" s="11"/>
+      <c r="O81" s="11"/>
+      <c r="P81" s="11"/>
+    </row>
+    <row r="82" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="42"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="L82" s="11"/>
+      <c r="M82" s="11"/>
+      <c r="N82" s="11"/>
+      <c r="O82" s="11"/>
+      <c r="P82" s="11"/>
+    </row>
+    <row r="83" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="42"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="L83" s="11"/>
+      <c r="M83" s="11"/>
+      <c r="N83" s="11"/>
+      <c r="O83" s="11"/>
+      <c r="P83" s="11"/>
+    </row>
+    <row r="84" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="42"/>
+      <c r="F84" s="13"/>
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11"/>
@@ -2759,18 +2832,22 @@
       <c r="O84" s="11"/>
       <c r="P84" s="11"/>
     </row>
-    <row r="85" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D85" s="13"/>
+    <row r="85" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="42"/>
+      <c r="F85" s="13"/>
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="11"/>
       <c r="L85" s="11"/>
       <c r="M85" s="11"/>
       <c r="N85" s="11"/>
       <c r="O85" s="11"/>
       <c r="P85" s="11"/>
     </row>
-    <row r="86" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D86" s="13"/>
+    <row r="86" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="42"/>
+      <c r="F86" s="13"/>
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
@@ -2781,8 +2858,9 @@
       <c r="O86" s="11"/>
       <c r="P86" s="11"/>
     </row>
-    <row r="87" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D87" s="13"/>
+    <row r="87" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="42"/>
+      <c r="F87" s="13"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
@@ -2793,8 +2871,9 @@
       <c r="O87" s="11"/>
       <c r="P87" s="11"/>
     </row>
-    <row r="88" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D88" s="13"/>
+    <row r="88" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="42"/>
+      <c r="F88" s="13"/>
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="11"/>
@@ -2805,8 +2884,9 @@
       <c r="O88" s="11"/>
       <c r="P88" s="11"/>
     </row>
-    <row r="89" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D89" s="13"/>
+    <row r="89" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="42"/>
+      <c r="F89" s="13"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="11"/>
@@ -2817,8 +2897,9 @@
       <c r="O89" s="11"/>
       <c r="P89" s="11"/>
     </row>
-    <row r="90" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D90" s="13"/>
+    <row r="90" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="42"/>
+      <c r="F90" s="13"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="11"/>
@@ -2829,44 +2910,42 @@
       <c r="O90" s="11"/>
       <c r="P90" s="11"/>
     </row>
-    <row r="91" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D91" s="13"/>
+    <row r="91" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="42"/>
+      <c r="F91" s="13"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
       <c r="L91" s="11"/>
       <c r="M91" s="11"/>
       <c r="N91" s="11"/>
       <c r="O91" s="11"/>
       <c r="P91" s="11"/>
     </row>
-    <row r="92" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D92" s="13"/>
+    <row r="92" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="42"/>
+      <c r="F92" s="13"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="11"/>
       <c r="L92" s="11"/>
       <c r="M92" s="11"/>
       <c r="N92" s="11"/>
       <c r="O92" s="11"/>
       <c r="P92" s="11"/>
     </row>
-    <row r="93" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D93" s="13"/>
+    <row r="93" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="42"/>
+      <c r="F93" s="13"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="11"/>
       <c r="L93" s="11"/>
       <c r="M93" s="11"/>
       <c r="N93" s="11"/>
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D94" s="13"/>
+    <row r="94" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="42"/>
+      <c r="F94" s="13"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
       <c r="L94" s="11"/>
@@ -2875,8 +2954,9 @@
       <c r="O94" s="11"/>
       <c r="P94" s="11"/>
     </row>
-    <row r="95" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D95" s="13"/>
+    <row r="95" spans="2:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="42"/>
+      <c r="F95" s="13"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
       <c r="L95" s="11"/>
@@ -2885,39 +2965,9 @@
       <c r="O95" s="11"/>
       <c r="P95" s="11"/>
     </row>
-    <row r="96" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D96" s="13"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="L96" s="11"/>
-      <c r="M96" s="11"/>
-      <c r="N96" s="11"/>
-      <c r="O96" s="11"/>
-      <c r="P96" s="11"/>
-    </row>
-    <row r="97" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D97" s="13"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="L97" s="11"/>
-      <c r="M97" s="11"/>
-      <c r="N97" s="11"/>
-      <c r="O97" s="11"/>
-      <c r="P97" s="11"/>
-    </row>
-    <row r="98" spans="4:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D98" s="13"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="L98" s="11"/>
-      <c r="M98" s="11"/>
-      <c r="N98" s="11"/>
-      <c r="O98" s="11"/>
-      <c r="P98" s="11"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F101">
-    <sortCondition ref="A2:A101"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D100">
+    <sortCondition ref="A2:A100"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>